<commit_message>
adding base capacity planning functionality
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
   <si>
     <t>NumBuses</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>UnitsByBus</t>
-  </si>
-  <si>
-    <t>Total</t>
   </si>
   <si>
     <t>NumYears</t>
@@ -219,14 +216,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S71"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +546,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6">
         <v>26</v>
@@ -569,23 +566,23 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="12">
+        <v>31</v>
+      </c>
+      <c r="B7" s="11">
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
-        <v>31</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
@@ -1084,17 +1081,17 @@
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="2"/>
-      <c r="G40" s="10" t="s">
+      <c r="G40" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
       <c r="J40" s="2"/>
       <c r="K40" s="4"/>
       <c r="N40" s="4"/>
@@ -1297,11 +1294,11 @@
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
       <c r="Q48" t="s">
         <v>18</v>
       </c>
@@ -2253,15 +2250,6 @@
       <c r="R69" s="6">
         <f t="shared" si="5"/>
         <v>3.06</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="F71" t="s">
-        <v>28</v>
-      </c>
-      <c r="G71">
-        <f>SUM(MaxGen)</f>
-        <v>8894.6999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added emissions and total cost to output sheet
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -16,6 +16,8 @@
   </sheets>
   <definedNames>
     <definedName name="BusDemand">Sheet2!$B$11:$D$36</definedName>
+    <definedName name="CH4_rate">Sheet2!$X$50:$X$69</definedName>
+    <definedName name="CO2_rate">Sheet2!$W$50:$W$69</definedName>
     <definedName name="LineCapacity">Sheet2!$O$42:$O$44</definedName>
     <definedName name="LineFromBus">Sheet2!$G$42:$I$44</definedName>
     <definedName name="LineReactance">Sheet2!$L$42:$L$44</definedName>
@@ -23,10 +25,13 @@
     <definedName name="MarginalC">Sheet2!$M$50:$M$69</definedName>
     <definedName name="MaxGen">Sheet2!$G$50:$G$69</definedName>
     <definedName name="MinGen">Sheet2!$J$50:$J$69</definedName>
+    <definedName name="N2O_rate">Sheet2!$Y$50:$Y$69</definedName>
+    <definedName name="NOx_rate">Sheet2!$U$50:$U$69</definedName>
     <definedName name="NumBuses">Sheet2!$B$1</definedName>
     <definedName name="NumLines">Sheet2!$B$2</definedName>
     <definedName name="NumUnits">Sheet2!$B$3</definedName>
     <definedName name="NumYears">Sheet2!$B$4</definedName>
+    <definedName name="SO2_rate">Sheet2!$V$50:$V$69</definedName>
     <definedName name="UnitsByBus">Sheet2!$B$50:$D$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
   <si>
     <t>NumBuses</t>
   </si>
@@ -135,6 +140,30 @@
   </si>
   <si>
     <t>Annual Demand Growth</t>
+  </si>
+  <si>
+    <t>Annual NOx total output emission rate (lb/MWh)</t>
+  </si>
+  <si>
+    <t>Annual SO2 total output emission rate (lb/MWh)</t>
+  </si>
+  <si>
+    <t>Annual CO2 total output emission rate (lb/MWh)</t>
+  </si>
+  <si>
+    <t>Annual CH4 total output emission rate (lb/MWh)</t>
+  </si>
+  <si>
+    <t>Annual N2O total output emission rate (lb/MWh)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Peak Hour? (Y/N)</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -195,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -213,17 +242,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -507,20 +548,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S69"/>
+  <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="K46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Y50" sqref="Y50:Y69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
     <col min="17" max="17" width="9.54296875" customWidth="1"/>
     <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="21" max="21" width="16.36328125" customWidth="1"/>
+    <col min="22" max="23" width="16.26953125" customWidth="1"/>
+    <col min="24" max="24" width="16.1796875" customWidth="1"/>
+    <col min="25" max="25" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -528,51 +574,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="6">
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="6">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6">
-        <v>4765</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="11">
-        <v>8.9999999999999993E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
@@ -580,8 +630,8 @@
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="2">
@@ -593,477 +643,557 @@
       <c r="D10" s="2">
         <v>3</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>2020</v>
       </c>
       <c r="B11" s="7">
-        <f>0.15*B5</f>
+        <f>0.15*E11</f>
         <v>714.75</v>
       </c>
       <c r="C11" s="7">
-        <f>0.5*B5</f>
+        <f>0.5*E11</f>
         <v>2382.5</v>
       </c>
       <c r="D11" s="7">
-        <f>0.35*B5</f>
+        <f>0.35*E11</f>
         <v>1667.75</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E11" s="2">
+        <f>F2</f>
+        <v>4765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>2021</v>
       </c>
       <c r="B12" s="7">
-        <f>B11*(1+$B$7)</f>
-        <v>721.18274999999994</v>
+        <f t="shared" ref="B12:B36" si="0">0.15*E12</f>
+        <v>721.18274999999983</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" ref="C12:D12" si="0">C11*(1+$B$7)</f>
+        <f t="shared" ref="C12:C36" si="1">0.5*E12</f>
         <v>2403.9424999999997</v>
       </c>
       <c r="D12" s="7">
-        <f t="shared" si="0"/>
-        <v>1682.7597499999999</v>
-      </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" ref="D12:D36" si="2">0.35*E12</f>
+        <v>1682.7597499999997</v>
+      </c>
+      <c r="E12" s="16">
+        <f>E11*(1+$F$3)</f>
+        <v>4807.8849999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>2022</v>
       </c>
       <c r="B13" s="7">
-        <f t="shared" ref="B13:B36" si="1">B12*(1+$B$7)</f>
+        <f t="shared" si="0"/>
         <v>727.67339474999983</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:C36" si="2">C12*(1+$B$7)</f>
+        <f t="shared" si="1"/>
         <v>2425.5779824999995</v>
       </c>
       <c r="D13" s="7">
-        <f t="shared" ref="D13:D36" si="3">D12*(1+$B$7)</f>
-        <v>1697.9045877499998</v>
-      </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <f t="shared" si="2"/>
+        <v>1697.9045877499996</v>
+      </c>
+      <c r="E13" s="16">
+        <f>E12*(1+$F$3)</f>
+        <v>4851.155964999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>2023</v>
       </c>
       <c r="B14" s="7">
+        <f t="shared" si="0"/>
+        <v>734.22245530274972</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="1"/>
-        <v>734.22245530274972</v>
-      </c>
-      <c r="C14" s="7">
+        <v>2447.4081843424992</v>
+      </c>
+      <c r="D14" s="7">
         <f t="shared" si="2"/>
-        <v>2447.4081843424992</v>
-      </c>
-      <c r="D14" s="7">
-        <f t="shared" si="3"/>
-        <v>1713.1857290397495</v>
-      </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1713.1857290397493</v>
+      </c>
+      <c r="E14" s="16">
+        <f>E13*(1+$F$3)</f>
+        <v>4894.8163686849985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>2024</v>
       </c>
       <c r="B15" s="7">
+        <f t="shared" si="0"/>
+        <v>740.83045740047453</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="1"/>
-        <v>740.83045740047442</v>
-      </c>
-      <c r="C15" s="7">
+        <v>2469.4348580015817</v>
+      </c>
+      <c r="D15" s="7">
         <f t="shared" si="2"/>
-        <v>2469.4348580015817</v>
-      </c>
-      <c r="D15" s="7">
-        <f t="shared" si="3"/>
         <v>1728.604400601107</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E15" s="16">
+        <f>E14*(1+$F$3)</f>
+        <v>4938.8697160031634</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>2025</v>
       </c>
       <c r="B16" s="7">
+        <f t="shared" si="0"/>
+        <v>747.49793151707877</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="1"/>
-        <v>747.49793151707865</v>
-      </c>
-      <c r="C16" s="7">
+        <v>2491.6597717235959</v>
+      </c>
+      <c r="D16" s="7">
         <f t="shared" si="2"/>
-        <v>2491.6597717235959</v>
-      </c>
-      <c r="D16" s="7">
-        <f t="shared" si="3"/>
-        <v>1744.1618402065169</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>1744.1618402065171</v>
+      </c>
+      <c r="E16" s="16">
+        <f>E15*(1+$F$3)</f>
+        <v>4983.3195434471918</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>2026</v>
       </c>
       <c r="B17" s="7">
+        <f t="shared" si="0"/>
+        <v>754.22541290073241</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="1"/>
-        <v>754.22541290073229</v>
-      </c>
-      <c r="C17" s="7">
+        <v>2514.0847096691082</v>
+      </c>
+      <c r="D17" s="7">
         <f t="shared" si="2"/>
-        <v>2514.0847096691082</v>
-      </c>
-      <c r="D17" s="7">
-        <f t="shared" si="3"/>
-        <v>1759.8592967683753</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>1759.8592967683755</v>
+      </c>
+      <c r="E17" s="16">
+        <f>E16*(1+$F$3)</f>
+        <v>5028.1694193382164</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>2027</v>
       </c>
       <c r="B18" s="7">
+        <f t="shared" si="0"/>
+        <v>761.01344161683892</v>
+      </c>
+      <c r="C18" s="7">
         <f t="shared" si="1"/>
-        <v>761.0134416168388</v>
-      </c>
-      <c r="C18" s="7">
+        <v>2536.7114720561299</v>
+      </c>
+      <c r="D18" s="7">
         <f t="shared" si="2"/>
-        <v>2536.7114720561299</v>
-      </c>
-      <c r="D18" s="7">
-        <f t="shared" si="3"/>
-        <v>1775.6980304392905</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>1775.6980304392907</v>
+      </c>
+      <c r="E18" s="16">
+        <f>E17*(1+$F$3)</f>
+        <v>5073.4229441122598</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>2028</v>
       </c>
       <c r="B19" s="7">
+        <f t="shared" si="0"/>
+        <v>767.86256259139043</v>
+      </c>
+      <c r="C19" s="7">
         <f t="shared" si="1"/>
-        <v>767.86256259139031</v>
-      </c>
-      <c r="C19" s="7">
+        <v>2559.5418753046347</v>
+      </c>
+      <c r="D19" s="7">
         <f t="shared" si="2"/>
-        <v>2559.5418753046347</v>
-      </c>
-      <c r="D19" s="7">
-        <f t="shared" si="3"/>
-        <v>1791.6793127132439</v>
-      </c>
-      <c r="E19" s="9"/>
+        <v>1791.6793127132441</v>
+      </c>
+      <c r="E19" s="16">
+        <f>E18*(1+$F$3)</f>
+        <v>5119.0837506092694</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>2029</v>
       </c>
       <c r="B20" s="7">
+        <f t="shared" si="0"/>
+        <v>774.77332565471283</v>
+      </c>
+      <c r="C20" s="7">
         <f t="shared" si="1"/>
-        <v>774.77332565471272</v>
-      </c>
-      <c r="C20" s="7">
+        <v>2582.5777521823761</v>
+      </c>
+      <c r="D20" s="7">
         <f t="shared" si="2"/>
-        <v>2582.5777521823761</v>
-      </c>
-      <c r="D20" s="7">
-        <f t="shared" si="3"/>
-        <v>1807.8044265276628</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>1807.8044265276631</v>
+      </c>
+      <c r="E20" s="16">
+        <f>E19*(1+$F$3)</f>
+        <v>5165.1555043647522</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>2030</v>
       </c>
       <c r="B21" s="7">
+        <f t="shared" si="0"/>
+        <v>781.74628558560516</v>
+      </c>
+      <c r="C21" s="7">
         <f t="shared" si="1"/>
-        <v>781.74628558560505</v>
-      </c>
-      <c r="C21" s="7">
+        <v>2605.8209519520174</v>
+      </c>
+      <c r="D21" s="7">
         <f t="shared" si="2"/>
-        <v>2605.8209519520174</v>
-      </c>
-      <c r="D21" s="7">
-        <f t="shared" si="3"/>
-        <v>1824.0746663664115</v>
-      </c>
-      <c r="E21" s="9"/>
+        <v>1824.074666366412</v>
+      </c>
+      <c r="E21" s="16">
+        <f>E20*(1+$F$3)</f>
+        <v>5211.6419039040347</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>2031</v>
       </c>
       <c r="B22" s="7">
+        <f t="shared" si="0"/>
+        <v>788.7820021558756</v>
+      </c>
+      <c r="C22" s="7">
         <f t="shared" si="1"/>
-        <v>788.78200215587538</v>
-      </c>
-      <c r="C22" s="7">
+        <v>2629.2733405195854</v>
+      </c>
+      <c r="D22" s="7">
         <f t="shared" si="2"/>
-        <v>2629.2733405195854</v>
-      </c>
-      <c r="D22" s="7">
-        <f t="shared" si="3"/>
-        <v>1840.491338363709</v>
-      </c>
-      <c r="E22" s="9"/>
+        <v>1840.4913383637097</v>
+      </c>
+      <c r="E22" s="16">
+        <f>E21*(1+$F$3)</f>
+        <v>5258.5466810391708</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>2032</v>
       </c>
       <c r="B23" s="7">
+        <f t="shared" si="0"/>
+        <v>795.88104017527849</v>
+      </c>
+      <c r="C23" s="7">
         <f t="shared" si="1"/>
-        <v>795.88104017527814</v>
-      </c>
-      <c r="C23" s="7">
+        <v>2652.9368005842616</v>
+      </c>
+      <c r="D23" s="7">
         <f t="shared" si="2"/>
-        <v>2652.9368005842616</v>
-      </c>
-      <c r="D23" s="7">
-        <f t="shared" si="3"/>
-        <v>1857.0557604089822</v>
-      </c>
-      <c r="E23" s="9"/>
+        <v>1857.0557604089829</v>
+      </c>
+      <c r="E23" s="16">
+        <f>E22*(1+$F$3)</f>
+        <v>5305.8736011685232</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>2033</v>
       </c>
       <c r="B24" s="7">
+        <f t="shared" si="0"/>
+        <v>803.04396953685591</v>
+      </c>
+      <c r="C24" s="7">
         <f t="shared" si="1"/>
-        <v>803.04396953685557</v>
-      </c>
-      <c r="C24" s="7">
+        <v>2676.8132317895197</v>
+      </c>
+      <c r="D24" s="7">
         <f t="shared" si="2"/>
-        <v>2676.8132317895197</v>
-      </c>
-      <c r="D24" s="7">
-        <f t="shared" si="3"/>
-        <v>1873.7692622526629</v>
-      </c>
-      <c r="E24" s="9"/>
+        <v>1873.7692622526636</v>
+      </c>
+      <c r="E24" s="16">
+        <f>E23*(1+$F$3)</f>
+        <v>5353.6264635790394</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>2034</v>
       </c>
       <c r="B25" s="7">
+        <f t="shared" si="0"/>
+        <v>810.2713652626876</v>
+      </c>
+      <c r="C25" s="7">
         <f t="shared" si="1"/>
-        <v>810.27136526268714</v>
-      </c>
-      <c r="C25" s="7">
+        <v>2700.9045508756253</v>
+      </c>
+      <c r="D25" s="7">
         <f t="shared" si="2"/>
-        <v>2700.9045508756253</v>
-      </c>
-      <c r="D25" s="7">
-        <f t="shared" si="3"/>
-        <v>1890.6331856129366</v>
-      </c>
-      <c r="E25" s="9"/>
+        <v>1890.6331856129375</v>
+      </c>
+      <c r="E25" s="16">
+        <f>E24*(1+$F$3)</f>
+        <v>5401.8091017512506</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>2035</v>
       </c>
       <c r="B26" s="7">
+        <f t="shared" si="0"/>
+        <v>817.56380755005171</v>
+      </c>
+      <c r="C26" s="7">
         <f t="shared" si="1"/>
-        <v>817.56380755005125</v>
-      </c>
-      <c r="C26" s="7">
+        <v>2725.2126918335057</v>
+      </c>
+      <c r="D26" s="7">
         <f t="shared" si="2"/>
-        <v>2725.2126918335057</v>
-      </c>
-      <c r="D26" s="7">
-        <f t="shared" si="3"/>
-        <v>1907.6488842834528</v>
-      </c>
-      <c r="E26" s="9"/>
+        <v>1907.6488842834538</v>
+      </c>
+      <c r="E26" s="16">
+        <f>E25*(1+$F$3)</f>
+        <v>5450.4253836670114</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>2036</v>
       </c>
       <c r="B27" s="7">
+        <f t="shared" si="0"/>
+        <v>824.92188181800202</v>
+      </c>
+      <c r="C27" s="7">
         <f t="shared" si="1"/>
-        <v>824.92188181800168</v>
-      </c>
-      <c r="C27" s="7">
+        <v>2749.7396060600067</v>
+      </c>
+      <c r="D27" s="7">
         <f t="shared" si="2"/>
-        <v>2749.7396060600067</v>
-      </c>
-      <c r="D27" s="7">
-        <f t="shared" si="3"/>
-        <v>1924.8177242420038</v>
-      </c>
-      <c r="E27" s="9"/>
+        <v>1924.8177242420045</v>
+      </c>
+      <c r="E27" s="16">
+        <f>E26*(1+$F$3)</f>
+        <v>5499.4792121200135</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>2037</v>
       </c>
       <c r="B28" s="7">
+        <f t="shared" si="0"/>
+        <v>832.34617875436402</v>
+      </c>
+      <c r="C28" s="7">
         <f t="shared" si="1"/>
-        <v>832.34617875436356</v>
-      </c>
-      <c r="C28" s="7">
+        <v>2774.4872625145467</v>
+      </c>
+      <c r="D28" s="7">
         <f t="shared" si="2"/>
-        <v>2774.4872625145467</v>
-      </c>
-      <c r="D28" s="7">
-        <f t="shared" si="3"/>
-        <v>1942.1410837601816</v>
-      </c>
-      <c r="E28" s="9"/>
+        <v>1942.1410837601825</v>
+      </c>
+      <c r="E28" s="16">
+        <f>E27*(1+$F$3)</f>
+        <v>5548.9745250290935</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>2038</v>
       </c>
       <c r="B29" s="7">
+        <f t="shared" si="0"/>
+        <v>839.83729436315321</v>
+      </c>
+      <c r="C29" s="7">
         <f t="shared" si="1"/>
-        <v>839.83729436315275</v>
-      </c>
-      <c r="C29" s="7">
+        <v>2799.4576478771774</v>
+      </c>
+      <c r="D29" s="7">
         <f t="shared" si="2"/>
-        <v>2799.4576478771774</v>
-      </c>
-      <c r="D29" s="7">
-        <f t="shared" si="3"/>
-        <v>1959.620353514023</v>
-      </c>
-      <c r="E29" s="9"/>
+        <v>1959.6203535140239</v>
+      </c>
+      <c r="E29" s="16">
+        <f>E28*(1+$F$3)</f>
+        <v>5598.9152957543547</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>2039</v>
       </c>
       <c r="B30" s="7">
+        <f t="shared" si="0"/>
+        <v>847.39583001242147</v>
+      </c>
+      <c r="C30" s="7">
         <f t="shared" si="1"/>
-        <v>847.39583001242102</v>
-      </c>
-      <c r="C30" s="7">
+        <v>2824.6527667080718</v>
+      </c>
+      <c r="D30" s="7">
         <f t="shared" si="2"/>
-        <v>2824.6527667080718</v>
-      </c>
-      <c r="D30" s="7">
-        <f t="shared" si="3"/>
-        <v>1977.2569366956491</v>
-      </c>
-      <c r="E30" s="9"/>
+        <v>1977.2569366956502</v>
+      </c>
+      <c r="E30" s="16">
+        <f>E29*(1+$F$3)</f>
+        <v>5649.3055334161436</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>2040</v>
       </c>
       <c r="B31" s="7">
+        <f t="shared" si="0"/>
+        <v>855.02239248253318</v>
+      </c>
+      <c r="C31" s="7">
         <f t="shared" si="1"/>
-        <v>855.02239248253272</v>
-      </c>
-      <c r="C31" s="7">
+        <v>2850.0746416084439</v>
+      </c>
+      <c r="D31" s="7">
         <f t="shared" si="2"/>
-        <v>2850.0746416084439</v>
-      </c>
-      <c r="D31" s="7">
-        <f t="shared" si="3"/>
-        <v>1995.0522491259096</v>
-      </c>
-      <c r="E31" s="9"/>
+        <v>1995.0522491259105</v>
+      </c>
+      <c r="E31" s="16">
+        <f>E30*(1+$F$3)</f>
+        <v>5700.1492832168879</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>2041</v>
       </c>
       <c r="B32" s="7">
+        <f t="shared" si="0"/>
+        <v>862.71759401487577</v>
+      </c>
+      <c r="C32" s="7">
         <f t="shared" si="1"/>
-        <v>862.71759401487543</v>
-      </c>
-      <c r="C32" s="7">
+        <v>2875.7253133829195</v>
+      </c>
+      <c r="D32" s="7">
         <f t="shared" si="2"/>
-        <v>2875.7253133829195</v>
-      </c>
-      <c r="D32" s="7">
-        <f t="shared" si="3"/>
-        <v>2013.0077193680427</v>
-      </c>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2013.0077193680436</v>
+      </c>
+      <c r="E32" s="16">
+        <f>E31*(1+$F$3)</f>
+        <v>5751.4506267658389</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>2042</v>
       </c>
       <c r="B33" s="7">
+        <f t="shared" si="0"/>
+        <v>870.48205236100966</v>
+      </c>
+      <c r="C33" s="7">
         <f t="shared" si="1"/>
-        <v>870.48205236100921</v>
-      </c>
-      <c r="C33" s="7">
+        <v>2901.6068412033655</v>
+      </c>
+      <c r="D33" s="7">
         <f t="shared" si="2"/>
-        <v>2901.6068412033655</v>
-      </c>
-      <c r="D33" s="7">
-        <f t="shared" si="3"/>
-        <v>2031.1247888423547</v>
-      </c>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2031.1247888423557</v>
+      </c>
+      <c r="E33" s="16">
+        <f>E32*(1+$F$3)</f>
+        <v>5803.2136824067311</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>2043</v>
       </c>
       <c r="B34" s="7">
+        <f t="shared" si="0"/>
+        <v>878.31639083225866</v>
+      </c>
+      <c r="C34" s="7">
         <f t="shared" si="1"/>
-        <v>878.31639083225821</v>
-      </c>
-      <c r="C34" s="7">
+        <v>2927.7213027741955</v>
+      </c>
+      <c r="D34" s="7">
         <f t="shared" si="2"/>
-        <v>2927.7213027741955</v>
-      </c>
-      <c r="D34" s="7">
-        <f t="shared" si="3"/>
-        <v>2049.4049119419356</v>
-      </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2049.4049119419369</v>
+      </c>
+      <c r="E34" s="16">
+        <f>E33*(1+$F$3)</f>
+        <v>5855.4426055483909</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>2044</v>
       </c>
       <c r="B35" s="7">
+        <f t="shared" si="0"/>
+        <v>886.22123834974877</v>
+      </c>
+      <c r="C35" s="7">
         <f t="shared" si="1"/>
-        <v>886.22123834974843</v>
-      </c>
-      <c r="C35" s="7">
+        <v>2954.0707944991627</v>
+      </c>
+      <c r="D35" s="7">
         <f t="shared" si="2"/>
-        <v>2954.0707944991627</v>
-      </c>
-      <c r="D35" s="7">
-        <f t="shared" si="3"/>
-        <v>2067.8495561494128</v>
-      </c>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2067.8495561494137</v>
+      </c>
+      <c r="E35" s="16">
+        <f>E34*(1+$F$3)</f>
+        <v>5908.1415889983255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>2045</v>
       </c>
       <c r="B36" s="7">
+        <f t="shared" si="0"/>
+        <v>894.19722949489642</v>
+      </c>
+      <c r="C36" s="7">
         <f t="shared" si="1"/>
-        <v>894.19722949489608</v>
-      </c>
-      <c r="C36" s="7">
+        <v>2980.6574316496549</v>
+      </c>
+      <c r="D36" s="7">
         <f t="shared" si="2"/>
-        <v>2980.6574316496549</v>
-      </c>
-      <c r="D36" s="7">
-        <f t="shared" si="3"/>
-        <v>2086.4602021547571</v>
-      </c>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2086.4602021547585</v>
+      </c>
+      <c r="E36" s="16">
+        <f>E35*(1+$F$3)</f>
+        <v>5961.3148632993098</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>3</v>
       </c>
@@ -1080,7 +1210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B40" s="13" t="s">
         <v>8</v>
       </c>
@@ -1096,7 +1226,7 @@
       <c r="K40" s="4"/>
       <c r="N40" s="4"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>5</v>
       </c>
@@ -1177,7 +1307,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1351,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1398,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>27</v>
       </c>
@@ -1292,8 +1422,24 @@
       <c r="R47" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="U47" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="V47" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="W47" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="X47" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y47" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z47" s="14"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B48" s="13" t="s">
         <v>8</v>
       </c>
@@ -1305,8 +1451,14 @@
       <c r="R48" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="U48" s="15"/>
+      <c r="V48" s="15"/>
+      <c r="W48" s="15"/>
+      <c r="X48" s="15"/>
+      <c r="Y48" s="15"/>
+      <c r="Z48" s="14"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -1331,8 +1483,17 @@
       <c r="O49" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T49" t="s">
+        <v>10</v>
+      </c>
+      <c r="U49" s="15"/>
+      <c r="V49" s="15"/>
+      <c r="W49" s="15"/>
+      <c r="X49" s="15"/>
+      <c r="Y49" s="15"/>
+      <c r="Z49" s="14"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>1</v>
       </c>
@@ -1377,8 +1538,26 @@
         <f>IF(EXACT(P50,$Q$42),$R$42,IF(EXACT(P50,$Q$43),$R$43,IF(EXACT(P50,$Q$44),$R$44,0)))</f>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T50" s="11">
+        <v>1</v>
+      </c>
+      <c r="U50" s="6">
+        <v>1.4370000000000001</v>
+      </c>
+      <c r="V50" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="W50" s="6">
+        <v>1540.787</v>
+      </c>
+      <c r="X50" s="6">
+        <v>2.4E-2</v>
+      </c>
+      <c r="Y50" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -1407,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="M51" s="8">
-        <f t="shared" ref="M51:M69" si="4">Q51*R51*1000/1000000</f>
+        <f t="shared" ref="M51:M69" si="3">Q51*R51*1000/1000000</f>
         <v>23.617080000000001</v>
       </c>
       <c r="O51" s="3">
@@ -1420,11 +1599,29 @@
         <v>7718</v>
       </c>
       <c r="R51" s="6">
-        <f t="shared" ref="R51:R69" si="5">IF(EXACT(P51,$Q$42),$R$42,IF(EXACT(P51,$Q$43),$R$43,IF(EXACT(P51,$Q$44),$R$44,0)))</f>
+        <f t="shared" ref="R51:R69" si="4">IF(EXACT(P51,$Q$42),$R$42,IF(EXACT(P51,$Q$43),$R$43,IF(EXACT(P51,$Q$44),$R$44,0)))</f>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T51" s="11">
+        <v>2</v>
+      </c>
+      <c r="U51" s="6">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="V51" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="W51" s="6">
+        <v>917.32500000000005</v>
+      </c>
+      <c r="X51" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="Y51" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>3</v>
       </c>
@@ -1453,7 +1650,7 @@
         <v>3</v>
       </c>
       <c r="M52" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>28.115279999999998</v>
       </c>
       <c r="O52" s="3">
@@ -1466,11 +1663,29 @@
         <v>9188</v>
       </c>
       <c r="R52" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T52" s="11">
+        <v>3</v>
+      </c>
+      <c r="U52" s="6">
+        <v>24.811</v>
+      </c>
+      <c r="V52" s="6">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="W52" s="6">
+        <v>1073.9280000000001</v>
+      </c>
+      <c r="X52" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="Y52" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>4</v>
       </c>
@@ -1499,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="M53" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>21.77496</v>
       </c>
       <c r="O53" s="3">
@@ -1512,11 +1727,29 @@
         <v>7116</v>
       </c>
       <c r="R53" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T53" s="11">
+        <v>4</v>
+      </c>
+      <c r="U53" s="6">
+        <v>1.056</v>
+      </c>
+      <c r="V53" s="6">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W53" s="6">
+        <v>845.83</v>
+      </c>
+      <c r="X53" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Y53" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>5</v>
       </c>
@@ -1545,7 +1778,7 @@
         <v>5</v>
       </c>
       <c r="M54" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23.94144</v>
       </c>
       <c r="O54" s="3">
@@ -1558,11 +1791,29 @@
         <v>7824</v>
       </c>
       <c r="R54" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T54" s="11">
+        <v>5</v>
+      </c>
+      <c r="U54" s="6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="V54" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W54" s="6">
+        <v>930.02099999999996</v>
+      </c>
+      <c r="X54" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="Y54" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>6</v>
       </c>
@@ -1591,7 +1842,7 @@
         <v>6</v>
       </c>
       <c r="M55" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>38.22552000000001</v>
       </c>
       <c r="O55" s="3">
@@ -1604,11 +1855,29 @@
         <v>12492</v>
       </c>
       <c r="R55" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T55" s="11">
+        <v>6</v>
+      </c>
+      <c r="U55" s="6">
+        <v>1.1240000000000001</v>
+      </c>
+      <c r="V55" s="6">
+        <v>0</v>
+      </c>
+      <c r="W55" s="6">
+        <v>1460.1579999999999</v>
+      </c>
+      <c r="X55" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Y55" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>7</v>
       </c>
@@ -1637,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="M56" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.6982999999999999</v>
       </c>
       <c r="O56" s="3">
@@ -1650,11 +1919,29 @@
         <v>555</v>
       </c>
       <c r="R56" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T56" s="11">
+        <v>7</v>
+      </c>
+      <c r="U56" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="V56" s="6">
+        <v>0</v>
+      </c>
+      <c r="W56" s="6">
+        <v>65.930999999999997</v>
+      </c>
+      <c r="X56" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Y56" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>8</v>
       </c>
@@ -1683,7 +1970,7 @@
         <v>8</v>
       </c>
       <c r="M57" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36.677160000000001</v>
       </c>
       <c r="O57" s="3">
@@ -1696,11 +1983,29 @@
         <v>11986</v>
       </c>
       <c r="R57" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T57" s="11">
+        <v>8</v>
+      </c>
+      <c r="U57" s="6">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="V57" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="W57" s="6">
+        <v>1424.5930000000001</v>
+      </c>
+      <c r="X57" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Y57" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>9</v>
       </c>
@@ -1729,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="M58" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23.494679999999999</v>
       </c>
       <c r="O58" s="3">
@@ -1742,11 +2047,29 @@
         <v>7678</v>
       </c>
       <c r="R58" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T58" s="11">
+        <v>9</v>
+      </c>
+      <c r="U58" s="6">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V58" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W58" s="6">
+        <v>912.65499999999997</v>
+      </c>
+      <c r="X58" s="6">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="Y58" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>10</v>
       </c>
@@ -1775,7 +2098,7 @@
         <v>10</v>
       </c>
       <c r="M59" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>31.606739999999999</v>
       </c>
       <c r="O59" s="3">
@@ -1788,11 +2111,29 @@
         <v>10329</v>
       </c>
       <c r="R59" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T59" s="11">
+        <v>10</v>
+      </c>
+      <c r="U59" s="6">
+        <v>1.306</v>
+      </c>
+      <c r="V59" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="W59" s="6">
+        <v>1235.3320000000001</v>
+      </c>
+      <c r="X59" s="6">
+        <v>2.4E-2</v>
+      </c>
+      <c r="Y59" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>11</v>
       </c>
@@ -1821,7 +2162,7 @@
         <v>11</v>
       </c>
       <c r="M60" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>38.996639999999999</v>
       </c>
       <c r="O60" s="3">
@@ -1834,11 +2175,29 @@
         <v>12744</v>
       </c>
       <c r="R60" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T60" s="11">
+        <v>11</v>
+      </c>
+      <c r="U60" s="6">
+        <v>2.9769999999999999</v>
+      </c>
+      <c r="V60" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="W60" s="6">
+        <v>1514.692</v>
+      </c>
+      <c r="X60" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="Y60" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>12</v>
       </c>
@@ -1867,7 +2226,7 @@
         <v>12</v>
       </c>
       <c r="M61" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>35.954999999999998</v>
       </c>
       <c r="O61" s="3">
@@ -1880,11 +2239,29 @@
         <v>11750</v>
       </c>
       <c r="R61" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T61" s="11">
+        <v>12</v>
+      </c>
+      <c r="U61" s="6">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="V61" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="W61" s="6">
+        <v>1397.9780000000001</v>
+      </c>
+      <c r="X61" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Y61" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>13</v>
       </c>
@@ -1913,7 +2290,7 @@
         <v>13</v>
       </c>
       <c r="M62" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>26.289359999999999</v>
       </c>
       <c r="O62" s="3">
@@ -1926,11 +2303,29 @@
         <v>12171</v>
       </c>
       <c r="R62" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.16</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T62" s="11">
+        <v>13</v>
+      </c>
+      <c r="U62" s="6">
+        <v>2.74</v>
+      </c>
+      <c r="V62" s="6">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="W62" s="6">
+        <v>2551.596</v>
+      </c>
+      <c r="X62" s="6">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="Y62" s="6">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>14</v>
       </c>
@@ -1959,7 +2354,7 @@
         <v>14</v>
       </c>
       <c r="M63" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>34.819740000000003</v>
       </c>
       <c r="O63" s="3">
@@ -1972,11 +2367,29 @@
         <v>11379</v>
       </c>
       <c r="R63" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T63" s="11">
+        <v>14</v>
+      </c>
+      <c r="U63" s="6">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="V63" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="W63" s="6">
+        <v>1352.424</v>
+      </c>
+      <c r="X63" s="6">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Y63" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>15</v>
       </c>
@@ -2005,7 +2418,7 @@
         <v>15</v>
       </c>
       <c r="M64" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>37.647179999999999</v>
       </c>
       <c r="O64" s="3">
@@ -2018,11 +2431,29 @@
         <v>12303</v>
       </c>
       <c r="R64" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T64" s="11">
+        <v>15</v>
+      </c>
+      <c r="U64" s="6">
+        <v>3.8889999999999998</v>
+      </c>
+      <c r="V64" s="6">
+        <v>3.9E-2</v>
+      </c>
+      <c r="W64" s="6">
+        <v>1436.3489999999999</v>
+      </c>
+      <c r="X64" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Y64" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>16</v>
       </c>
@@ -2051,7 +2482,7 @@
         <v>16</v>
       </c>
       <c r="M65" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25.404119999999999</v>
       </c>
       <c r="O65" s="3">
@@ -2064,11 +2495,29 @@
         <v>8302</v>
       </c>
       <c r="R65" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T65" s="11">
+        <v>16</v>
+      </c>
+      <c r="U65" s="6">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="V65" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W65" s="6">
+        <v>986.73699999999997</v>
+      </c>
+      <c r="X65" s="6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="Y65" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>17</v>
       </c>
@@ -2097,7 +2546,7 @@
         <v>17</v>
       </c>
       <c r="M66" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23.453280000000003</v>
       </c>
       <c r="O66" s="3">
@@ -2110,11 +2559,29 @@
         <v>10858</v>
       </c>
       <c r="R66" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.16</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T66" s="11">
+        <v>17</v>
+      </c>
+      <c r="U66" s="6">
+        <v>3.786</v>
+      </c>
+      <c r="V66" s="6">
+        <v>1.365</v>
+      </c>
+      <c r="W66" s="6">
+        <v>2277.605</v>
+      </c>
+      <c r="X66" s="6">
+        <v>0.249</v>
+      </c>
+      <c r="Y66" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>18</v>
       </c>
@@ -2143,7 +2610,7 @@
         <v>18</v>
       </c>
       <c r="M67" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23.647680000000001</v>
       </c>
       <c r="O67" s="3">
@@ -2156,11 +2623,29 @@
         <v>10948</v>
       </c>
       <c r="R67" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.16</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T67" s="11">
+        <v>18</v>
+      </c>
+      <c r="U67" s="6">
+        <v>1.2689999999999999</v>
+      </c>
+      <c r="V67" s="6">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="W67" s="6">
+        <v>2246.4659999999999</v>
+      </c>
+      <c r="X67" s="6">
+        <v>0.223</v>
+      </c>
+      <c r="Y67" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>19</v>
       </c>
@@ -2189,7 +2674,7 @@
         <v>19</v>
       </c>
       <c r="M68" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>223.99503999999999</v>
       </c>
       <c r="O68" s="3">
@@ -2202,11 +2687,29 @@
         <v>17834</v>
       </c>
       <c r="R68" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>12.56</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T68" s="11">
+        <v>19</v>
+      </c>
+      <c r="U68" s="6">
+        <v>15.976000000000001</v>
+      </c>
+      <c r="V68" s="6">
+        <v>9.0060000000000002</v>
+      </c>
+      <c r="W68" s="6">
+        <v>2912.8049999999998</v>
+      </c>
+      <c r="X68" s="6">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="Y68" s="6">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>20</v>
       </c>
@@ -2235,7 +2738,7 @@
         <v>20</v>
       </c>
       <c r="M69" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>36.931139999999999</v>
       </c>
       <c r="O69" s="3">
@@ -2248,16 +2751,42 @@
         <v>12069</v>
       </c>
       <c r="R69" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.06</v>
       </c>
+      <c r="T69" s="11">
+        <v>20</v>
+      </c>
+      <c r="U69" s="6">
+        <v>2.1019999999999999</v>
+      </c>
+      <c r="V69" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="W69" s="6">
+        <v>1434.461</v>
+      </c>
+      <c r="X69" s="6">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Y69" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="12">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="V47:V49"/>
+    <mergeCell ref="W47:W49"/>
+    <mergeCell ref="X47:X49"/>
+    <mergeCell ref="Y47:Y49"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="G40:I40"/>
     <mergeCell ref="B48:D48"/>
+    <mergeCell ref="U47:U49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added discount rate, changed emissions to output yearly
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -18,6 +18,7 @@
     <definedName name="BusDemand">Sheet2!$C$11:$E$36</definedName>
     <definedName name="CH4_rate">Sheet2!$Y$50:$Y$89</definedName>
     <definedName name="CO2_rate">Sheet2!$X$50:$X$89</definedName>
+    <definedName name="DiscRate">Sheet2!$G$1</definedName>
     <definedName name="LineCapacity">Sheet2!$P$42:$P$44</definedName>
     <definedName name="LineFromBus">Sheet2!$H$42:$J$44</definedName>
     <definedName name="LineReactance">Sheet2!$M$42:$M$44</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
   <si>
     <t>NumBuses</t>
   </si>
@@ -293,6 +294,9 @@
   </si>
   <si>
     <t>Nameplate Capacity (MW)</t>
+  </si>
+  <si>
+    <t>Discount Rate</t>
   </si>
 </sst>
 </file>
@@ -360,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -416,6 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,7 +705,7 @@
   <dimension ref="A1:AG89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,6 +728,13 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
+      <c r="E1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="23">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
@@ -4629,7 +4641,8 @@
       <c r="AG89" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="56">
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AF87:AG87"/>
     <mergeCell ref="AF88:AG88"/>
     <mergeCell ref="AF89:AG89"/>

</xml_diff>

<commit_message>
added new wind and solar functionality
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -16,24 +16,33 @@
   </sheets>
   <definedNames>
     <definedName name="BusDemand">Sheet2!$C$11:$E$36</definedName>
-    <definedName name="CH4_rate">Sheet2!$Y$50:$Y$89</definedName>
-    <definedName name="CO2_rate">Sheet2!$X$50:$X$89</definedName>
+    <definedName name="CAPEX_solar">Sheet2!$Q$1</definedName>
+    <definedName name="CAPEX_wind">Sheet2!$Q$3</definedName>
+    <definedName name="CH4_rate">Sheet2!$Y$50:$Y$91</definedName>
+    <definedName name="CO2_rate">Sheet2!$X$50:$X$91</definedName>
     <definedName name="DiscRate">Sheet2!$G$1</definedName>
     <definedName name="LineCapacity">Sheet2!$P$42:$P$44</definedName>
     <definedName name="LineFromBus">Sheet2!$H$42:$J$44</definedName>
     <definedName name="LineReactance">Sheet2!$M$42:$M$44</definedName>
     <definedName name="LineToBus">Sheet2!$C$42:$E$44</definedName>
-    <definedName name="MarginalC">Sheet2!$N$50:$N$89</definedName>
-    <definedName name="MaxGen">Sheet2!$H$50:$H$89</definedName>
-    <definedName name="MinGen">Sheet2!$K$50:$K$89</definedName>
-    <definedName name="N2O_rate">Sheet2!$Z$50:$Z$89</definedName>
-    <definedName name="NOx_rate">Sheet2!$V$50:$V$89</definedName>
+    <definedName name="MarginalC">Sheet2!$N$50:$N$91</definedName>
+    <definedName name="maxCO2">Sheet2!$L$2</definedName>
+    <definedName name="MaxGen">Sheet2!$H$50:$H$91</definedName>
+    <definedName name="MinGen">Sheet2!$K$50:$K$91</definedName>
+    <definedName name="N2O_rate">Sheet2!$Z$50:$Z$91</definedName>
+    <definedName name="NOx_rate">Sheet2!$V$50:$V$91</definedName>
     <definedName name="NumBuses">Sheet2!$C$1</definedName>
     <definedName name="NumLines">Sheet2!$C$2</definedName>
     <definedName name="NumUnits">Sheet2!$C$3</definedName>
     <definedName name="NumYears">Sheet2!$C$4</definedName>
-    <definedName name="SO2_rate">Sheet2!$W$50:$W$89</definedName>
-    <definedName name="UnitsByBus">Sheet2!$C$50:$E$89</definedName>
+    <definedName name="OPEX_solar">Sheet2!$Q$2</definedName>
+    <definedName name="OPEX_wind">Sheet2!$Q$4</definedName>
+    <definedName name="SO2_rate">Sheet2!$W$50:$W$91</definedName>
+    <definedName name="solar_cap_factor">Sheet2!$G$4</definedName>
+    <definedName name="solar_inc">Sheet2!$Q$5</definedName>
+    <definedName name="UnitsByBus">Sheet2!$C$50:$E$91</definedName>
+    <definedName name="wind_cap_factor">Sheet2!$G$5</definedName>
+    <definedName name="wind_inc">Sheet2!$Q$6</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -45,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
   <si>
     <t>NumBuses</t>
   </si>
@@ -161,12 +170,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Peak Hour? (Y/N)</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>ALT</t>
   </si>
   <si>
@@ -297,16 +300,56 @@
   </si>
   <si>
     <t>Discount Rate</t>
+  </si>
+  <si>
+    <t>Solar Scale Factor</t>
+  </si>
+  <si>
+    <t>2020 CO2 Emissions (lb):</t>
+  </si>
+  <si>
+    <t>Max 2045 CO2 Emissions (lb):</t>
+  </si>
+  <si>
+    <t>NEWSOLAR</t>
+  </si>
+  <si>
+    <t>NEWWIND</t>
+  </si>
+  <si>
+    <t>WIND</t>
+  </si>
+  <si>
+    <t>CAPEX of new solar ($):</t>
+  </si>
+  <si>
+    <t>OPEX of new solar ($/MW):</t>
+  </si>
+  <si>
+    <t>CAPEX of new wind ($):</t>
+  </si>
+  <si>
+    <t>OPEX of new wind ($/MW):</t>
+  </si>
+  <si>
+    <t>Size of each wind module (MW):</t>
+  </si>
+  <si>
+    <t>Size of each solar module (MW):</t>
+  </si>
+  <si>
+    <t>Wind Scale Factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,8 +379,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,11 +399,97 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -364,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,10 +533,30 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -411,16 +566,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG89"/>
+  <dimension ref="A1:AG91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,6 +903,12 @@
     <col min="1" max="1" width="6.54296875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="6" max="6" width="13.36328125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="12" max="12" width="8.6328125" customWidth="1"/>
+    <col min="14" max="14" width="9.26953125" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="17" max="17" width="13.26953125" customWidth="1"/>
     <col min="18" max="18" width="9.54296875" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
     <col min="22" max="22" width="16.36328125" customWidth="1"/>
@@ -721,81 +917,158 @@
     <col min="26" max="26" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="I1" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="23">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="17">
+        <v>7256200.8565999996</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="26">
+        <v>2221460.4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="17"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="6">
         <v>4765</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I2" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="25">
+        <f>L1*0.25</f>
+        <v>1814050.2141499999</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="26">
+        <v>19867.2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>40</v>
-      </c>
-      <c r="E3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="17"/>
+      <c r="F3" s="29"/>
       <c r="G3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I3" s="4"/>
+      <c r="L3" s="27"/>
+      <c r="N3" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="26">
+        <v>1596613.3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="6">
         <v>26</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D4" s="15"/>
+      <c r="E4" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="17">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="N4" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="26">
+        <v>43560</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="17" t="s">
+      <c r="E5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="17">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="N5" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="I6" s="4"/>
+      <c r="N6" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="C9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
@@ -812,7 +1085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>2020</v>
       </c>
@@ -833,7 +1106,7 @@
         <v>4765</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>2021</v>
       </c>
@@ -854,7 +1127,7 @@
         <v>4807.8849999999993</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>2022</v>
       </c>
@@ -875,7 +1148,7 @@
         <v>4851.155964999999</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>2023</v>
       </c>
@@ -896,7 +1169,7 @@
         <v>4894.8163686849985</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>2024</v>
       </c>
@@ -917,7 +1190,7 @@
         <v>4938.8697160031634</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>2025</v>
       </c>
@@ -1376,17 +1649,17 @@
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C40" s="19" t="s">
+      <c r="C40" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="2"/>
-      <c r="H40" s="19" t="s">
+      <c r="H40" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
       <c r="O40" s="4"/>
@@ -1587,45 +1860,45 @@
       <c r="S47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V47" s="18" t="s">
+      <c r="V47" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="W47" s="18" t="s">
+      <c r="W47" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="X47" s="18" t="s">
+      <c r="X47" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="Y47" s="18" t="s">
+      <c r="Y47" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="Z47" s="18" t="s">
+      <c r="Z47" s="30" t="s">
         <v>36</v>
       </c>
       <c r="AA47" s="13"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
       <c r="R48" t="s">
         <v>18</v>
       </c>
       <c r="S48" t="s">
         <v>21</v>
       </c>
-      <c r="V48" s="18"/>
-      <c r="W48" s="18"/>
-      <c r="X48" s="18"/>
-      <c r="Y48" s="18"/>
-      <c r="Z48" s="18"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
       <c r="AA48" s="13"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>10</v>
@@ -1654,16 +1927,16 @@
       <c r="U49" t="s">
         <v>10</v>
       </c>
-      <c r="V49" s="18"/>
-      <c r="W49" s="18"/>
-      <c r="X49" s="18"/>
-      <c r="Y49" s="18"/>
-      <c r="Z49" s="18"/>
+      <c r="V49" s="30"/>
+      <c r="W49" s="30"/>
+      <c r="X49" s="30"/>
+      <c r="Y49" s="30"/>
+      <c r="Z49" s="30"/>
       <c r="AA49" s="13"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B50" s="2">
         <v>1</v>
@@ -1730,7 +2003,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B51" s="2">
         <v>2</v>
@@ -1760,7 +2033,7 @@
         <v>2</v>
       </c>
       <c r="N51" s="8">
-        <f t="shared" ref="N51:N89" si="4">R51*S51*1000/1000000</f>
+        <f t="shared" ref="N51:N91" si="4">R51*S51*1000/1000000</f>
         <v>23.617080000000001</v>
       </c>
       <c r="P51" s="3">
@@ -1797,7 +2070,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B52" s="2">
         <v>3</v>
@@ -1864,7 +2137,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B53" s="2">
         <v>4</v>
@@ -1931,7 +2204,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B54" s="3">
         <v>5</v>
@@ -1998,7 +2271,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B55" s="3">
         <v>6</v>
@@ -2065,7 +2338,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B56" s="3">
         <v>7</v>
@@ -2132,7 +2405,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B57" s="3">
         <v>8</v>
@@ -2199,7 +2472,7 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3">
         <v>9</v>
@@ -2266,7 +2539,7 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3">
         <v>10</v>
@@ -2333,7 +2606,7 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B60" s="3">
         <v>11</v>
@@ -2400,7 +2673,7 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B61" s="3">
         <v>12</v>
@@ -2467,7 +2740,7 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B62" s="3">
         <v>13</v>
@@ -2534,7 +2807,7 @@
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B63" s="3">
         <v>14</v>
@@ -2601,7 +2874,7 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B64" s="3">
         <v>15</v>
@@ -2668,7 +2941,7 @@
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B65" s="3">
         <v>16</v>
@@ -2735,7 +3008,7 @@
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B66" s="3">
         <v>17</v>
@@ -2802,7 +3075,7 @@
     </row>
     <row r="67" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B67" s="3">
         <v>18</v>
@@ -2866,21 +3139,21 @@
       <c r="Z67" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AC67" s="20" t="s">
+      <c r="AC67" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD67" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE67" s="34"/>
+      <c r="AF67" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="AD67" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="AE67" s="20"/>
-      <c r="AF67" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG67" s="20"/>
+      <c r="AG67" s="43"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B68" s="3">
         <v>19</v>
@@ -2944,15 +3217,15 @@
       <c r="Z68" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AC68" s="20"/>
-      <c r="AD68" s="20"/>
-      <c r="AE68" s="20"/>
-      <c r="AF68" s="20"/>
-      <c r="AG68" s="20"/>
+      <c r="AC68" s="33"/>
+      <c r="AD68" s="35"/>
+      <c r="AE68" s="35"/>
+      <c r="AF68" s="35"/>
+      <c r="AG68" s="44"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69" s="3">
         <v>20</v>
@@ -3022,7 +3295,7 @@
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B70" s="12">
         <v>21</v>
@@ -3040,7 +3313,7 @@
         <v>21</v>
       </c>
       <c r="H70" s="6">
-        <f>IF(EXACT($G$4,$D$4),AF70,0)</f>
+        <f>$G$4*AF70</f>
         <v>28.1</v>
       </c>
       <c r="J70" s="12">
@@ -3060,7 +3333,7 @@
         <v>21</v>
       </c>
       <c r="Q70" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R70" s="6">
         <v>0</v>
@@ -3086,24 +3359,24 @@
       <c r="Z70" s="6">
         <v>0</v>
       </c>
-      <c r="AB70" s="12">
+      <c r="AB70" s="18">
         <v>21</v>
       </c>
-      <c r="AC70">
+      <c r="AC70" s="19">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AD70" s="21">
+      <c r="AD70" s="36">
         <v>72154</v>
       </c>
-      <c r="AE70" s="21"/>
-      <c r="AF70" s="22">
+      <c r="AE70" s="36"/>
+      <c r="AF70" s="45">
         <v>28.1</v>
       </c>
-      <c r="AG70" s="22"/>
+      <c r="AG70" s="46"/>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B71" s="12">
         <v>22</v>
@@ -3121,7 +3394,7 @@
         <v>22</v>
       </c>
       <c r="H71" s="6">
-        <f t="shared" ref="H71:H89" si="6">IF(EXACT($G$4,$D$4),AF71,0)</f>
+        <f t="shared" ref="H71:H89" si="6">$G$4*AF71</f>
         <v>25</v>
       </c>
       <c r="J71" s="12">
@@ -3141,7 +3414,7 @@
         <v>22</v>
       </c>
       <c r="Q71" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R71" s="6">
         <v>0</v>
@@ -3167,24 +3440,24 @@
       <c r="Z71" s="6">
         <v>0</v>
       </c>
-      <c r="AB71" s="12">
+      <c r="AB71" s="20">
         <v>22</v>
       </c>
-      <c r="AC71">
+      <c r="AC71" s="21">
         <v>0.31</v>
       </c>
-      <c r="AD71" s="21">
+      <c r="AD71" s="37">
         <v>67811</v>
       </c>
-      <c r="AE71" s="21"/>
-      <c r="AF71" s="22">
+      <c r="AE71" s="37"/>
+      <c r="AF71" s="38">
         <v>25</v>
       </c>
-      <c r="AG71" s="22"/>
+      <c r="AG71" s="39"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B72" s="12">
         <v>23</v>
@@ -3222,7 +3495,7 @@
         <v>23</v>
       </c>
       <c r="Q72" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R72" s="6">
         <v>0</v>
@@ -3248,24 +3521,24 @@
       <c r="Z72" s="6">
         <v>0</v>
       </c>
-      <c r="AB72" s="12">
+      <c r="AB72" s="20">
         <v>23</v>
       </c>
-      <c r="AC72">
+      <c r="AC72" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD72" s="21">
+      <c r="AD72" s="37">
         <v>187455</v>
       </c>
-      <c r="AE72" s="21"/>
-      <c r="AF72" s="22">
+      <c r="AE72" s="37"/>
+      <c r="AF72" s="38">
         <v>70</v>
       </c>
-      <c r="AG72" s="22"/>
+      <c r="AG72" s="39"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B73" s="12">
         <v>24</v>
@@ -3303,7 +3576,7 @@
         <v>24</v>
       </c>
       <c r="Q73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R73" s="6">
         <v>0</v>
@@ -3329,24 +3602,24 @@
       <c r="Z73" s="6">
         <v>0</v>
       </c>
-      <c r="AB73" s="12">
+      <c r="AB73" s="20">
         <v>24</v>
       </c>
-      <c r="AC73">
+      <c r="AC73" s="21">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AD73" s="21">
+      <c r="AD73" s="37">
         <v>63266</v>
       </c>
-      <c r="AE73" s="21"/>
-      <c r="AF73" s="22">
+      <c r="AE73" s="37"/>
+      <c r="AF73" s="38">
         <v>30.6</v>
       </c>
-      <c r="AG73" s="22"/>
+      <c r="AG73" s="39"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B74" s="12">
         <v>25</v>
@@ -3384,7 +3657,7 @@
         <v>25</v>
       </c>
       <c r="Q74" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R74" s="6">
         <v>0</v>
@@ -3410,24 +3683,24 @@
       <c r="Z74" s="6">
         <v>0</v>
       </c>
-      <c r="AB74" s="12">
+      <c r="AB74" s="20">
         <v>25</v>
       </c>
-      <c r="AC74">
+      <c r="AC74" s="21">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AD74" s="21">
+      <c r="AD74" s="37">
         <v>26553</v>
       </c>
-      <c r="AE74" s="21"/>
-      <c r="AF74" s="22">
+      <c r="AE74" s="37"/>
+      <c r="AF74" s="38">
         <v>10</v>
       </c>
-      <c r="AG74" s="22"/>
+      <c r="AG74" s="39"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B75" s="12">
         <v>26</v>
@@ -3465,7 +3738,7 @@
         <v>26</v>
       </c>
       <c r="Q75" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R75" s="6">
         <v>0</v>
@@ -3491,24 +3764,24 @@
       <c r="Z75" s="6">
         <v>0</v>
       </c>
-      <c r="AB75" s="12">
+      <c r="AB75" s="20">
         <v>26</v>
       </c>
-      <c r="AC75">
+      <c r="AC75" s="21">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AD75" s="21">
+      <c r="AD75" s="37">
         <v>24949</v>
       </c>
-      <c r="AE75" s="21"/>
-      <c r="AF75" s="22">
+      <c r="AE75" s="37"/>
+      <c r="AF75" s="38">
         <v>10</v>
       </c>
-      <c r="AG75" s="22"/>
+      <c r="AG75" s="39"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B76" s="12">
         <v>27</v>
@@ -3546,7 +3819,7 @@
         <v>27</v>
       </c>
       <c r="Q76" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R76" s="6">
         <v>0</v>
@@ -3572,24 +3845,24 @@
       <c r="Z76" s="6">
         <v>0</v>
       </c>
-      <c r="AB76" s="12">
+      <c r="AB76" s="20">
         <v>27</v>
       </c>
-      <c r="AC76">
+      <c r="AC76" s="21">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AD76" s="21">
+      <c r="AD76" s="37">
         <v>22870</v>
       </c>
-      <c r="AE76" s="21"/>
-      <c r="AF76" s="22">
+      <c r="AE76" s="37"/>
+      <c r="AF76" s="38">
         <v>10</v>
       </c>
-      <c r="AG76" s="22"/>
+      <c r="AG76" s="39"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B77" s="12">
         <v>28</v>
@@ -3627,7 +3900,7 @@
         <v>28</v>
       </c>
       <c r="Q77" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R77" s="6">
         <v>0</v>
@@ -3653,24 +3926,24 @@
       <c r="Z77" s="6">
         <v>0</v>
       </c>
-      <c r="AB77" s="12">
+      <c r="AB77" s="20">
         <v>28</v>
       </c>
-      <c r="AC77">
+      <c r="AC77" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD77" s="21">
+      <c r="AD77" s="37">
         <v>139836</v>
       </c>
-      <c r="AE77" s="21"/>
-      <c r="AF77" s="22">
+      <c r="AE77" s="37"/>
+      <c r="AF77" s="38">
         <v>52.2</v>
       </c>
-      <c r="AG77" s="22"/>
+      <c r="AG77" s="39"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B78" s="12">
         <v>29</v>
@@ -3708,7 +3981,7 @@
         <v>29</v>
       </c>
       <c r="Q78" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R78" s="6">
         <v>0</v>
@@ -3734,24 +4007,24 @@
       <c r="Z78" s="6">
         <v>0</v>
       </c>
-      <c r="AB78" s="12">
+      <c r="AB78" s="20">
         <v>29</v>
       </c>
-      <c r="AC78">
+      <c r="AC78" s="21">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AD78" s="21">
+      <c r="AD78" s="37">
         <v>23515</v>
       </c>
-      <c r="AE78" s="21"/>
-      <c r="AF78" s="22">
+      <c r="AE78" s="37"/>
+      <c r="AF78" s="38">
         <v>10</v>
       </c>
-      <c r="AG78" s="22"/>
+      <c r="AG78" s="39"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B79" s="12">
         <v>30</v>
@@ -3789,7 +4062,7 @@
         <v>30</v>
       </c>
       <c r="Q79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R79" s="6">
         <v>0</v>
@@ -3815,24 +4088,24 @@
       <c r="Z79" s="6">
         <v>0</v>
       </c>
-      <c r="AB79" s="12">
+      <c r="AB79" s="20">
         <v>30</v>
       </c>
-      <c r="AC79">
+      <c r="AC79" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AD79" s="21">
+      <c r="AD79" s="37">
         <v>49503</v>
       </c>
-      <c r="AE79" s="21"/>
-      <c r="AF79" s="22">
+      <c r="AE79" s="37"/>
+      <c r="AF79" s="38">
         <v>20.2</v>
       </c>
-      <c r="AG79" s="22"/>
+      <c r="AG79" s="39"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B80" s="12">
         <v>31</v>
@@ -3870,7 +4143,7 @@
         <v>31</v>
       </c>
       <c r="Q80" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R80" s="6">
         <v>0</v>
@@ -3896,24 +4169,24 @@
       <c r="Z80" s="6">
         <v>0</v>
       </c>
-      <c r="AB80" s="12">
+      <c r="AB80" s="20">
         <v>31</v>
       </c>
-      <c r="AC80">
+      <c r="AC80" s="21">
         <v>0.307</v>
       </c>
-      <c r="AD80" s="21">
+      <c r="AD80" s="37">
         <v>188420</v>
       </c>
-      <c r="AE80" s="21"/>
-      <c r="AF80" s="22">
+      <c r="AE80" s="37"/>
+      <c r="AF80" s="38">
         <v>70</v>
       </c>
-      <c r="AG80" s="22"/>
+      <c r="AG80" s="39"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B81" s="12">
         <v>32</v>
@@ -3951,7 +4224,7 @@
         <v>32</v>
       </c>
       <c r="Q81" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R81" s="6">
         <v>0</v>
@@ -3977,24 +4250,24 @@
       <c r="Z81" s="6">
         <v>0</v>
       </c>
-      <c r="AB81" s="12">
+      <c r="AB81" s="20">
         <v>32</v>
       </c>
-      <c r="AC81">
+      <c r="AC81" s="21">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AD81" s="21">
+      <c r="AD81" s="37">
         <v>26573</v>
       </c>
-      <c r="AE81" s="21"/>
-      <c r="AF81" s="22">
+      <c r="AE81" s="37"/>
+      <c r="AF81" s="38">
         <v>10.5</v>
       </c>
-      <c r="AG81" s="22"/>
+      <c r="AG81" s="39"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B82" s="12">
         <v>33</v>
@@ -4032,7 +4305,7 @@
         <v>33</v>
       </c>
       <c r="Q82" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R82" s="6">
         <v>0</v>
@@ -4058,24 +4331,24 @@
       <c r="Z82" s="6">
         <v>0</v>
       </c>
-      <c r="AB82" s="12">
+      <c r="AB82" s="20">
         <v>33</v>
       </c>
-      <c r="AC82">
+      <c r="AC82" s="21">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AD82" s="21">
+      <c r="AD82" s="37">
         <v>25253</v>
       </c>
-      <c r="AE82" s="21"/>
-      <c r="AF82" s="22">
+      <c r="AE82" s="37"/>
+      <c r="AF82" s="38">
         <v>10</v>
       </c>
-      <c r="AG82" s="22"/>
+      <c r="AG82" s="39"/>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B83" s="12">
         <v>34</v>
@@ -4113,7 +4386,7 @@
         <v>34</v>
       </c>
       <c r="Q83" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R83" s="6">
         <v>0</v>
@@ -4139,24 +4412,24 @@
       <c r="Z83" s="6">
         <v>0</v>
       </c>
-      <c r="AB83" s="12">
+      <c r="AB83" s="20">
         <v>34</v>
       </c>
-      <c r="AC83">
+      <c r="AC83" s="21">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AD83" s="21">
+      <c r="AD83" s="37">
         <v>17610</v>
       </c>
-      <c r="AE83" s="21"/>
-      <c r="AF83" s="22">
+      <c r="AE83" s="37"/>
+      <c r="AF83" s="38">
         <v>10</v>
       </c>
-      <c r="AG83" s="22"/>
+      <c r="AG83" s="39"/>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B84" s="12">
         <v>35</v>
@@ -4194,7 +4467,7 @@
         <v>35</v>
       </c>
       <c r="Q84" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R84" s="6">
         <v>0</v>
@@ -4220,24 +4493,24 @@
       <c r="Z84" s="6">
         <v>0</v>
       </c>
-      <c r="AB84" s="12">
+      <c r="AB84" s="20">
         <v>35</v>
       </c>
-      <c r="AC84">
+      <c r="AC84" s="21">
         <v>0.221</v>
       </c>
-      <c r="AD84" s="21">
+      <c r="AD84" s="37">
         <v>19372</v>
       </c>
-      <c r="AE84" s="21"/>
-      <c r="AF84" s="22">
+      <c r="AE84" s="37"/>
+      <c r="AF84" s="38">
         <v>10</v>
       </c>
-      <c r="AG84" s="22"/>
+      <c r="AG84" s="39"/>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B85" s="12">
         <v>36</v>
@@ -4275,7 +4548,7 @@
         <v>36</v>
       </c>
       <c r="Q85" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R85" s="6">
         <v>0</v>
@@ -4301,24 +4574,24 @@
       <c r="Z85" s="6">
         <v>0</v>
       </c>
-      <c r="AB85" s="12">
+      <c r="AB85" s="20">
         <v>36</v>
       </c>
-      <c r="AC85">
+      <c r="AC85" s="21">
         <v>0.216</v>
       </c>
-      <c r="AD85" s="21">
+      <c r="AD85" s="37">
         <v>18939</v>
       </c>
-      <c r="AE85" s="21"/>
-      <c r="AF85" s="22">
+      <c r="AE85" s="37"/>
+      <c r="AF85" s="38">
         <v>10</v>
       </c>
-      <c r="AG85" s="22"/>
+      <c r="AG85" s="39"/>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B86" s="12">
         <v>37</v>
@@ -4356,7 +4629,7 @@
         <v>37</v>
       </c>
       <c r="Q86" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R86" s="6">
         <v>0</v>
@@ -4382,24 +4655,24 @@
       <c r="Z86" s="6">
         <v>0</v>
       </c>
-      <c r="AB86" s="12">
+      <c r="AB86" s="20">
         <v>37</v>
       </c>
-      <c r="AC86">
+      <c r="AC86" s="21">
         <v>0.23</v>
       </c>
-      <c r="AD86" s="21">
+      <c r="AD86" s="37">
         <v>20382</v>
       </c>
-      <c r="AE86" s="21"/>
-      <c r="AF86" s="22">
+      <c r="AE86" s="37"/>
+      <c r="AF86" s="38">
         <v>10.1</v>
       </c>
-      <c r="AG86" s="22"/>
+      <c r="AG86" s="39"/>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B87" s="12">
         <v>38</v>
@@ -4437,7 +4710,7 @@
         <v>38</v>
       </c>
       <c r="Q87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R87" s="6">
         <v>0</v>
@@ -4463,24 +4736,24 @@
       <c r="Z87" s="6">
         <v>0</v>
       </c>
-      <c r="AB87" s="12">
+      <c r="AB87" s="20">
         <v>38</v>
       </c>
-      <c r="AC87">
+      <c r="AC87" s="21">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AD87" s="21">
+      <c r="AD87" s="37">
         <v>19968</v>
       </c>
-      <c r="AE87" s="21"/>
-      <c r="AF87" s="22">
+      <c r="AE87" s="37"/>
+      <c r="AF87" s="38">
         <v>10.1</v>
       </c>
-      <c r="AG87" s="22"/>
+      <c r="AG87" s="39"/>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B88" s="12">
         <v>39</v>
@@ -4518,7 +4791,7 @@
         <v>39</v>
       </c>
       <c r="Q88" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R88" s="6">
         <v>0</v>
@@ -4544,24 +4817,24 @@
       <c r="Z88" s="6">
         <v>0</v>
       </c>
-      <c r="AB88" s="12">
+      <c r="AB88" s="20">
         <v>39</v>
       </c>
-      <c r="AC88">
+      <c r="AC88" s="21">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AD88" s="21">
+      <c r="AD88" s="37">
         <v>23240</v>
       </c>
-      <c r="AE88" s="21"/>
-      <c r="AF88" s="22">
+      <c r="AE88" s="37"/>
+      <c r="AF88" s="38">
         <v>10</v>
       </c>
-      <c r="AG88" s="22"/>
+      <c r="AG88" s="39"/>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B89" s="12">
         <v>40</v>
@@ -4599,7 +4872,7 @@
         <v>40</v>
       </c>
       <c r="Q89" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="R89" s="6">
         <v>0</v>
@@ -4625,23 +4898,160 @@
       <c r="Z89" s="6">
         <v>0</v>
       </c>
-      <c r="AB89" s="12">
+      <c r="AB89" s="22">
         <v>40</v>
       </c>
-      <c r="AC89">
+      <c r="AC89" s="23">
         <v>0.254</v>
       </c>
-      <c r="AD89" s="21">
+      <c r="AD89" s="42">
         <v>26709</v>
       </c>
-      <c r="AE89" s="21"/>
-      <c r="AF89" s="22">
+      <c r="AE89" s="42"/>
+      <c r="AF89" s="40">
         <v>12</v>
       </c>
-      <c r="AG89" s="22"/>
+      <c r="AG89" s="41"/>
+    </row>
+    <row r="90" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="24">
+        <v>41</v>
+      </c>
+      <c r="C90" s="6">
+        <v>0</v>
+      </c>
+      <c r="D90" s="6">
+        <v>1</v>
+      </c>
+      <c r="E90" s="6">
+        <v>0</v>
+      </c>
+      <c r="G90" s="24">
+        <v>41</v>
+      </c>
+      <c r="H90" s="6">
+        <v>10000</v>
+      </c>
+      <c r="J90" s="24">
+        <v>41</v>
+      </c>
+      <c r="K90" s="6">
+        <v>0</v>
+      </c>
+      <c r="M90" s="24">
+        <v>41</v>
+      </c>
+      <c r="N90" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P90" s="24">
+        <v>41</v>
+      </c>
+      <c r="Q90" t="s">
+        <v>39</v>
+      </c>
+      <c r="R90" s="6">
+        <v>0</v>
+      </c>
+      <c r="S90" s="6">
+        <v>0</v>
+      </c>
+      <c r="U90" s="24">
+        <v>41</v>
+      </c>
+      <c r="V90" s="6">
+        <v>0</v>
+      </c>
+      <c r="W90" s="6">
+        <v>0</v>
+      </c>
+      <c r="X90" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y90" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91" s="24">
+        <v>42</v>
+      </c>
+      <c r="C91" s="6">
+        <v>0</v>
+      </c>
+      <c r="D91" s="6">
+        <v>0</v>
+      </c>
+      <c r="E91" s="6">
+        <v>1</v>
+      </c>
+      <c r="G91" s="24">
+        <v>42</v>
+      </c>
+      <c r="H91" s="6">
+        <v>10000</v>
+      </c>
+      <c r="J91" s="24">
+        <v>42</v>
+      </c>
+      <c r="K91" s="6">
+        <v>0</v>
+      </c>
+      <c r="M91" s="24">
+        <v>42</v>
+      </c>
+      <c r="N91" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P91" s="24">
+        <v>42</v>
+      </c>
+      <c r="Q91" t="s">
+        <v>87</v>
+      </c>
+      <c r="R91" s="6">
+        <v>0</v>
+      </c>
+      <c r="S91" s="6">
+        <v>0</v>
+      </c>
+      <c r="U91" s="24">
+        <v>42</v>
+      </c>
+      <c r="V91" s="6">
+        <v>0</v>
+      </c>
+      <c r="W91" s="6">
+        <v>0</v>
+      </c>
+      <c r="X91" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="65">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="AF87:AG87"/>
     <mergeCell ref="AF88:AG88"/>
@@ -4698,6 +5108,10 @@
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="W47:W49"/>
     <mergeCell ref="X47:X49"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added some ev stuff to input file
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -21,6 +21,7 @@
     <definedName name="CH4_rate">Sheet2!$Y$50:$Y$91</definedName>
     <definedName name="CO2_rate">Sheet2!$X$50:$X$91</definedName>
     <definedName name="DiscRate">Sheet2!$G$1</definedName>
+    <definedName name="EV_subsidy_cost">Sheet2!$V$1</definedName>
     <definedName name="LineCapacity">Sheet2!$P$42:$P$44</definedName>
     <definedName name="LineFromBus">Sheet2!$H$42:$J$44</definedName>
     <definedName name="LineReactance">Sheet2!$M$42:$M$44</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="105">
   <si>
     <t>NumBuses</t>
   </si>
@@ -339,6 +340,36 @@
   </si>
   <si>
     <t>Wind Scale Factor</t>
+  </si>
+  <si>
+    <t>EV 20% Subsidy Capital Cost ($):</t>
+  </si>
+  <si>
+    <t>Number of EVs without subsidy:</t>
+  </si>
+  <si>
+    <t>Number of EVs with subsidy:</t>
+  </si>
+  <si>
+    <t>Emissions from conventional car:</t>
+  </si>
+  <si>
+    <t>(lb CO2/year)</t>
+  </si>
+  <si>
+    <t>(lb CO2/car/year)</t>
+  </si>
+  <si>
+    <t>CO2 Emissions without Subsidy:</t>
+  </si>
+  <si>
+    <t>CO2 Emissions with Subsidy:</t>
+  </si>
+  <si>
+    <t># of conventional cars with subsidy:</t>
+  </si>
+  <si>
+    <t># of conventional cars w/o subsidy:</t>
   </si>
 </sst>
 </file>
@@ -499,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -560,6 +591,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,19 +627,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -596,21 +642,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,7 +928,7 @@
   <dimension ref="A1:AG91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -910,14 +943,16 @@
     <col min="16" max="16" width="9" customWidth="1"/>
     <col min="17" max="17" width="13.26953125" customWidth="1"/>
     <col min="18" max="18" width="9.54296875" customWidth="1"/>
-    <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="22" max="22" width="16.36328125" customWidth="1"/>
+    <col min="19" max="19" width="10.54296875" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" customWidth="1"/>
+    <col min="21" max="21" width="10.54296875" customWidth="1"/>
+    <col min="22" max="22" width="16.7265625" customWidth="1"/>
     <col min="23" max="24" width="16.26953125" customWidth="1"/>
     <col min="25" max="25" width="16.1796875" customWidth="1"/>
     <col min="26" max="26" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -947,8 +982,16 @@
       <c r="Q1" s="26">
         <v>2221460.4</v>
       </c>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S1" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="26">
+        <v>8809340386.1000004</v>
+      </c>
+    </row>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
@@ -979,8 +1022,16 @@
       <c r="Q2" s="26">
         <v>19867.2</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S2" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="47">
+        <v>348494.96600000001</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1004,8 +1055,16 @@
       <c r="Q3" s="26">
         <v>1596613.3</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S3" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="48">
+        <v>2066077.2990000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1029,8 +1088,17 @@
       <c r="Q4" s="26">
         <v>43560</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S4" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="47">
+        <f>0.86*2489249.757</f>
+        <v>2140754.7910200004</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="E5" s="29" t="s">
         <v>94</v>
@@ -1048,8 +1116,17 @@
       <c r="Q5" s="28">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S5" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="47">
+        <f>0.17*2489249.757</f>
+        <v>423172.45869000006</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I6" s="4"/>
       <c r="N6" s="29" t="s">
         <v>92</v>
@@ -1059,8 +1136,48 @@
       <c r="Q6" s="28">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="S6" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="T6" s="29"/>
+      <c r="U6" s="29"/>
+      <c r="V6" s="47">
+        <f>(18000/25)*8.8*2.20462</f>
+        <v>13968.472320000001</v>
+      </c>
+      <c r="W6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="S7" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="T7" s="29"/>
+      <c r="U7" s="29"/>
+      <c r="V7" s="47">
+        <f>V4*V6</f>
+        <v>29903074042.27026</v>
+      </c>
+      <c r="W7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="S8" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="T8" s="29"/>
+      <c r="U8" s="29"/>
+      <c r="V8" s="47">
+        <f>V5*V6</f>
+        <v>5911072775.7976093</v>
+      </c>
+      <c r="W8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
       <c r="C9" s="29" t="s">
         <v>29</v>
       </c>
@@ -1068,7 +1185,7 @@
       <c r="E9" s="29"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>30</v>
       </c>
@@ -1085,7 +1202,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>2020</v>
       </c>
@@ -1106,7 +1223,7 @@
         <v>4765</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
         <v>2021</v>
       </c>
@@ -1127,7 +1244,7 @@
         <v>4807.8849999999993</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>2022</v>
       </c>
@@ -1148,7 +1265,7 @@
         <v>4851.155964999999</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>2023</v>
       </c>
@@ -1169,7 +1286,7 @@
         <v>4894.8163686849985</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>2024</v>
       </c>
@@ -1190,7 +1307,7 @@
         <v>4938.8697160031634</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>2025</v>
       </c>
@@ -1649,17 +1766,17 @@
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C40" s="46" t="s">
+      <c r="C40" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
       <c r="F40" s="2"/>
-      <c r="H40" s="46" t="s">
+      <c r="H40" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
       <c r="O40" s="4"/>
@@ -1860,40 +1977,40 @@
       <c r="S47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V47" s="45" t="s">
+      <c r="V47" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="W47" s="45" t="s">
+      <c r="W47" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="X47" s="45" t="s">
+      <c r="X47" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="Y47" s="45" t="s">
+      <c r="Y47" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="Z47" s="45" t="s">
+      <c r="Z47" s="30" t="s">
         <v>36</v>
       </c>
       <c r="AA47" s="13"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C48" s="46" t="s">
+      <c r="C48" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
       <c r="R48" t="s">
         <v>18</v>
       </c>
       <c r="S48" t="s">
         <v>21</v>
       </c>
-      <c r="V48" s="45"/>
-      <c r="W48" s="45"/>
-      <c r="X48" s="45"/>
-      <c r="Y48" s="45"/>
-      <c r="Z48" s="45"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
       <c r="AA48" s="13"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.35">
@@ -1927,11 +2044,11 @@
       <c r="U49" t="s">
         <v>10</v>
       </c>
-      <c r="V49" s="45"/>
-      <c r="W49" s="45"/>
-      <c r="X49" s="45"/>
-      <c r="Y49" s="45"/>
-      <c r="Z49" s="45"/>
+      <c r="V49" s="30"/>
+      <c r="W49" s="30"/>
+      <c r="X49" s="30"/>
+      <c r="Y49" s="30"/>
+      <c r="Z49" s="30"/>
       <c r="AA49" s="13"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.35">
@@ -3139,17 +3256,17 @@
       <c r="Z67" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AC67" s="42" t="s">
+      <c r="AC67" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="AD67" s="36" t="s">
+      <c r="AD67" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="AE67" s="36"/>
-      <c r="AF67" s="36" t="s">
+      <c r="AE67" s="34"/>
+      <c r="AF67" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="AG67" s="37"/>
+      <c r="AG67" s="43"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -3217,11 +3334,11 @@
       <c r="Z68" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AC68" s="43"/>
-      <c r="AD68" s="38"/>
-      <c r="AE68" s="38"/>
-      <c r="AF68" s="38"/>
-      <c r="AG68" s="39"/>
+      <c r="AC68" s="33"/>
+      <c r="AD68" s="35"/>
+      <c r="AE68" s="35"/>
+      <c r="AF68" s="35"/>
+      <c r="AG68" s="44"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -3365,14 +3482,14 @@
       <c r="AC70" s="19">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AD70" s="44">
+      <c r="AD70" s="36">
         <v>72154</v>
       </c>
-      <c r="AE70" s="44"/>
-      <c r="AF70" s="40">
+      <c r="AE70" s="36"/>
+      <c r="AF70" s="45">
         <v>28.1</v>
       </c>
-      <c r="AG70" s="41"/>
+      <c r="AG70" s="46"/>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -3446,14 +3563,14 @@
       <c r="AC71" s="21">
         <v>0.31</v>
       </c>
-      <c r="AD71" s="34">
+      <c r="AD71" s="37">
         <v>67811</v>
       </c>
-      <c r="AE71" s="34"/>
-      <c r="AF71" s="30">
+      <c r="AE71" s="37"/>
+      <c r="AF71" s="38">
         <v>25</v>
       </c>
-      <c r="AG71" s="31"/>
+      <c r="AG71" s="39"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
@@ -3527,14 +3644,14 @@
       <c r="AC72" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD72" s="34">
+      <c r="AD72" s="37">
         <v>187455</v>
       </c>
-      <c r="AE72" s="34"/>
-      <c r="AF72" s="30">
+      <c r="AE72" s="37"/>
+      <c r="AF72" s="38">
         <v>70</v>
       </c>
-      <c r="AG72" s="31"/>
+      <c r="AG72" s="39"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -3608,14 +3725,14 @@
       <c r="AC73" s="21">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AD73" s="34">
+      <c r="AD73" s="37">
         <v>63266</v>
       </c>
-      <c r="AE73" s="34"/>
-      <c r="AF73" s="30">
+      <c r="AE73" s="37"/>
+      <c r="AF73" s="38">
         <v>30.6</v>
       </c>
-      <c r="AG73" s="31"/>
+      <c r="AG73" s="39"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -3689,14 +3806,14 @@
       <c r="AC74" s="21">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AD74" s="34">
+      <c r="AD74" s="37">
         <v>26553</v>
       </c>
-      <c r="AE74" s="34"/>
-      <c r="AF74" s="30">
+      <c r="AE74" s="37"/>
+      <c r="AF74" s="38">
         <v>10</v>
       </c>
-      <c r="AG74" s="31"/>
+      <c r="AG74" s="39"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -3770,14 +3887,14 @@
       <c r="AC75" s="21">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AD75" s="34">
+      <c r="AD75" s="37">
         <v>24949</v>
       </c>
-      <c r="AE75" s="34"/>
-      <c r="AF75" s="30">
+      <c r="AE75" s="37"/>
+      <c r="AF75" s="38">
         <v>10</v>
       </c>
-      <c r="AG75" s="31"/>
+      <c r="AG75" s="39"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
@@ -3851,14 +3968,14 @@
       <c r="AC76" s="21">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AD76" s="34">
+      <c r="AD76" s="37">
         <v>22870</v>
       </c>
-      <c r="AE76" s="34"/>
-      <c r="AF76" s="30">
+      <c r="AE76" s="37"/>
+      <c r="AF76" s="38">
         <v>10</v>
       </c>
-      <c r="AG76" s="31"/>
+      <c r="AG76" s="39"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -3932,14 +4049,14 @@
       <c r="AC77" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD77" s="34">
+      <c r="AD77" s="37">
         <v>139836</v>
       </c>
-      <c r="AE77" s="34"/>
-      <c r="AF77" s="30">
+      <c r="AE77" s="37"/>
+      <c r="AF77" s="38">
         <v>52.2</v>
       </c>
-      <c r="AG77" s="31"/>
+      <c r="AG77" s="39"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -4013,14 +4130,14 @@
       <c r="AC78" s="21">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AD78" s="34">
+      <c r="AD78" s="37">
         <v>23515</v>
       </c>
-      <c r="AE78" s="34"/>
-      <c r="AF78" s="30">
+      <c r="AE78" s="37"/>
+      <c r="AF78" s="38">
         <v>10</v>
       </c>
-      <c r="AG78" s="31"/>
+      <c r="AG78" s="39"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
@@ -4094,14 +4211,14 @@
       <c r="AC79" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AD79" s="34">
+      <c r="AD79" s="37">
         <v>49503</v>
       </c>
-      <c r="AE79" s="34"/>
-      <c r="AF79" s="30">
+      <c r="AE79" s="37"/>
+      <c r="AF79" s="38">
         <v>20.2</v>
       </c>
-      <c r="AG79" s="31"/>
+      <c r="AG79" s="39"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -4175,14 +4292,14 @@
       <c r="AC80" s="21">
         <v>0.307</v>
       </c>
-      <c r="AD80" s="34">
+      <c r="AD80" s="37">
         <v>188420</v>
       </c>
-      <c r="AE80" s="34"/>
-      <c r="AF80" s="30">
+      <c r="AE80" s="37"/>
+      <c r="AF80" s="38">
         <v>70</v>
       </c>
-      <c r="AG80" s="31"/>
+      <c r="AG80" s="39"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
@@ -4256,14 +4373,14 @@
       <c r="AC81" s="21">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AD81" s="34">
+      <c r="AD81" s="37">
         <v>26573</v>
       </c>
-      <c r="AE81" s="34"/>
-      <c r="AF81" s="30">
+      <c r="AE81" s="37"/>
+      <c r="AF81" s="38">
         <v>10.5</v>
       </c>
-      <c r="AG81" s="31"/>
+      <c r="AG81" s="39"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
@@ -4337,14 +4454,14 @@
       <c r="AC82" s="21">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AD82" s="34">
+      <c r="AD82" s="37">
         <v>25253</v>
       </c>
-      <c r="AE82" s="34"/>
-      <c r="AF82" s="30">
+      <c r="AE82" s="37"/>
+      <c r="AF82" s="38">
         <v>10</v>
       </c>
-      <c r="AG82" s="31"/>
+      <c r="AG82" s="39"/>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -4418,14 +4535,14 @@
       <c r="AC83" s="21">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AD83" s="34">
+      <c r="AD83" s="37">
         <v>17610</v>
       </c>
-      <c r="AE83" s="34"/>
-      <c r="AF83" s="30">
+      <c r="AE83" s="37"/>
+      <c r="AF83" s="38">
         <v>10</v>
       </c>
-      <c r="AG83" s="31"/>
+      <c r="AG83" s="39"/>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -4499,14 +4616,14 @@
       <c r="AC84" s="21">
         <v>0.221</v>
       </c>
-      <c r="AD84" s="34">
+      <c r="AD84" s="37">
         <v>19372</v>
       </c>
-      <c r="AE84" s="34"/>
-      <c r="AF84" s="30">
+      <c r="AE84" s="37"/>
+      <c r="AF84" s="38">
         <v>10</v>
       </c>
-      <c r="AG84" s="31"/>
+      <c r="AG84" s="39"/>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
@@ -4580,14 +4697,14 @@
       <c r="AC85" s="21">
         <v>0.216</v>
       </c>
-      <c r="AD85" s="34">
+      <c r="AD85" s="37">
         <v>18939</v>
       </c>
-      <c r="AE85" s="34"/>
-      <c r="AF85" s="30">
+      <c r="AE85" s="37"/>
+      <c r="AF85" s="38">
         <v>10</v>
       </c>
-      <c r="AG85" s="31"/>
+      <c r="AG85" s="39"/>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -4661,14 +4778,14 @@
       <c r="AC86" s="21">
         <v>0.23</v>
       </c>
-      <c r="AD86" s="34">
+      <c r="AD86" s="37">
         <v>20382</v>
       </c>
-      <c r="AE86" s="34"/>
-      <c r="AF86" s="30">
+      <c r="AE86" s="37"/>
+      <c r="AF86" s="38">
         <v>10.1</v>
       </c>
-      <c r="AG86" s="31"/>
+      <c r="AG86" s="39"/>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -4742,14 +4859,14 @@
       <c r="AC87" s="21">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AD87" s="34">
+      <c r="AD87" s="37">
         <v>19968</v>
       </c>
-      <c r="AE87" s="34"/>
-      <c r="AF87" s="30">
+      <c r="AE87" s="37"/>
+      <c r="AF87" s="38">
         <v>10.1</v>
       </c>
-      <c r="AG87" s="31"/>
+      <c r="AG87" s="39"/>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -4823,14 +4940,14 @@
       <c r="AC88" s="21">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AD88" s="34">
+      <c r="AD88" s="37">
         <v>23240</v>
       </c>
-      <c r="AE88" s="34"/>
-      <c r="AF88" s="30">
+      <c r="AE88" s="37"/>
+      <c r="AF88" s="38">
         <v>10</v>
       </c>
-      <c r="AG88" s="31"/>
+      <c r="AG88" s="39"/>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
@@ -4904,14 +5021,14 @@
       <c r="AC89" s="23">
         <v>0.254</v>
       </c>
-      <c r="AD89" s="35">
+      <c r="AD89" s="42">
         <v>26709</v>
       </c>
-      <c r="AE89" s="35"/>
-      <c r="AF89" s="32">
+      <c r="AE89" s="42"/>
+      <c r="AF89" s="40">
         <v>12</v>
       </c>
-      <c r="AG89" s="33"/>
+      <c r="AG89" s="41"/>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -5046,51 +5163,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="W47:W49"/>
-    <mergeCell ref="X47:X49"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="Y47:Y49"/>
-    <mergeCell ref="Z47:Z49"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="V47:V49"/>
-    <mergeCell ref="AC67:AC68"/>
-    <mergeCell ref="AD67:AE68"/>
-    <mergeCell ref="AD70:AE70"/>
-    <mergeCell ref="AD71:AE71"/>
-    <mergeCell ref="AD72:AE72"/>
-    <mergeCell ref="AD73:AE73"/>
-    <mergeCell ref="AD74:AE74"/>
-    <mergeCell ref="AD75:AE75"/>
-    <mergeCell ref="AD76:AE76"/>
-    <mergeCell ref="AD77:AE77"/>
-    <mergeCell ref="AD85:AE85"/>
-    <mergeCell ref="AD86:AE86"/>
-    <mergeCell ref="AD87:AE87"/>
-    <mergeCell ref="AD78:AE78"/>
-    <mergeCell ref="AD79:AE79"/>
-    <mergeCell ref="AD80:AE80"/>
-    <mergeCell ref="AD81:AE81"/>
-    <mergeCell ref="AD82:AE82"/>
-    <mergeCell ref="AF79:AG79"/>
-    <mergeCell ref="AF80:AG80"/>
-    <mergeCell ref="AF81:AG81"/>
-    <mergeCell ref="AD83:AE83"/>
-    <mergeCell ref="AD84:AE84"/>
-    <mergeCell ref="AF74:AG74"/>
-    <mergeCell ref="AF75:AG75"/>
-    <mergeCell ref="AF76:AG76"/>
-    <mergeCell ref="AF77:AG77"/>
-    <mergeCell ref="AF78:AG78"/>
+  <mergeCells count="73">
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="AF87:AG87"/>
     <mergeCell ref="AF88:AG88"/>
@@ -5107,11 +5192,51 @@
     <mergeCell ref="AF71:AG71"/>
     <mergeCell ref="AF72:AG72"/>
     <mergeCell ref="AF73:AG73"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="AF74:AG74"/>
+    <mergeCell ref="AF75:AG75"/>
+    <mergeCell ref="AF76:AG76"/>
+    <mergeCell ref="AF77:AG77"/>
+    <mergeCell ref="AF78:AG78"/>
+    <mergeCell ref="AF79:AG79"/>
+    <mergeCell ref="AF80:AG80"/>
+    <mergeCell ref="AF81:AG81"/>
+    <mergeCell ref="AD83:AE83"/>
+    <mergeCell ref="AD84:AE84"/>
+    <mergeCell ref="AD85:AE85"/>
+    <mergeCell ref="AD86:AE86"/>
+    <mergeCell ref="AD87:AE87"/>
+    <mergeCell ref="AD78:AE78"/>
+    <mergeCell ref="AD79:AE79"/>
+    <mergeCell ref="AD80:AE80"/>
+    <mergeCell ref="AD81:AE81"/>
+    <mergeCell ref="AD82:AE82"/>
+    <mergeCell ref="AD73:AE73"/>
+    <mergeCell ref="AD74:AE74"/>
+    <mergeCell ref="AD75:AE75"/>
+    <mergeCell ref="AD76:AE76"/>
+    <mergeCell ref="AD77:AE77"/>
+    <mergeCell ref="AC67:AC68"/>
+    <mergeCell ref="AD67:AE68"/>
+    <mergeCell ref="AD70:AE70"/>
+    <mergeCell ref="AD71:AE71"/>
+    <mergeCell ref="AD72:AE72"/>
+    <mergeCell ref="Y47:Y49"/>
+    <mergeCell ref="Z47:Z49"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="V47:V49"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="W47:W49"/>
+    <mergeCell ref="X47:X49"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="S8:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more inputs etc
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -18,30 +18,30 @@
     <definedName name="BusDemand">Sheet2!$C$11:$E$36</definedName>
     <definedName name="CAPEX_solar">Sheet2!$Q$1</definedName>
     <definedName name="CAPEX_wind">Sheet2!$Q$3</definedName>
-    <definedName name="CH4_rate">Sheet2!$Y$50:$Y$91</definedName>
-    <definedName name="CO2_rate">Sheet2!$X$50:$X$91</definedName>
+    <definedName name="CH4_rate">Sheet2!$Y$50:$Y$92</definedName>
+    <definedName name="CO2_rate">Sheet2!$X$50:$X$92</definedName>
     <definedName name="DiscRate">Sheet2!$G$1</definedName>
     <definedName name="EV_subsidy_cost">Sheet2!$V$1</definedName>
     <definedName name="LineCapacity">Sheet2!$P$42:$P$44</definedName>
     <definedName name="LineFromBus">Sheet2!$H$42:$J$44</definedName>
     <definedName name="LineReactance">Sheet2!$M$42:$M$44</definedName>
     <definedName name="LineToBus">Sheet2!$C$42:$E$44</definedName>
-    <definedName name="MarginalC">Sheet2!$N$50:$N$91</definedName>
+    <definedName name="MarginalC">Sheet2!$N$50:$N$92</definedName>
     <definedName name="maxCO2">Sheet2!$L$2</definedName>
-    <definedName name="MaxGen">Sheet2!$H$50:$H$91</definedName>
-    <definedName name="MinGen">Sheet2!$K$50:$K$91</definedName>
-    <definedName name="N2O_rate">Sheet2!$Z$50:$Z$91</definedName>
-    <definedName name="NOx_rate">Sheet2!$V$50:$V$91</definedName>
+    <definedName name="MaxGen">Sheet2!$H$50:$H$92</definedName>
+    <definedName name="MinGen">Sheet2!$K$50:$K$92</definedName>
+    <definedName name="N2O_rate">Sheet2!$Z$50:$Z$92</definedName>
+    <definedName name="NOx_rate">Sheet2!$V$50:$V$92</definedName>
     <definedName name="NumBuses">Sheet2!$C$1</definedName>
     <definedName name="NumLines">Sheet2!$C$2</definedName>
     <definedName name="NumUnits">Sheet2!$C$3</definedName>
     <definedName name="NumYears">Sheet2!$C$4</definedName>
     <definedName name="OPEX_solar">Sheet2!$Q$2</definedName>
     <definedName name="OPEX_wind">Sheet2!$Q$4</definedName>
-    <definedName name="SO2_rate">Sheet2!$W$50:$W$91</definedName>
+    <definedName name="SO2_rate">Sheet2!$W$50:$W$92</definedName>
     <definedName name="solar_cap_factor">Sheet2!$G$4</definedName>
     <definedName name="solar_inc">Sheet2!$Q$5</definedName>
-    <definedName name="UnitsByBus">Sheet2!$C$50:$E$91</definedName>
+    <definedName name="UnitsByBus">Sheet2!$C$50:$E$92</definedName>
     <definedName name="wind_cap_factor">Sheet2!$G$5</definedName>
     <definedName name="wind_inc">Sheet2!$Q$6</definedName>
   </definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>NumBuses</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>(in 2045)</t>
+  </si>
+  <si>
+    <t>STOR</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -593,7 +596,34 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -608,19 +638,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -630,21 +651,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -928,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG91"/>
+  <dimension ref="A1:AG92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -962,34 +968,34 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="31"/>
+      <c r="F1" s="32"/>
       <c r="G1" s="16">
         <v>0.1</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
       <c r="L1" s="17">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
       <c r="Q1" s="26">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
       <c r="V1" s="26">
         <v>8809340386.1000004</v>
       </c>
@@ -1001,35 +1007,35 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="31"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="6">
         <v>4765</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="25">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="31" t="s">
+      <c r="N2" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
       <c r="Q2" s="26">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="31" t="s">
+      <c r="S2" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
       <c r="V2" s="29">
         <v>348494.96600000001</v>
       </c>
@@ -1042,30 +1048,30 @@
         <v>2</v>
       </c>
       <c r="C3" s="6">
-        <v>42</v>
-      </c>
-      <c r="E3" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="31"/>
+      <c r="F3" s="32"/>
       <c r="G3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I3" s="4"/>
       <c r="L3" s="27"/>
-      <c r="N3" s="31" t="s">
+      <c r="N3" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
       <c r="Q3" s="26">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="31" t="s">
+      <c r="S3" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="T3" s="31"/>
-      <c r="U3" s="31"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
       <c r="V3" s="30">
         <v>2066077.2990000001</v>
       </c>
@@ -1081,27 +1087,27 @@
         <v>26</v>
       </c>
       <c r="D4" s="15"/>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="31"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="17">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="N4" s="31" t="s">
+      <c r="N4" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
       <c r="Q4" s="26">
         <v>43560</v>
       </c>
-      <c r="S4" s="31" t="s">
+      <c r="S4" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="T4" s="31"/>
-      <c r="U4" s="31"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
       <c r="V4" s="29">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1112,27 +1118,27 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="17">
         <v>1</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="N5" s="31" t="s">
+      <c r="N5" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
       <c r="Q5" s="28">
         <v>50</v>
       </c>
-      <c r="S5" s="31" t="s">
+      <c r="S5" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
       <c r="V5" s="29">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1143,19 +1149,19 @@
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I6" s="4"/>
-      <c r="N6" s="31" t="s">
+      <c r="N6" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" s="31"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
       <c r="Q6" s="28">
         <v>10</v>
       </c>
-      <c r="S6" s="31" t="s">
+      <c r="S6" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
       <c r="V6" s="29">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1165,11 +1171,11 @@
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="S7" s="31" t="s">
+      <c r="S7" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
       <c r="V7" s="29">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1179,11 +1185,11 @@
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="S8" s="31" t="s">
+      <c r="S8" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
       <c r="V8" s="29">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1193,11 +1199,11 @@
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.35">
@@ -1781,17 +1787,17 @@
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
       <c r="F40" s="2"/>
-      <c r="H40" s="48" t="s">
+      <c r="H40" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
       <c r="O40" s="4"/>
@@ -1992,40 +1998,40 @@
       <c r="S47" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V47" s="47" t="s">
+      <c r="V47" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="W47" s="47" t="s">
+      <c r="W47" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="X47" s="47" t="s">
+      <c r="X47" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="Y47" s="47" t="s">
+      <c r="Y47" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="Z47" s="47" t="s">
+      <c r="Z47" s="33" t="s">
         <v>36</v>
       </c>
       <c r="AA47" s="13"/>
     </row>
     <row r="48" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="C48" s="48" t="s">
+      <c r="C48" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
       <c r="R48" t="s">
         <v>18</v>
       </c>
       <c r="S48" t="s">
         <v>21</v>
       </c>
-      <c r="V48" s="47"/>
-      <c r="W48" s="47"/>
-      <c r="X48" s="47"/>
-      <c r="Y48" s="47"/>
-      <c r="Z48" s="47"/>
+      <c r="V48" s="33"/>
+      <c r="W48" s="33"/>
+      <c r="X48" s="33"/>
+      <c r="Y48" s="33"/>
+      <c r="Z48" s="33"/>
       <c r="AA48" s="13"/>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.35">
@@ -2059,11 +2065,11 @@
       <c r="U49" t="s">
         <v>10</v>
       </c>
-      <c r="V49" s="47"/>
-      <c r="W49" s="47"/>
-      <c r="X49" s="47"/>
-      <c r="Y49" s="47"/>
-      <c r="Z49" s="47"/>
+      <c r="V49" s="33"/>
+      <c r="W49" s="33"/>
+      <c r="X49" s="33"/>
+      <c r="Y49" s="33"/>
+      <c r="Z49" s="33"/>
       <c r="AA49" s="13"/>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.35">
@@ -2165,7 +2171,7 @@
         <v>2</v>
       </c>
       <c r="N51" s="8">
-        <f t="shared" ref="N51:N91" si="4">R51*S51*1000/1000000</f>
+        <f t="shared" ref="N51:N92" si="4">R51*S51*1000/1000000</f>
         <v>23.617080000000001</v>
       </c>
       <c r="P51" s="3">
@@ -3271,17 +3277,17 @@
       <c r="Z67" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AC67" s="44" t="s">
+      <c r="AC67" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="AD67" s="38" t="s">
+      <c r="AD67" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="AE67" s="38"/>
-      <c r="AF67" s="38" t="s">
+      <c r="AE67" s="37"/>
+      <c r="AF67" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="AG67" s="39"/>
+      <c r="AG67" s="46"/>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -3349,11 +3355,11 @@
       <c r="Z68" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AC68" s="45"/>
-      <c r="AD68" s="40"/>
-      <c r="AE68" s="40"/>
-      <c r="AF68" s="40"/>
-      <c r="AG68" s="41"/>
+      <c r="AC68" s="36"/>
+      <c r="AD68" s="38"/>
+      <c r="AE68" s="38"/>
+      <c r="AF68" s="38"/>
+      <c r="AG68" s="47"/>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -3497,14 +3503,14 @@
       <c r="AC70" s="19">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AD70" s="46">
+      <c r="AD70" s="39">
         <v>72154</v>
       </c>
-      <c r="AE70" s="46"/>
-      <c r="AF70" s="42">
+      <c r="AE70" s="39"/>
+      <c r="AF70" s="48">
         <v>28.1</v>
       </c>
-      <c r="AG70" s="43"/>
+      <c r="AG70" s="49"/>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -3578,14 +3584,14 @@
       <c r="AC71" s="21">
         <v>0.31</v>
       </c>
-      <c r="AD71" s="36">
+      <c r="AD71" s="40">
         <v>67811</v>
       </c>
-      <c r="AE71" s="36"/>
-      <c r="AF71" s="32">
+      <c r="AE71" s="40"/>
+      <c r="AF71" s="41">
         <v>25</v>
       </c>
-      <c r="AG71" s="33"/>
+      <c r="AG71" s="42"/>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
@@ -3659,14 +3665,14 @@
       <c r="AC72" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD72" s="36">
+      <c r="AD72" s="40">
         <v>187455</v>
       </c>
-      <c r="AE72" s="36"/>
-      <c r="AF72" s="32">
+      <c r="AE72" s="40"/>
+      <c r="AF72" s="41">
         <v>70</v>
       </c>
-      <c r="AG72" s="33"/>
+      <c r="AG72" s="42"/>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -3740,14 +3746,14 @@
       <c r="AC73" s="21">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AD73" s="36">
+      <c r="AD73" s="40">
         <v>63266</v>
       </c>
-      <c r="AE73" s="36"/>
-      <c r="AF73" s="32">
+      <c r="AE73" s="40"/>
+      <c r="AF73" s="41">
         <v>30.6</v>
       </c>
-      <c r="AG73" s="33"/>
+      <c r="AG73" s="42"/>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -3821,14 +3827,14 @@
       <c r="AC74" s="21">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AD74" s="36">
+      <c r="AD74" s="40">
         <v>26553</v>
       </c>
-      <c r="AE74" s="36"/>
-      <c r="AF74" s="32">
+      <c r="AE74" s="40"/>
+      <c r="AF74" s="41">
         <v>10</v>
       </c>
-      <c r="AG74" s="33"/>
+      <c r="AG74" s="42"/>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -3902,14 +3908,14 @@
       <c r="AC75" s="21">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AD75" s="36">
+      <c r="AD75" s="40">
         <v>24949</v>
       </c>
-      <c r="AE75" s="36"/>
-      <c r="AF75" s="32">
+      <c r="AE75" s="40"/>
+      <c r="AF75" s="41">
         <v>10</v>
       </c>
-      <c r="AG75" s="33"/>
+      <c r="AG75" s="42"/>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
@@ -3983,14 +3989,14 @@
       <c r="AC76" s="21">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AD76" s="36">
+      <c r="AD76" s="40">
         <v>22870</v>
       </c>
-      <c r="AE76" s="36"/>
-      <c r="AF76" s="32">
+      <c r="AE76" s="40"/>
+      <c r="AF76" s="41">
         <v>10</v>
       </c>
-      <c r="AG76" s="33"/>
+      <c r="AG76" s="42"/>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -4064,14 +4070,14 @@
       <c r="AC77" s="21">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AD77" s="36">
+      <c r="AD77" s="40">
         <v>139836</v>
       </c>
-      <c r="AE77" s="36"/>
-      <c r="AF77" s="32">
+      <c r="AE77" s="40"/>
+      <c r="AF77" s="41">
         <v>52.2</v>
       </c>
-      <c r="AG77" s="33"/>
+      <c r="AG77" s="42"/>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -4145,14 +4151,14 @@
       <c r="AC78" s="21">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AD78" s="36">
+      <c r="AD78" s="40">
         <v>23515</v>
       </c>
-      <c r="AE78" s="36"/>
-      <c r="AF78" s="32">
+      <c r="AE78" s="40"/>
+      <c r="AF78" s="41">
         <v>10</v>
       </c>
-      <c r="AG78" s="33"/>
+      <c r="AG78" s="42"/>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
@@ -4226,14 +4232,14 @@
       <c r="AC79" s="21">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AD79" s="36">
+      <c r="AD79" s="40">
         <v>49503</v>
       </c>
-      <c r="AE79" s="36"/>
-      <c r="AF79" s="32">
+      <c r="AE79" s="40"/>
+      <c r="AF79" s="41">
         <v>20.2</v>
       </c>
-      <c r="AG79" s="33"/>
+      <c r="AG79" s="42"/>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -4307,14 +4313,14 @@
       <c r="AC80" s="21">
         <v>0.307</v>
       </c>
-      <c r="AD80" s="36">
+      <c r="AD80" s="40">
         <v>188420</v>
       </c>
-      <c r="AE80" s="36"/>
-      <c r="AF80" s="32">
+      <c r="AE80" s="40"/>
+      <c r="AF80" s="41">
         <v>70</v>
       </c>
-      <c r="AG80" s="33"/>
+      <c r="AG80" s="42"/>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
@@ -4388,14 +4394,14 @@
       <c r="AC81" s="21">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AD81" s="36">
+      <c r="AD81" s="40">
         <v>26573</v>
       </c>
-      <c r="AE81" s="36"/>
-      <c r="AF81" s="32">
+      <c r="AE81" s="40"/>
+      <c r="AF81" s="41">
         <v>10.5</v>
       </c>
-      <c r="AG81" s="33"/>
+      <c r="AG81" s="42"/>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
@@ -4469,14 +4475,14 @@
       <c r="AC82" s="21">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AD82" s="36">
+      <c r="AD82" s="40">
         <v>25253</v>
       </c>
-      <c r="AE82" s="36"/>
-      <c r="AF82" s="32">
+      <c r="AE82" s="40"/>
+      <c r="AF82" s="41">
         <v>10</v>
       </c>
-      <c r="AG82" s="33"/>
+      <c r="AG82" s="42"/>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -4550,14 +4556,14 @@
       <c r="AC83" s="21">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AD83" s="36">
+      <c r="AD83" s="40">
         <v>17610</v>
       </c>
-      <c r="AE83" s="36"/>
-      <c r="AF83" s="32">
+      <c r="AE83" s="40"/>
+      <c r="AF83" s="41">
         <v>10</v>
       </c>
-      <c r="AG83" s="33"/>
+      <c r="AG83" s="42"/>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -4631,14 +4637,14 @@
       <c r="AC84" s="21">
         <v>0.221</v>
       </c>
-      <c r="AD84" s="36">
+      <c r="AD84" s="40">
         <v>19372</v>
       </c>
-      <c r="AE84" s="36"/>
-      <c r="AF84" s="32">
+      <c r="AE84" s="40"/>
+      <c r="AF84" s="41">
         <v>10</v>
       </c>
-      <c r="AG84" s="33"/>
+      <c r="AG84" s="42"/>
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
@@ -4712,14 +4718,14 @@
       <c r="AC85" s="21">
         <v>0.216</v>
       </c>
-      <c r="AD85" s="36">
+      <c r="AD85" s="40">
         <v>18939</v>
       </c>
-      <c r="AE85" s="36"/>
-      <c r="AF85" s="32">
+      <c r="AE85" s="40"/>
+      <c r="AF85" s="41">
         <v>10</v>
       </c>
-      <c r="AG85" s="33"/>
+      <c r="AG85" s="42"/>
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -4793,14 +4799,14 @@
       <c r="AC86" s="21">
         <v>0.23</v>
       </c>
-      <c r="AD86" s="36">
+      <c r="AD86" s="40">
         <v>20382</v>
       </c>
-      <c r="AE86" s="36"/>
-      <c r="AF86" s="32">
+      <c r="AE86" s="40"/>
+      <c r="AF86" s="41">
         <v>10.1</v>
       </c>
-      <c r="AG86" s="33"/>
+      <c r="AG86" s="42"/>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -4874,14 +4880,14 @@
       <c r="AC87" s="21">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AD87" s="36">
+      <c r="AD87" s="40">
         <v>19968</v>
       </c>
-      <c r="AE87" s="36"/>
-      <c r="AF87" s="32">
+      <c r="AE87" s="40"/>
+      <c r="AF87" s="41">
         <v>10.1</v>
       </c>
-      <c r="AG87" s="33"/>
+      <c r="AG87" s="42"/>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -4955,14 +4961,14 @@
       <c r="AC88" s="21">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AD88" s="36">
+      <c r="AD88" s="40">
         <v>23240</v>
       </c>
-      <c r="AE88" s="36"/>
-      <c r="AF88" s="32">
+      <c r="AE88" s="40"/>
+      <c r="AF88" s="41">
         <v>10</v>
       </c>
-      <c r="AG88" s="33"/>
+      <c r="AG88" s="42"/>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
@@ -5036,14 +5042,14 @@
       <c r="AC89" s="23">
         <v>0.254</v>
       </c>
-      <c r="AD89" s="37">
+      <c r="AD89" s="45">
         <v>26709</v>
       </c>
-      <c r="AE89" s="37"/>
-      <c r="AF89" s="34">
+      <c r="AE89" s="45"/>
+      <c r="AF89" s="43">
         <v>12</v>
       </c>
-      <c r="AG89" s="35"/>
+      <c r="AG89" s="44"/>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -5177,53 +5183,83 @@
         <v>0</v>
       </c>
     </row>
+    <row r="92" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="31">
+        <v>43</v>
+      </c>
+      <c r="C92" s="6">
+        <v>0</v>
+      </c>
+      <c r="D92" s="6">
+        <v>1</v>
+      </c>
+      <c r="E92" s="6">
+        <v>0</v>
+      </c>
+      <c r="G92" s="31">
+        <v>43</v>
+      </c>
+      <c r="H92" s="6">
+        <v>0</v>
+      </c>
+      <c r="J92" s="31">
+        <v>43</v>
+      </c>
+      <c r="K92" s="6">
+        <v>0</v>
+      </c>
+      <c r="M92" s="31">
+        <v>43</v>
+      </c>
+      <c r="N92" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P92" s="31">
+        <v>43</v>
+      </c>
+      <c r="R92" s="6">
+        <v>0</v>
+      </c>
+      <c r="S92" s="6">
+        <v>0</v>
+      </c>
+      <c r="U92" s="31">
+        <v>43</v>
+      </c>
+      <c r="V92" s="6">
+        <v>0</v>
+      </c>
+      <c r="W92" s="6">
+        <v>0</v>
+      </c>
+      <c r="X92" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="6">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="W47:W49"/>
-    <mergeCell ref="X47:X49"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="Y47:Y49"/>
-    <mergeCell ref="Z47:Z49"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="V47:V49"/>
-    <mergeCell ref="AC67:AC68"/>
-    <mergeCell ref="AD67:AE68"/>
-    <mergeCell ref="AD70:AE70"/>
-    <mergeCell ref="AD71:AE71"/>
-    <mergeCell ref="AD72:AE72"/>
-    <mergeCell ref="AD73:AE73"/>
-    <mergeCell ref="AD74:AE74"/>
-    <mergeCell ref="AD75:AE75"/>
-    <mergeCell ref="AD76:AE76"/>
-    <mergeCell ref="AD77:AE77"/>
-    <mergeCell ref="AD85:AE85"/>
-    <mergeCell ref="AD86:AE86"/>
-    <mergeCell ref="AD87:AE87"/>
-    <mergeCell ref="AD78:AE78"/>
-    <mergeCell ref="AD79:AE79"/>
-    <mergeCell ref="AD80:AE80"/>
-    <mergeCell ref="AD81:AE81"/>
-    <mergeCell ref="AD82:AE82"/>
-    <mergeCell ref="AF79:AG79"/>
-    <mergeCell ref="AF80:AG80"/>
-    <mergeCell ref="AF81:AG81"/>
-    <mergeCell ref="AD83:AE83"/>
-    <mergeCell ref="AD84:AE84"/>
-    <mergeCell ref="AF74:AG74"/>
-    <mergeCell ref="AF75:AG75"/>
-    <mergeCell ref="AF76:AG76"/>
-    <mergeCell ref="AF77:AG77"/>
-    <mergeCell ref="AF78:AG78"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="AF87:AG87"/>
     <mergeCell ref="AF88:AG88"/>
@@ -5240,18 +5276,51 @@
     <mergeCell ref="AF71:AG71"/>
     <mergeCell ref="AF72:AG72"/>
     <mergeCell ref="AF73:AG73"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="AF74:AG74"/>
+    <mergeCell ref="AF75:AG75"/>
+    <mergeCell ref="AF76:AG76"/>
+    <mergeCell ref="AF77:AG77"/>
+    <mergeCell ref="AF78:AG78"/>
+    <mergeCell ref="AF79:AG79"/>
+    <mergeCell ref="AF80:AG80"/>
+    <mergeCell ref="AF81:AG81"/>
+    <mergeCell ref="AD83:AE83"/>
+    <mergeCell ref="AD84:AE84"/>
+    <mergeCell ref="AD85:AE85"/>
+    <mergeCell ref="AD86:AE86"/>
+    <mergeCell ref="AD87:AE87"/>
+    <mergeCell ref="AD78:AE78"/>
+    <mergeCell ref="AD79:AE79"/>
+    <mergeCell ref="AD80:AE80"/>
+    <mergeCell ref="AD81:AE81"/>
+    <mergeCell ref="AD82:AE82"/>
+    <mergeCell ref="AD73:AE73"/>
+    <mergeCell ref="AD74:AE74"/>
+    <mergeCell ref="AD75:AE75"/>
+    <mergeCell ref="AD76:AE76"/>
+    <mergeCell ref="AD77:AE77"/>
+    <mergeCell ref="AC67:AC68"/>
+    <mergeCell ref="AD67:AE68"/>
+    <mergeCell ref="AD70:AE70"/>
+    <mergeCell ref="AD71:AE71"/>
+    <mergeCell ref="AD72:AE72"/>
+    <mergeCell ref="Y47:Y49"/>
+    <mergeCell ref="Z47:Z49"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="V47:V49"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="W47:W49"/>
+    <mergeCell ref="X47:X49"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="S8:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Full dispatch of Off-Peak
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -627,27 +627,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,10 +639,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -673,6 +661,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N98" sqref="N98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2345,17 +2345,17 @@
       </c>
     </row>
     <row r="40" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
       <c r="F40" s="2"/>
-      <c r="H40" s="35" t="s">
+      <c r="H40" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="35"/>
-      <c r="J40" s="35"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="50"/>
       <c r="K40" s="2"/>
       <c r="L40" s="4"/>
       <c r="O40" s="4"/>
@@ -2578,11 +2578,11 @@
       <c r="AD47" s="12"/>
     </row>
     <row r="48" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
       <c r="U48" t="s">
         <v>17</v>
       </c>
@@ -3950,17 +3950,17 @@
       <c r="AC67" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AF67" s="36" t="s">
+      <c r="AF67" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="AG67" s="38" t="s">
+      <c r="AG67" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="AH67" s="38"/>
-      <c r="AI67" s="38" t="s">
+      <c r="AH67" s="41"/>
+      <c r="AI67" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="AJ67" s="47"/>
+      <c r="AJ67" s="42"/>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -4034,11 +4034,11 @@
       <c r="AC68" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AF68" s="37"/>
-      <c r="AG68" s="39"/>
-      <c r="AH68" s="39"/>
-      <c r="AI68" s="39"/>
-      <c r="AJ68" s="48"/>
+      <c r="AF68" s="48"/>
+      <c r="AG68" s="43"/>
+      <c r="AH68" s="43"/>
+      <c r="AI68" s="43"/>
+      <c r="AJ68" s="44"/>
     </row>
     <row r="69" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -4195,14 +4195,14 @@
       <c r="AF70" s="18">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AG70" s="40">
+      <c r="AG70" s="49">
         <v>72154</v>
       </c>
-      <c r="AH70" s="40"/>
-      <c r="AI70" s="49">
+      <c r="AH70" s="49"/>
+      <c r="AI70" s="45">
         <v>28.1</v>
       </c>
-      <c r="AJ70" s="50"/>
+      <c r="AJ70" s="46"/>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -4283,14 +4283,14 @@
       <c r="AF71" s="20">
         <v>0.31</v>
       </c>
-      <c r="AG71" s="41">
+      <c r="AG71" s="39">
         <v>67811</v>
       </c>
-      <c r="AH71" s="41"/>
-      <c r="AI71" s="42">
+      <c r="AH71" s="39"/>
+      <c r="AI71" s="35">
         <v>25</v>
       </c>
-      <c r="AJ71" s="43"/>
+      <c r="AJ71" s="36"/>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
@@ -4371,14 +4371,14 @@
       <c r="AF72" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG72" s="41">
+      <c r="AG72" s="39">
         <v>187455</v>
       </c>
-      <c r="AH72" s="41"/>
-      <c r="AI72" s="42">
+      <c r="AH72" s="39"/>
+      <c r="AI72" s="35">
         <v>70</v>
       </c>
-      <c r="AJ72" s="43"/>
+      <c r="AJ72" s="36"/>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -4459,14 +4459,14 @@
       <c r="AF73" s="20">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AG73" s="41">
+      <c r="AG73" s="39">
         <v>63266</v>
       </c>
-      <c r="AH73" s="41"/>
-      <c r="AI73" s="42">
+      <c r="AH73" s="39"/>
+      <c r="AI73" s="35">
         <v>30.6</v>
       </c>
-      <c r="AJ73" s="43"/>
+      <c r="AJ73" s="36"/>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -4547,14 +4547,14 @@
       <c r="AF74" s="20">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AG74" s="41">
+      <c r="AG74" s="39">
         <v>26553</v>
       </c>
-      <c r="AH74" s="41"/>
-      <c r="AI74" s="42">
+      <c r="AH74" s="39"/>
+      <c r="AI74" s="35">
         <v>10</v>
       </c>
-      <c r="AJ74" s="43"/>
+      <c r="AJ74" s="36"/>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -4635,14 +4635,14 @@
       <c r="AF75" s="20">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AG75" s="41">
+      <c r="AG75" s="39">
         <v>24949</v>
       </c>
-      <c r="AH75" s="41"/>
-      <c r="AI75" s="42">
+      <c r="AH75" s="39"/>
+      <c r="AI75" s="35">
         <v>10</v>
       </c>
-      <c r="AJ75" s="43"/>
+      <c r="AJ75" s="36"/>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
@@ -4723,14 +4723,14 @@
       <c r="AF76" s="20">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AG76" s="41">
+      <c r="AG76" s="39">
         <v>22870</v>
       </c>
-      <c r="AH76" s="41"/>
-      <c r="AI76" s="42">
+      <c r="AH76" s="39"/>
+      <c r="AI76" s="35">
         <v>10</v>
       </c>
-      <c r="AJ76" s="43"/>
+      <c r="AJ76" s="36"/>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -4811,14 +4811,14 @@
       <c r="AF77" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG77" s="41">
+      <c r="AG77" s="39">
         <v>139836</v>
       </c>
-      <c r="AH77" s="41"/>
-      <c r="AI77" s="42">
+      <c r="AH77" s="39"/>
+      <c r="AI77" s="35">
         <v>52.2</v>
       </c>
-      <c r="AJ77" s="43"/>
+      <c r="AJ77" s="36"/>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -4899,14 +4899,14 @@
       <c r="AF78" s="20">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AG78" s="41">
+      <c r="AG78" s="39">
         <v>23515</v>
       </c>
-      <c r="AH78" s="41"/>
-      <c r="AI78" s="42">
+      <c r="AH78" s="39"/>
+      <c r="AI78" s="35">
         <v>10</v>
       </c>
-      <c r="AJ78" s="43"/>
+      <c r="AJ78" s="36"/>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
@@ -4987,14 +4987,14 @@
       <c r="AF79" s="20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AG79" s="41">
+      <c r="AG79" s="39">
         <v>49503</v>
       </c>
-      <c r="AH79" s="41"/>
-      <c r="AI79" s="42">
+      <c r="AH79" s="39"/>
+      <c r="AI79" s="35">
         <v>20.2</v>
       </c>
-      <c r="AJ79" s="43"/>
+      <c r="AJ79" s="36"/>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -5075,14 +5075,14 @@
       <c r="AF80" s="20">
         <v>0.307</v>
       </c>
-      <c r="AG80" s="41">
+      <c r="AG80" s="39">
         <v>188420</v>
       </c>
-      <c r="AH80" s="41"/>
-      <c r="AI80" s="42">
+      <c r="AH80" s="39"/>
+      <c r="AI80" s="35">
         <v>70</v>
       </c>
-      <c r="AJ80" s="43"/>
+      <c r="AJ80" s="36"/>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
@@ -5163,14 +5163,14 @@
       <c r="AF81" s="20">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AG81" s="41">
+      <c r="AG81" s="39">
         <v>26573</v>
       </c>
-      <c r="AH81" s="41"/>
-      <c r="AI81" s="42">
+      <c r="AH81" s="39"/>
+      <c r="AI81" s="35">
         <v>10.5</v>
       </c>
-      <c r="AJ81" s="43"/>
+      <c r="AJ81" s="36"/>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
@@ -5251,14 +5251,14 @@
       <c r="AF82" s="20">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AG82" s="41">
+      <c r="AG82" s="39">
         <v>25253</v>
       </c>
-      <c r="AH82" s="41"/>
-      <c r="AI82" s="42">
+      <c r="AH82" s="39"/>
+      <c r="AI82" s="35">
         <v>10</v>
       </c>
-      <c r="AJ82" s="43"/>
+      <c r="AJ82" s="36"/>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -5339,14 +5339,14 @@
       <c r="AF83" s="20">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AG83" s="41">
+      <c r="AG83" s="39">
         <v>17610</v>
       </c>
-      <c r="AH83" s="41"/>
-      <c r="AI83" s="42">
+      <c r="AH83" s="39"/>
+      <c r="AI83" s="35">
         <v>10</v>
       </c>
-      <c r="AJ83" s="43"/>
+      <c r="AJ83" s="36"/>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -5427,14 +5427,14 @@
       <c r="AF84" s="20">
         <v>0.221</v>
       </c>
-      <c r="AG84" s="41">
+      <c r="AG84" s="39">
         <v>19372</v>
       </c>
-      <c r="AH84" s="41"/>
-      <c r="AI84" s="42">
+      <c r="AH84" s="39"/>
+      <c r="AI84" s="35">
         <v>10</v>
       </c>
-      <c r="AJ84" s="43"/>
+      <c r="AJ84" s="36"/>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
@@ -5515,14 +5515,14 @@
       <c r="AF85" s="20">
         <v>0.216</v>
       </c>
-      <c r="AG85" s="41">
+      <c r="AG85" s="39">
         <v>18939</v>
       </c>
-      <c r="AH85" s="41"/>
-      <c r="AI85" s="42">
+      <c r="AH85" s="39"/>
+      <c r="AI85" s="35">
         <v>10</v>
       </c>
-      <c r="AJ85" s="43"/>
+      <c r="AJ85" s="36"/>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -5603,14 +5603,14 @@
       <c r="AF86" s="20">
         <v>0.23</v>
       </c>
-      <c r="AG86" s="41">
+      <c r="AG86" s="39">
         <v>20382</v>
       </c>
-      <c r="AH86" s="41"/>
-      <c r="AI86" s="42">
+      <c r="AH86" s="39"/>
+      <c r="AI86" s="35">
         <v>10.1</v>
       </c>
-      <c r="AJ86" s="43"/>
+      <c r="AJ86" s="36"/>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -5691,14 +5691,14 @@
       <c r="AF87" s="20">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AG87" s="41">
+      <c r="AG87" s="39">
         <v>19968</v>
       </c>
-      <c r="AH87" s="41"/>
-      <c r="AI87" s="42">
+      <c r="AH87" s="39"/>
+      <c r="AI87" s="35">
         <v>10.1</v>
       </c>
-      <c r="AJ87" s="43"/>
+      <c r="AJ87" s="36"/>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -5779,14 +5779,14 @@
       <c r="AF88" s="20">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AG88" s="41">
+      <c r="AG88" s="39">
         <v>23240</v>
       </c>
-      <c r="AH88" s="41"/>
-      <c r="AI88" s="42">
+      <c r="AH88" s="39"/>
+      <c r="AI88" s="35">
         <v>10</v>
       </c>
-      <c r="AJ88" s="43"/>
+      <c r="AJ88" s="36"/>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
@@ -5867,14 +5867,14 @@
       <c r="AF89" s="22">
         <v>0.254</v>
       </c>
-      <c r="AG89" s="46">
+      <c r="AG89" s="40">
         <v>26709</v>
       </c>
-      <c r="AH89" s="46"/>
-      <c r="AI89" s="44">
+      <c r="AH89" s="40"/>
+      <c r="AI89" s="37">
         <v>12</v>
       </c>
-      <c r="AJ89" s="45"/>
+      <c r="AJ89" s="38"/>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -6046,13 +6046,13 @@
         <v>43</v>
       </c>
       <c r="K92" s="6">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="M92" s="30">
         <v>43</v>
       </c>
       <c r="N92" s="6">
-        <v>-10000</v>
+        <v>0</v>
       </c>
       <c r="P92" s="33">
         <v>43</v>
@@ -6091,18 +6091,48 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="AF67:AF68"/>
+    <mergeCell ref="AG67:AH68"/>
+    <mergeCell ref="AG70:AH70"/>
+    <mergeCell ref="AG71:AH71"/>
+    <mergeCell ref="AG72:AH72"/>
+    <mergeCell ref="AG73:AH73"/>
+    <mergeCell ref="AG74:AH74"/>
+    <mergeCell ref="AG75:AH75"/>
+    <mergeCell ref="AG76:AH76"/>
+    <mergeCell ref="AG77:AH77"/>
+    <mergeCell ref="AG85:AH85"/>
+    <mergeCell ref="AG86:AH86"/>
+    <mergeCell ref="AG87:AH87"/>
+    <mergeCell ref="AG78:AH78"/>
+    <mergeCell ref="AG79:AH79"/>
+    <mergeCell ref="AG80:AH80"/>
+    <mergeCell ref="AG81:AH81"/>
+    <mergeCell ref="AG82:AH82"/>
+    <mergeCell ref="AI79:AJ79"/>
+    <mergeCell ref="AI80:AJ80"/>
+    <mergeCell ref="AI81:AJ81"/>
+    <mergeCell ref="AG83:AH83"/>
+    <mergeCell ref="AG84:AH84"/>
+    <mergeCell ref="AI74:AJ74"/>
+    <mergeCell ref="AI75:AJ75"/>
+    <mergeCell ref="AI76:AJ76"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AI78:AJ78"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="AI87:AJ87"/>
     <mergeCell ref="AI88:AJ88"/>
@@ -6119,48 +6149,18 @@
     <mergeCell ref="AI71:AJ71"/>
     <mergeCell ref="AI72:AJ72"/>
     <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AI74:AJ74"/>
-    <mergeCell ref="AI75:AJ75"/>
-    <mergeCell ref="AI76:AJ76"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AI78:AJ78"/>
-    <mergeCell ref="AI79:AJ79"/>
-    <mergeCell ref="AI80:AJ80"/>
-    <mergeCell ref="AI81:AJ81"/>
-    <mergeCell ref="AG83:AH83"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="AG85:AH85"/>
-    <mergeCell ref="AG86:AH86"/>
-    <mergeCell ref="AG87:AH87"/>
-    <mergeCell ref="AG78:AH78"/>
-    <mergeCell ref="AG79:AH79"/>
-    <mergeCell ref="AG80:AH80"/>
-    <mergeCell ref="AG81:AH81"/>
-    <mergeCell ref="AG82:AH82"/>
-    <mergeCell ref="AG73:AH73"/>
-    <mergeCell ref="AG74:AH74"/>
-    <mergeCell ref="AG75:AH75"/>
-    <mergeCell ref="AG76:AH76"/>
-    <mergeCell ref="AG77:AH77"/>
-    <mergeCell ref="AF67:AF68"/>
-    <mergeCell ref="AG67:AH68"/>
-    <mergeCell ref="AG70:AH70"/>
-    <mergeCell ref="AG71:AH71"/>
-    <mergeCell ref="AG72:AH72"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed input file not allowing batteries to discahrge
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -642,27 +642,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,10 +654,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -688,6 +676,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2396,17 +2396,17 @@
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
       <c r="F42" s="2"/>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
       <c r="K42" s="2"/>
       <c r="L42" s="4"/>
       <c r="O42" s="4"/>
@@ -2629,11 +2629,11 @@
       <c r="AD49" s="12"/>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
       <c r="U50" t="s">
         <v>17</v>
       </c>
@@ -4001,17 +4001,17 @@
       <c r="AC69" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AF69" s="37" t="s">
+      <c r="AF69" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="AG69" s="39" t="s">
+      <c r="AG69" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="AH69" s="39"/>
-      <c r="AI69" s="39" t="s">
+      <c r="AH69" s="42"/>
+      <c r="AI69" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="AJ69" s="48"/>
+      <c r="AJ69" s="43"/>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -4085,11 +4085,11 @@
       <c r="AC70" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AF70" s="38"/>
-      <c r="AG70" s="40"/>
-      <c r="AH70" s="40"/>
-      <c r="AI70" s="40"/>
-      <c r="AJ70" s="49"/>
+      <c r="AF70" s="49"/>
+      <c r="AG70" s="44"/>
+      <c r="AH70" s="44"/>
+      <c r="AI70" s="44"/>
+      <c r="AJ70" s="45"/>
     </row>
     <row r="71" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -4246,14 +4246,14 @@
       <c r="AF72" s="18">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AG72" s="41">
+      <c r="AG72" s="50">
         <v>72154</v>
       </c>
-      <c r="AH72" s="41"/>
-      <c r="AI72" s="50">
+      <c r="AH72" s="50"/>
+      <c r="AI72" s="46">
         <v>28.1</v>
       </c>
-      <c r="AJ72" s="51"/>
+      <c r="AJ72" s="47"/>
     </row>
     <row r="73" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -4334,14 +4334,14 @@
       <c r="AF73" s="20">
         <v>0.31</v>
       </c>
-      <c r="AG73" s="42">
+      <c r="AG73" s="40">
         <v>67811</v>
       </c>
-      <c r="AH73" s="42"/>
-      <c r="AI73" s="43">
+      <c r="AH73" s="40"/>
+      <c r="AI73" s="36">
         <v>25</v>
       </c>
-      <c r="AJ73" s="44"/>
+      <c r="AJ73" s="37"/>
     </row>
     <row r="74" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -4422,14 +4422,14 @@
       <c r="AF74" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG74" s="42">
+      <c r="AG74" s="40">
         <v>187455</v>
       </c>
-      <c r="AH74" s="42"/>
-      <c r="AI74" s="43">
+      <c r="AH74" s="40"/>
+      <c r="AI74" s="36">
         <v>70</v>
       </c>
-      <c r="AJ74" s="44"/>
+      <c r="AJ74" s="37"/>
     </row>
     <row r="75" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -4510,14 +4510,14 @@
       <c r="AF75" s="20">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AG75" s="42">
+      <c r="AG75" s="40">
         <v>63266</v>
       </c>
-      <c r="AH75" s="42"/>
-      <c r="AI75" s="43">
+      <c r="AH75" s="40"/>
+      <c r="AI75" s="36">
         <v>30.6</v>
       </c>
-      <c r="AJ75" s="44"/>
+      <c r="AJ75" s="37"/>
     </row>
     <row r="76" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
@@ -4598,14 +4598,14 @@
       <c r="AF76" s="20">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AG76" s="42">
+      <c r="AG76" s="40">
         <v>26553</v>
       </c>
-      <c r="AH76" s="42"/>
-      <c r="AI76" s="43">
+      <c r="AH76" s="40"/>
+      <c r="AI76" s="36">
         <v>10</v>
       </c>
-      <c r="AJ76" s="44"/>
+      <c r="AJ76" s="37"/>
     </row>
     <row r="77" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -4686,14 +4686,14 @@
       <c r="AF77" s="20">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AG77" s="42">
+      <c r="AG77" s="40">
         <v>24949</v>
       </c>
-      <c r="AH77" s="42"/>
-      <c r="AI77" s="43">
+      <c r="AH77" s="40"/>
+      <c r="AI77" s="36">
         <v>10</v>
       </c>
-      <c r="AJ77" s="44"/>
+      <c r="AJ77" s="37"/>
     </row>
     <row r="78" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -4774,14 +4774,14 @@
       <c r="AF78" s="20">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AG78" s="42">
+      <c r="AG78" s="40">
         <v>22870</v>
       </c>
-      <c r="AH78" s="42"/>
-      <c r="AI78" s="43">
+      <c r="AH78" s="40"/>
+      <c r="AI78" s="36">
         <v>10</v>
       </c>
-      <c r="AJ78" s="44"/>
+      <c r="AJ78" s="37"/>
     </row>
     <row r="79" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
@@ -4862,14 +4862,14 @@
       <c r="AF79" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG79" s="42">
+      <c r="AG79" s="40">
         <v>139836</v>
       </c>
-      <c r="AH79" s="42"/>
-      <c r="AI79" s="43">
+      <c r="AH79" s="40"/>
+      <c r="AI79" s="36">
         <v>52.2</v>
       </c>
-      <c r="AJ79" s="44"/>
+      <c r="AJ79" s="37"/>
     </row>
     <row r="80" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -4950,14 +4950,14 @@
       <c r="AF80" s="20">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AG80" s="42">
+      <c r="AG80" s="40">
         <v>23515</v>
       </c>
-      <c r="AH80" s="42"/>
-      <c r="AI80" s="43">
+      <c r="AH80" s="40"/>
+      <c r="AI80" s="36">
         <v>10</v>
       </c>
-      <c r="AJ80" s="44"/>
+      <c r="AJ80" s="37"/>
     </row>
     <row r="81" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
@@ -5038,14 +5038,14 @@
       <c r="AF81" s="20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AG81" s="42">
+      <c r="AG81" s="40">
         <v>49503</v>
       </c>
-      <c r="AH81" s="42"/>
-      <c r="AI81" s="43">
+      <c r="AH81" s="40"/>
+      <c r="AI81" s="36">
         <v>20.2</v>
       </c>
-      <c r="AJ81" s="44"/>
+      <c r="AJ81" s="37"/>
     </row>
     <row r="82" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
@@ -5126,14 +5126,14 @@
       <c r="AF82" s="20">
         <v>0.307</v>
       </c>
-      <c r="AG82" s="42">
+      <c r="AG82" s="40">
         <v>188420</v>
       </c>
-      <c r="AH82" s="42"/>
-      <c r="AI82" s="43">
+      <c r="AH82" s="40"/>
+      <c r="AI82" s="36">
         <v>70</v>
       </c>
-      <c r="AJ82" s="44"/>
+      <c r="AJ82" s="37"/>
     </row>
     <row r="83" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -5214,14 +5214,14 @@
       <c r="AF83" s="20">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AG83" s="42">
+      <c r="AG83" s="40">
         <v>26573</v>
       </c>
-      <c r="AH83" s="42"/>
-      <c r="AI83" s="43">
+      <c r="AH83" s="40"/>
+      <c r="AI83" s="36">
         <v>10.5</v>
       </c>
-      <c r="AJ83" s="44"/>
+      <c r="AJ83" s="37"/>
     </row>
     <row r="84" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
@@ -5302,14 +5302,14 @@
       <c r="AF84" s="20">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AG84" s="42">
+      <c r="AG84" s="40">
         <v>25253</v>
       </c>
-      <c r="AH84" s="42"/>
-      <c r="AI84" s="43">
+      <c r="AH84" s="40"/>
+      <c r="AI84" s="36">
         <v>10</v>
       </c>
-      <c r="AJ84" s="44"/>
+      <c r="AJ84" s="37"/>
     </row>
     <row r="85" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
@@ -5390,14 +5390,14 @@
       <c r="AF85" s="20">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AG85" s="42">
+      <c r="AG85" s="40">
         <v>17610</v>
       </c>
-      <c r="AH85" s="42"/>
-      <c r="AI85" s="43">
+      <c r="AH85" s="40"/>
+      <c r="AI85" s="36">
         <v>10</v>
       </c>
-      <c r="AJ85" s="44"/>
+      <c r="AJ85" s="37"/>
     </row>
     <row r="86" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -5478,14 +5478,14 @@
       <c r="AF86" s="20">
         <v>0.221</v>
       </c>
-      <c r="AG86" s="42">
+      <c r="AG86" s="40">
         <v>19372</v>
       </c>
-      <c r="AH86" s="42"/>
-      <c r="AI86" s="43">
+      <c r="AH86" s="40"/>
+      <c r="AI86" s="36">
         <v>10</v>
       </c>
-      <c r="AJ86" s="44"/>
+      <c r="AJ86" s="37"/>
     </row>
     <row r="87" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
@@ -5566,14 +5566,14 @@
       <c r="AF87" s="20">
         <v>0.216</v>
       </c>
-      <c r="AG87" s="42">
+      <c r="AG87" s="40">
         <v>18939</v>
       </c>
-      <c r="AH87" s="42"/>
-      <c r="AI87" s="43">
+      <c r="AH87" s="40"/>
+      <c r="AI87" s="36">
         <v>10</v>
       </c>
-      <c r="AJ87" s="44"/>
+      <c r="AJ87" s="37"/>
     </row>
     <row r="88" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -5654,14 +5654,14 @@
       <c r="AF88" s="20">
         <v>0.23</v>
       </c>
-      <c r="AG88" s="42">
+      <c r="AG88" s="40">
         <v>20382</v>
       </c>
-      <c r="AH88" s="42"/>
-      <c r="AI88" s="43">
+      <c r="AH88" s="40"/>
+      <c r="AI88" s="36">
         <v>10.1</v>
       </c>
-      <c r="AJ88" s="44"/>
+      <c r="AJ88" s="37"/>
     </row>
     <row r="89" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
@@ -5742,14 +5742,14 @@
       <c r="AF89" s="20">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AG89" s="42">
+      <c r="AG89" s="40">
         <v>19968</v>
       </c>
-      <c r="AH89" s="42"/>
-      <c r="AI89" s="43">
+      <c r="AH89" s="40"/>
+      <c r="AI89" s="36">
         <v>10.1</v>
       </c>
-      <c r="AJ89" s="44"/>
+      <c r="AJ89" s="37"/>
     </row>
     <row r="90" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
@@ -5830,14 +5830,14 @@
       <c r="AF90" s="20">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AG90" s="42">
+      <c r="AG90" s="40">
         <v>23240</v>
       </c>
-      <c r="AH90" s="42"/>
-      <c r="AI90" s="43">
+      <c r="AH90" s="40"/>
+      <c r="AI90" s="36">
         <v>10</v>
       </c>
-      <c r="AJ90" s="44"/>
+      <c r="AJ90" s="37"/>
     </row>
     <row r="91" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
@@ -5918,14 +5918,14 @@
       <c r="AF91" s="22">
         <v>0.254</v>
       </c>
-      <c r="AG91" s="47">
+      <c r="AG91" s="41">
         <v>26709</v>
       </c>
-      <c r="AH91" s="47"/>
-      <c r="AI91" s="45">
+      <c r="AH91" s="41"/>
+      <c r="AI91" s="38">
         <v>12</v>
       </c>
-      <c r="AJ91" s="46"/>
+      <c r="AJ91" s="39"/>
     </row>
     <row r="92" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
@@ -6097,7 +6097,7 @@
         <v>43</v>
       </c>
       <c r="K94" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M94" s="30">
         <v>43</v>
@@ -6142,19 +6142,49 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="AF69:AF70"/>
+    <mergeCell ref="AG69:AH70"/>
+    <mergeCell ref="AG72:AH72"/>
+    <mergeCell ref="AG73:AH73"/>
+    <mergeCell ref="AG74:AH74"/>
+    <mergeCell ref="AG75:AH75"/>
+    <mergeCell ref="AG76:AH76"/>
+    <mergeCell ref="AG77:AH77"/>
+    <mergeCell ref="AG78:AH78"/>
+    <mergeCell ref="AG79:AH79"/>
+    <mergeCell ref="AG87:AH87"/>
+    <mergeCell ref="AG88:AH88"/>
+    <mergeCell ref="AG89:AH89"/>
+    <mergeCell ref="AG80:AH80"/>
+    <mergeCell ref="AG81:AH81"/>
+    <mergeCell ref="AG82:AH82"/>
+    <mergeCell ref="AG83:AH83"/>
+    <mergeCell ref="AG84:AH84"/>
+    <mergeCell ref="AI81:AJ81"/>
+    <mergeCell ref="AI82:AJ82"/>
+    <mergeCell ref="AI83:AJ83"/>
+    <mergeCell ref="AG85:AH85"/>
+    <mergeCell ref="AG86:AH86"/>
+    <mergeCell ref="AI76:AJ76"/>
+    <mergeCell ref="AI77:AJ77"/>
+    <mergeCell ref="AI78:AJ78"/>
+    <mergeCell ref="AI79:AJ79"/>
+    <mergeCell ref="AI80:AJ80"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="AI89:AJ89"/>
     <mergeCell ref="AI90:AJ90"/>
@@ -6171,50 +6201,20 @@
     <mergeCell ref="AI73:AJ73"/>
     <mergeCell ref="AI74:AJ74"/>
     <mergeCell ref="AI75:AJ75"/>
-    <mergeCell ref="AI76:AJ76"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AI78:AJ78"/>
-    <mergeCell ref="AI79:AJ79"/>
-    <mergeCell ref="AI80:AJ80"/>
-    <mergeCell ref="AI81:AJ81"/>
-    <mergeCell ref="AI82:AJ82"/>
-    <mergeCell ref="AI83:AJ83"/>
-    <mergeCell ref="AG85:AH85"/>
-    <mergeCell ref="AG86:AH86"/>
-    <mergeCell ref="AG87:AH87"/>
-    <mergeCell ref="AG88:AH88"/>
-    <mergeCell ref="AG89:AH89"/>
-    <mergeCell ref="AG80:AH80"/>
-    <mergeCell ref="AG81:AH81"/>
-    <mergeCell ref="AG82:AH82"/>
-    <mergeCell ref="AG83:AH83"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="AG75:AH75"/>
-    <mergeCell ref="AG76:AH76"/>
-    <mergeCell ref="AG77:AH77"/>
-    <mergeCell ref="AG78:AH78"/>
-    <mergeCell ref="AG79:AH79"/>
-    <mergeCell ref="AF69:AF70"/>
-    <mergeCell ref="AG69:AH70"/>
-    <mergeCell ref="AG72:AH72"/>
-    <mergeCell ref="AG73:AH73"/>
-    <mergeCell ref="AG74:AH74"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N8:P8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added no free energy constraint, storage still not built at all
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K95" sqref="K95"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O84" sqref="O84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6103,7 +6103,7 @@
         <v>43</v>
       </c>
       <c r="N94" s="6">
-        <v>0</v>
+        <v>-10000</v>
       </c>
       <c r="P94" s="33">
         <v>43</v>

</xml_diff>

<commit_message>
Updated new solar seasonality
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -753,28 +753,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,10 +771,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -804,8 +795,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1090,8 +1090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,34 +1122,34 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="38"/>
+      <c r="F1" s="39"/>
       <c r="G1" s="14">
         <v>0.1</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="38" t="s">
+      <c r="N1" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
       <c r="Q1" s="24">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="38" t="s">
+      <c r="S1" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1161,31 +1161,31 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="6"/>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="38" t="s">
+      <c r="S2" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1203,27 +1203,27 @@
       <c r="F3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
       <c r="Q3" s="24">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="S3" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="38"/>
-      <c r="U3" s="38"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1245,27 +1245,27 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
       <c r="L4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="N4" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
       <c r="Q4" s="24">
         <v>43560</v>
       </c>
-      <c r="S4" s="38" t="s">
+      <c r="S4" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1282,27 +1282,27 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="N5" s="38" t="s">
+      <c r="N5" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
       <c r="Q5" s="26">
         <v>50</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="39"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1325,23 +1325,23 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
       <c r="L6" s="10"/>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
       <c r="Q6" s="26">
         <v>10</v>
       </c>
-      <c r="S6" s="38" t="s">
+      <c r="S6" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="38"/>
+      <c r="T6" s="39"/>
+      <c r="U6" s="39"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1364,11 +1364,11 @@
       <c r="G7" s="6">
         <v>4050</v>
       </c>
-      <c r="S7" s="38" t="s">
+      <c r="S7" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="38"/>
-      <c r="U7" s="38"/>
+      <c r="T7" s="39"/>
+      <c r="U7" s="39"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1384,11 +1384,11 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="S8" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="38"/>
-      <c r="U8" s="38"/>
+      <c r="T8" s="39"/>
+      <c r="U8" s="39"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -5697,17 +5697,17 @@
       </c>
     </row>
     <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
       <c r="F45" s="2"/>
-      <c r="H45" s="39" t="s">
+      <c r="H45" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="O45" s="4"/>
@@ -5941,30 +5941,30 @@
       </c>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="G53" s="55" t="s">
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="G53" s="38" t="s">
         <v>137</v>
       </c>
       <c r="H53">
         <v>0.5</v>
       </c>
-      <c r="J53" s="55" t="s">
+      <c r="J53" s="38" t="s">
         <v>138</v>
       </c>
       <c r="K53">
         <v>0.7</v>
       </c>
-      <c r="M53" s="55" t="s">
+      <c r="M53" s="38" t="s">
         <v>139</v>
       </c>
       <c r="N53">
         <v>1</v>
       </c>
-      <c r="P53" s="55" t="s">
+      <c r="P53" s="38" t="s">
         <v>140</v>
       </c>
       <c r="Q53">
@@ -9999,27 +9999,27 @@
       </c>
     </row>
     <row r="103" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="D103" s="40" t="s">
+      <c r="D103" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="E103" s="42" t="s">
+      <c r="E103" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="F103" s="42"/>
-      <c r="G103" s="42" t="s">
+      <c r="F103" s="46"/>
+      <c r="G103" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="H103" s="51"/>
+      <c r="H103" s="47"/>
       <c r="N103" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="D104" s="41"/>
-      <c r="E104" s="43"/>
-      <c r="F104" s="43"/>
-      <c r="G104" s="43"/>
-      <c r="H104" s="52"/>
+      <c r="D104" s="55"/>
+      <c r="E104" s="48"/>
+      <c r="F104" s="48"/>
+      <c r="G104" s="48"/>
+      <c r="H104" s="49"/>
     </row>
     <row r="105" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
@@ -10033,14 +10033,14 @@
       <c r="D106" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E106" s="44">
+      <c r="E106" s="52">
         <v>72154</v>
       </c>
-      <c r="F106" s="44"/>
-      <c r="G106" s="53">
+      <c r="F106" s="52"/>
+      <c r="G106" s="50">
         <v>28.1</v>
       </c>
-      <c r="H106" s="54"/>
+      <c r="H106" s="51"/>
     </row>
     <row r="107" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C107" s="18">
@@ -10049,14 +10049,14 @@
       <c r="D107" s="19">
         <v>0.31</v>
       </c>
-      <c r="E107" s="45">
+      <c r="E107" s="44">
         <v>67811</v>
       </c>
-      <c r="F107" s="45"/>
-      <c r="G107" s="46">
+      <c r="F107" s="44"/>
+      <c r="G107" s="40">
         <v>25</v>
       </c>
-      <c r="H107" s="47"/>
+      <c r="H107" s="41"/>
     </row>
     <row r="108" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C108" s="18">
@@ -10065,14 +10065,14 @@
       <c r="D108" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E108" s="45">
+      <c r="E108" s="44">
         <v>187455</v>
       </c>
-      <c r="F108" s="45"/>
-      <c r="G108" s="46">
+      <c r="F108" s="44"/>
+      <c r="G108" s="40">
         <v>70</v>
       </c>
-      <c r="H108" s="47"/>
+      <c r="H108" s="41"/>
     </row>
     <row r="109" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C109" s="18">
@@ -10081,14 +10081,14 @@
       <c r="D109" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E109" s="45">
+      <c r="E109" s="44">
         <v>63266</v>
       </c>
-      <c r="F109" s="45"/>
-      <c r="G109" s="46">
+      <c r="F109" s="44"/>
+      <c r="G109" s="40">
         <v>30.6</v>
       </c>
-      <c r="H109" s="47"/>
+      <c r="H109" s="41"/>
     </row>
     <row r="110" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -10097,14 +10097,14 @@
       <c r="D110" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E110" s="45">
+      <c r="E110" s="44">
         <v>26553</v>
       </c>
-      <c r="F110" s="45"/>
-      <c r="G110" s="46">
+      <c r="F110" s="44"/>
+      <c r="G110" s="40">
         <v>10</v>
       </c>
-      <c r="H110" s="47"/>
+      <c r="H110" s="41"/>
     </row>
     <row r="111" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -10113,14 +10113,14 @@
       <c r="D111" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E111" s="45">
+      <c r="E111" s="44">
         <v>24949</v>
       </c>
-      <c r="F111" s="45"/>
-      <c r="G111" s="46">
+      <c r="F111" s="44"/>
+      <c r="G111" s="40">
         <v>10</v>
       </c>
-      <c r="H111" s="47"/>
+      <c r="H111" s="41"/>
     </row>
     <row r="112" spans="1:38" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -10129,14 +10129,14 @@
       <c r="D112" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E112" s="45">
+      <c r="E112" s="44">
         <v>22870</v>
       </c>
-      <c r="F112" s="45"/>
-      <c r="G112" s="46">
+      <c r="F112" s="44"/>
+      <c r="G112" s="40">
         <v>10</v>
       </c>
-      <c r="H112" s="47"/>
+      <c r="H112" s="41"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -10145,14 +10145,14 @@
       <c r="D113" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E113" s="45">
+      <c r="E113" s="44">
         <v>139836</v>
       </c>
-      <c r="F113" s="45"/>
-      <c r="G113" s="46">
+      <c r="F113" s="44"/>
+      <c r="G113" s="40">
         <v>52.2</v>
       </c>
-      <c r="H113" s="47"/>
+      <c r="H113" s="41"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -10161,14 +10161,14 @@
       <c r="D114" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E114" s="45">
+      <c r="E114" s="44">
         <v>23515</v>
       </c>
-      <c r="F114" s="45"/>
-      <c r="G114" s="46">
+      <c r="F114" s="44"/>
+      <c r="G114" s="40">
         <v>10</v>
       </c>
-      <c r="H114" s="47"/>
+      <c r="H114" s="41"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -10177,14 +10177,14 @@
       <c r="D115" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E115" s="45">
+      <c r="E115" s="44">
         <v>49503</v>
       </c>
-      <c r="F115" s="45"/>
-      <c r="G115" s="46">
+      <c r="F115" s="44"/>
+      <c r="G115" s="40">
         <v>20.2</v>
       </c>
-      <c r="H115" s="47"/>
+      <c r="H115" s="41"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -10193,14 +10193,14 @@
       <c r="D116" s="19">
         <v>0.307</v>
       </c>
-      <c r="E116" s="45">
+      <c r="E116" s="44">
         <v>188420</v>
       </c>
-      <c r="F116" s="45"/>
-      <c r="G116" s="46">
+      <c r="F116" s="44"/>
+      <c r="G116" s="40">
         <v>70</v>
       </c>
-      <c r="H116" s="47"/>
+      <c r="H116" s="41"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -10209,14 +10209,14 @@
       <c r="D117" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E117" s="45">
+      <c r="E117" s="44">
         <v>26573</v>
       </c>
-      <c r="F117" s="45"/>
-      <c r="G117" s="46">
+      <c r="F117" s="44"/>
+      <c r="G117" s="40">
         <v>10.5</v>
       </c>
-      <c r="H117" s="47"/>
+      <c r="H117" s="41"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -10225,14 +10225,14 @@
       <c r="D118" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E118" s="45">
+      <c r="E118" s="44">
         <v>25253</v>
       </c>
-      <c r="F118" s="45"/>
-      <c r="G118" s="46">
+      <c r="F118" s="44"/>
+      <c r="G118" s="40">
         <v>10</v>
       </c>
-      <c r="H118" s="47"/>
+      <c r="H118" s="41"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -10241,14 +10241,14 @@
       <c r="D119" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E119" s="45">
+      <c r="E119" s="44">
         <v>17610</v>
       </c>
-      <c r="F119" s="45"/>
-      <c r="G119" s="46">
+      <c r="F119" s="44"/>
+      <c r="G119" s="40">
         <v>10</v>
       </c>
-      <c r="H119" s="47"/>
+      <c r="H119" s="41"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -10257,14 +10257,14 @@
       <c r="D120" s="19">
         <v>0.221</v>
       </c>
-      <c r="E120" s="45">
+      <c r="E120" s="44">
         <v>19372</v>
       </c>
-      <c r="F120" s="45"/>
-      <c r="G120" s="46">
+      <c r="F120" s="44"/>
+      <c r="G120" s="40">
         <v>10</v>
       </c>
-      <c r="H120" s="47"/>
+      <c r="H120" s="41"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -10273,14 +10273,14 @@
       <c r="D121" s="19">
         <v>0.216</v>
       </c>
-      <c r="E121" s="45">
+      <c r="E121" s="44">
         <v>18939</v>
       </c>
-      <c r="F121" s="45"/>
-      <c r="G121" s="46">
+      <c r="F121" s="44"/>
+      <c r="G121" s="40">
         <v>10</v>
       </c>
-      <c r="H121" s="47"/>
+      <c r="H121" s="41"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -10289,14 +10289,14 @@
       <c r="D122" s="19">
         <v>0.23</v>
       </c>
-      <c r="E122" s="45">
+      <c r="E122" s="44">
         <v>20382</v>
       </c>
-      <c r="F122" s="45"/>
-      <c r="G122" s="46">
+      <c r="F122" s="44"/>
+      <c r="G122" s="40">
         <v>10.1</v>
       </c>
-      <c r="H122" s="47"/>
+      <c r="H122" s="41"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -10305,14 +10305,14 @@
       <c r="D123" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E123" s="45">
+      <c r="E123" s="44">
         <v>19968</v>
       </c>
-      <c r="F123" s="45"/>
-      <c r="G123" s="46">
+      <c r="F123" s="44"/>
+      <c r="G123" s="40">
         <v>10.1</v>
       </c>
-      <c r="H123" s="47"/>
+      <c r="H123" s="41"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -10321,14 +10321,14 @@
       <c r="D124" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E124" s="45">
+      <c r="E124" s="44">
         <v>23240</v>
       </c>
-      <c r="F124" s="45"/>
-      <c r="G124" s="46">
+      <c r="F124" s="44"/>
+      <c r="G124" s="40">
         <v>10</v>
       </c>
-      <c r="H124" s="47"/>
+      <c r="H124" s="41"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="20">
@@ -10337,29 +10337,57 @@
       <c r="D125" s="21">
         <v>0.254</v>
       </c>
-      <c r="E125" s="50">
+      <c r="E125" s="45">
         <v>26709</v>
       </c>
-      <c r="F125" s="50"/>
-      <c r="G125" s="48">
+      <c r="F125" s="45"/>
+      <c r="G125" s="42">
         <v>12</v>
       </c>
-      <c r="H125" s="49"/>
+      <c r="H125" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:F104"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="G124:H124"/>
@@ -10376,46 +10404,18 @@
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G108:H108"/>
     <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:F104"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
placeholders for reading in RampRate, constraint not yet constructed
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -21,10 +21,10 @@
     <definedName name="CAPEX_solar">Sheet2!$Q$1</definedName>
     <definedName name="CAPEX_storage">Sheet2!$Q$7</definedName>
     <definedName name="CAPEX_wind">Sheet2!$Q$3</definedName>
-    <definedName name="CH4_rate">Sheet2!$AB$52:$AB$94</definedName>
-    <definedName name="CO2_rate">Sheet2!$AA$52:$AA$94</definedName>
+    <definedName name="CH4_rate">Sheet2!$AE$52:$AE$94</definedName>
+    <definedName name="CO2_rate">Sheet2!$AD$52:$AD$94</definedName>
     <definedName name="DiscRate">Sheet2!$G$1</definedName>
-    <definedName name="EV_subsidy_cost">Sheet2!$V$1</definedName>
+    <definedName name="EV_subsidy_cost">Sheet2!$Y$1</definedName>
     <definedName name="LineCapacity">Sheet2!$P$44:$P$46</definedName>
     <definedName name="LineFromBus">Sheet2!$H$44:$J$46</definedName>
     <definedName name="LineReactance">Sheet2!$M$44:$M$46</definedName>
@@ -34,8 +34,8 @@
     <definedName name="MaxGenOff">Sheet2!$K$52:$K$94</definedName>
     <definedName name="MaxGenPeak">Sheet2!$H$52:$H$94</definedName>
     <definedName name="MinGen">Sheet2!$N$52:$N$94</definedName>
-    <definedName name="N2O_rate">Sheet2!$AC$52:$AC$94</definedName>
-    <definedName name="NOx_rate">Sheet2!$Y$52:$Y$94</definedName>
+    <definedName name="N2O_rate">Sheet2!$AF$52:$AF$94</definedName>
+    <definedName name="NOx_rate">Sheet2!$AB$52:$AB$94</definedName>
     <definedName name="NumBuses">Sheet2!$C$1</definedName>
     <definedName name="NumLines">Sheet2!$C$2</definedName>
     <definedName name="NumUnits">Sheet2!$C$3</definedName>
@@ -45,7 +45,8 @@
     <definedName name="OPEX_storage">Sheet2!$Q$8</definedName>
     <definedName name="OPEX_wind">Sheet2!$Q$4</definedName>
     <definedName name="PeakHours">Sheet2!$C$6</definedName>
-    <definedName name="SO2_rate">Sheet2!$Z$52:$Z$94</definedName>
+    <definedName name="RampRate">Sheet2!$T$52:$T$94</definedName>
+    <definedName name="SO2_rate">Sheet2!$AC$52:$AC$94</definedName>
     <definedName name="solar_cap_factor">Sheet2!$G$4</definedName>
     <definedName name="solar_inc">Sheet2!$Q$5</definedName>
     <definedName name="UnitsByBus">Sheet2!$C$52:$E$94</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
   <si>
     <t>NumBuses</t>
   </si>
@@ -407,6 +408,9 @@
   </si>
   <si>
     <t>Battery Efficiency</t>
+  </si>
+  <si>
+    <t>RampRate (MW/hr)</t>
   </si>
 </sst>
 </file>
@@ -567,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -639,7 +643,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -654,19 +682,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -678,18 +697,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ94"/>
+  <dimension ref="A1:AM94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O84" sqref="O84"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T52" sqref="T52:T94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -988,135 +999,145 @@
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="9" customWidth="1"/>
     <col min="17" max="17" width="13.26953125" customWidth="1"/>
-    <col min="18" max="18" width="9.54296875" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" customWidth="1"/>
-    <col min="20" max="20" width="10.6328125" customWidth="1"/>
-    <col min="21" max="21" width="10.54296875" customWidth="1"/>
-    <col min="22" max="22" width="16.7265625" customWidth="1"/>
-    <col min="23" max="24" width="16.26953125" customWidth="1"/>
-    <col min="25" max="25" width="16.1796875" customWidth="1"/>
-    <col min="26" max="29" width="16.26953125" customWidth="1"/>
+    <col min="18" max="20" width="8.7265625" customWidth="1"/>
+    <col min="21" max="21" width="9.54296875" customWidth="1"/>
+    <col min="22" max="22" width="10.54296875" customWidth="1"/>
+    <col min="23" max="23" width="10.6328125" customWidth="1"/>
+    <col min="24" max="24" width="10.54296875" customWidth="1"/>
+    <col min="25" max="25" width="16.7265625" customWidth="1"/>
+    <col min="26" max="27" width="16.26953125" customWidth="1"/>
+    <col min="28" max="28" width="16.1796875" customWidth="1"/>
+    <col min="29" max="32" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="35"/>
+      <c r="F1" s="36"/>
       <c r="G1" s="15">
         <v>0.1</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
       <c r="L1" s="16">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
       <c r="Q1" s="25">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="V1" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="25">
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="25">
         <v>8809340386.1000004</v>
       </c>
     </row>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="6">
         <v>7000</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
       <c r="L2" s="24">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
       <c r="Q2" s="25">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="V2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="28">
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="28">
         <v>348494.96600000001</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6">
         <v>43</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I3" s="4"/>
       <c r="L3" s="26"/>
-      <c r="N3" s="35" t="s">
+      <c r="N3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
       <c r="Q3" s="25">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="35" t="s">
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="V3" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="29">
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="29">
         <v>2066077.2990000001</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Z3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1124,67 +1145,73 @@
         <v>26</v>
       </c>
       <c r="D4" s="14"/>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="16">
         <v>1</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="N4" s="35" t="s">
+      <c r="N4" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
       <c r="Q4" s="25">
         <v>43560</v>
       </c>
-      <c r="S4" s="35" t="s">
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="V4" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="28">
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="28">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Z4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="16">
         <v>1</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="N5" s="35" t="s">
+      <c r="N5" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="36"/>
+      <c r="P5" s="36"/>
       <c r="Q5" s="27">
         <v>50</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="V5" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="28">
+      <c r="W5" s="36"/>
+      <c r="X5" s="36"/>
+      <c r="Y5" s="28">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Z5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>108</v>
       </c>
@@ -1192,36 +1219,39 @@
         <f>16*365</f>
         <v>5840</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="10">
         <v>0.3</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
       <c r="Q6" s="27">
         <v>10</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="R6" s="54"/>
+      <c r="S6" s="54"/>
+      <c r="T6" s="54"/>
+      <c r="V6" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="28">
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
+      <c r="Y6" s="28">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Z6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>109</v>
       </c>
@@ -1229,84 +1259,93 @@
         <f>8*365</f>
         <v>2920</v>
       </c>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
       <c r="Q7" s="25">
         <v>601000</v>
       </c>
-      <c r="S7" s="35" t="s">
+      <c r="R7" s="53"/>
+      <c r="S7" s="53"/>
+      <c r="T7" s="53"/>
+      <c r="V7" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="28">
-        <f>V4*V6</f>
+      <c r="W7" s="36"/>
+      <c r="X7" s="36"/>
+      <c r="Y7" s="28">
+        <f>Y4*Y6</f>
         <v>29903074042.27026</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Z7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="N8" s="35" t="s">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="N8" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
       <c r="Q8" s="25">
         <v>15025</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="V8" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="28">
-        <f>V5*V6</f>
+      <c r="W8" s="36"/>
+      <c r="X8" s="36"/>
+      <c r="Y8" s="28">
+        <f>Y5*Y6</f>
         <v>5911072775.7976093</v>
       </c>
-      <c r="W8" t="s">
+      <c r="Z8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="N9" s="35" t="s">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="N9" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
       <c r="Q9" s="27">
         <v>0.95</v>
       </c>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="28"/>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="28"/>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="C11" s="35" t="s">
+      <c r="R9" s="54"/>
+      <c r="S9" s="54"/>
+      <c r="T9" s="54"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="28"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="28"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="C11" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
       <c r="F11" s="2"/>
-      <c r="I11" s="35" t="s">
+      <c r="I11" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="33"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
         <v>28</v>
       </c>
@@ -1338,7 +1377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B13" s="4">
         <v>2020</v>
       </c>
@@ -1378,7 +1417,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B14" s="4">
         <v>2021</v>
       </c>
@@ -1418,7 +1457,7 @@
         <v>2118.8999999999996</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B15" s="4">
         <v>2022</v>
       </c>
@@ -1458,7 +1497,7 @@
         <v>2137.9700999999995</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>2023</v>
       </c>
@@ -2138,7 +2177,7 @@
         <v>2489.7254187143535</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <v>2040</v>
       </c>
@@ -2178,7 +2217,7 @@
         <v>2512.1329474827821</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>2041</v>
       </c>
@@ -2218,7 +2257,7 @@
         <v>2534.742144010127</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>2042</v>
       </c>
@@ -2258,7 +2297,7 @@
         <v>2557.5548233062182</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <v>2043</v>
       </c>
@@ -2298,7 +2337,7 @@
         <v>2580.5728167159737</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <v>2044</v>
       </c>
@@ -2338,7 +2377,7 @@
         <v>2603.7979720664175</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
         <v>2045</v>
       </c>
@@ -2378,7 +2417,7 @@
         <v>2627.2321538150145</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
         <v>3</v>
       </c>
@@ -2391,27 +2430,27 @@
       <c r="O41" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R41" s="4" t="s">
+      <c r="U41" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="C42" s="51" t="s">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="C42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="37"/>
       <c r="F42" s="2"/>
-      <c r="H42" s="51" t="s">
+      <c r="H42" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
       <c r="K42" s="2"/>
       <c r="L42" s="4"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
@@ -2444,11 +2483,11 @@
       <c r="O43" t="s">
         <v>4</v>
       </c>
-      <c r="R43" t="s">
+      <c r="U43" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
@@ -2485,14 +2524,14 @@
       <c r="P44" s="6">
         <v>1100</v>
       </c>
-      <c r="R44" t="s">
+      <c r="U44" t="s">
         <v>21</v>
       </c>
-      <c r="S44" s="6">
+      <c r="V44" s="6">
         <v>3.06</v>
       </c>
     </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>6</v>
       </c>
@@ -2529,14 +2568,14 @@
       <c r="P45" s="6">
         <v>2000</v>
       </c>
-      <c r="R45" t="s">
+      <c r="U45" t="s">
         <v>23</v>
       </c>
-      <c r="S45" s="6">
+      <c r="V45" s="6">
         <v>2.16</v>
       </c>
     </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
@@ -2573,17 +2612,17 @@
       <c r="P46" s="6">
         <v>1000</v>
       </c>
-      <c r="R46" t="s">
+      <c r="U46" t="s">
         <v>24</v>
       </c>
-      <c r="S46" s="6">
+      <c r="V46" s="6">
         <v>12.56</v>
       </c>
-      <c r="T46" t="s">
+      <c r="W46" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
         <v>26</v>
       </c>
@@ -2602,52 +2641,55 @@
       <c r="P49" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T49" s="4" t="s">
+      <c r="S49" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="W49" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U49" s="4" t="s">
+      <c r="X49" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V49" s="4" t="s">
+      <c r="Y49" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Y49" s="32" t="s">
+      <c r="AB49" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Z49" s="32" t="s">
+      <c r="AC49" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AA49" s="32" t="s">
+      <c r="AD49" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AB49" s="32" t="s">
+      <c r="AE49" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="AC49" s="32" t="s">
+      <c r="AF49" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="AD49" s="12"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="C50" s="51" t="s">
+      <c r="AG49" s="12"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="C50" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="U50" t="s">
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="X50" t="s">
         <v>17</v>
       </c>
-      <c r="V50" t="s">
+      <c r="Y50" t="s">
         <v>20</v>
       </c>
-      <c r="Y50" s="32"/>
-      <c r="Z50" s="32"/>
-      <c r="AA50" s="32"/>
       <c r="AB50" s="32"/>
       <c r="AC50" s="32"/>
-      <c r="AD50" s="12"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AD50" s="32"/>
+      <c r="AE50" s="32"/>
+      <c r="AF50" s="32"/>
+      <c r="AG50" s="12"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2675,20 +2717,23 @@
       <c r="P51" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="S51" s="33" t="s">
+      <c r="S51" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="X51" t="s">
+      <c r="V51" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="Y51" s="32"/>
-      <c r="Z51" s="32"/>
-      <c r="AA51" s="32"/>
+      <c r="AA51" t="s">
+        <v>10</v>
+      </c>
       <c r="AB51" s="32"/>
       <c r="AC51" s="32"/>
-      <c r="AD51" s="12"/>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AD51" s="32"/>
+      <c r="AE51" s="32"/>
+      <c r="AF51" s="32"/>
+      <c r="AG51" s="12"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2726,42 +2771,50 @@
         <v>1</v>
       </c>
       <c r="Q52" s="8">
-        <f t="shared" ref="Q52:Q94" si="8">U52*V52*1000/1000000</f>
+        <f t="shared" ref="Q52:Q94" si="8">X52*Y52*1000/1000000</f>
         <v>39.666780000000003</v>
       </c>
-      <c r="S52" s="33">
+      <c r="R52" s="55"/>
+      <c r="S52" s="35">
         <v>1</v>
       </c>
-      <c r="T52" t="s">
+      <c r="T52" s="56">
+        <v>2520</v>
+      </c>
+      <c r="U52" s="55"/>
+      <c r="V52" s="33">
+        <v>1</v>
+      </c>
+      <c r="W52" t="s">
         <v>21</v>
       </c>
-      <c r="U52" s="6">
+      <c r="X52" s="6">
         <v>12963</v>
       </c>
-      <c r="V52" s="6">
-        <f t="shared" ref="V52:V71" si="9">IF(EXACT(T52,$R$44),$S$44,IF(EXACT(T52,$R$45),$S$45,IF(EXACT(T52,$R$46),$S$46,0)))</f>
+      <c r="Y52" s="6">
+        <f t="shared" ref="Y52:Y71" si="9">IF(EXACT(W52,$U$44),$V$44,IF(EXACT(W52,$U$45),$V$45,IF(EXACT(W52,$U$46),$V$46,0)))</f>
         <v>3.06</v>
       </c>
-      <c r="X52" s="33">
+      <c r="AA52" s="33">
         <v>1</v>
       </c>
-      <c r="Y52" s="6">
+      <c r="AB52" s="6">
         <v>1.4370000000000001</v>
       </c>
-      <c r="Z52" s="6">
+      <c r="AC52" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AA52" s="6">
+      <c r="AD52" s="6">
         <v>1540.787</v>
       </c>
-      <c r="AB52" s="6">
+      <c r="AE52" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AC52" s="6">
+      <c r="AF52" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2802,39 +2855,47 @@
         <f t="shared" si="8"/>
         <v>23.617080000000001</v>
       </c>
-      <c r="S53" s="33">
+      <c r="R53" s="55"/>
+      <c r="S53" s="35">
         <v>2</v>
       </c>
-      <c r="T53" t="s">
+      <c r="T53" s="56">
+        <v>1980</v>
+      </c>
+      <c r="U53" s="55"/>
+      <c r="V53" s="33">
+        <v>2</v>
+      </c>
+      <c r="W53" t="s">
         <v>21</v>
       </c>
-      <c r="U53" s="6">
+      <c r="X53" s="6">
         <v>7718</v>
       </c>
-      <c r="V53" s="6">
+      <c r="Y53" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X53" s="33">
+      <c r="AA53" s="33">
         <v>2</v>
       </c>
-      <c r="Y53" s="6">
+      <c r="AB53" s="6">
         <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="Z53" s="6">
-        <v>2E-3</v>
-      </c>
-      <c r="AA53" s="6">
-        <v>917.32500000000005</v>
-      </c>
-      <c r="AB53" s="6">
-        <v>1.6E-2</v>
       </c>
       <c r="AC53" s="6">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AD53" s="6">
+        <v>917.32500000000005</v>
+      </c>
+      <c r="AE53" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AF53" s="6">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2875,39 +2936,47 @@
         <f t="shared" si="8"/>
         <v>28.115279999999998</v>
       </c>
-      <c r="S54" s="33">
+      <c r="R54" s="55"/>
+      <c r="S54" s="35">
         <v>3</v>
       </c>
-      <c r="T54" t="s">
+      <c r="T54" s="56">
+        <v>240</v>
+      </c>
+      <c r="U54" s="55"/>
+      <c r="V54" s="33">
+        <v>3</v>
+      </c>
+      <c r="W54" t="s">
         <v>21</v>
       </c>
-      <c r="U54" s="6">
+      <c r="X54" s="6">
         <v>9188</v>
       </c>
-      <c r="V54" s="6">
+      <c r="Y54" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X54" s="33">
+      <c r="AA54" s="33">
         <v>3</v>
       </c>
-      <c r="Y54" s="6">
+      <c r="AB54" s="6">
         <v>24.811</v>
       </c>
-      <c r="Z54" s="6">
+      <c r="AC54" s="6">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AA54" s="6">
+      <c r="AD54" s="6">
         <v>1073.9280000000001</v>
       </c>
-      <c r="AB54" s="6">
+      <c r="AE54" s="6">
         <v>0.02</v>
       </c>
-      <c r="AC54" s="6">
+      <c r="AF54" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2948,39 +3017,47 @@
         <f t="shared" si="8"/>
         <v>21.77496</v>
       </c>
-      <c r="S55" s="33">
+      <c r="R55" s="55"/>
+      <c r="S55" s="35">
         <v>4</v>
       </c>
-      <c r="T55" t="s">
+      <c r="T55" s="56">
+        <v>1020</v>
+      </c>
+      <c r="U55" s="55"/>
+      <c r="V55" s="33">
+        <v>4</v>
+      </c>
+      <c r="W55" t="s">
         <v>21</v>
       </c>
-      <c r="U55" s="6">
+      <c r="X55" s="6">
         <v>7116</v>
       </c>
-      <c r="V55" s="6">
+      <c r="Y55" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X55" s="33">
+      <c r="AA55" s="33">
         <v>4</v>
       </c>
-      <c r="Y55" s="6">
+      <c r="AB55" s="6">
         <v>1.056</v>
       </c>
-      <c r="Z55" s="6">
+      <c r="AC55" s="6">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="AA55" s="6">
+      <c r="AD55" s="6">
         <v>845.83</v>
       </c>
-      <c r="AB55" s="6">
+      <c r="AE55" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AC55" s="6">
+      <c r="AF55" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -3021,39 +3098,47 @@
         <f t="shared" si="8"/>
         <v>23.94144</v>
       </c>
-      <c r="S56" s="33">
+      <c r="R56" s="55"/>
+      <c r="S56" s="35">
         <v>5</v>
       </c>
-      <c r="T56" t="s">
+      <c r="T56" s="56">
+        <v>2220</v>
+      </c>
+      <c r="U56" s="55"/>
+      <c r="V56" s="33">
+        <v>5</v>
+      </c>
+      <c r="W56" t="s">
         <v>21</v>
       </c>
-      <c r="U56" s="6">
+      <c r="X56" s="6">
         <v>7824</v>
       </c>
-      <c r="V56" s="6">
+      <c r="Y56" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X56" s="33">
+      <c r="AA56" s="33">
         <v>5</v>
       </c>
-      <c r="Y56" s="6">
+      <c r="AB56" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="Z56" s="6">
+      <c r="AC56" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AA56" s="6">
+      <c r="AD56" s="6">
         <v>930.02099999999996</v>
       </c>
-      <c r="AB56" s="6">
+      <c r="AE56" s="6">
         <v>1.6E-2</v>
       </c>
-      <c r="AC56" s="6">
+      <c r="AF56" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -3094,39 +3179,47 @@
         <f t="shared" si="8"/>
         <v>38.22552000000001</v>
       </c>
-      <c r="S57" s="33">
+      <c r="R57" s="55"/>
+      <c r="S57" s="35">
         <v>6</v>
       </c>
-      <c r="T57" t="s">
+      <c r="T57" s="56">
+        <v>300</v>
+      </c>
+      <c r="U57" s="55"/>
+      <c r="V57" s="33">
+        <v>6</v>
+      </c>
+      <c r="W57" t="s">
         <v>21</v>
       </c>
-      <c r="U57" s="6">
+      <c r="X57" s="6">
         <v>12492</v>
       </c>
-      <c r="V57" s="6">
+      <c r="Y57" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X57" s="33">
+      <c r="AA57" s="33">
         <v>6</v>
       </c>
-      <c r="Y57" s="6">
+      <c r="AB57" s="6">
         <v>1.1240000000000001</v>
       </c>
-      <c r="Z57" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="6">
+      <c r="AC57" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD57" s="6">
         <v>1460.1579999999999</v>
       </c>
-      <c r="AB57" s="6">
+      <c r="AE57" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AC57" s="6">
+      <c r="AF57" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -3167,39 +3260,47 @@
         <f t="shared" si="8"/>
         <v>1.6982999999999999</v>
       </c>
-      <c r="S58" s="33">
+      <c r="R58" s="55"/>
+      <c r="S58" s="35">
         <v>7</v>
       </c>
-      <c r="T58" t="s">
+      <c r="T58" s="56">
+        <v>420</v>
+      </c>
+      <c r="U58" s="55"/>
+      <c r="V58" s="33">
+        <v>7</v>
+      </c>
+      <c r="W58" t="s">
         <v>21</v>
       </c>
-      <c r="U58" s="6">
+      <c r="X58" s="6">
         <v>555</v>
       </c>
-      <c r="V58" s="6">
+      <c r="Y58" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X58" s="33">
+      <c r="AA58" s="33">
         <v>7</v>
       </c>
-      <c r="Y58" s="6">
+      <c r="AB58" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="Z58" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA58" s="6">
+      <c r="AC58" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD58" s="6">
         <v>65.930999999999997</v>
       </c>
-      <c r="AB58" s="6">
+      <c r="AE58" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AC58" s="6">
+      <c r="AF58" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -3240,39 +3341,47 @@
         <f t="shared" si="8"/>
         <v>36.677160000000001</v>
       </c>
-      <c r="S59" s="33">
+      <c r="R59" s="55"/>
+      <c r="S59" s="35">
         <v>8</v>
       </c>
-      <c r="T59" t="s">
+      <c r="T59" s="56">
+        <v>420</v>
+      </c>
+      <c r="U59" s="55"/>
+      <c r="V59" s="33">
+        <v>8</v>
+      </c>
+      <c r="W59" t="s">
         <v>21</v>
       </c>
-      <c r="U59" s="6">
+      <c r="X59" s="6">
         <v>11986</v>
       </c>
-      <c r="V59" s="6">
+      <c r="Y59" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X59" s="33">
+      <c r="AA59" s="33">
         <v>8</v>
       </c>
-      <c r="Y59" s="6">
+      <c r="AB59" s="6">
         <v>1.3009999999999999</v>
       </c>
-      <c r="Z59" s="6">
+      <c r="AC59" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AA59" s="6">
+      <c r="AD59" s="6">
         <v>1424.5930000000001</v>
       </c>
-      <c r="AB59" s="6">
+      <c r="AE59" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="AC59" s="6">
+      <c r="AF59" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -3313,39 +3422,47 @@
         <f t="shared" si="8"/>
         <v>23.494679999999999</v>
       </c>
-      <c r="S60" s="33">
+      <c r="R60" s="55"/>
+      <c r="S60" s="35">
         <v>9</v>
       </c>
-      <c r="T60" t="s">
+      <c r="T60" s="56">
+        <v>1980</v>
+      </c>
+      <c r="U60" s="55"/>
+      <c r="V60" s="33">
+        <v>9</v>
+      </c>
+      <c r="W60" t="s">
         <v>21</v>
       </c>
-      <c r="U60" s="6">
+      <c r="X60" s="6">
         <v>7678</v>
       </c>
-      <c r="V60" s="6">
+      <c r="Y60" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X60" s="33">
+      <c r="AA60" s="33">
         <v>9</v>
       </c>
-      <c r="Y60" s="6">
+      <c r="AB60" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="Z60" s="6">
+      <c r="AC60" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AA60" s="6">
+      <c r="AD60" s="6">
         <v>912.65499999999997</v>
       </c>
-      <c r="AB60" s="6">
+      <c r="AE60" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="AC60" s="6">
+      <c r="AF60" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -3386,39 +3503,47 @@
         <f t="shared" si="8"/>
         <v>31.606739999999999</v>
       </c>
-      <c r="S61" s="33">
+      <c r="R61" s="55"/>
+      <c r="S61" s="35">
         <v>10</v>
       </c>
-      <c r="T61" t="s">
+      <c r="T61" s="56">
+        <v>900</v>
+      </c>
+      <c r="U61" s="55"/>
+      <c r="V61" s="33">
+        <v>10</v>
+      </c>
+      <c r="W61" t="s">
         <v>21</v>
       </c>
-      <c r="U61" s="6">
+      <c r="X61" s="6">
         <v>10329</v>
       </c>
-      <c r="V61" s="6">
+      <c r="Y61" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X61" s="33">
+      <c r="AA61" s="33">
         <v>10</v>
       </c>
-      <c r="Y61" s="6">
+      <c r="AB61" s="6">
         <v>1.306</v>
       </c>
-      <c r="Z61" s="6">
+      <c r="AC61" s="6">
         <v>0.01</v>
       </c>
-      <c r="AA61" s="6">
+      <c r="AD61" s="6">
         <v>1235.3320000000001</v>
       </c>
-      <c r="AB61" s="6">
+      <c r="AE61" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AC61" s="6">
+      <c r="AF61" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -3459,39 +3584,47 @@
         <f t="shared" si="8"/>
         <v>38.996639999999999</v>
       </c>
-      <c r="S62" s="33">
+      <c r="R62" s="55"/>
+      <c r="S62" s="35">
         <v>11</v>
       </c>
-      <c r="T62" t="s">
+      <c r="T62" s="56">
+        <v>480</v>
+      </c>
+      <c r="U62" s="55"/>
+      <c r="V62" s="33">
+        <v>11</v>
+      </c>
+      <c r="W62" t="s">
         <v>21</v>
       </c>
-      <c r="U62" s="6">
+      <c r="X62" s="6">
         <v>12744</v>
       </c>
-      <c r="V62" s="6">
+      <c r="Y62" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X62" s="33">
+      <c r="AA62" s="33">
         <v>11</v>
       </c>
-      <c r="Y62" s="6">
+      <c r="AB62" s="6">
         <v>2.9769999999999999</v>
       </c>
-      <c r="Z62" s="6">
+      <c r="AC62" s="6">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="AA62" s="6">
+      <c r="AD62" s="6">
         <v>1514.692</v>
       </c>
-      <c r="AB62" s="6">
+      <c r="AE62" s="6">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="AC62" s="6">
+      <c r="AF62" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -3532,39 +3665,47 @@
         <f t="shared" si="8"/>
         <v>35.954999999999998</v>
       </c>
-      <c r="S63" s="33">
+      <c r="R63" s="55"/>
+      <c r="S63" s="35">
         <v>12</v>
       </c>
-      <c r="T63" t="s">
+      <c r="T63" s="56">
+        <v>720</v>
+      </c>
+      <c r="U63" s="55"/>
+      <c r="V63" s="33">
+        <v>12</v>
+      </c>
+      <c r="W63" t="s">
         <v>21</v>
       </c>
-      <c r="U63" s="6">
+      <c r="X63" s="6">
         <v>11750</v>
       </c>
-      <c r="V63" s="6">
+      <c r="Y63" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X63" s="33">
+      <c r="AA63" s="33">
         <v>12</v>
       </c>
-      <c r="Y63" s="6">
+      <c r="AB63" s="6">
         <v>0.41199999999999998</v>
       </c>
-      <c r="Z63" s="6">
+      <c r="AC63" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AA63" s="6">
+      <c r="AD63" s="6">
         <v>1397.9780000000001</v>
       </c>
-      <c r="AB63" s="6">
+      <c r="AE63" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AC63" s="6">
+      <c r="AF63" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -3605,39 +3746,47 @@
         <f t="shared" si="8"/>
         <v>26.289359999999999</v>
       </c>
-      <c r="S64" s="33">
+      <c r="R64" s="55"/>
+      <c r="S64" s="35">
         <v>13</v>
       </c>
-      <c r="T64" t="s">
+      <c r="T64" s="56">
+        <v>2220</v>
+      </c>
+      <c r="U64" s="55"/>
+      <c r="V64" s="33">
+        <v>13</v>
+      </c>
+      <c r="W64" t="s">
         <v>23</v>
       </c>
-      <c r="U64" s="6">
+      <c r="X64" s="6">
         <v>12171</v>
       </c>
-      <c r="V64" s="6">
+      <c r="Y64" s="6">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="X64" s="33">
+      <c r="AA64" s="33">
         <v>13</v>
       </c>
-      <c r="Y64" s="6">
+      <c r="AB64" s="6">
         <v>2.74</v>
       </c>
-      <c r="Z64" s="6">
+      <c r="AC64" s="6">
         <v>0.53300000000000003</v>
       </c>
-      <c r="AA64" s="6">
+      <c r="AD64" s="6">
         <v>2551.596</v>
       </c>
-      <c r="AB64" s="6">
+      <c r="AE64" s="6">
         <v>0.27400000000000002</v>
       </c>
-      <c r="AC64" s="6">
+      <c r="AF64" s="6">
         <v>0.04</v>
       </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -3678,39 +3827,47 @@
         <f t="shared" si="8"/>
         <v>34.819740000000003</v>
       </c>
-      <c r="S65" s="33">
+      <c r="R65" s="55"/>
+      <c r="S65" s="35">
         <v>14</v>
       </c>
-      <c r="T65" t="s">
+      <c r="T65" s="56">
+        <v>3120</v>
+      </c>
+      <c r="U65" s="55"/>
+      <c r="V65" s="33">
+        <v>14</v>
+      </c>
+      <c r="W65" t="s">
         <v>21</v>
       </c>
-      <c r="U65" s="6">
+      <c r="X65" s="6">
         <v>11379</v>
       </c>
-      <c r="V65" s="6">
+      <c r="Y65" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X65" s="33">
+      <c r="AA65" s="33">
         <v>14</v>
       </c>
-      <c r="Y65" s="6">
+      <c r="AB65" s="6">
         <v>0.38900000000000001</v>
       </c>
-      <c r="Z65" s="6">
+      <c r="AC65" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AA65" s="6">
+      <c r="AD65" s="6">
         <v>1352.424</v>
       </c>
-      <c r="AB65" s="6">
+      <c r="AE65" s="6">
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="AC65" s="6">
+      <c r="AF65" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -3751,39 +3908,47 @@
         <f t="shared" si="8"/>
         <v>37.647179999999999</v>
       </c>
-      <c r="S66" s="33">
+      <c r="R66" s="55"/>
+      <c r="S66" s="35">
         <v>15</v>
       </c>
-      <c r="T66" t="s">
+      <c r="T66" s="56">
+        <v>180</v>
+      </c>
+      <c r="U66" s="55"/>
+      <c r="V66" s="33">
+        <v>15</v>
+      </c>
+      <c r="W66" t="s">
         <v>21</v>
       </c>
-      <c r="U66" s="6">
+      <c r="X66" s="6">
         <v>12303</v>
       </c>
-      <c r="V66" s="6">
+      <c r="Y66" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X66" s="33">
+      <c r="AA66" s="33">
         <v>15</v>
       </c>
-      <c r="Y66" s="6">
+      <c r="AB66" s="6">
         <v>3.8889999999999998</v>
       </c>
-      <c r="Z66" s="6">
+      <c r="AC66" s="6">
         <v>3.9E-2</v>
       </c>
-      <c r="AA66" s="6">
+      <c r="AD66" s="6">
         <v>1436.3489999999999</v>
       </c>
-      <c r="AB66" s="6">
+      <c r="AE66" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="AC66" s="6">
+      <c r="AF66" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -3824,39 +3989,47 @@
         <f t="shared" si="8"/>
         <v>25.404119999999999</v>
       </c>
-      <c r="S67" s="33">
+      <c r="R67" s="55"/>
+      <c r="S67" s="35">
         <v>16</v>
       </c>
-      <c r="T67" t="s">
+      <c r="T67" s="56">
+        <v>180</v>
+      </c>
+      <c r="U67" s="55"/>
+      <c r="V67" s="33">
+        <v>16</v>
+      </c>
+      <c r="W67" t="s">
         <v>21</v>
       </c>
-      <c r="U67" s="6">
+      <c r="X67" s="6">
         <v>8302</v>
       </c>
-      <c r="V67" s="6">
+      <c r="Y67" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X67" s="33">
+      <c r="AA67" s="33">
         <v>16</v>
       </c>
-      <c r="Y67" s="6">
+      <c r="AB67" s="6">
         <v>0.35699999999999998</v>
       </c>
-      <c r="Z67" s="6">
+      <c r="AC67" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AA67" s="6">
+      <c r="AD67" s="6">
         <v>986.73699999999997</v>
       </c>
-      <c r="AB67" s="6">
+      <c r="AE67" s="6">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="AC67" s="6">
+      <c r="AF67" s="6">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -3897,39 +4070,47 @@
         <f t="shared" si="8"/>
         <v>23.453280000000003</v>
       </c>
-      <c r="S68" s="33">
+      <c r="R68" s="55"/>
+      <c r="S68" s="35">
         <v>17</v>
       </c>
-      <c r="T68" t="s">
+      <c r="T68" s="56">
+        <v>300</v>
+      </c>
+      <c r="U68" s="55"/>
+      <c r="V68" s="33">
+        <v>17</v>
+      </c>
+      <c r="W68" t="s">
         <v>23</v>
       </c>
-      <c r="U68" s="6">
+      <c r="X68" s="6">
         <v>10858</v>
       </c>
-      <c r="V68" s="6">
+      <c r="Y68" s="6">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="X68" s="33">
+      <c r="AA68" s="33">
         <v>17</v>
       </c>
-      <c r="Y68" s="6">
+      <c r="AB68" s="6">
         <v>3.786</v>
       </c>
-      <c r="Z68" s="6">
+      <c r="AC68" s="6">
         <v>1.365</v>
       </c>
-      <c r="AA68" s="6">
+      <c r="AD68" s="6">
         <v>2277.605</v>
       </c>
-      <c r="AB68" s="6">
+      <c r="AE68" s="6">
         <v>0.249</v>
       </c>
-      <c r="AC68" s="6">
+      <c r="AF68" s="6">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -3970,50 +4151,58 @@
         <f t="shared" si="8"/>
         <v>23.647680000000001</v>
       </c>
-      <c r="S69" s="33">
+      <c r="R69" s="55"/>
+      <c r="S69" s="35">
         <v>18</v>
       </c>
-      <c r="T69" t="s">
+      <c r="T69" s="56">
+        <v>2700</v>
+      </c>
+      <c r="U69" s="55"/>
+      <c r="V69" s="33">
+        <v>18</v>
+      </c>
+      <c r="W69" t="s">
         <v>23</v>
       </c>
-      <c r="U69" s="6">
+      <c r="X69" s="6">
         <v>10948</v>
       </c>
-      <c r="V69" s="6">
+      <c r="Y69" s="6">
         <f t="shared" si="9"/>
         <v>2.16</v>
       </c>
-      <c r="X69" s="33">
+      <c r="AA69" s="33">
         <v>18</v>
       </c>
-      <c r="Y69" s="6">
+      <c r="AB69" s="6">
         <v>1.2689999999999999</v>
       </c>
-      <c r="Z69" s="6">
+      <c r="AC69" s="6">
         <v>0.40300000000000002</v>
       </c>
-      <c r="AA69" s="6">
+      <c r="AD69" s="6">
         <v>2246.4659999999999</v>
       </c>
-      <c r="AB69" s="6">
+      <c r="AE69" s="6">
         <v>0.223</v>
       </c>
-      <c r="AC69" s="6">
+      <c r="AF69" s="6">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="AF69" s="48" t="s">
+      <c r="AI69" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="AG69" s="42" t="s">
+      <c r="AJ69" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="AH69" s="42"/>
-      <c r="AI69" s="42" t="s">
+      <c r="AK69" s="40"/>
+      <c r="AL69" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="AJ69" s="43"/>
-    </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM69" s="49"/>
+    </row>
+    <row r="70" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -4054,44 +4243,52 @@
         <f t="shared" si="8"/>
         <v>223.99503999999999</v>
       </c>
-      <c r="S70" s="33">
+      <c r="R70" s="55"/>
+      <c r="S70" s="35">
         <v>19</v>
       </c>
-      <c r="T70" t="s">
+      <c r="T70" s="56">
+        <v>120</v>
+      </c>
+      <c r="U70" s="55"/>
+      <c r="V70" s="33">
+        <v>19</v>
+      </c>
+      <c r="W70" t="s">
         <v>24</v>
       </c>
-      <c r="U70" s="6">
+      <c r="X70" s="6">
         <v>17834</v>
       </c>
-      <c r="V70" s="6">
+      <c r="Y70" s="6">
         <f t="shared" si="9"/>
         <v>12.56</v>
       </c>
-      <c r="X70" s="33">
+      <c r="AA70" s="33">
         <v>19</v>
       </c>
-      <c r="Y70" s="6">
+      <c r="AB70" s="6">
         <v>15.976000000000001</v>
       </c>
-      <c r="Z70" s="6">
+      <c r="AC70" s="6">
         <v>9.0060000000000002</v>
       </c>
-      <c r="AA70" s="6">
+      <c r="AD70" s="6">
         <v>2912.8049999999998</v>
       </c>
-      <c r="AB70" s="6">
+      <c r="AE70" s="6">
         <v>0.11799999999999999</v>
       </c>
-      <c r="AC70" s="6">
+      <c r="AF70" s="6">
         <v>2.4E-2</v>
       </c>
-      <c r="AF70" s="49"/>
-      <c r="AG70" s="44"/>
-      <c r="AH70" s="44"/>
-      <c r="AI70" s="44"/>
-      <c r="AJ70" s="45"/>
-    </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AI70" s="39"/>
+      <c r="AJ70" s="41"/>
+      <c r="AK70" s="41"/>
+      <c r="AL70" s="41"/>
+      <c r="AM70" s="50"/>
+    </row>
+    <row r="71" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -4132,42 +4329,50 @@
         <f t="shared" si="8"/>
         <v>36.931139999999999</v>
       </c>
-      <c r="S71" s="33">
+      <c r="R71" s="55"/>
+      <c r="S71" s="35">
         <v>20</v>
       </c>
-      <c r="T71" t="s">
+      <c r="T71" s="56">
+        <v>1920</v>
+      </c>
+      <c r="U71" s="55"/>
+      <c r="V71" s="33">
+        <v>20</v>
+      </c>
+      <c r="W71" t="s">
         <v>21</v>
       </c>
-      <c r="U71" s="6">
+      <c r="X71" s="6">
         <v>12069</v>
       </c>
-      <c r="V71" s="6">
+      <c r="Y71" s="6">
         <f t="shared" si="9"/>
         <v>3.06</v>
       </c>
-      <c r="X71" s="33">
+      <c r="AA71" s="33">
         <v>20</v>
       </c>
-      <c r="Y71" s="6">
+      <c r="AB71" s="6">
         <v>2.1019999999999999</v>
       </c>
-      <c r="Z71" s="6">
+      <c r="AC71" s="6">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AA71" s="6">
+      <c r="AD71" s="6">
         <v>1434.461</v>
       </c>
-      <c r="AB71" s="6">
+      <c r="AE71" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="AC71" s="6">
+      <c r="AF71" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="AE71" t="s">
+      <c r="AH71" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -4187,14 +4392,14 @@
         <v>21</v>
       </c>
       <c r="H72" s="6">
-        <f>$G$4*AI72</f>
+        <f>$G$4*AL72</f>
         <v>28.1</v>
       </c>
       <c r="J72" s="33">
         <v>21</v>
       </c>
       <c r="K72" s="6">
-        <f>$G$4*AL72</f>
+        <f>$G$4*AO72</f>
         <v>0</v>
       </c>
       <c r="M72" s="11">
@@ -4210,52 +4415,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S72" s="33">
+      <c r="R72" s="55"/>
+      <c r="S72" s="35">
         <v>21</v>
       </c>
-      <c r="T72" t="s">
+      <c r="T72" s="56">
+        <f>H72</f>
+        <v>28.1</v>
+      </c>
+      <c r="V72" s="33">
+        <v>21</v>
+      </c>
+      <c r="W72" t="s">
         <v>37</v>
       </c>
-      <c r="U72" s="6">
-        <v>0</v>
-      </c>
-      <c r="V72" s="6">
-        <v>0</v>
-      </c>
-      <c r="X72" s="33">
+      <c r="X72" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA72" s="33">
         <v>21</v>
       </c>
-      <c r="Y72" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z72" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA72" s="6">
-        <v>0</v>
-      </c>
       <c r="AB72" s="6">
         <v>0</v>
       </c>
       <c r="AC72" s="6">
         <v>0</v>
       </c>
-      <c r="AE72" s="17">
+      <c r="AD72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="17">
         <v>21</v>
       </c>
-      <c r="AF72" s="18">
+      <c r="AI72" s="18">
         <v>0.29299999999999998</v>
       </c>
-      <c r="AG72" s="50">
+      <c r="AJ72" s="42">
         <v>72154</v>
       </c>
-      <c r="AH72" s="50"/>
-      <c r="AI72" s="46">
+      <c r="AK72" s="42"/>
+      <c r="AL72" s="51">
         <v>28.1</v>
       </c>
-      <c r="AJ72" s="47"/>
-    </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM72" s="52"/>
+    </row>
+    <row r="73" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -4275,14 +4488,14 @@
         <v>22</v>
       </c>
       <c r="H73" s="6">
-        <f t="shared" ref="H73:H91" si="10">$G$4*AI73</f>
+        <f t="shared" ref="H73:H91" si="10">$G$4*AL73</f>
         <v>25</v>
       </c>
       <c r="J73" s="33">
         <v>22</v>
       </c>
       <c r="K73" s="6">
-        <f t="shared" ref="K73:K91" si="11">$G$4*AL73</f>
+        <f t="shared" ref="K73:K91" si="11">$G$4*AO73</f>
         <v>0</v>
       </c>
       <c r="M73" s="11">
@@ -4298,52 +4511,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S73" s="33">
+      <c r="R73" s="55"/>
+      <c r="S73" s="35">
         <v>22</v>
       </c>
-      <c r="T73" t="s">
+      <c r="T73" s="56">
+        <f t="shared" ref="T73:T91" si="12">H73</f>
+        <v>25</v>
+      </c>
+      <c r="V73" s="33">
+        <v>22</v>
+      </c>
+      <c r="W73" t="s">
         <v>37</v>
       </c>
-      <c r="U73" s="6">
-        <v>0</v>
-      </c>
-      <c r="V73" s="6">
-        <v>0</v>
-      </c>
-      <c r="X73" s="33">
+      <c r="X73" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y73" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA73" s="33">
         <v>22</v>
       </c>
-      <c r="Y73" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z73" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA73" s="6">
-        <v>0</v>
-      </c>
       <c r="AB73" s="6">
         <v>0</v>
       </c>
       <c r="AC73" s="6">
         <v>0</v>
       </c>
-      <c r="AE73" s="19">
+      <c r="AD73" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE73" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF73" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH73" s="19">
         <v>22</v>
       </c>
-      <c r="AF73" s="20">
+      <c r="AI73" s="20">
         <v>0.31</v>
       </c>
-      <c r="AG73" s="40">
+      <c r="AJ73" s="43">
         <v>67811</v>
       </c>
-      <c r="AH73" s="40"/>
-      <c r="AI73" s="36">
+      <c r="AK73" s="43"/>
+      <c r="AL73" s="44">
         <v>25</v>
       </c>
-      <c r="AJ73" s="37"/>
-    </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM73" s="45"/>
+    </row>
+    <row r="74" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>39</v>
       </c>
@@ -4386,52 +4607,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S74" s="33">
+      <c r="R74" s="55"/>
+      <c r="S74" s="35">
         <v>23</v>
       </c>
-      <c r="T74" t="s">
+      <c r="T74" s="56">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="V74" s="33">
+        <v>23</v>
+      </c>
+      <c r="W74" t="s">
         <v>37</v>
       </c>
-      <c r="U74" s="6">
-        <v>0</v>
-      </c>
-      <c r="V74" s="6">
-        <v>0</v>
-      </c>
-      <c r="X74" s="33">
+      <c r="X74" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y74" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA74" s="33">
         <v>23</v>
       </c>
-      <c r="Y74" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z74" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA74" s="6">
-        <v>0</v>
-      </c>
       <c r="AB74" s="6">
         <v>0</v>
       </c>
       <c r="AC74" s="6">
         <v>0</v>
       </c>
-      <c r="AE74" s="19">
+      <c r="AD74" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE74" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="19">
         <v>23</v>
       </c>
-      <c r="AF74" s="20">
+      <c r="AI74" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG74" s="40">
+      <c r="AJ74" s="43">
         <v>187455</v>
       </c>
-      <c r="AH74" s="40"/>
-      <c r="AI74" s="36">
+      <c r="AK74" s="43"/>
+      <c r="AL74" s="44">
         <v>70</v>
       </c>
-      <c r="AJ74" s="37"/>
-    </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM74" s="45"/>
+    </row>
+    <row r="75" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>40</v>
       </c>
@@ -4474,52 +4703,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S75" s="33">
+      <c r="R75" s="55"/>
+      <c r="S75" s="35">
         <v>24</v>
       </c>
-      <c r="T75" t="s">
+      <c r="T75" s="56">
+        <f t="shared" si="12"/>
+        <v>30.6</v>
+      </c>
+      <c r="V75" s="33">
+        <v>24</v>
+      </c>
+      <c r="W75" t="s">
         <v>37</v>
       </c>
-      <c r="U75" s="6">
-        <v>0</v>
-      </c>
-      <c r="V75" s="6">
-        <v>0</v>
-      </c>
-      <c r="X75" s="33">
+      <c r="X75" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y75" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA75" s="33">
         <v>24</v>
       </c>
-      <c r="Y75" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z75" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA75" s="6">
-        <v>0</v>
-      </c>
       <c r="AB75" s="6">
         <v>0</v>
       </c>
       <c r="AC75" s="6">
         <v>0</v>
       </c>
-      <c r="AE75" s="19">
+      <c r="AD75" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE75" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF75" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH75" s="19">
         <v>24</v>
       </c>
-      <c r="AF75" s="20">
+      <c r="AI75" s="20">
         <v>0.23599999999999999</v>
       </c>
-      <c r="AG75" s="40">
+      <c r="AJ75" s="43">
         <v>63266</v>
       </c>
-      <c r="AH75" s="40"/>
-      <c r="AI75" s="36">
+      <c r="AK75" s="43"/>
+      <c r="AL75" s="44">
         <v>30.6</v>
       </c>
-      <c r="AJ75" s="37"/>
-    </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM75" s="45"/>
+    </row>
+    <row r="76" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>41</v>
       </c>
@@ -4562,52 +4799,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S76" s="33">
+      <c r="R76" s="55"/>
+      <c r="S76" s="35">
         <v>25</v>
       </c>
-      <c r="T76" t="s">
+      <c r="T76" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V76" s="33">
+        <v>25</v>
+      </c>
+      <c r="W76" t="s">
         <v>37</v>
       </c>
-      <c r="U76" s="6">
-        <v>0</v>
-      </c>
-      <c r="V76" s="6">
-        <v>0</v>
-      </c>
-      <c r="X76" s="33">
+      <c r="X76" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA76" s="33">
         <v>25</v>
       </c>
-      <c r="Y76" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z76" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA76" s="6">
-        <v>0</v>
-      </c>
       <c r="AB76" s="6">
         <v>0</v>
       </c>
       <c r="AC76" s="6">
         <v>0</v>
       </c>
-      <c r="AE76" s="19">
+      <c r="AD76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH76" s="19">
         <v>25</v>
       </c>
-      <c r="AF76" s="20">
+      <c r="AI76" s="20">
         <v>0.30299999999999999</v>
       </c>
-      <c r="AG76" s="40">
+      <c r="AJ76" s="43">
         <v>26553</v>
       </c>
-      <c r="AH76" s="40"/>
-      <c r="AI76" s="36">
+      <c r="AK76" s="43"/>
+      <c r="AL76" s="44">
         <v>10</v>
       </c>
-      <c r="AJ76" s="37"/>
-    </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM76" s="45"/>
+    </row>
+    <row r="77" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -4650,52 +4895,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S77" s="33">
+      <c r="R77" s="55"/>
+      <c r="S77" s="35">
         <v>26</v>
       </c>
-      <c r="T77" t="s">
+      <c r="T77" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V77" s="33">
+        <v>26</v>
+      </c>
+      <c r="W77" t="s">
         <v>37</v>
       </c>
-      <c r="U77" s="6">
-        <v>0</v>
-      </c>
-      <c r="V77" s="6">
-        <v>0</v>
-      </c>
-      <c r="X77" s="33">
+      <c r="X77" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA77" s="33">
         <v>26</v>
       </c>
-      <c r="Y77" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z77" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA77" s="6">
-        <v>0</v>
-      </c>
       <c r="AB77" s="6">
         <v>0</v>
       </c>
       <c r="AC77" s="6">
         <v>0</v>
       </c>
-      <c r="AE77" s="19">
+      <c r="AD77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH77" s="19">
         <v>26</v>
       </c>
-      <c r="AF77" s="20">
+      <c r="AI77" s="20">
         <v>0.28499999999999998</v>
       </c>
-      <c r="AG77" s="40">
+      <c r="AJ77" s="43">
         <v>24949</v>
       </c>
-      <c r="AH77" s="40"/>
-      <c r="AI77" s="36">
+      <c r="AK77" s="43"/>
+      <c r="AL77" s="44">
         <v>10</v>
       </c>
-      <c r="AJ77" s="37"/>
-    </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM77" s="45"/>
+    </row>
+    <row r="78" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>43</v>
       </c>
@@ -4738,52 +4991,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S78" s="33">
+      <c r="R78" s="55"/>
+      <c r="S78" s="35">
         <v>27</v>
       </c>
-      <c r="T78" t="s">
+      <c r="T78" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V78" s="33">
+        <v>27</v>
+      </c>
+      <c r="W78" t="s">
         <v>37</v>
       </c>
-      <c r="U78" s="6">
-        <v>0</v>
-      </c>
-      <c r="V78" s="6">
-        <v>0</v>
-      </c>
-      <c r="X78" s="33">
+      <c r="X78" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA78" s="33">
         <v>27</v>
       </c>
-      <c r="Y78" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z78" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA78" s="6">
-        <v>0</v>
-      </c>
       <c r="AB78" s="6">
         <v>0</v>
       </c>
       <c r="AC78" s="6">
         <v>0</v>
       </c>
-      <c r="AE78" s="19">
+      <c r="AD78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="19">
         <v>27</v>
       </c>
-      <c r="AF78" s="20">
+      <c r="AI78" s="20">
         <v>0.26100000000000001</v>
       </c>
-      <c r="AG78" s="40">
+      <c r="AJ78" s="43">
         <v>22870</v>
       </c>
-      <c r="AH78" s="40"/>
-      <c r="AI78" s="36">
+      <c r="AK78" s="43"/>
+      <c r="AL78" s="44">
         <v>10</v>
       </c>
-      <c r="AJ78" s="37"/>
-    </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM78" s="45"/>
+    </row>
+    <row r="79" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>44</v>
       </c>
@@ -4826,52 +5087,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S79" s="33">
+      <c r="R79" s="55"/>
+      <c r="S79" s="35">
         <v>28</v>
       </c>
-      <c r="T79" t="s">
+      <c r="T79" s="56">
+        <f t="shared" si="12"/>
+        <v>52.2</v>
+      </c>
+      <c r="V79" s="33">
+        <v>28</v>
+      </c>
+      <c r="W79" t="s">
         <v>37</v>
       </c>
-      <c r="U79" s="6">
-        <v>0</v>
-      </c>
-      <c r="V79" s="6">
-        <v>0</v>
-      </c>
-      <c r="X79" s="33">
+      <c r="X79" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA79" s="33">
         <v>28</v>
       </c>
-      <c r="Y79" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z79" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA79" s="6">
-        <v>0</v>
-      </c>
       <c r="AB79" s="6">
         <v>0</v>
       </c>
       <c r="AC79" s="6">
         <v>0</v>
       </c>
-      <c r="AE79" s="19">
+      <c r="AD79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="19">
         <v>28</v>
       </c>
-      <c r="AF79" s="20">
+      <c r="AI79" s="20">
         <v>0.30599999999999999</v>
       </c>
-      <c r="AG79" s="40">
+      <c r="AJ79" s="43">
         <v>139836</v>
       </c>
-      <c r="AH79" s="40"/>
-      <c r="AI79" s="36">
+      <c r="AK79" s="43"/>
+      <c r="AL79" s="44">
         <v>52.2</v>
       </c>
-      <c r="AJ79" s="37"/>
-    </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM79" s="45"/>
+    </row>
+    <row r="80" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>45</v>
       </c>
@@ -4914,52 +5183,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S80" s="33">
+      <c r="R80" s="55"/>
+      <c r="S80" s="35">
         <v>29</v>
       </c>
-      <c r="T80" t="s">
+      <c r="T80" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V80" s="33">
+        <v>29</v>
+      </c>
+      <c r="W80" t="s">
         <v>37</v>
       </c>
-      <c r="U80" s="6">
-        <v>0</v>
-      </c>
-      <c r="V80" s="6">
-        <v>0</v>
-      </c>
-      <c r="X80" s="33">
+      <c r="X80" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA80" s="33">
         <v>29</v>
       </c>
-      <c r="Y80" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z80" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA80" s="6">
-        <v>0</v>
-      </c>
       <c r="AB80" s="6">
         <v>0</v>
       </c>
       <c r="AC80" s="6">
         <v>0</v>
       </c>
-      <c r="AE80" s="19">
+      <c r="AD80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="19">
         <v>29</v>
       </c>
-      <c r="AF80" s="20">
+      <c r="AI80" s="20">
         <v>0.26800000000000002</v>
       </c>
-      <c r="AG80" s="40">
+      <c r="AJ80" s="43">
         <v>23515</v>
       </c>
-      <c r="AH80" s="40"/>
-      <c r="AI80" s="36">
+      <c r="AK80" s="43"/>
+      <c r="AL80" s="44">
         <v>10</v>
       </c>
-      <c r="AJ80" s="37"/>
-    </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM80" s="45"/>
+    </row>
+    <row r="81" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>46</v>
       </c>
@@ -5002,52 +5279,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S81" s="33">
+      <c r="R81" s="55"/>
+      <c r="S81" s="35">
         <v>30</v>
       </c>
-      <c r="T81" t="s">
+      <c r="T81" s="56">
+        <f t="shared" si="12"/>
+        <v>20.2</v>
+      </c>
+      <c r="V81" s="33">
+        <v>30</v>
+      </c>
+      <c r="W81" t="s">
         <v>37</v>
       </c>
-      <c r="U81" s="6">
-        <v>0</v>
-      </c>
-      <c r="V81" s="6">
-        <v>0</v>
-      </c>
-      <c r="X81" s="33">
+      <c r="X81" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA81" s="33">
         <v>30</v>
       </c>
-      <c r="Y81" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z81" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA81" s="6">
-        <v>0</v>
-      </c>
       <c r="AB81" s="6">
         <v>0</v>
       </c>
       <c r="AC81" s="6">
         <v>0</v>
       </c>
-      <c r="AE81" s="19">
+      <c r="AD81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH81" s="19">
         <v>30</v>
       </c>
-      <c r="AF81" s="20">
+      <c r="AI81" s="20">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AG81" s="40">
+      <c r="AJ81" s="43">
         <v>49503</v>
       </c>
-      <c r="AH81" s="40"/>
-      <c r="AI81" s="36">
+      <c r="AK81" s="43"/>
+      <c r="AL81" s="44">
         <v>20.2</v>
       </c>
-      <c r="AJ81" s="37"/>
-    </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM81" s="45"/>
+    </row>
+    <row r="82" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>47</v>
       </c>
@@ -5090,52 +5375,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S82" s="33">
+      <c r="R82" s="55"/>
+      <c r="S82" s="35">
         <v>31</v>
       </c>
-      <c r="T82" t="s">
+      <c r="T82" s="56">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="V82" s="33">
+        <v>31</v>
+      </c>
+      <c r="W82" t="s">
         <v>37</v>
       </c>
-      <c r="U82" s="6">
-        <v>0</v>
-      </c>
-      <c r="V82" s="6">
-        <v>0</v>
-      </c>
-      <c r="X82" s="33">
+      <c r="X82" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA82" s="33">
         <v>31</v>
       </c>
-      <c r="Y82" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z82" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA82" s="6">
-        <v>0</v>
-      </c>
       <c r="AB82" s="6">
         <v>0</v>
       </c>
       <c r="AC82" s="6">
         <v>0</v>
       </c>
-      <c r="AE82" s="19">
+      <c r="AD82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="19">
         <v>31</v>
       </c>
-      <c r="AF82" s="20">
+      <c r="AI82" s="20">
         <v>0.307</v>
       </c>
-      <c r="AG82" s="40">
+      <c r="AJ82" s="43">
         <v>188420</v>
       </c>
-      <c r="AH82" s="40"/>
-      <c r="AI82" s="36">
+      <c r="AK82" s="43"/>
+      <c r="AL82" s="44">
         <v>70</v>
       </c>
-      <c r="AJ82" s="37"/>
-    </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM82" s="45"/>
+    </row>
+    <row r="83" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -5178,52 +5471,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S83" s="33">
+      <c r="R83" s="55"/>
+      <c r="S83" s="35">
         <v>32</v>
       </c>
-      <c r="T83" t="s">
+      <c r="T83" s="56">
+        <f t="shared" si="12"/>
+        <v>10.5</v>
+      </c>
+      <c r="V83" s="33">
+        <v>32</v>
+      </c>
+      <c r="W83" t="s">
         <v>37</v>
       </c>
-      <c r="U83" s="6">
-        <v>0</v>
-      </c>
-      <c r="V83" s="6">
-        <v>0</v>
-      </c>
-      <c r="X83" s="33">
+      <c r="X83" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y83" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA83" s="33">
         <v>32</v>
       </c>
-      <c r="Y83" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z83" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA83" s="6">
-        <v>0</v>
-      </c>
       <c r="AB83" s="6">
         <v>0</v>
       </c>
       <c r="AC83" s="6">
         <v>0</v>
       </c>
-      <c r="AE83" s="19">
+      <c r="AD83" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE83" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF83" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="19">
         <v>32</v>
       </c>
-      <c r="AF83" s="20">
+      <c r="AI83" s="20">
         <v>0.28899999999999998</v>
       </c>
-      <c r="AG83" s="40">
+      <c r="AJ83" s="43">
         <v>26573</v>
       </c>
-      <c r="AH83" s="40"/>
-      <c r="AI83" s="36">
+      <c r="AK83" s="43"/>
+      <c r="AL83" s="44">
         <v>10.5</v>
       </c>
-      <c r="AJ83" s="37"/>
-    </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM83" s="45"/>
+    </row>
+    <row r="84" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>49</v>
       </c>
@@ -5266,52 +5567,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S84" s="33">
+      <c r="R84" s="55"/>
+      <c r="S84" s="35">
         <v>33</v>
       </c>
-      <c r="T84" t="s">
+      <c r="T84" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V84" s="33">
+        <v>33</v>
+      </c>
+      <c r="W84" t="s">
         <v>37</v>
       </c>
-      <c r="U84" s="6">
-        <v>0</v>
-      </c>
-      <c r="V84" s="6">
-        <v>0</v>
-      </c>
-      <c r="X84" s="33">
+      <c r="X84" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA84" s="33">
         <v>33</v>
       </c>
-      <c r="Y84" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z84" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA84" s="6">
-        <v>0</v>
-      </c>
       <c r="AB84" s="6">
         <v>0</v>
       </c>
       <c r="AC84" s="6">
         <v>0</v>
       </c>
-      <c r="AE84" s="19">
+      <c r="AD84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="19">
         <v>33</v>
       </c>
-      <c r="AF84" s="20">
+      <c r="AI84" s="20">
         <v>0.28799999999999998</v>
       </c>
-      <c r="AG84" s="40">
+      <c r="AJ84" s="43">
         <v>25253</v>
       </c>
-      <c r="AH84" s="40"/>
-      <c r="AI84" s="36">
+      <c r="AK84" s="43"/>
+      <c r="AL84" s="44">
         <v>10</v>
       </c>
-      <c r="AJ84" s="37"/>
-    </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM84" s="45"/>
+    </row>
+    <row r="85" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>50</v>
       </c>
@@ -5354,52 +5663,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S85" s="33">
+      <c r="R85" s="55"/>
+      <c r="S85" s="35">
         <v>34</v>
       </c>
-      <c r="T85" t="s">
+      <c r="T85" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V85" s="33">
+        <v>34</v>
+      </c>
+      <c r="W85" t="s">
         <v>37</v>
       </c>
-      <c r="U85" s="6">
-        <v>0</v>
-      </c>
-      <c r="V85" s="6">
-        <v>0</v>
-      </c>
-      <c r="X85" s="33">
+      <c r="X85" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA85" s="33">
         <v>34</v>
       </c>
-      <c r="Y85" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z85" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA85" s="6">
-        <v>0</v>
-      </c>
       <c r="AB85" s="6">
         <v>0</v>
       </c>
       <c r="AC85" s="6">
         <v>0</v>
       </c>
-      <c r="AE85" s="19">
+      <c r="AD85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="19">
         <v>34</v>
       </c>
-      <c r="AF85" s="20">
+      <c r="AI85" s="20">
         <v>0.20100000000000001</v>
       </c>
-      <c r="AG85" s="40">
+      <c r="AJ85" s="43">
         <v>17610</v>
       </c>
-      <c r="AH85" s="40"/>
-      <c r="AI85" s="36">
+      <c r="AK85" s="43"/>
+      <c r="AL85" s="44">
         <v>10</v>
       </c>
-      <c r="AJ85" s="37"/>
-    </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM85" s="45"/>
+    </row>
+    <row r="86" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>51</v>
       </c>
@@ -5442,52 +5759,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S86" s="33">
+      <c r="R86" s="55"/>
+      <c r="S86" s="35">
         <v>35</v>
       </c>
-      <c r="T86" t="s">
+      <c r="T86" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V86" s="33">
+        <v>35</v>
+      </c>
+      <c r="W86" t="s">
         <v>37</v>
       </c>
-      <c r="U86" s="6">
-        <v>0</v>
-      </c>
-      <c r="V86" s="6">
-        <v>0</v>
-      </c>
-      <c r="X86" s="33">
+      <c r="X86" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA86" s="33">
         <v>35</v>
       </c>
-      <c r="Y86" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z86" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA86" s="6">
-        <v>0</v>
-      </c>
       <c r="AB86" s="6">
         <v>0</v>
       </c>
       <c r="AC86" s="6">
         <v>0</v>
       </c>
-      <c r="AE86" s="19">
+      <c r="AD86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="19">
         <v>35</v>
       </c>
-      <c r="AF86" s="20">
+      <c r="AI86" s="20">
         <v>0.221</v>
       </c>
-      <c r="AG86" s="40">
+      <c r="AJ86" s="43">
         <v>19372</v>
       </c>
-      <c r="AH86" s="40"/>
-      <c r="AI86" s="36">
+      <c r="AK86" s="43"/>
+      <c r="AL86" s="44">
         <v>10</v>
       </c>
-      <c r="AJ86" s="37"/>
-    </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM86" s="45"/>
+    </row>
+    <row r="87" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>52</v>
       </c>
@@ -5530,52 +5855,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S87" s="33">
+      <c r="R87" s="55"/>
+      <c r="S87" s="35">
         <v>36</v>
       </c>
-      <c r="T87" t="s">
+      <c r="T87" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V87" s="33">
+        <v>36</v>
+      </c>
+      <c r="W87" t="s">
         <v>37</v>
       </c>
-      <c r="U87" s="6">
-        <v>0</v>
-      </c>
-      <c r="V87" s="6">
-        <v>0</v>
-      </c>
-      <c r="X87" s="33">
+      <c r="X87" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA87" s="33">
         <v>36</v>
       </c>
-      <c r="Y87" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z87" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA87" s="6">
-        <v>0</v>
-      </c>
       <c r="AB87" s="6">
         <v>0</v>
       </c>
       <c r="AC87" s="6">
         <v>0</v>
       </c>
-      <c r="AE87" s="19">
+      <c r="AD87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH87" s="19">
         <v>36</v>
       </c>
-      <c r="AF87" s="20">
+      <c r="AI87" s="20">
         <v>0.216</v>
       </c>
-      <c r="AG87" s="40">
+      <c r="AJ87" s="43">
         <v>18939</v>
       </c>
-      <c r="AH87" s="40"/>
-      <c r="AI87" s="36">
+      <c r="AK87" s="43"/>
+      <c r="AL87" s="44">
         <v>10</v>
       </c>
-      <c r="AJ87" s="37"/>
-    </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM87" s="45"/>
+    </row>
+    <row r="88" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>53</v>
       </c>
@@ -5618,29 +5951,28 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S88" s="33">
+      <c r="R88" s="55"/>
+      <c r="S88" s="35">
         <v>37</v>
       </c>
-      <c r="T88" t="s">
+      <c r="T88" s="56">
+        <f t="shared" si="12"/>
+        <v>10.1</v>
+      </c>
+      <c r="V88" s="33">
         <v>37</v>
       </c>
-      <c r="U88" s="6">
-        <v>0</v>
-      </c>
-      <c r="V88" s="6">
-        <v>0</v>
-      </c>
-      <c r="X88" s="33">
+      <c r="W88" t="s">
         <v>37</v>
       </c>
+      <c r="X88" s="6">
+        <v>0</v>
+      </c>
       <c r="Y88" s="6">
         <v>0</v>
       </c>
-      <c r="Z88" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA88" s="6">
-        <v>0</v>
+      <c r="AA88" s="33">
+        <v>37</v>
       </c>
       <c r="AB88" s="6">
         <v>0</v>
@@ -5648,22 +5980,31 @@
       <c r="AC88" s="6">
         <v>0</v>
       </c>
-      <c r="AE88" s="19">
+      <c r="AD88" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE88" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF88" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH88" s="19">
         <v>37</v>
       </c>
-      <c r="AF88" s="20">
+      <c r="AI88" s="20">
         <v>0.23</v>
       </c>
-      <c r="AG88" s="40">
+      <c r="AJ88" s="43">
         <v>20382</v>
       </c>
-      <c r="AH88" s="40"/>
-      <c r="AI88" s="36">
+      <c r="AK88" s="43"/>
+      <c r="AL88" s="44">
         <v>10.1</v>
       </c>
-      <c r="AJ88" s="37"/>
-    </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM88" s="45"/>
+    </row>
+    <row r="89" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>54</v>
       </c>
@@ -5706,52 +6047,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S89" s="33">
+      <c r="R89" s="55"/>
+      <c r="S89" s="35">
         <v>38</v>
       </c>
-      <c r="T89" t="s">
+      <c r="T89" s="56">
+        <f t="shared" si="12"/>
+        <v>10.1</v>
+      </c>
+      <c r="V89" s="33">
+        <v>38</v>
+      </c>
+      <c r="W89" t="s">
         <v>37</v>
       </c>
-      <c r="U89" s="6">
-        <v>0</v>
-      </c>
-      <c r="V89" s="6">
-        <v>0</v>
-      </c>
-      <c r="X89" s="33">
+      <c r="X89" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA89" s="33">
         <v>38</v>
       </c>
-      <c r="Y89" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z89" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA89" s="6">
-        <v>0</v>
-      </c>
       <c r="AB89" s="6">
         <v>0</v>
       </c>
       <c r="AC89" s="6">
         <v>0</v>
       </c>
-      <c r="AE89" s="19">
+      <c r="AD89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH89" s="19">
         <v>38</v>
       </c>
-      <c r="AF89" s="20">
+      <c r="AI89" s="20">
         <v>0.22600000000000001</v>
       </c>
-      <c r="AG89" s="40">
+      <c r="AJ89" s="43">
         <v>19968</v>
       </c>
-      <c r="AH89" s="40"/>
-      <c r="AI89" s="36">
+      <c r="AK89" s="43"/>
+      <c r="AL89" s="44">
         <v>10.1</v>
       </c>
-      <c r="AJ89" s="37"/>
-    </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM89" s="45"/>
+    </row>
+    <row r="90" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>55</v>
       </c>
@@ -5794,52 +6143,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S90" s="33">
+      <c r="R90" s="55"/>
+      <c r="S90" s="35">
         <v>39</v>
       </c>
-      <c r="T90" t="s">
+      <c r="T90" s="56">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="V90" s="33">
+        <v>39</v>
+      </c>
+      <c r="W90" t="s">
         <v>37</v>
       </c>
-      <c r="U90" s="6">
-        <v>0</v>
-      </c>
-      <c r="V90" s="6">
-        <v>0</v>
-      </c>
-      <c r="X90" s="33">
+      <c r="X90" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA90" s="33">
         <v>39</v>
       </c>
-      <c r="Y90" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z90" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA90" s="6">
-        <v>0</v>
-      </c>
       <c r="AB90" s="6">
         <v>0</v>
       </c>
       <c r="AC90" s="6">
         <v>0</v>
       </c>
-      <c r="AE90" s="19">
+      <c r="AD90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="19">
         <v>39</v>
       </c>
-      <c r="AF90" s="20">
+      <c r="AI90" s="20">
         <v>0.26500000000000001</v>
       </c>
-      <c r="AG90" s="40">
+      <c r="AJ90" s="43">
         <v>23240</v>
       </c>
-      <c r="AH90" s="40"/>
-      <c r="AI90" s="36">
+      <c r="AK90" s="43"/>
+      <c r="AL90" s="44">
         <v>10</v>
       </c>
-      <c r="AJ90" s="37"/>
-    </row>
-    <row r="91" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM90" s="45"/>
+    </row>
+    <row r="91" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>56</v>
       </c>
@@ -5882,52 +6239,60 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S91" s="33">
+      <c r="R91" s="55"/>
+      <c r="S91" s="35">
         <v>40</v>
       </c>
-      <c r="T91" t="s">
+      <c r="T91" s="56">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="V91" s="33">
+        <v>40</v>
+      </c>
+      <c r="W91" t="s">
         <v>37</v>
       </c>
-      <c r="U91" s="6">
-        <v>0</v>
-      </c>
-      <c r="V91" s="6">
-        <v>0</v>
-      </c>
-      <c r="X91" s="33">
+      <c r="X91" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA91" s="33">
         <v>40</v>
       </c>
-      <c r="Y91" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z91" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA91" s="6">
-        <v>0</v>
-      </c>
       <c r="AB91" s="6">
         <v>0</v>
       </c>
       <c r="AC91" s="6">
         <v>0</v>
       </c>
-      <c r="AE91" s="21">
+      <c r="AD91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="21">
         <v>40</v>
       </c>
-      <c r="AF91" s="22">
+      <c r="AI91" s="22">
         <v>0.254</v>
       </c>
-      <c r="AG91" s="41">
+      <c r="AJ91" s="48">
         <v>26709</v>
       </c>
-      <c r="AH91" s="41"/>
-      <c r="AI91" s="38">
+      <c r="AK91" s="48"/>
+      <c r="AL91" s="46">
         <v>12</v>
       </c>
-      <c r="AJ91" s="39"/>
-    </row>
-    <row r="92" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AM91" s="47"/>
+    </row>
+    <row r="92" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>83</v>
       </c>
@@ -5968,38 +6333,45 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S92" s="33">
+      <c r="R92" s="55"/>
+      <c r="S92" s="35">
         <v>41</v>
       </c>
-      <c r="T92" t="s">
+      <c r="T92" s="56">
+        <v>0</v>
+      </c>
+      <c r="V92" s="33">
+        <v>41</v>
+      </c>
+      <c r="W92" t="s">
         <v>37</v>
       </c>
-      <c r="U92" s="6">
-        <v>0</v>
-      </c>
-      <c r="V92" s="6">
-        <v>0</v>
-      </c>
-      <c r="X92" s="33">
+      <c r="X92" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA92" s="33">
         <v>41</v>
       </c>
-      <c r="Y92" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z92" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA92" s="6">
-        <v>0</v>
-      </c>
       <c r="AB92" s="6">
         <v>0</v>
       </c>
       <c r="AC92" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AD92" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE92" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>84</v>
       </c>
@@ -6040,38 +6412,45 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S93" s="33">
+      <c r="R93" s="55"/>
+      <c r="S93" s="35">
         <v>42</v>
       </c>
-      <c r="T93" t="s">
+      <c r="T93" s="56">
+        <v>0</v>
+      </c>
+      <c r="V93" s="33">
+        <v>42</v>
+      </c>
+      <c r="W93" t="s">
         <v>85</v>
       </c>
-      <c r="U93" s="6">
-        <v>0</v>
-      </c>
-      <c r="V93" s="6">
-        <v>0</v>
-      </c>
-      <c r="X93" s="33">
+      <c r="X93" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y93" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA93" s="33">
         <v>42</v>
       </c>
-      <c r="Y93" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z93" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA93" s="6">
-        <v>0</v>
-      </c>
       <c r="AB93" s="6">
         <v>0</v>
       </c>
       <c r="AC93" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AD93" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE93" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF93" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>102</v>
       </c>
@@ -6112,38 +6491,111 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="S94" s="33">
+      <c r="R94" s="55"/>
+      <c r="S94" s="35">
         <v>43</v>
       </c>
-      <c r="U94" s="6">
-        <v>0</v>
-      </c>
-      <c r="V94" s="6">
-        <v>0</v>
-      </c>
-      <c r="X94" s="33">
+      <c r="T94" s="56">
+        <v>10000</v>
+      </c>
+      <c r="V94" s="33">
         <v>43</v>
       </c>
+      <c r="W94" t="s">
+        <v>102</v>
+      </c>
+      <c r="X94" s="6">
+        <v>0</v>
+      </c>
       <c r="Y94" s="6">
         <v>0</v>
       </c>
-      <c r="Z94" s="6">
-        <v>0</v>
-      </c>
-      <c r="AA94" s="6">
-        <v>0</v>
+      <c r="AA94" s="33">
+        <v>43</v>
       </c>
       <c r="AB94" s="6">
         <v>0</v>
       </c>
       <c r="AC94" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD94" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE94" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF94" s="6">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="73">
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="V6:X6"/>
+    <mergeCell ref="V7:X7"/>
+    <mergeCell ref="V4:X4"/>
+    <mergeCell ref="V5:X5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="AL89:AM89"/>
+    <mergeCell ref="AL90:AM90"/>
+    <mergeCell ref="AL91:AM91"/>
+    <mergeCell ref="AL84:AM84"/>
+    <mergeCell ref="AL85:AM85"/>
+    <mergeCell ref="AL86:AM86"/>
+    <mergeCell ref="AL87:AM87"/>
+    <mergeCell ref="AL88:AM88"/>
+    <mergeCell ref="AJ90:AK90"/>
+    <mergeCell ref="AJ91:AK91"/>
+    <mergeCell ref="AL69:AM70"/>
+    <mergeCell ref="AL72:AM72"/>
+    <mergeCell ref="AL73:AM73"/>
+    <mergeCell ref="AL74:AM74"/>
+    <mergeCell ref="AL75:AM75"/>
+    <mergeCell ref="AL76:AM76"/>
+    <mergeCell ref="AL77:AM77"/>
+    <mergeCell ref="AL78:AM78"/>
+    <mergeCell ref="AL79:AM79"/>
+    <mergeCell ref="AL80:AM80"/>
+    <mergeCell ref="AL81:AM81"/>
+    <mergeCell ref="AL82:AM82"/>
+    <mergeCell ref="AL83:AM83"/>
+    <mergeCell ref="AJ85:AK85"/>
+    <mergeCell ref="AJ86:AK86"/>
+    <mergeCell ref="AJ87:AK87"/>
+    <mergeCell ref="AJ88:AK88"/>
+    <mergeCell ref="AJ89:AK89"/>
+    <mergeCell ref="AJ80:AK80"/>
+    <mergeCell ref="AJ81:AK81"/>
+    <mergeCell ref="AJ82:AK82"/>
+    <mergeCell ref="AJ83:AK83"/>
+    <mergeCell ref="AJ84:AK84"/>
+    <mergeCell ref="AJ75:AK75"/>
+    <mergeCell ref="AJ76:AK76"/>
+    <mergeCell ref="AJ77:AK77"/>
+    <mergeCell ref="AJ78:AK78"/>
+    <mergeCell ref="AJ79:AK79"/>
+    <mergeCell ref="AI69:AI70"/>
+    <mergeCell ref="AJ69:AK70"/>
+    <mergeCell ref="AJ72:AK72"/>
+    <mergeCell ref="AJ73:AK73"/>
+    <mergeCell ref="AJ74:AK74"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="I11:K11"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="V8:X8"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
@@ -6152,69 +6604,6 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N7:P7"/>
     <mergeCell ref="N8:P8"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="AF69:AF70"/>
-    <mergeCell ref="AG69:AH70"/>
-    <mergeCell ref="AG72:AH72"/>
-    <mergeCell ref="AG73:AH73"/>
-    <mergeCell ref="AG74:AH74"/>
-    <mergeCell ref="AG75:AH75"/>
-    <mergeCell ref="AG76:AH76"/>
-    <mergeCell ref="AG77:AH77"/>
-    <mergeCell ref="AG78:AH78"/>
-    <mergeCell ref="AG79:AH79"/>
-    <mergeCell ref="AG87:AH87"/>
-    <mergeCell ref="AG88:AH88"/>
-    <mergeCell ref="AG89:AH89"/>
-    <mergeCell ref="AG80:AH80"/>
-    <mergeCell ref="AG81:AH81"/>
-    <mergeCell ref="AG82:AH82"/>
-    <mergeCell ref="AG83:AH83"/>
-    <mergeCell ref="AG84:AH84"/>
-    <mergeCell ref="AI81:AJ81"/>
-    <mergeCell ref="AI82:AJ82"/>
-    <mergeCell ref="AI83:AJ83"/>
-    <mergeCell ref="AG85:AH85"/>
-    <mergeCell ref="AG86:AH86"/>
-    <mergeCell ref="AI76:AJ76"/>
-    <mergeCell ref="AI77:AJ77"/>
-    <mergeCell ref="AI78:AJ78"/>
-    <mergeCell ref="AI79:AJ79"/>
-    <mergeCell ref="AI80:AJ80"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="AI89:AJ89"/>
-    <mergeCell ref="AI90:AJ90"/>
-    <mergeCell ref="AI91:AJ91"/>
-    <mergeCell ref="AI84:AJ84"/>
-    <mergeCell ref="AI85:AJ85"/>
-    <mergeCell ref="AI86:AJ86"/>
-    <mergeCell ref="AI87:AJ87"/>
-    <mergeCell ref="AI88:AJ88"/>
-    <mergeCell ref="AG90:AH90"/>
-    <mergeCell ref="AG91:AH91"/>
-    <mergeCell ref="AI69:AJ70"/>
-    <mergeCell ref="AI72:AJ72"/>
-    <mergeCell ref="AI73:AJ73"/>
-    <mergeCell ref="AI74:AJ74"/>
-    <mergeCell ref="AI75:AJ75"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="N6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change to battery free energy constraints
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -775,28 +775,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,10 +791,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -826,7 +815,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC55" sqref="AC55:AC97"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1142,34 +1142,34 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="40"/>
+      <c r="F1" s="41"/>
       <c r="G1" s="14">
         <v>0.1</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="Q1" s="24">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="S1" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1181,31 +1181,31 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
       <c r="G2" s="6"/>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1223,27 +1223,27 @@
       <c r="F3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="41" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
       <c r="Q3" s="24">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="40" t="s">
+      <c r="S3" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1265,27 +1265,27 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="40" t="s">
+      <c r="N4" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
       <c r="Q4" s="24">
         <v>43560</v>
       </c>
-      <c r="S4" s="40" t="s">
+      <c r="S4" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1302,27 +1302,27 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="N5" s="40" t="s">
+      <c r="N5" s="41" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
       <c r="Q5" s="24">
         <v>601000</v>
       </c>
-      <c r="S5" s="40" t="s">
+      <c r="S5" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="T5" s="40"/>
-      <c r="U5" s="40"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1345,23 +1345,23 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
       <c r="L6" s="10"/>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="40"/>
-      <c r="P6" s="40"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
       <c r="Q6" s="24">
         <v>15025</v>
       </c>
-      <c r="S6" s="40" t="s">
+      <c r="S6" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="40"/>
-      <c r="U6" s="40"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1384,19 +1384,19 @@
       <c r="G7" s="6">
         <v>4050</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="41"/>
       <c r="Q7" s="26">
         <v>0.95</v>
       </c>
-      <c r="S7" s="40" t="s">
+      <c r="S7" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="40"/>
-      <c r="U7" s="40"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1412,19 +1412,19 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="40"/>
-      <c r="P8" s="40"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
       <c r="Q8" s="26">
         <v>50</v>
       </c>
-      <c r="S8" s="40" t="s">
+      <c r="S8" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="40"/>
-      <c r="U8" s="40"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1440,11 +1440,11 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="N9" s="40" t="s">
+      <c r="N9" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
       <c r="Q9" s="26">
         <v>10</v>
       </c>
@@ -5741,17 +5741,17 @@
       </c>
     </row>
     <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
       <c r="F45" s="2"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="55"/>
+      <c r="J45" s="55"/>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="O45" s="4"/>
@@ -5988,11 +5988,11 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="55"/>
       <c r="G53" s="38" t="s">
         <v>137</v>
       </c>
@@ -6137,13 +6137,13 @@
         <v>1</v>
       </c>
       <c r="Z55" s="8">
-        <f>AG55*AH55*1000/1000000</f>
+        <f t="shared" ref="Z55:Z97" si="32">AG55*AH55*1000/1000000</f>
         <v>39.666780000000003</v>
       </c>
       <c r="AB55" s="39">
         <v>1</v>
       </c>
-      <c r="AC55" s="57">
+      <c r="AC55" s="40">
         <v>2520</v>
       </c>
       <c r="AE55" s="32">
@@ -6156,7 +6156,7 @@
         <v>12963</v>
       </c>
       <c r="AH55" s="6">
-        <f t="shared" ref="AH55:AH74" si="32">IF(EXACT(AF55,$R$47),$S$47,IF(EXACT(AF55,$R$48),$S$48,IF(EXACT(AF55,$R$49),$S$49,0)))</f>
+        <f t="shared" ref="AH55:AH74" si="33">IF(EXACT(AF55,$R$47),$S$47,IF(EXACT(AF55,$R$48),$S$48,IF(EXACT(AF55,$R$49),$S$49,0)))</f>
         <v>3.06</v>
       </c>
       <c r="AJ55" s="32">
@@ -6234,13 +6234,13 @@
         <v>2</v>
       </c>
       <c r="Z56" s="8">
-        <f>AG56*AH56*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>23.617080000000001</v>
       </c>
       <c r="AB56" s="39">
         <v>2</v>
       </c>
-      <c r="AC56" s="57">
+      <c r="AC56" s="40">
         <v>1980</v>
       </c>
       <c r="AE56" s="32">
@@ -6253,7 +6253,7 @@
         <v>7718</v>
       </c>
       <c r="AH56" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ56" s="32">
@@ -6331,13 +6331,13 @@
         <v>3</v>
       </c>
       <c r="Z57" s="8">
-        <f>AG57*AH57*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>28.115279999999998</v>
       </c>
       <c r="AB57" s="39">
         <v>3</v>
       </c>
-      <c r="AC57" s="57">
+      <c r="AC57" s="40">
         <v>240</v>
       </c>
       <c r="AE57" s="32">
@@ -6350,7 +6350,7 @@
         <v>9188</v>
       </c>
       <c r="AH57" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ57" s="32">
@@ -6428,13 +6428,13 @@
         <v>4</v>
       </c>
       <c r="Z58" s="8">
-        <f>AG58*AH58*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>21.77496</v>
       </c>
       <c r="AB58" s="39">
         <v>4</v>
       </c>
-      <c r="AC58" s="57">
+      <c r="AC58" s="40">
         <v>1020</v>
       </c>
       <c r="AE58" s="32">
@@ -6447,7 +6447,7 @@
         <v>7116</v>
       </c>
       <c r="AH58" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ58" s="32">
@@ -6525,13 +6525,13 @@
         <v>5</v>
       </c>
       <c r="Z59" s="8">
-        <f>AG59*AH59*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>23.94144</v>
       </c>
       <c r="AB59" s="39">
         <v>5</v>
       </c>
-      <c r="AC59" s="57">
+      <c r="AC59" s="40">
         <v>2220</v>
       </c>
       <c r="AE59" s="32">
@@ -6544,7 +6544,7 @@
         <v>7824</v>
       </c>
       <c r="AH59" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ59" s="32">
@@ -6622,13 +6622,13 @@
         <v>6</v>
       </c>
       <c r="Z60" s="8">
-        <f>AG60*AH60*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>38.22552000000001</v>
       </c>
       <c r="AB60" s="39">
         <v>6</v>
       </c>
-      <c r="AC60" s="57">
+      <c r="AC60" s="40">
         <v>300</v>
       </c>
       <c r="AE60" s="32">
@@ -6641,7 +6641,7 @@
         <v>12492</v>
       </c>
       <c r="AH60" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ60" s="32">
@@ -6719,13 +6719,13 @@
         <v>7</v>
       </c>
       <c r="Z61" s="8">
-        <f>AG61*AH61*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>1.6982999999999999</v>
       </c>
       <c r="AB61" s="39">
         <v>7</v>
       </c>
-      <c r="AC61" s="57">
+      <c r="AC61" s="40">
         <v>420</v>
       </c>
       <c r="AE61" s="32">
@@ -6738,7 +6738,7 @@
         <v>555</v>
       </c>
       <c r="AH61" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ61" s="32">
@@ -6816,13 +6816,13 @@
         <v>8</v>
       </c>
       <c r="Z62" s="8">
-        <f>AG62*AH62*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>36.677160000000001</v>
       </c>
       <c r="AB62" s="39">
         <v>8</v>
       </c>
-      <c r="AC62" s="57">
+      <c r="AC62" s="40">
         <v>420</v>
       </c>
       <c r="AE62" s="32">
@@ -6835,7 +6835,7 @@
         <v>11986</v>
       </c>
       <c r="AH62" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ62" s="32">
@@ -6913,13 +6913,13 @@
         <v>9</v>
       </c>
       <c r="Z63" s="8">
-        <f>AG63*AH63*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>23.494679999999999</v>
       </c>
       <c r="AB63" s="39">
         <v>9</v>
       </c>
-      <c r="AC63" s="57">
+      <c r="AC63" s="40">
         <v>1980</v>
       </c>
       <c r="AE63" s="32">
@@ -6932,7 +6932,7 @@
         <v>7678</v>
       </c>
       <c r="AH63" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ63" s="32">
@@ -7010,13 +7010,13 @@
         <v>10</v>
       </c>
       <c r="Z64" s="8">
-        <f>AG64*AH64*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>31.606739999999999</v>
       </c>
       <c r="AB64" s="39">
         <v>10</v>
       </c>
-      <c r="AC64" s="57">
+      <c r="AC64" s="40">
         <v>900</v>
       </c>
       <c r="AE64" s="32">
@@ -7029,7 +7029,7 @@
         <v>10329</v>
       </c>
       <c r="AH64" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ64" s="32">
@@ -7107,13 +7107,13 @@
         <v>11</v>
       </c>
       <c r="Z65" s="8">
-        <f>AG65*AH65*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>38.996639999999999</v>
       </c>
       <c r="AB65" s="39">
         <v>11</v>
       </c>
-      <c r="AC65" s="57">
+      <c r="AC65" s="40">
         <v>480</v>
       </c>
       <c r="AE65" s="32">
@@ -7126,7 +7126,7 @@
         <v>12744</v>
       </c>
       <c r="AH65" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ65" s="32">
@@ -7204,13 +7204,13 @@
         <v>12</v>
       </c>
       <c r="Z66" s="8">
-        <f>AG66*AH66*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>35.954999999999998</v>
       </c>
       <c r="AB66" s="39">
         <v>12</v>
       </c>
-      <c r="AC66" s="57">
+      <c r="AC66" s="40">
         <v>720</v>
       </c>
       <c r="AE66" s="32">
@@ -7223,7 +7223,7 @@
         <v>11750</v>
       </c>
       <c r="AH66" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ66" s="32">
@@ -7301,13 +7301,13 @@
         <v>13</v>
       </c>
       <c r="Z67" s="8">
-        <f>AG67*AH67*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>26.289359999999999</v>
       </c>
       <c r="AB67" s="39">
         <v>13</v>
       </c>
-      <c r="AC67" s="57">
+      <c r="AC67" s="40">
         <v>2220</v>
       </c>
       <c r="AE67" s="32">
@@ -7320,7 +7320,7 @@
         <v>12171</v>
       </c>
       <c r="AH67" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.16</v>
       </c>
       <c r="AJ67" s="32">
@@ -7398,13 +7398,13 @@
         <v>14</v>
       </c>
       <c r="Z68" s="8">
-        <f>AG68*AH68*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>34.819740000000003</v>
       </c>
       <c r="AB68" s="39">
         <v>14</v>
       </c>
-      <c r="AC68" s="57">
+      <c r="AC68" s="40">
         <v>3120</v>
       </c>
       <c r="AE68" s="32">
@@ -7417,7 +7417,7 @@
         <v>11379</v>
       </c>
       <c r="AH68" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ68" s="32">
@@ -7495,13 +7495,13 @@
         <v>15</v>
       </c>
       <c r="Z69" s="8">
-        <f>AG69*AH69*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>37.647179999999999</v>
       </c>
       <c r="AB69" s="39">
         <v>15</v>
       </c>
-      <c r="AC69" s="57">
+      <c r="AC69" s="40">
         <v>180</v>
       </c>
       <c r="AE69" s="32">
@@ -7514,7 +7514,7 @@
         <v>12303</v>
       </c>
       <c r="AH69" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ69" s="32">
@@ -7592,13 +7592,13 @@
         <v>16</v>
       </c>
       <c r="Z70" s="8">
-        <f>AG70*AH70*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>25.404119999999999</v>
       </c>
       <c r="AB70" s="39">
         <v>16</v>
       </c>
-      <c r="AC70" s="57">
+      <c r="AC70" s="40">
         <v>180</v>
       </c>
       <c r="AE70" s="32">
@@ -7611,7 +7611,7 @@
         <v>8302</v>
       </c>
       <c r="AH70" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ70" s="32">
@@ -7689,13 +7689,13 @@
         <v>17</v>
       </c>
       <c r="Z71" s="8">
-        <f>AG71*AH71*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>23.453280000000003</v>
       </c>
       <c r="AB71" s="39">
         <v>17</v>
       </c>
-      <c r="AC71" s="57">
+      <c r="AC71" s="40">
         <v>300</v>
       </c>
       <c r="AE71" s="32">
@@ -7708,7 +7708,7 @@
         <v>10858</v>
       </c>
       <c r="AH71" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.16</v>
       </c>
       <c r="AJ71" s="32">
@@ -7786,13 +7786,13 @@
         <v>18</v>
       </c>
       <c r="Z72" s="8">
-        <f>AG72*AH72*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>23.647680000000001</v>
       </c>
       <c r="AB72" s="39">
         <v>18</v>
       </c>
-      <c r="AC72" s="57">
+      <c r="AC72" s="40">
         <v>2700</v>
       </c>
       <c r="AE72" s="32">
@@ -7805,7 +7805,7 @@
         <v>10948</v>
       </c>
       <c r="AH72" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>2.16</v>
       </c>
       <c r="AJ72" s="32">
@@ -7883,13 +7883,13 @@
         <v>19</v>
       </c>
       <c r="Z73" s="8">
-        <f>AG73*AH73*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>223.99503999999999</v>
       </c>
       <c r="AB73" s="39">
         <v>19</v>
       </c>
-      <c r="AC73" s="57">
+      <c r="AC73" s="40">
         <v>120</v>
       </c>
       <c r="AE73" s="32">
@@ -7902,7 +7902,7 @@
         <v>17834</v>
       </c>
       <c r="AH73" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>12.56</v>
       </c>
       <c r="AJ73" s="32">
@@ -7980,13 +7980,13 @@
         <v>20</v>
       </c>
       <c r="Z74" s="8">
-        <f>AG74*AH74*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>36.931139999999999</v>
       </c>
       <c r="AB74" s="39">
         <v>20</v>
       </c>
-      <c r="AC74" s="57">
+      <c r="AC74" s="40">
         <v>1920</v>
       </c>
       <c r="AE74" s="32">
@@ -7999,7 +7999,7 @@
         <v>12069</v>
       </c>
       <c r="AH74" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>3.06</v>
       </c>
       <c r="AJ74" s="32">
@@ -8041,14 +8041,14 @@
         <v>21</v>
       </c>
       <c r="H75" s="6">
-        <f t="shared" ref="H75:H94" si="33">$L$4*$G106*H$53</f>
+        <f t="shared" ref="H75:H94" si="34">$L$4*$G106*H$53</f>
         <v>14.05</v>
       </c>
       <c r="J75" s="35">
         <v>21</v>
       </c>
       <c r="K75" s="6">
-        <f t="shared" ref="K75:K94" si="34">$L$4*$G106*K$53</f>
+        <f t="shared" ref="K75:K94" si="35">$L$4*$G106*K$53</f>
         <v>19.669999999999998</v>
       </c>
       <c r="M75" s="35">
@@ -8062,7 +8062,7 @@
         <v>21</v>
       </c>
       <c r="Q75" s="6">
-        <f t="shared" ref="Q75:Q94" si="35">$L$4*$G106*Q$53</f>
+        <f t="shared" ref="Q75:Q94" si="36">$L$4*$G106*Q$53</f>
         <v>19.669999999999998</v>
       </c>
       <c r="S75" s="32">
@@ -8081,13 +8081,13 @@
         <v>21</v>
       </c>
       <c r="Z75" s="8">
-        <f>AG75*AH75*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB75" s="39">
         <v>21</v>
       </c>
-      <c r="AC75" s="57">
+      <c r="AC75" s="40">
         <f>Q75</f>
         <v>19.669999999999998</v>
       </c>
@@ -8142,28 +8142,28 @@
         <v>22</v>
       </c>
       <c r="H76" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>12.5</v>
       </c>
       <c r="J76" s="35">
         <v>22</v>
       </c>
       <c r="K76" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>17.5</v>
       </c>
       <c r="M76" s="35">
         <v>22</v>
       </c>
       <c r="N76" s="6">
-        <f t="shared" ref="N76:N94" si="36">$L$4*$G107</f>
+        <f t="shared" ref="N76:N94" si="37">$L$4*$G107</f>
         <v>25</v>
       </c>
       <c r="P76" s="35">
         <v>22</v>
       </c>
       <c r="Q76" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>17.5</v>
       </c>
       <c r="S76" s="32">
@@ -8182,14 +8182,14 @@
         <v>22</v>
       </c>
       <c r="Z76" s="8">
-        <f>AG76*AH76*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB76" s="39">
         <v>22</v>
       </c>
-      <c r="AC76" s="57">
-        <f t="shared" ref="AC76:AC94" si="37">Q76</f>
+      <c r="AC76" s="40">
+        <f t="shared" ref="AC76:AC94" si="38">Q76</f>
         <v>17.5</v>
       </c>
       <c r="AE76" s="32">
@@ -8243,28 +8243,28 @@
         <v>23</v>
       </c>
       <c r="H77" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>35</v>
       </c>
       <c r="J77" s="35">
         <v>23</v>
       </c>
       <c r="K77" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>49</v>
       </c>
       <c r="M77" s="35">
         <v>23</v>
       </c>
       <c r="N77" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>70</v>
       </c>
       <c r="P77" s="35">
         <v>23</v>
       </c>
       <c r="Q77" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>49</v>
       </c>
       <c r="S77" s="32">
@@ -8283,14 +8283,14 @@
         <v>23</v>
       </c>
       <c r="Z77" s="8">
-        <f>AG77*AH77*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB77" s="39">
         <v>23</v>
       </c>
-      <c r="AC77" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC77" s="40">
+        <f t="shared" si="38"/>
         <v>49</v>
       </c>
       <c r="AE77" s="32">
@@ -8344,28 +8344,28 @@
         <v>24</v>
       </c>
       <c r="H78" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>15.3</v>
       </c>
       <c r="J78" s="35">
         <v>24</v>
       </c>
       <c r="K78" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>21.419999999999998</v>
       </c>
       <c r="M78" s="35">
         <v>24</v>
       </c>
       <c r="N78" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>30.6</v>
       </c>
       <c r="P78" s="35">
         <v>24</v>
       </c>
       <c r="Q78" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>21.419999999999998</v>
       </c>
       <c r="S78" s="32">
@@ -8384,14 +8384,14 @@
         <v>24</v>
       </c>
       <c r="Z78" s="8">
-        <f>AG78*AH78*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB78" s="39">
         <v>24</v>
       </c>
-      <c r="AC78" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC78" s="40">
+        <f t="shared" si="38"/>
         <v>21.419999999999998</v>
       </c>
       <c r="AE78" s="32">
@@ -8445,28 +8445,28 @@
         <v>25</v>
       </c>
       <c r="H79" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J79" s="35">
         <v>25</v>
       </c>
       <c r="K79" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M79" s="35">
         <v>25</v>
       </c>
       <c r="N79" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P79" s="35">
         <v>25</v>
       </c>
       <c r="Q79" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S79" s="32">
@@ -8485,14 +8485,14 @@
         <v>25</v>
       </c>
       <c r="Z79" s="8">
-        <f>AG79*AH79*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB79" s="39">
         <v>25</v>
       </c>
-      <c r="AC79" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC79" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE79" s="32">
@@ -8546,28 +8546,28 @@
         <v>26</v>
       </c>
       <c r="H80" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J80" s="35">
         <v>26</v>
       </c>
       <c r="K80" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M80" s="35">
         <v>26</v>
       </c>
       <c r="N80" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P80" s="35">
         <v>26</v>
       </c>
       <c r="Q80" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S80" s="32">
@@ -8586,14 +8586,14 @@
         <v>26</v>
       </c>
       <c r="Z80" s="8">
-        <f>AG80*AH80*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB80" s="39">
         <v>26</v>
       </c>
-      <c r="AC80" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC80" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE80" s="32">
@@ -8647,28 +8647,28 @@
         <v>27</v>
       </c>
       <c r="H81" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J81" s="35">
         <v>27</v>
       </c>
       <c r="K81" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M81" s="35">
         <v>27</v>
       </c>
       <c r="N81" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P81" s="35">
         <v>27</v>
       </c>
       <c r="Q81" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S81" s="32">
@@ -8687,14 +8687,14 @@
         <v>27</v>
       </c>
       <c r="Z81" s="8">
-        <f>AG81*AH81*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB81" s="39">
         <v>27</v>
       </c>
-      <c r="AC81" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC81" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE81" s="32">
@@ -8748,28 +8748,28 @@
         <v>28</v>
       </c>
       <c r="H82" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>26.1</v>
       </c>
       <c r="J82" s="35">
         <v>28</v>
       </c>
       <c r="K82" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>36.54</v>
       </c>
       <c r="M82" s="35">
         <v>28</v>
       </c>
       <c r="N82" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>52.2</v>
       </c>
       <c r="P82" s="35">
         <v>28</v>
       </c>
       <c r="Q82" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>36.54</v>
       </c>
       <c r="S82" s="32">
@@ -8788,14 +8788,14 @@
         <v>28</v>
       </c>
       <c r="Z82" s="8">
-        <f>AG82*AH82*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB82" s="39">
         <v>28</v>
       </c>
-      <c r="AC82" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC82" s="40">
+        <f t="shared" si="38"/>
         <v>36.54</v>
       </c>
       <c r="AE82" s="32">
@@ -8849,28 +8849,28 @@
         <v>29</v>
       </c>
       <c r="H83" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J83" s="35">
         <v>29</v>
       </c>
       <c r="K83" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M83" s="35">
         <v>29</v>
       </c>
       <c r="N83" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P83" s="35">
         <v>29</v>
       </c>
       <c r="Q83" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S83" s="32">
@@ -8889,14 +8889,14 @@
         <v>29</v>
       </c>
       <c r="Z83" s="8">
-        <f>AG83*AH83*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB83" s="39">
         <v>29</v>
       </c>
-      <c r="AC83" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC83" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE83" s="32">
@@ -8950,28 +8950,28 @@
         <v>30</v>
       </c>
       <c r="H84" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>10.1</v>
       </c>
       <c r="J84" s="35">
         <v>30</v>
       </c>
       <c r="K84" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>14.139999999999999</v>
       </c>
       <c r="M84" s="35">
         <v>30</v>
       </c>
       <c r="N84" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>20.2</v>
       </c>
       <c r="P84" s="35">
         <v>30</v>
       </c>
       <c r="Q84" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>14.139999999999999</v>
       </c>
       <c r="S84" s="32">
@@ -8990,14 +8990,14 @@
         <v>30</v>
       </c>
       <c r="Z84" s="8">
-        <f>AG84*AH84*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB84" s="39">
         <v>30</v>
       </c>
-      <c r="AC84" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC84" s="40">
+        <f t="shared" si="38"/>
         <v>14.139999999999999</v>
       </c>
       <c r="AE84" s="32">
@@ -9051,28 +9051,28 @@
         <v>31</v>
       </c>
       <c r="H85" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>35</v>
       </c>
       <c r="J85" s="35">
         <v>31</v>
       </c>
       <c r="K85" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>49</v>
       </c>
       <c r="M85" s="35">
         <v>31</v>
       </c>
       <c r="N85" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>70</v>
       </c>
       <c r="P85" s="35">
         <v>31</v>
       </c>
       <c r="Q85" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>49</v>
       </c>
       <c r="S85" s="32">
@@ -9091,14 +9091,14 @@
         <v>31</v>
       </c>
       <c r="Z85" s="8">
-        <f>AG85*AH85*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB85" s="39">
         <v>31</v>
       </c>
-      <c r="AC85" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC85" s="40">
+        <f t="shared" si="38"/>
         <v>49</v>
       </c>
       <c r="AE85" s="32">
@@ -9152,28 +9152,28 @@
         <v>32</v>
       </c>
       <c r="H86" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.25</v>
       </c>
       <c r="J86" s="35">
         <v>32</v>
       </c>
       <c r="K86" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.35</v>
       </c>
       <c r="M86" s="35">
         <v>32</v>
       </c>
       <c r="N86" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10.5</v>
       </c>
       <c r="P86" s="35">
         <v>32</v>
       </c>
       <c r="Q86" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7.35</v>
       </c>
       <c r="S86" s="32">
@@ -9192,14 +9192,14 @@
         <v>32</v>
       </c>
       <c r="Z86" s="8">
-        <f>AG86*AH86*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB86" s="39">
         <v>32</v>
       </c>
-      <c r="AC86" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC86" s="40">
+        <f t="shared" si="38"/>
         <v>7.35</v>
       </c>
       <c r="AE86" s="32">
@@ -9253,28 +9253,28 @@
         <v>33</v>
       </c>
       <c r="H87" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J87" s="35">
         <v>33</v>
       </c>
       <c r="K87" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M87" s="35">
         <v>33</v>
       </c>
       <c r="N87" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P87" s="35">
         <v>33</v>
       </c>
       <c r="Q87" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S87" s="32">
@@ -9293,14 +9293,14 @@
         <v>33</v>
       </c>
       <c r="Z87" s="8">
-        <f>AG87*AH87*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB87" s="39">
         <v>33</v>
       </c>
-      <c r="AC87" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC87" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE87" s="32">
@@ -9354,28 +9354,28 @@
         <v>34</v>
       </c>
       <c r="H88" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J88" s="35">
         <v>34</v>
       </c>
       <c r="K88" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M88" s="35">
         <v>34</v>
       </c>
       <c r="N88" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P88" s="35">
         <v>34</v>
       </c>
       <c r="Q88" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S88" s="32">
@@ -9394,14 +9394,14 @@
         <v>34</v>
       </c>
       <c r="Z88" s="8">
-        <f>AG88*AH88*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB88" s="39">
         <v>34</v>
       </c>
-      <c r="AC88" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC88" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE88" s="32">
@@ -9455,28 +9455,28 @@
         <v>35</v>
       </c>
       <c r="H89" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J89" s="35">
         <v>35</v>
       </c>
       <c r="K89" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M89" s="35">
         <v>35</v>
       </c>
       <c r="N89" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P89" s="35">
         <v>35</v>
       </c>
       <c r="Q89" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S89" s="32">
@@ -9495,14 +9495,14 @@
         <v>35</v>
       </c>
       <c r="Z89" s="8">
-        <f>AG89*AH89*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB89" s="39">
         <v>35</v>
       </c>
-      <c r="AC89" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC89" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE89" s="32">
@@ -9556,28 +9556,28 @@
         <v>36</v>
       </c>
       <c r="H90" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J90" s="35">
         <v>36</v>
       </c>
       <c r="K90" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M90" s="35">
         <v>36</v>
       </c>
       <c r="N90" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P90" s="35">
         <v>36</v>
       </c>
       <c r="Q90" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S90" s="32">
@@ -9596,14 +9596,14 @@
         <v>36</v>
       </c>
       <c r="Z90" s="8">
-        <f>AG90*AH90*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB90" s="39">
         <v>36</v>
       </c>
-      <c r="AC90" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC90" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE90" s="32">
@@ -9657,28 +9657,28 @@
         <v>37</v>
       </c>
       <c r="H91" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.05</v>
       </c>
       <c r="J91" s="35">
         <v>37</v>
       </c>
       <c r="K91" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="M91" s="35">
         <v>37</v>
       </c>
       <c r="N91" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10.1</v>
       </c>
       <c r="P91" s="35">
         <v>37</v>
       </c>
       <c r="Q91" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="S91" s="32">
@@ -9697,14 +9697,14 @@
         <v>37</v>
       </c>
       <c r="Z91" s="8">
-        <f>AG91*AH91*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB91" s="39">
         <v>37</v>
       </c>
-      <c r="AC91" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC91" s="40">
+        <f t="shared" si="38"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="AE91" s="32">
@@ -9758,28 +9758,28 @@
         <v>38</v>
       </c>
       <c r="H92" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5.05</v>
       </c>
       <c r="J92" s="35">
         <v>38</v>
       </c>
       <c r="K92" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="M92" s="35">
         <v>38</v>
       </c>
       <c r="N92" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10.1</v>
       </c>
       <c r="P92" s="35">
         <v>38</v>
       </c>
       <c r="Q92" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="S92" s="32">
@@ -9798,14 +9798,14 @@
         <v>38</v>
       </c>
       <c r="Z92" s="8">
-        <f>AG92*AH92*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB92" s="39">
         <v>38</v>
       </c>
-      <c r="AC92" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC92" s="40">
+        <f t="shared" si="38"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="AE92" s="32">
@@ -9859,28 +9859,28 @@
         <v>39</v>
       </c>
       <c r="H93" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="J93" s="35">
         <v>39</v>
       </c>
       <c r="K93" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>7</v>
       </c>
       <c r="M93" s="35">
         <v>39</v>
       </c>
       <c r="N93" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>10</v>
       </c>
       <c r="P93" s="35">
         <v>39</v>
       </c>
       <c r="Q93" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>7</v>
       </c>
       <c r="S93" s="32">
@@ -9899,14 +9899,14 @@
         <v>39</v>
       </c>
       <c r="Z93" s="8">
-        <f>AG93*AH93*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB93" s="39">
         <v>39</v>
       </c>
-      <c r="AC93" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC93" s="40">
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="AE93" s="32">
@@ -9960,28 +9960,28 @@
         <v>40</v>
       </c>
       <c r="H94" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="J94" s="35">
         <v>40</v>
       </c>
       <c r="K94" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="M94" s="35">
         <v>40</v>
       </c>
       <c r="N94" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>12</v>
       </c>
       <c r="P94" s="35">
         <v>40</v>
       </c>
       <c r="Q94" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="S94" s="32">
@@ -10000,14 +10000,14 @@
         <v>40</v>
       </c>
       <c r="Z94" s="8">
-        <f>AG94*AH94*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB94" s="39">
         <v>40</v>
       </c>
-      <c r="AC94" s="57">
-        <f t="shared" si="37"/>
+      <c r="AC94" s="40">
+        <f t="shared" si="38"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="AE94" s="32">
@@ -10097,13 +10097,13 @@
         <v>41</v>
       </c>
       <c r="Z95" s="8">
-        <f>AG95*AH95*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB95" s="39">
         <v>41</v>
       </c>
-      <c r="AC95" s="57">
+      <c r="AC95" s="40">
         <v>10000</v>
       </c>
       <c r="AE95" s="32">
@@ -10193,13 +10193,13 @@
         <v>42</v>
       </c>
       <c r="Z96" s="8">
-        <f>AG96*AH96*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB96" s="39">
         <v>42</v>
       </c>
-      <c r="AC96" s="57">
+      <c r="AC96" s="40">
         <v>10000</v>
       </c>
       <c r="AE96" s="32">
@@ -10277,25 +10277,25 @@
         <v>43</v>
       </c>
       <c r="T97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V97" s="29">
         <v>43</v>
       </c>
       <c r="W97" s="6">
-        <v>0</v>
+        <v>-10000</v>
       </c>
       <c r="Y97" s="32">
         <v>43</v>
       </c>
       <c r="Z97" s="8">
-        <f>AG97*AH97*1000/1000000</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AB97" s="39">
         <v>43</v>
       </c>
-      <c r="AC97" s="57">
+      <c r="AC97" s="40">
         <v>10000</v>
       </c>
       <c r="AE97" s="32">
@@ -10327,27 +10327,27 @@
       </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D103" s="42" t="s">
+      <c r="D103" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="E103" s="44" t="s">
+      <c r="E103" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="F103" s="44"/>
-      <c r="G103" s="44" t="s">
+      <c r="F103" s="48"/>
+      <c r="G103" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="H103" s="53"/>
+      <c r="H103" s="49"/>
       <c r="N103" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D104" s="43"/>
-      <c r="E104" s="45"/>
-      <c r="F104" s="45"/>
-      <c r="G104" s="45"/>
-      <c r="H104" s="54"/>
+      <c r="D104" s="57"/>
+      <c r="E104" s="50"/>
+      <c r="F104" s="50"/>
+      <c r="G104" s="50"/>
+      <c r="H104" s="51"/>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
@@ -10361,14 +10361,14 @@
       <c r="D106" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E106" s="46">
+      <c r="E106" s="54">
         <v>72154</v>
       </c>
-      <c r="F106" s="46"/>
-      <c r="G106" s="55">
+      <c r="F106" s="54"/>
+      <c r="G106" s="52">
         <v>28.1</v>
       </c>
-      <c r="H106" s="56"/>
+      <c r="H106" s="53"/>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C107" s="18">
@@ -10377,14 +10377,14 @@
       <c r="D107" s="19">
         <v>0.31</v>
       </c>
-      <c r="E107" s="47">
+      <c r="E107" s="46">
         <v>67811</v>
       </c>
-      <c r="F107" s="47"/>
-      <c r="G107" s="48">
+      <c r="F107" s="46"/>
+      <c r="G107" s="42">
         <v>25</v>
       </c>
-      <c r="H107" s="49"/>
+      <c r="H107" s="43"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C108" s="18">
@@ -10393,14 +10393,14 @@
       <c r="D108" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E108" s="47">
+      <c r="E108" s="46">
         <v>187455</v>
       </c>
-      <c r="F108" s="47"/>
-      <c r="G108" s="48">
+      <c r="F108" s="46"/>
+      <c r="G108" s="42">
         <v>70</v>
       </c>
-      <c r="H108" s="49"/>
+      <c r="H108" s="43"/>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C109" s="18">
@@ -10409,14 +10409,14 @@
       <c r="D109" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E109" s="47">
+      <c r="E109" s="46">
         <v>63266</v>
       </c>
-      <c r="F109" s="47"/>
-      <c r="G109" s="48">
+      <c r="F109" s="46"/>
+      <c r="G109" s="42">
         <v>30.6</v>
       </c>
-      <c r="H109" s="49"/>
+      <c r="H109" s="43"/>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -10425,14 +10425,14 @@
       <c r="D110" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E110" s="47">
+      <c r="E110" s="46">
         <v>26553</v>
       </c>
-      <c r="F110" s="47"/>
-      <c r="G110" s="48">
+      <c r="F110" s="46"/>
+      <c r="G110" s="42">
         <v>10</v>
       </c>
-      <c r="H110" s="49"/>
+      <c r="H110" s="43"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -10441,14 +10441,14 @@
       <c r="D111" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E111" s="47">
+      <c r="E111" s="46">
         <v>24949</v>
       </c>
-      <c r="F111" s="47"/>
-      <c r="G111" s="48">
+      <c r="F111" s="46"/>
+      <c r="G111" s="42">
         <v>10</v>
       </c>
-      <c r="H111" s="49"/>
+      <c r="H111" s="43"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -10457,14 +10457,14 @@
       <c r="D112" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E112" s="47">
+      <c r="E112" s="46">
         <v>22870</v>
       </c>
-      <c r="F112" s="47"/>
-      <c r="G112" s="48">
+      <c r="F112" s="46"/>
+      <c r="G112" s="42">
         <v>10</v>
       </c>
-      <c r="H112" s="49"/>
+      <c r="H112" s="43"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -10473,14 +10473,14 @@
       <c r="D113" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E113" s="47">
+      <c r="E113" s="46">
         <v>139836</v>
       </c>
-      <c r="F113" s="47"/>
-      <c r="G113" s="48">
+      <c r="F113" s="46"/>
+      <c r="G113" s="42">
         <v>52.2</v>
       </c>
-      <c r="H113" s="49"/>
+      <c r="H113" s="43"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -10489,14 +10489,14 @@
       <c r="D114" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E114" s="47">
+      <c r="E114" s="46">
         <v>23515</v>
       </c>
-      <c r="F114" s="47"/>
-      <c r="G114" s="48">
+      <c r="F114" s="46"/>
+      <c r="G114" s="42">
         <v>10</v>
       </c>
-      <c r="H114" s="49"/>
+      <c r="H114" s="43"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -10505,14 +10505,14 @@
       <c r="D115" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E115" s="47">
+      <c r="E115" s="46">
         <v>49503</v>
       </c>
-      <c r="F115" s="47"/>
-      <c r="G115" s="48">
+      <c r="F115" s="46"/>
+      <c r="G115" s="42">
         <v>20.2</v>
       </c>
-      <c r="H115" s="49"/>
+      <c r="H115" s="43"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -10521,14 +10521,14 @@
       <c r="D116" s="19">
         <v>0.307</v>
       </c>
-      <c r="E116" s="47">
+      <c r="E116" s="46">
         <v>188420</v>
       </c>
-      <c r="F116" s="47"/>
-      <c r="G116" s="48">
+      <c r="F116" s="46"/>
+      <c r="G116" s="42">
         <v>70</v>
       </c>
-      <c r="H116" s="49"/>
+      <c r="H116" s="43"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -10537,14 +10537,14 @@
       <c r="D117" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E117" s="47">
+      <c r="E117" s="46">
         <v>26573</v>
       </c>
-      <c r="F117" s="47"/>
-      <c r="G117" s="48">
+      <c r="F117" s="46"/>
+      <c r="G117" s="42">
         <v>10.5</v>
       </c>
-      <c r="H117" s="49"/>
+      <c r="H117" s="43"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -10553,14 +10553,14 @@
       <c r="D118" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E118" s="47">
+      <c r="E118" s="46">
         <v>25253</v>
       </c>
-      <c r="F118" s="47"/>
-      <c r="G118" s="48">
+      <c r="F118" s="46"/>
+      <c r="G118" s="42">
         <v>10</v>
       </c>
-      <c r="H118" s="49"/>
+      <c r="H118" s="43"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -10569,14 +10569,14 @@
       <c r="D119" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E119" s="47">
+      <c r="E119" s="46">
         <v>17610</v>
       </c>
-      <c r="F119" s="47"/>
-      <c r="G119" s="48">
+      <c r="F119" s="46"/>
+      <c r="G119" s="42">
         <v>10</v>
       </c>
-      <c r="H119" s="49"/>
+      <c r="H119" s="43"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -10585,14 +10585,14 @@
       <c r="D120" s="19">
         <v>0.221</v>
       </c>
-      <c r="E120" s="47">
+      <c r="E120" s="46">
         <v>19372</v>
       </c>
-      <c r="F120" s="47"/>
-      <c r="G120" s="48">
+      <c r="F120" s="46"/>
+      <c r="G120" s="42">
         <v>10</v>
       </c>
-      <c r="H120" s="49"/>
+      <c r="H120" s="43"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -10601,14 +10601,14 @@
       <c r="D121" s="19">
         <v>0.216</v>
       </c>
-      <c r="E121" s="47">
+      <c r="E121" s="46">
         <v>18939</v>
       </c>
-      <c r="F121" s="47"/>
-      <c r="G121" s="48">
+      <c r="F121" s="46"/>
+      <c r="G121" s="42">
         <v>10</v>
       </c>
-      <c r="H121" s="49"/>
+      <c r="H121" s="43"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -10617,14 +10617,14 @@
       <c r="D122" s="19">
         <v>0.23</v>
       </c>
-      <c r="E122" s="47">
+      <c r="E122" s="46">
         <v>20382</v>
       </c>
-      <c r="F122" s="47"/>
-      <c r="G122" s="48">
+      <c r="F122" s="46"/>
+      <c r="G122" s="42">
         <v>10.1</v>
       </c>
-      <c r="H122" s="49"/>
+      <c r="H122" s="43"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -10633,14 +10633,14 @@
       <c r="D123" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E123" s="47">
+      <c r="E123" s="46">
         <v>19968</v>
       </c>
-      <c r="F123" s="47"/>
-      <c r="G123" s="48">
+      <c r="F123" s="46"/>
+      <c r="G123" s="42">
         <v>10.1</v>
       </c>
-      <c r="H123" s="49"/>
+      <c r="H123" s="43"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -10649,14 +10649,14 @@
       <c r="D124" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E124" s="47">
+      <c r="E124" s="46">
         <v>23240</v>
       </c>
-      <c r="F124" s="47"/>
-      <c r="G124" s="48">
+      <c r="F124" s="46"/>
+      <c r="G124" s="42">
         <v>10</v>
       </c>
-      <c r="H124" s="49"/>
+      <c r="H124" s="43"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="20">
@@ -10665,29 +10665,60 @@
       <c r="D125" s="21">
         <v>0.254</v>
       </c>
-      <c r="E125" s="52">
+      <c r="E125" s="47">
         <v>26709</v>
       </c>
-      <c r="F125" s="52"/>
-      <c r="G125" s="50">
+      <c r="F125" s="47"/>
+      <c r="G125" s="44">
         <v>12</v>
       </c>
-      <c r="H125" s="51"/>
+      <c r="H125" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:F104"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="G124:H124"/>
@@ -10704,49 +10735,18 @@
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G108:H108"/>
     <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:F104"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solar and Wind Build Times
-Adds build times for solar and wind to constraints that dictate available new capacity
-Adds input for solar and wind build times on data_in
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -52,6 +52,7 @@
     <definedName name="SO2_rate">Sheet2!$AL$55:$AL$97</definedName>
     <definedName name="solar_cap_factor">Sheet2!$L$4</definedName>
     <definedName name="solar_inc">Sheet2!$Q$8</definedName>
+    <definedName name="SolarBuildTime">Sheet2!$Q$10</definedName>
     <definedName name="SpringDemandOff">Sheet2!$U$16:$W$41</definedName>
     <definedName name="SpringDemandPeak">Sheet2!$O$16:$Q$41</definedName>
     <definedName name="SpringMaxGenPeak">Sheet2!$K$55:$K$97</definedName>
@@ -67,6 +68,7 @@
     <definedName name="UnitsByBus">Sheet2!$C$55:$E$97</definedName>
     <definedName name="wind_cap_factor">Sheet2!$L$5</definedName>
     <definedName name="wind_inc">Sheet2!$Q$9</definedName>
+    <definedName name="WindBuildTime">Sheet2!$Q$11</definedName>
     <definedName name="WinterDemandOff">Sheet2!$I$16:$K$41</definedName>
     <definedName name="WinterDemandPeak">Sheet2!$C$16:$E$41</definedName>
     <definedName name="WinterMaxGenPeak">Sheet2!$H$55:$H$97</definedName>
@@ -84,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="147">
   <si>
     <t>NumBuses</t>
   </si>
@@ -519,6 +521,12 @@
   </si>
   <si>
     <t>RampRate (MW/hr)</t>
+  </si>
+  <si>
+    <t>Solar Build Time (years):</t>
+  </si>
+  <si>
+    <t>Wind Build Time (years):</t>
   </si>
 </sst>
 </file>
@@ -1110,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,6 +1468,14 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
+      <c r="N10" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="26">
+        <v>1</v>
+      </c>
       <c r="S10" s="33"/>
       <c r="T10" s="33"/>
       <c r="U10" s="33"/>
@@ -1471,6 +1487,14 @@
       </c>
       <c r="G11" s="6">
         <v>3780</v>
+      </c>
+      <c r="N11" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="26">
+        <v>3</v>
       </c>
       <c r="S11" s="33"/>
       <c r="T11" s="33"/>
@@ -10675,9 +10699,7 @@
       <c r="H125" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S8:U8"/>
+  <mergeCells count="73">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="N8:P8"/>
@@ -10740,6 +10762,8 @@
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N10:P10"/>
+    <mergeCell ref="N11:P11"/>
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="S3:U3"/>
@@ -10747,6 +10771,8 @@
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="S5:U5"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="S8:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
minor changes, no change in output
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -776,7 +776,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,19 +814,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -815,20 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1112,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W98" sqref="W98"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V91" sqref="V91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1144,34 +1144,34 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="41"/>
+      <c r="F1" s="43"/>
       <c r="G1" s="14">
         <v>0.1</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
       <c r="Q1" s="24">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1183,31 +1183,31 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1225,27 +1225,27 @@
       <c r="F3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
       <c r="Q3" s="24">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="41" t="s">
+      <c r="S3" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1267,27 +1267,27 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
       <c r="L4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="N4" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
       <c r="Q4" s="24">
         <v>43560</v>
       </c>
-      <c r="S4" s="41" t="s">
+      <c r="S4" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1304,27 +1304,27 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="N5" s="41" t="s">
+      <c r="N5" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
       <c r="Q5" s="24">
         <v>601000</v>
       </c>
-      <c r="S5" s="41" t="s">
+      <c r="S5" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
+      <c r="T5" s="43"/>
+      <c r="U5" s="43"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1347,23 +1347,23 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="58"/>
-      <c r="N6" s="41" t="s">
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="41"/>
+      <c r="N6" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
       <c r="Q6" s="24">
         <v>15025</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S6" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
+      <c r="T6" s="43"/>
+      <c r="U6" s="43"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1386,19 +1386,19 @@
       <c r="G7" s="6">
         <v>4050</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
       <c r="Q7" s="26">
         <v>0.95</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1414,19 +1414,19 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
       <c r="Q8" s="26">
         <v>50</v>
       </c>
-      <c r="S8" s="41" t="s">
+      <c r="S8" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1442,11 +1442,11 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
       <c r="Q9" s="26">
         <v>10</v>
       </c>
@@ -5743,17 +5743,17 @@
       </c>
     </row>
     <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="C45" s="55" t="s">
+      <c r="C45" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="2"/>
-      <c r="H45" s="55" t="s">
+      <c r="H45" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="O45" s="4"/>
@@ -5990,11 +5990,11 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="C53" s="55" t="s">
+      <c r="C53" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
       <c r="G53" s="38" t="s">
         <v>137</v>
       </c>
@@ -10279,7 +10279,7 @@
         <v>43</v>
       </c>
       <c r="T97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V97" s="29">
         <v>43</v>
@@ -10329,27 +10329,27 @@
       </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D103" s="56" t="s">
+      <c r="D103" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E103" s="48" t="s">
+      <c r="E103" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="F103" s="48"/>
-      <c r="G103" s="48" t="s">
+      <c r="F103" s="47"/>
+      <c r="G103" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="H103" s="49"/>
+      <c r="H103" s="56"/>
       <c r="N103" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D104" s="57"/>
-      <c r="E104" s="50"/>
-      <c r="F104" s="50"/>
-      <c r="G104" s="50"/>
-      <c r="H104" s="51"/>
+      <c r="D104" s="46"/>
+      <c r="E104" s="48"/>
+      <c r="F104" s="48"/>
+      <c r="G104" s="48"/>
+      <c r="H104" s="57"/>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
@@ -10363,14 +10363,14 @@
       <c r="D106" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E106" s="54">
+      <c r="E106" s="49">
         <v>72154</v>
       </c>
-      <c r="F106" s="54"/>
-      <c r="G106" s="52">
+      <c r="F106" s="49"/>
+      <c r="G106" s="58">
         <v>28.1</v>
       </c>
-      <c r="H106" s="53"/>
+      <c r="H106" s="59"/>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C107" s="18">
@@ -10379,14 +10379,14 @@
       <c r="D107" s="19">
         <v>0.31</v>
       </c>
-      <c r="E107" s="46">
+      <c r="E107" s="50">
         <v>67811</v>
       </c>
-      <c r="F107" s="46"/>
-      <c r="G107" s="42">
+      <c r="F107" s="50"/>
+      <c r="G107" s="51">
         <v>25</v>
       </c>
-      <c r="H107" s="43"/>
+      <c r="H107" s="52"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C108" s="18">
@@ -10395,14 +10395,14 @@
       <c r="D108" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E108" s="46">
+      <c r="E108" s="50">
         <v>187455</v>
       </c>
-      <c r="F108" s="46"/>
-      <c r="G108" s="42">
+      <c r="F108" s="50"/>
+      <c r="G108" s="51">
         <v>70</v>
       </c>
-      <c r="H108" s="43"/>
+      <c r="H108" s="52"/>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C109" s="18">
@@ -10411,14 +10411,14 @@
       <c r="D109" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E109" s="46">
+      <c r="E109" s="50">
         <v>63266</v>
       </c>
-      <c r="F109" s="46"/>
-      <c r="G109" s="42">
+      <c r="F109" s="50"/>
+      <c r="G109" s="51">
         <v>30.6</v>
       </c>
-      <c r="H109" s="43"/>
+      <c r="H109" s="52"/>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -10427,14 +10427,14 @@
       <c r="D110" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E110" s="46">
+      <c r="E110" s="50">
         <v>26553</v>
       </c>
-      <c r="F110" s="46"/>
-      <c r="G110" s="42">
+      <c r="F110" s="50"/>
+      <c r="G110" s="51">
         <v>10</v>
       </c>
-      <c r="H110" s="43"/>
+      <c r="H110" s="52"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -10443,14 +10443,14 @@
       <c r="D111" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E111" s="46">
+      <c r="E111" s="50">
         <v>24949</v>
       </c>
-      <c r="F111" s="46"/>
-      <c r="G111" s="42">
+      <c r="F111" s="50"/>
+      <c r="G111" s="51">
         <v>10</v>
       </c>
-      <c r="H111" s="43"/>
+      <c r="H111" s="52"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -10459,14 +10459,14 @@
       <c r="D112" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E112" s="46">
+      <c r="E112" s="50">
         <v>22870</v>
       </c>
-      <c r="F112" s="46"/>
-      <c r="G112" s="42">
+      <c r="F112" s="50"/>
+      <c r="G112" s="51">
         <v>10</v>
       </c>
-      <c r="H112" s="43"/>
+      <c r="H112" s="52"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -10475,14 +10475,14 @@
       <c r="D113" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E113" s="46">
+      <c r="E113" s="50">
         <v>139836</v>
       </c>
-      <c r="F113" s="46"/>
-      <c r="G113" s="42">
+      <c r="F113" s="50"/>
+      <c r="G113" s="51">
         <v>52.2</v>
       </c>
-      <c r="H113" s="43"/>
+      <c r="H113" s="52"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -10491,14 +10491,14 @@
       <c r="D114" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E114" s="46">
+      <c r="E114" s="50">
         <v>23515</v>
       </c>
-      <c r="F114" s="46"/>
-      <c r="G114" s="42">
+      <c r="F114" s="50"/>
+      <c r="G114" s="51">
         <v>10</v>
       </c>
-      <c r="H114" s="43"/>
+      <c r="H114" s="52"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -10507,14 +10507,14 @@
       <c r="D115" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E115" s="46">
+      <c r="E115" s="50">
         <v>49503</v>
       </c>
-      <c r="F115" s="46"/>
-      <c r="G115" s="42">
+      <c r="F115" s="50"/>
+      <c r="G115" s="51">
         <v>20.2</v>
       </c>
-      <c r="H115" s="43"/>
+      <c r="H115" s="52"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -10523,14 +10523,14 @@
       <c r="D116" s="19">
         <v>0.307</v>
       </c>
-      <c r="E116" s="46">
+      <c r="E116" s="50">
         <v>188420</v>
       </c>
-      <c r="F116" s="46"/>
-      <c r="G116" s="42">
+      <c r="F116" s="50"/>
+      <c r="G116" s="51">
         <v>70</v>
       </c>
-      <c r="H116" s="43"/>
+      <c r="H116" s="52"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -10539,14 +10539,14 @@
       <c r="D117" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E117" s="46">
+      <c r="E117" s="50">
         <v>26573</v>
       </c>
-      <c r="F117" s="46"/>
-      <c r="G117" s="42">
+      <c r="F117" s="50"/>
+      <c r="G117" s="51">
         <v>10.5</v>
       </c>
-      <c r="H117" s="43"/>
+      <c r="H117" s="52"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -10555,14 +10555,14 @@
       <c r="D118" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E118" s="46">
+      <c r="E118" s="50">
         <v>25253</v>
       </c>
-      <c r="F118" s="46"/>
-      <c r="G118" s="42">
+      <c r="F118" s="50"/>
+      <c r="G118" s="51">
         <v>10</v>
       </c>
-      <c r="H118" s="43"/>
+      <c r="H118" s="52"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -10571,14 +10571,14 @@
       <c r="D119" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E119" s="46">
+      <c r="E119" s="50">
         <v>17610</v>
       </c>
-      <c r="F119" s="46"/>
-      <c r="G119" s="42">
+      <c r="F119" s="50"/>
+      <c r="G119" s="51">
         <v>10</v>
       </c>
-      <c r="H119" s="43"/>
+      <c r="H119" s="52"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -10587,14 +10587,14 @@
       <c r="D120" s="19">
         <v>0.221</v>
       </c>
-      <c r="E120" s="46">
+      <c r="E120" s="50">
         <v>19372</v>
       </c>
-      <c r="F120" s="46"/>
-      <c r="G120" s="42">
+      <c r="F120" s="50"/>
+      <c r="G120" s="51">
         <v>10</v>
       </c>
-      <c r="H120" s="43"/>
+      <c r="H120" s="52"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -10603,14 +10603,14 @@
       <c r="D121" s="19">
         <v>0.216</v>
       </c>
-      <c r="E121" s="46">
+      <c r="E121" s="50">
         <v>18939</v>
       </c>
-      <c r="F121" s="46"/>
-      <c r="G121" s="42">
+      <c r="F121" s="50"/>
+      <c r="G121" s="51">
         <v>10</v>
       </c>
-      <c r="H121" s="43"/>
+      <c r="H121" s="52"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -10619,14 +10619,14 @@
       <c r="D122" s="19">
         <v>0.23</v>
       </c>
-      <c r="E122" s="46">
+      <c r="E122" s="50">
         <v>20382</v>
       </c>
-      <c r="F122" s="46"/>
-      <c r="G122" s="42">
+      <c r="F122" s="50"/>
+      <c r="G122" s="51">
         <v>10.1</v>
       </c>
-      <c r="H122" s="43"/>
+      <c r="H122" s="52"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -10635,14 +10635,14 @@
       <c r="D123" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E123" s="46">
+      <c r="E123" s="50">
         <v>19968</v>
       </c>
-      <c r="F123" s="46"/>
-      <c r="G123" s="42">
+      <c r="F123" s="50"/>
+      <c r="G123" s="51">
         <v>10.1</v>
       </c>
-      <c r="H123" s="43"/>
+      <c r="H123" s="52"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -10651,14 +10651,14 @@
       <c r="D124" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E124" s="46">
+      <c r="E124" s="50">
         <v>23240</v>
       </c>
-      <c r="F124" s="46"/>
-      <c r="G124" s="42">
+      <c r="F124" s="50"/>
+      <c r="G124" s="51">
         <v>10</v>
       </c>
-      <c r="H124" s="43"/>
+      <c r="H124" s="52"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="20">
@@ -10667,59 +10667,29 @@
       <c r="D125" s="21">
         <v>0.254</v>
       </c>
-      <c r="E125" s="47">
+      <c r="E125" s="55">
         <v>26709</v>
       </c>
-      <c r="F125" s="47"/>
-      <c r="G125" s="44">
+      <c r="F125" s="55"/>
+      <c r="G125" s="53">
         <v>12</v>
       </c>
-      <c r="H125" s="45"/>
+      <c r="H125" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:F104"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="G124:H124"/>
@@ -10736,18 +10706,48 @@
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G108:H108"/>
     <mergeCell ref="G109:H109"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:F104"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
introduced some redundancies to try to find why storage isn't being chosen; no luck yet
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -688,7 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -779,6 +779,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,19 +812,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -815,18 +827,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,7 +1113,7 @@
   <dimension ref="A1:AV125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+      <selection activeCell="M92" sqref="M92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1345,10 +1347,10 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="10"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
       <c r="N6" s="41" t="s">
         <v>142</v>
       </c>
@@ -1479,7 +1481,7 @@
     </row>
     <row r="12" spans="2:48" x14ac:dyDescent="0.35">
       <c r="F12" s="36"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="25"/>
       <c r="S12" s="33"/>
       <c r="T12" s="33"/>
       <c r="U12" s="33"/>
@@ -5741,17 +5743,17 @@
       </c>
     </row>
     <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="C45" s="55" t="s">
+      <c r="C45" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
       <c r="F45" s="2"/>
-      <c r="H45" s="55" t="s">
+      <c r="H45" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42"/>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="O45" s="4"/>
@@ -5988,11 +5990,11 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="C53" s="55" t="s">
+      <c r="C53" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="55"/>
-      <c r="E53" s="55"/>
+      <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
       <c r="G53" s="38" t="s">
         <v>137</v>
       </c>
@@ -10253,25 +10255,25 @@
         <v>43</v>
       </c>
       <c r="H97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J97" s="35">
         <v>43</v>
       </c>
       <c r="K97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M97" s="35">
         <v>43</v>
       </c>
       <c r="N97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="P97" s="35">
         <v>43</v>
       </c>
       <c r="Q97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="S97" s="32">
         <v>43</v>
@@ -10327,27 +10329,27 @@
       </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D103" s="56" t="s">
+      <c r="D103" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="E103" s="48" t="s">
+      <c r="E103" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F103" s="48"/>
-      <c r="G103" s="48" t="s">
+      <c r="F103" s="45"/>
+      <c r="G103" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="H103" s="49"/>
+      <c r="H103" s="54"/>
       <c r="N103" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D104" s="57"/>
-      <c r="E104" s="50"/>
-      <c r="F104" s="50"/>
-      <c r="G104" s="50"/>
-      <c r="H104" s="51"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="46"/>
+      <c r="F104" s="46"/>
+      <c r="G104" s="46"/>
+      <c r="H104" s="55"/>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
@@ -10361,14 +10363,14 @@
       <c r="D106" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E106" s="54">
+      <c r="E106" s="47">
         <v>72154</v>
       </c>
-      <c r="F106" s="54"/>
-      <c r="G106" s="52">
+      <c r="F106" s="47"/>
+      <c r="G106" s="56">
         <v>28.1</v>
       </c>
-      <c r="H106" s="53"/>
+      <c r="H106" s="57"/>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C107" s="18">
@@ -10377,14 +10379,14 @@
       <c r="D107" s="19">
         <v>0.31</v>
       </c>
-      <c r="E107" s="46">
+      <c r="E107" s="48">
         <v>67811</v>
       </c>
-      <c r="F107" s="46"/>
-      <c r="G107" s="42">
+      <c r="F107" s="48"/>
+      <c r="G107" s="49">
         <v>25</v>
       </c>
-      <c r="H107" s="43"/>
+      <c r="H107" s="50"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C108" s="18">
@@ -10393,14 +10395,14 @@
       <c r="D108" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E108" s="46">
+      <c r="E108" s="48">
         <v>187455</v>
       </c>
-      <c r="F108" s="46"/>
-      <c r="G108" s="42">
+      <c r="F108" s="48"/>
+      <c r="G108" s="49">
         <v>70</v>
       </c>
-      <c r="H108" s="43"/>
+      <c r="H108" s="50"/>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C109" s="18">
@@ -10409,14 +10411,14 @@
       <c r="D109" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E109" s="46">
+      <c r="E109" s="48">
         <v>63266</v>
       </c>
-      <c r="F109" s="46"/>
-      <c r="G109" s="42">
+      <c r="F109" s="48"/>
+      <c r="G109" s="49">
         <v>30.6</v>
       </c>
-      <c r="H109" s="43"/>
+      <c r="H109" s="50"/>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -10425,14 +10427,14 @@
       <c r="D110" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E110" s="46">
+      <c r="E110" s="48">
         <v>26553</v>
       </c>
-      <c r="F110" s="46"/>
-      <c r="G110" s="42">
+      <c r="F110" s="48"/>
+      <c r="G110" s="49">
         <v>10</v>
       </c>
-      <c r="H110" s="43"/>
+      <c r="H110" s="50"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -10441,14 +10443,14 @@
       <c r="D111" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E111" s="46">
+      <c r="E111" s="48">
         <v>24949</v>
       </c>
-      <c r="F111" s="46"/>
-      <c r="G111" s="42">
+      <c r="F111" s="48"/>
+      <c r="G111" s="49">
         <v>10</v>
       </c>
-      <c r="H111" s="43"/>
+      <c r="H111" s="50"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -10457,14 +10459,14 @@
       <c r="D112" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E112" s="46">
+      <c r="E112" s="48">
         <v>22870</v>
       </c>
-      <c r="F112" s="46"/>
-      <c r="G112" s="42">
+      <c r="F112" s="48"/>
+      <c r="G112" s="49">
         <v>10</v>
       </c>
-      <c r="H112" s="43"/>
+      <c r="H112" s="50"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -10473,14 +10475,14 @@
       <c r="D113" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E113" s="46">
+      <c r="E113" s="48">
         <v>139836</v>
       </c>
-      <c r="F113" s="46"/>
-      <c r="G113" s="42">
+      <c r="F113" s="48"/>
+      <c r="G113" s="49">
         <v>52.2</v>
       </c>
-      <c r="H113" s="43"/>
+      <c r="H113" s="50"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -10489,14 +10491,14 @@
       <c r="D114" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E114" s="46">
+      <c r="E114" s="48">
         <v>23515</v>
       </c>
-      <c r="F114" s="46"/>
-      <c r="G114" s="42">
+      <c r="F114" s="48"/>
+      <c r="G114" s="49">
         <v>10</v>
       </c>
-      <c r="H114" s="43"/>
+      <c r="H114" s="50"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -10505,14 +10507,14 @@
       <c r="D115" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E115" s="46">
+      <c r="E115" s="48">
         <v>49503</v>
       </c>
-      <c r="F115" s="46"/>
-      <c r="G115" s="42">
+      <c r="F115" s="48"/>
+      <c r="G115" s="49">
         <v>20.2</v>
       </c>
-      <c r="H115" s="43"/>
+      <c r="H115" s="50"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -10521,14 +10523,14 @@
       <c r="D116" s="19">
         <v>0.307</v>
       </c>
-      <c r="E116" s="46">
+      <c r="E116" s="48">
         <v>188420</v>
       </c>
-      <c r="F116" s="46"/>
-      <c r="G116" s="42">
+      <c r="F116" s="48"/>
+      <c r="G116" s="49">
         <v>70</v>
       </c>
-      <c r="H116" s="43"/>
+      <c r="H116" s="50"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -10537,14 +10539,14 @@
       <c r="D117" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E117" s="46">
+      <c r="E117" s="48">
         <v>26573</v>
       </c>
-      <c r="F117" s="46"/>
-      <c r="G117" s="42">
+      <c r="F117" s="48"/>
+      <c r="G117" s="49">
         <v>10.5</v>
       </c>
-      <c r="H117" s="43"/>
+      <c r="H117" s="50"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -10553,14 +10555,14 @@
       <c r="D118" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E118" s="46">
+      <c r="E118" s="48">
         <v>25253</v>
       </c>
-      <c r="F118" s="46"/>
-      <c r="G118" s="42">
+      <c r="F118" s="48"/>
+      <c r="G118" s="49">
         <v>10</v>
       </c>
-      <c r="H118" s="43"/>
+      <c r="H118" s="50"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -10569,14 +10571,14 @@
       <c r="D119" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E119" s="46">
+      <c r="E119" s="48">
         <v>17610</v>
       </c>
-      <c r="F119" s="46"/>
-      <c r="G119" s="42">
+      <c r="F119" s="48"/>
+      <c r="G119" s="49">
         <v>10</v>
       </c>
-      <c r="H119" s="43"/>
+      <c r="H119" s="50"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -10585,14 +10587,14 @@
       <c r="D120" s="19">
         <v>0.221</v>
       </c>
-      <c r="E120" s="46">
+      <c r="E120" s="48">
         <v>19372</v>
       </c>
-      <c r="F120" s="46"/>
-      <c r="G120" s="42">
+      <c r="F120" s="48"/>
+      <c r="G120" s="49">
         <v>10</v>
       </c>
-      <c r="H120" s="43"/>
+      <c r="H120" s="50"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -10601,14 +10603,14 @@
       <c r="D121" s="19">
         <v>0.216</v>
       </c>
-      <c r="E121" s="46">
+      <c r="E121" s="48">
         <v>18939</v>
       </c>
-      <c r="F121" s="46"/>
-      <c r="G121" s="42">
+      <c r="F121" s="48"/>
+      <c r="G121" s="49">
         <v>10</v>
       </c>
-      <c r="H121" s="43"/>
+      <c r="H121" s="50"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -10617,14 +10619,14 @@
       <c r="D122" s="19">
         <v>0.23</v>
       </c>
-      <c r="E122" s="46">
+      <c r="E122" s="48">
         <v>20382</v>
       </c>
-      <c r="F122" s="46"/>
-      <c r="G122" s="42">
+      <c r="F122" s="48"/>
+      <c r="G122" s="49">
         <v>10.1</v>
       </c>
-      <c r="H122" s="43"/>
+      <c r="H122" s="50"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -10633,14 +10635,14 @@
       <c r="D123" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E123" s="46">
+      <c r="E123" s="48">
         <v>19968</v>
       </c>
-      <c r="F123" s="46"/>
-      <c r="G123" s="42">
+      <c r="F123" s="48"/>
+      <c r="G123" s="49">
         <v>10.1</v>
       </c>
-      <c r="H123" s="43"/>
+      <c r="H123" s="50"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -10649,14 +10651,14 @@
       <c r="D124" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E124" s="46">
+      <c r="E124" s="48">
         <v>23240</v>
       </c>
-      <c r="F124" s="46"/>
-      <c r="G124" s="42">
+      <c r="F124" s="48"/>
+      <c r="G124" s="49">
         <v>10</v>
       </c>
-      <c r="H124" s="43"/>
+      <c r="H124" s="50"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="20">
@@ -10665,60 +10667,29 @@
       <c r="D125" s="21">
         <v>0.254</v>
       </c>
-      <c r="E125" s="47">
+      <c r="E125" s="53">
         <v>26709</v>
       </c>
-      <c r="F125" s="47"/>
-      <c r="G125" s="44">
+      <c r="F125" s="53"/>
+      <c r="G125" s="51">
         <v>12</v>
       </c>
-      <c r="H125" s="45"/>
+      <c r="H125" s="52"/>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N8:P8"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="E103:F104"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
+  <mergeCells count="70">
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="G124:H124"/>
@@ -10735,18 +10706,48 @@
     <mergeCell ref="G107:H107"/>
     <mergeCell ref="G108:H108"/>
     <mergeCell ref="G109:H109"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="E103:F104"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N8:P8"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added energy efficiency programs (refrigerator and LED lights)
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -29,6 +29,10 @@
     <definedName name="FallOffHours">Sheet2!$AV$13</definedName>
     <definedName name="FallPeakHours">Sheet2!$AP$13</definedName>
     <definedName name="FallSolarFactor">Sheet2!$Q$53</definedName>
+    <definedName name="fridge_eff_benefit">Sheet2!$AY$16:$BA$41</definedName>
+    <definedName name="fridge_eff_cost">Sheet2!$BB$13</definedName>
+    <definedName name="led_eff_benefit">Sheet2!$BE$16:$BG$41</definedName>
+    <definedName name="led_eff_cost">Sheet2!$BH$13</definedName>
     <definedName name="LineCapacity">Sheet2!$P$47:$P$49</definedName>
     <definedName name="LineFromBus">Sheet2!$H$47:$J$49</definedName>
     <definedName name="LineReactance">Sheet2!$M$47:$M$49</definedName>
@@ -84,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="148">
   <si>
     <t>NumBuses</t>
   </si>
@@ -519,14 +523,24 @@
   </si>
   <si>
     <t>RampRate (MW/hr)</t>
+  </si>
+  <si>
+    <t>Refrigerator Energy Efficiency Benefits (MW)</t>
+  </si>
+  <si>
+    <t>LED Lights Energy Efficiency Benefits (MW)</t>
+  </si>
+  <si>
+    <t>Annual Cost ($):</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -684,11 +698,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -776,6 +791,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -806,12 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -827,10 +840,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1110,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV125"/>
+  <dimension ref="A1:BL125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M92" sqref="M92"/>
+    <sheetView tabSelected="1" topLeftCell="AJ4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AV10" sqref="AV10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,79 +1153,84 @@
     <col min="23" max="24" width="16.26953125" customWidth="1"/>
     <col min="25" max="25" width="16.1796875" customWidth="1"/>
     <col min="26" max="29" width="16.26953125" customWidth="1"/>
+    <col min="54" max="54" width="15" customWidth="1"/>
+    <col min="55" max="56" width="8.7265625" customWidth="1"/>
+    <col min="60" max="60" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="41"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="14">
         <v>0.1</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
       <c r="Q1" s="24">
         <v>2221460.4</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
     </row>
-    <row r="2" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="6"/>
-      <c r="I2" s="41" t="s">
+      <c r="I2" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1215,7 +1238,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1225,35 +1248,39 @@
       <c r="F3" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="N3" s="41" t="s">
+      <c r="N3" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
       <c r="Q3" s="24">
         <v>1596613.3</v>
       </c>
-      <c r="S3" s="41" t="s">
+      <c r="S3" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
       <c r="W3" t="s">
         <v>102</v>
       </c>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
     </row>
-    <row r="4" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1267,27 +1294,27 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="41" t="s">
+      <c r="I4" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
       <c r="L4" s="15">
         <v>1</v>
       </c>
-      <c r="N4" s="41" t="s">
+      <c r="N4" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="O4" s="41"/>
-      <c r="P4" s="41"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
       <c r="Q4" s="24">
         <v>43560</v>
       </c>
-      <c r="S4" s="41" t="s">
+      <c r="S4" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="T4" s="41"/>
-      <c r="U4" s="41"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1296,7 +1323,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
       <c r="F5" s="36" t="s">
         <v>111</v>
@@ -1304,27 +1331,27 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
-      <c r="N5" s="41" t="s">
+      <c r="N5" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
       <c r="Q5" s="24">
         <v>601000</v>
       </c>
-      <c r="S5" s="41" t="s">
+      <c r="S5" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="T5" s="41"/>
-      <c r="U5" s="41"/>
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1333,7 +1360,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>105</v>
       </c>
@@ -1347,23 +1374,23 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="59"/>
-      <c r="N6" s="41" t="s">
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="42"/>
+      <c r="N6" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
       <c r="Q6" s="24">
         <v>15025</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S6" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1372,7 +1399,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
@@ -1386,19 +1413,19 @@
       <c r="G7" s="6">
         <v>4050</v>
       </c>
-      <c r="N7" s="41" t="s">
+      <c r="N7" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
+      <c r="O7" s="45"/>
+      <c r="P7" s="45"/>
       <c r="Q7" s="26">
         <v>0.95</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1407,26 +1434,26 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:64" x14ac:dyDescent="0.35">
       <c r="F8" s="36" t="s">
         <v>114</v>
       </c>
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="N8" s="41" t="s">
+      <c r="N8" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
+      <c r="O8" s="45"/>
+      <c r="P8" s="45"/>
       <c r="Q8" s="26">
         <v>50</v>
       </c>
-      <c r="S8" s="41" t="s">
+      <c r="S8" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1434,19 +1461,20 @@
       <c r="W8" t="s">
         <v>96</v>
       </c>
+      <c r="AA8" s="44"/>
     </row>
-    <row r="9" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:64" x14ac:dyDescent="0.35">
       <c r="F9" s="36" t="s">
         <v>115</v>
       </c>
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="N9" s="41" t="s">
+      <c r="N9" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="45"/>
       <c r="Q9" s="26">
         <v>10</v>
       </c>
@@ -1455,7 +1483,7 @@
       <c r="U9" s="33"/>
       <c r="V9" s="25"/>
     </row>
-    <row r="10" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:64" x14ac:dyDescent="0.35">
       <c r="F10" s="36" t="s">
         <v>116</v>
       </c>
@@ -1467,7 +1495,7 @@
       <c r="U10" s="33"/>
       <c r="V10" s="25"/>
     </row>
-    <row r="11" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:64" x14ac:dyDescent="0.35">
       <c r="F11" s="36" t="s">
         <v>117</v>
       </c>
@@ -1479,7 +1507,7 @@
       <c r="U11" s="33"/>
       <c r="V11" s="25"/>
     </row>
-    <row r="12" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:64" x14ac:dyDescent="0.35">
       <c r="F12" s="36"/>
       <c r="G12" s="25"/>
       <c r="S12" s="33"/>
@@ -1487,7 +1515,7 @@
       <c r="U12" s="33"/>
       <c r="V12" s="25"/>
     </row>
-    <row r="13" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:64" x14ac:dyDescent="0.35">
       <c r="E13" s="36" t="s">
         <v>125</v>
       </c>
@@ -1556,8 +1584,22 @@
         <f>92*8</f>
         <v>736</v>
       </c>
+      <c r="AZ13" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="BA13" s="45"/>
+      <c r="BB13" s="43">
+        <v>16054000</v>
+      </c>
+      <c r="BF13" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="BG13" s="45"/>
+      <c r="BH13" s="43">
+        <v>10000000</v>
+      </c>
     </row>
-    <row r="14" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:64" x14ac:dyDescent="0.35">
       <c r="D14" s="33" t="s">
         <v>108</v>
       </c>
@@ -1598,8 +1640,24 @@
       </c>
       <c r="AU14" s="33"/>
       <c r="AV14" s="34"/>
+      <c r="AX14" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY14" s="45"/>
+      <c r="AZ14" s="45"/>
+      <c r="BA14" s="45"/>
+      <c r="BB14" s="45"/>
+      <c r="BD14" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="BE14" s="45"/>
+      <c r="BF14" s="45"/>
+      <c r="BG14" s="45"/>
+      <c r="BH14" s="45"/>
+      <c r="BK14" s="41"/>
+      <c r="BL14" s="41"/>
     </row>
-    <row r="15" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
@@ -1720,8 +1778,38 @@
       <c r="AV15" s="34" t="s">
         <v>34</v>
       </c>
+      <c r="AX15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY15">
+        <v>1</v>
+      </c>
+      <c r="AZ15">
+        <v>2</v>
+      </c>
+      <c r="BA15">
+        <v>3</v>
+      </c>
+      <c r="BB15" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE15">
+        <v>1</v>
+      </c>
+      <c r="BF15">
+        <v>2</v>
+      </c>
+      <c r="BG15">
+        <v>3</v>
+      </c>
+      <c r="BH15" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="16" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:64" x14ac:dyDescent="0.35">
       <c r="B16" s="4">
         <v>2020</v>
       </c>
@@ -1874,8 +1962,44 @@
         <f>G11</f>
         <v>3780</v>
       </c>
+      <c r="AX16" s="4">
+        <v>2020</v>
+      </c>
+      <c r="AY16" s="27">
+        <f>0.15*BB16</f>
+        <v>1.7458725000000002</v>
+      </c>
+      <c r="AZ16" s="27">
+        <f>0.5*BB16</f>
+        <v>5.8195750000000004</v>
+      </c>
+      <c r="BA16" s="27">
+        <f>0.35*BB16</f>
+        <v>4.0737025000000004</v>
+      </c>
+      <c r="BB16">
+        <v>11.639150000000001</v>
+      </c>
+      <c r="BD16" s="4">
+        <v>2020</v>
+      </c>
+      <c r="BE16" s="27">
+        <f>0.15*BH16</f>
+        <v>10.5</v>
+      </c>
+      <c r="BF16" s="27">
+        <f>0.5*BH16</f>
+        <v>35</v>
+      </c>
+      <c r="BG16" s="27">
+        <f>0.35*BH16</f>
+        <v>24.5</v>
+      </c>
+      <c r="BH16">
+        <v>70</v>
+      </c>
     </row>
-    <row r="17" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B17" s="4">
         <v>2021</v>
       </c>
@@ -2028,8 +2152,44 @@
         <f>AV16*(1+$L$3)</f>
         <v>3814.0199999999995</v>
       </c>
+      <c r="AX17" s="4">
+        <v>2021</v>
+      </c>
+      <c r="AY17" s="27">
+        <f t="shared" ref="AY17:AY41" si="28">0.15*BB17</f>
+        <v>3.4917450000000003</v>
+      </c>
+      <c r="AZ17" s="27">
+        <f t="shared" ref="AZ17:AZ41" si="29">0.5*BB17</f>
+        <v>11.639150000000001</v>
+      </c>
+      <c r="BA17" s="27">
+        <f t="shared" ref="BA17:BA41" si="30">0.35*BB17</f>
+        <v>8.1474050000000009</v>
+      </c>
+      <c r="BB17">
+        <v>23.278300000000002</v>
+      </c>
+      <c r="BD17" s="4">
+        <v>2021</v>
+      </c>
+      <c r="BE17" s="27">
+        <f t="shared" ref="BE17:BE41" si="31">0.15*BH17</f>
+        <v>21</v>
+      </c>
+      <c r="BF17" s="27">
+        <f t="shared" ref="BF17:BF41" si="32">0.5*BH17</f>
+        <v>70</v>
+      </c>
+      <c r="BG17" s="27">
+        <f t="shared" ref="BG17:BG41" si="33">0.35*BH17</f>
+        <v>49</v>
+      </c>
+      <c r="BH17">
+        <v>140</v>
+      </c>
     </row>
-    <row r="18" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B18" s="4">
         <v>2022</v>
       </c>
@@ -2065,7 +2225,7 @@
         <v>1327.6794320999998</v>
       </c>
       <c r="L18" s="12">
-        <f t="shared" ref="L18:L41" si="28">L17*(1+$L$3)</f>
+        <f t="shared" ref="L18:L41" si="34">L17*(1+$L$3)</f>
         <v>3793.3698059999992</v>
       </c>
       <c r="N18" s="4">
@@ -2103,7 +2263,7 @@
         <v>1443.1298174999995</v>
       </c>
       <c r="X18" s="12">
-        <f t="shared" ref="X18:X41" si="29">X17*(1+$L$3)</f>
+        <f t="shared" ref="X18:X41" si="35">X17*(1+$L$3)</f>
         <v>4123.2280499999988</v>
       </c>
       <c r="Z18" s="4">
@@ -2141,7 +2301,7 @@
         <v>1784.8487051499994</v>
       </c>
       <c r="AJ18" s="12">
-        <f t="shared" ref="AJ18:AJ41" si="30">AJ17*(1+$L$3)</f>
+        <f t="shared" ref="AJ18:AJ41" si="36">AJ17*(1+$L$3)</f>
         <v>5099.5677289999985</v>
       </c>
       <c r="AL18" s="4">
@@ -2179,11 +2339,47 @@
         <v>1346.9211629999995</v>
       </c>
       <c r="AV18" s="12">
-        <f t="shared" ref="AV18:AV41" si="31">AV17*(1+$L$3)</f>
+        <f t="shared" ref="AV18:AV41" si="37">AV17*(1+$L$3)</f>
         <v>3848.3461799999991</v>
       </c>
+      <c r="AX18" s="4">
+        <v>2022</v>
+      </c>
+      <c r="AY18" s="27">
+        <f t="shared" si="28"/>
+        <v>5.2376174999999998</v>
+      </c>
+      <c r="AZ18" s="27">
+        <f t="shared" si="29"/>
+        <v>17.458725000000001</v>
+      </c>
+      <c r="BA18" s="27">
+        <f t="shared" si="30"/>
+        <v>12.2211075</v>
+      </c>
+      <c r="BB18">
+        <v>34.917450000000002</v>
+      </c>
+      <c r="BD18" s="4">
+        <v>2022</v>
+      </c>
+      <c r="BE18" s="27">
+        <f t="shared" si="31"/>
+        <v>31.5</v>
+      </c>
+      <c r="BF18" s="27">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+      <c r="BG18" s="27">
+        <f t="shared" si="33"/>
+        <v>73.5</v>
+      </c>
+      <c r="BH18">
+        <v>210</v>
+      </c>
     </row>
-    <row r="19" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B19" s="4">
         <v>2023</v>
       </c>
@@ -2219,7 +2415,7 @@
         <v>1339.6285469888994</v>
       </c>
       <c r="L19" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>3827.5101342539988</v>
       </c>
       <c r="N19" s="4">
@@ -2257,7 +2453,7 @@
         <v>1456.1179858574994</v>
       </c>
       <c r="X19" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4160.3371024499984</v>
       </c>
       <c r="Z19" s="4">
@@ -2295,7 +2491,7 @@
         <v>1800.9123434963492</v>
       </c>
       <c r="AJ19" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5145.4638385609978</v>
       </c>
       <c r="AL19" s="4">
@@ -2333,11 +2529,47 @@
         <v>1359.0434534669994</v>
       </c>
       <c r="AV19" s="12">
+        <f t="shared" si="37"/>
+        <v>3882.9812956199985</v>
+      </c>
+      <c r="AX19" s="4">
+        <v>2023</v>
+      </c>
+      <c r="AY19" s="27">
+        <f t="shared" si="28"/>
+        <v>6.9834900000000006</v>
+      </c>
+      <c r="AZ19" s="27">
+        <f t="shared" si="29"/>
+        <v>23.278300000000002</v>
+      </c>
+      <c r="BA19" s="27">
+        <f t="shared" si="30"/>
+        <v>16.294810000000002</v>
+      </c>
+      <c r="BB19">
+        <v>46.556600000000003</v>
+      </c>
+      <c r="BD19" s="4">
+        <v>2023</v>
+      </c>
+      <c r="BE19" s="27">
         <f t="shared" si="31"/>
-        <v>3882.9812956199985</v>
+        <v>42</v>
+      </c>
+      <c r="BF19" s="27">
+        <f t="shared" si="32"/>
+        <v>140</v>
+      </c>
+      <c r="BG19" s="27">
+        <f t="shared" si="33"/>
+        <v>98</v>
+      </c>
+      <c r="BH19">
+        <v>280</v>
       </c>
     </row>
-    <row r="20" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <v>2024</v>
       </c>
@@ -2373,7 +2605,7 @@
         <v>1351.6852039117996</v>
       </c>
       <c r="L20" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>3861.9577254622845</v>
       </c>
       <c r="N20" s="4">
@@ -2411,7 +2643,7 @@
         <v>1469.2230477302169</v>
       </c>
       <c r="X20" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4197.7801363720482</v>
       </c>
       <c r="Z20" s="4">
@@ -2449,7 +2681,7 @@
         <v>1817.1205545878161</v>
       </c>
       <c r="AJ20" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5191.7730131080461</v>
       </c>
       <c r="AL20" s="4">
@@ -2487,11 +2719,47 @@
         <v>1371.2748445482023</v>
       </c>
       <c r="AV20" s="12">
+        <f t="shared" si="37"/>
+        <v>3917.9281272805779</v>
+      </c>
+      <c r="AX20" s="4">
+        <v>2024</v>
+      </c>
+      <c r="AY20" s="27">
+        <f t="shared" si="28"/>
+        <v>8.7293625000000006</v>
+      </c>
+      <c r="AZ20" s="27">
+        <f t="shared" si="29"/>
+        <v>29.097875000000002</v>
+      </c>
+      <c r="BA20" s="27">
+        <f t="shared" si="30"/>
+        <v>20.368512500000001</v>
+      </c>
+      <c r="BB20">
+        <v>58.195750000000004</v>
+      </c>
+      <c r="BD20" s="4">
+        <v>2024</v>
+      </c>
+      <c r="BE20" s="27">
         <f t="shared" si="31"/>
-        <v>3917.9281272805779</v>
+        <v>52.5</v>
+      </c>
+      <c r="BF20" s="27">
+        <f t="shared" si="32"/>
+        <v>175</v>
+      </c>
+      <c r="BG20" s="27">
+        <f t="shared" si="33"/>
+        <v>122.49999999999999</v>
+      </c>
+      <c r="BH20">
+        <v>350</v>
       </c>
     </row>
-    <row r="21" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B21" s="4">
         <v>2025</v>
       </c>
@@ -2527,7 +2795,7 @@
         <v>1363.8503707470056</v>
       </c>
       <c r="L21" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>3896.7153449914449</v>
       </c>
       <c r="N21" s="4">
@@ -2565,7 +2833,7 @@
         <v>1482.4460551597886</v>
       </c>
       <c r="X21" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4235.560157599396</v>
       </c>
       <c r="Z21" s="4">
@@ -2603,7 +2871,7 @@
         <v>1833.4746395791062</v>
       </c>
       <c r="AJ21" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5238.4989702260182</v>
       </c>
       <c r="AL21" s="4">
@@ -2641,11 +2909,47 @@
         <v>1383.6163181491359</v>
       </c>
       <c r="AV21" s="12">
+        <f t="shared" si="37"/>
+        <v>3953.1894804261028</v>
+      </c>
+      <c r="AX21" s="4">
+        <v>2025</v>
+      </c>
+      <c r="AY21" s="27">
+        <f t="shared" si="28"/>
+        <v>10.475235</v>
+      </c>
+      <c r="AZ21" s="27">
+        <f t="shared" si="29"/>
+        <v>34.917450000000002</v>
+      </c>
+      <c r="BA21" s="27">
+        <f t="shared" si="30"/>
+        <v>24.442215000000001</v>
+      </c>
+      <c r="BB21">
+        <v>69.834900000000005</v>
+      </c>
+      <c r="BD21" s="4">
+        <v>2025</v>
+      </c>
+      <c r="BE21" s="27">
         <f t="shared" si="31"/>
-        <v>3953.1894804261028</v>
+        <v>63</v>
+      </c>
+      <c r="BF21" s="27">
+        <f t="shared" si="32"/>
+        <v>210</v>
+      </c>
+      <c r="BG21" s="27">
+        <f t="shared" si="33"/>
+        <v>147</v>
+      </c>
+      <c r="BH21">
+        <v>420</v>
       </c>
     </row>
-    <row r="22" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>2026</v>
       </c>
@@ -2681,7 +2985,7 @@
         <v>1376.1250240837285</v>
       </c>
       <c r="L22" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>3931.7857830963676</v>
       </c>
       <c r="N22" s="4">
@@ -2719,7 +3023,7 @@
         <v>1495.7880696562265</v>
       </c>
       <c r="X22" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4273.6801990177901</v>
       </c>
       <c r="Z22" s="4">
@@ -2757,7 +3061,7 @@
         <v>1849.975911335318</v>
       </c>
       <c r="AJ22" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5285.6454609580514</v>
       </c>
       <c r="AL22" s="4">
@@ -2795,11 +3099,47 @@
         <v>1396.068865012478</v>
       </c>
       <c r="AV22" s="12">
+        <f t="shared" si="37"/>
+        <v>3988.7681857499374</v>
+      </c>
+      <c r="AX22" s="4">
+        <v>2026</v>
+      </c>
+      <c r="AY22" s="27">
+        <f t="shared" si="28"/>
+        <v>12.2211075</v>
+      </c>
+      <c r="AZ22" s="27">
+        <f t="shared" si="29"/>
+        <v>40.737025000000003</v>
+      </c>
+      <c r="BA22" s="27">
+        <f t="shared" si="30"/>
+        <v>28.5159175</v>
+      </c>
+      <c r="BB22">
+        <v>81.474050000000005</v>
+      </c>
+      <c r="BD22" s="4">
+        <v>2026</v>
+      </c>
+      <c r="BE22" s="27">
         <f t="shared" si="31"/>
-        <v>3988.7681857499374</v>
+        <v>73.5</v>
+      </c>
+      <c r="BF22" s="27">
+        <f t="shared" si="32"/>
+        <v>245</v>
+      </c>
+      <c r="BG22" s="27">
+        <f t="shared" si="33"/>
+        <v>171.5</v>
+      </c>
+      <c r="BH22">
+        <v>490</v>
       </c>
     </row>
-    <row r="23" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B23" s="4">
         <v>2027</v>
       </c>
@@ -2835,7 +3175,7 @@
         <v>1388.510149300482</v>
       </c>
       <c r="L23" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>3967.1718551442345</v>
       </c>
       <c r="N23" s="4">
@@ -2873,7 +3213,7 @@
         <v>1509.2501622831326</v>
       </c>
       <c r="X23" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4312.1433208089502</v>
       </c>
       <c r="Z23" s="4">
@@ -2911,7 +3251,7 @@
         <v>1866.6256945373357</v>
       </c>
       <c r="AJ23" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5333.2162701066736</v>
       </c>
       <c r="AL23" s="4">
@@ -2949,11 +3289,47 @@
         <v>1408.6334847975902</v>
       </c>
       <c r="AV23" s="12">
+        <f t="shared" si="37"/>
+        <v>4024.6670994216865</v>
+      </c>
+      <c r="AX23" s="4">
+        <v>2027</v>
+      </c>
+      <c r="AY23" s="27">
+        <f t="shared" si="28"/>
+        <v>13.966980000000001</v>
+      </c>
+      <c r="AZ23" s="27">
+        <f t="shared" si="29"/>
+        <v>46.556600000000003</v>
+      </c>
+      <c r="BA23" s="27">
+        <f t="shared" si="30"/>
+        <v>32.589620000000004</v>
+      </c>
+      <c r="BB23">
+        <v>93.113200000000006</v>
+      </c>
+      <c r="BD23" s="4">
+        <v>2027</v>
+      </c>
+      <c r="BE23" s="27">
         <f t="shared" si="31"/>
-        <v>4024.6670994216865</v>
+        <v>84</v>
+      </c>
+      <c r="BF23" s="27">
+        <f t="shared" si="32"/>
+        <v>280</v>
+      </c>
+      <c r="BG23" s="27">
+        <f t="shared" si="33"/>
+        <v>196</v>
+      </c>
+      <c r="BH23">
+        <v>560</v>
       </c>
     </row>
-    <row r="24" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B24" s="4">
         <v>2028</v>
       </c>
@@ -2989,7 +3365,7 @@
         <v>1401.0067406441863</v>
       </c>
       <c r="L24" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4002.8764018405323</v>
       </c>
       <c r="N24" s="4">
@@ -3027,7 +3403,7 @@
         <v>1522.8334137436805</v>
       </c>
       <c r="X24" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4350.9526106962303</v>
       </c>
       <c r="Z24" s="4">
@@ -3065,7 +3441,7 @@
         <v>1883.4253257881714</v>
       </c>
       <c r="AJ24" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5381.2152165376328</v>
       </c>
       <c r="AL24" s="4">
@@ -3103,11 +3479,47 @@
         <v>1421.3111861607683</v>
       </c>
       <c r="AV24" s="12">
+        <f t="shared" si="37"/>
+        <v>4060.8891033164814</v>
+      </c>
+      <c r="AX24" s="4">
+        <v>2028</v>
+      </c>
+      <c r="AY24" s="27">
+        <f t="shared" si="28"/>
+        <v>15.7128525</v>
+      </c>
+      <c r="AZ24" s="27">
+        <f t="shared" si="29"/>
+        <v>52.376175000000003</v>
+      </c>
+      <c r="BA24" s="27">
+        <f t="shared" si="30"/>
+        <v>36.6633225</v>
+      </c>
+      <c r="BB24">
+        <v>104.75235000000001</v>
+      </c>
+      <c r="BD24" s="4">
+        <v>2028</v>
+      </c>
+      <c r="BE24" s="27">
         <f t="shared" si="31"/>
-        <v>4060.8891033164814</v>
+        <v>94.5</v>
+      </c>
+      <c r="BF24" s="27">
+        <f t="shared" si="32"/>
+        <v>315</v>
+      </c>
+      <c r="BG24" s="27">
+        <f t="shared" si="33"/>
+        <v>220.5</v>
+      </c>
+      <c r="BH24">
+        <v>630</v>
       </c>
     </row>
-    <row r="25" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B25" s="4">
         <v>2029</v>
       </c>
@@ -3143,7 +3555,7 @@
         <v>1413.6158013099837</v>
       </c>
       <c r="L25" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4038.9022894570967</v>
       </c>
       <c r="N25" s="4">
@@ -3181,7 +3593,7 @@
         <v>1536.5389144673734</v>
       </c>
       <c r="X25" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4390.1111841924958</v>
       </c>
       <c r="Z25" s="4">
@@ -3219,7 +3631,7 @@
         <v>1900.3761537202647</v>
       </c>
       <c r="AJ25" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5429.6461534864711</v>
       </c>
       <c r="AL25" s="4">
@@ -3257,11 +3669,47 @@
         <v>1434.1029868362152</v>
       </c>
       <c r="AV25" s="12">
+        <f t="shared" si="37"/>
+        <v>4097.4371052463293</v>
+      </c>
+      <c r="AX25" s="4">
+        <v>2029</v>
+      </c>
+      <c r="AY25" s="27">
+        <f t="shared" si="28"/>
+        <v>17.458725000000001</v>
+      </c>
+      <c r="AZ25" s="27">
+        <f t="shared" si="29"/>
+        <v>58.195750000000004</v>
+      </c>
+      <c r="BA25" s="27">
+        <f t="shared" si="30"/>
+        <v>40.737025000000003</v>
+      </c>
+      <c r="BB25">
+        <v>116.39150000000001</v>
+      </c>
+      <c r="BD25" s="4">
+        <v>2029</v>
+      </c>
+      <c r="BE25" s="27">
         <f t="shared" si="31"/>
-        <v>4097.4371052463293</v>
+        <v>105</v>
+      </c>
+      <c r="BF25" s="27">
+        <f t="shared" si="32"/>
+        <v>350</v>
+      </c>
+      <c r="BG25" s="27">
+        <f t="shared" si="33"/>
+        <v>244.99999999999997</v>
+      </c>
+      <c r="BH25">
+        <v>700</v>
       </c>
     </row>
-    <row r="26" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B26" s="4">
         <v>2030</v>
       </c>
@@ -3297,7 +3745,7 @@
         <v>1426.3383435217734</v>
       </c>
       <c r="L26" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4075.2524100622099</v>
       </c>
       <c r="N26" s="4">
@@ -3335,7 +3783,7 @@
         <v>1550.3677646975798</v>
       </c>
       <c r="X26" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4429.6221848502282</v>
       </c>
       <c r="Z26" s="4">
@@ -3373,7 +3821,7 @@
         <v>1917.4795391037469</v>
       </c>
       <c r="AJ26" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5478.5129688678489</v>
       </c>
       <c r="AL26" s="4">
@@ -3411,11 +3859,47 @@
         <v>1447.009913717741</v>
       </c>
       <c r="AV26" s="12">
+        <f t="shared" si="37"/>
+        <v>4134.3140391935458</v>
+      </c>
+      <c r="AX26" s="4">
+        <v>2030</v>
+      </c>
+      <c r="AY26" s="27">
+        <f t="shared" si="28"/>
+        <v>19.204597500000002</v>
+      </c>
+      <c r="AZ26" s="27">
+        <f t="shared" si="29"/>
+        <v>64.015325000000004</v>
+      </c>
+      <c r="BA26" s="27">
+        <f t="shared" si="30"/>
+        <v>44.810727499999999</v>
+      </c>
+      <c r="BB26">
+        <v>128.03065000000001</v>
+      </c>
+      <c r="BD26" s="4">
+        <v>2030</v>
+      </c>
+      <c r="BE26" s="27">
         <f t="shared" si="31"/>
-        <v>4134.3140391935458</v>
+        <v>115.5</v>
+      </c>
+      <c r="BF26" s="27">
+        <f t="shared" si="32"/>
+        <v>385</v>
+      </c>
+      <c r="BG26" s="27">
+        <f t="shared" si="33"/>
+        <v>269.5</v>
+      </c>
+      <c r="BH26">
+        <v>770</v>
       </c>
     </row>
-    <row r="27" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B27" s="4">
         <v>2031</v>
       </c>
@@ -3451,7 +3935,7 @@
         <v>1439.1753886134691</v>
       </c>
       <c r="L27" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4111.9296817527693</v>
       </c>
       <c r="N27" s="4">
@@ -3489,7 +3973,7 @@
         <v>1564.3210745798579</v>
       </c>
       <c r="X27" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4469.4887845138801</v>
       </c>
       <c r="Z27" s="4">
@@ -3527,7 +4011,7 @@
         <v>1934.7368549556807</v>
       </c>
       <c r="AJ27" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5527.8195855876593</v>
       </c>
       <c r="AL27" s="4">
@@ -3565,11 +4049,47 @@
         <v>1460.0330029412003</v>
       </c>
       <c r="AV27" s="12">
+        <f t="shared" si="37"/>
+        <v>4171.522865546287</v>
+      </c>
+      <c r="AX27" s="4">
+        <v>2031</v>
+      </c>
+      <c r="AY27" s="27">
+        <f t="shared" si="28"/>
+        <v>20.950469999999999</v>
+      </c>
+      <c r="AZ27" s="27">
+        <f t="shared" si="29"/>
+        <v>69.834900000000005</v>
+      </c>
+      <c r="BA27" s="27">
+        <f t="shared" si="30"/>
+        <v>48.884430000000002</v>
+      </c>
+      <c r="BB27">
+        <v>139.66980000000001</v>
+      </c>
+      <c r="BD27" s="4">
+        <v>2031</v>
+      </c>
+      <c r="BE27" s="27">
         <f t="shared" si="31"/>
-        <v>4171.522865546287</v>
+        <v>126</v>
+      </c>
+      <c r="BF27" s="27">
+        <f t="shared" si="32"/>
+        <v>420</v>
+      </c>
+      <c r="BG27" s="27">
+        <f t="shared" si="33"/>
+        <v>294</v>
+      </c>
+      <c r="BH27">
+        <v>840</v>
       </c>
     </row>
-    <row r="28" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B28" s="4">
         <v>2032</v>
       </c>
@@ -3605,7 +4125,7 @@
         <v>1452.1279671109901</v>
       </c>
       <c r="L28" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4148.9370488885434</v>
       </c>
       <c r="N28" s="4">
@@ -3643,7 +4163,7 @@
         <v>1578.3999642510764</v>
       </c>
       <c r="X28" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4509.7141835745042</v>
       </c>
       <c r="Z28" s="4">
@@ -3681,7 +4201,7 @@
         <v>1952.1494866502815</v>
       </c>
       <c r="AJ28" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5577.5699618579474</v>
       </c>
       <c r="AL28" s="4">
@@ -3719,11 +4239,47 @@
         <v>1473.173299967671</v>
       </c>
       <c r="AV28" s="12">
+        <f t="shared" si="37"/>
+        <v>4209.0665713362032</v>
+      </c>
+      <c r="AX28" s="4">
+        <v>2032</v>
+      </c>
+      <c r="AY28" s="27">
+        <f t="shared" si="28"/>
+        <v>22.6963425</v>
+      </c>
+      <c r="AZ28" s="27">
+        <f t="shared" si="29"/>
+        <v>75.654475000000005</v>
+      </c>
+      <c r="BA28" s="27">
+        <f t="shared" si="30"/>
+        <v>52.958132499999998</v>
+      </c>
+      <c r="BB28">
+        <v>151.30895000000001</v>
+      </c>
+      <c r="BD28" s="4">
+        <v>2032</v>
+      </c>
+      <c r="BE28" s="27">
         <f t="shared" si="31"/>
-        <v>4209.0665713362032</v>
+        <v>136.5</v>
+      </c>
+      <c r="BF28" s="27">
+        <f t="shared" si="32"/>
+        <v>455</v>
+      </c>
+      <c r="BG28" s="27">
+        <f t="shared" si="33"/>
+        <v>318.5</v>
+      </c>
+      <c r="BH28">
+        <v>910</v>
       </c>
     </row>
-    <row r="29" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B29" s="4">
         <v>2033</v>
       </c>
@@ -3759,7 +4315,7 @@
         <v>1465.1971188149889</v>
       </c>
       <c r="L29" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4186.2774823285399</v>
       </c>
       <c r="N29" s="4">
@@ -3797,7 +4353,7 @@
         <v>1592.6055639293359</v>
       </c>
       <c r="X29" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4550.3016112266741</v>
       </c>
       <c r="Z29" s="4">
@@ -3835,7 +4391,7 @@
         <v>1969.7188320301339</v>
       </c>
       <c r="AJ29" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5627.7680915146684</v>
       </c>
       <c r="AL29" s="4">
@@ -3873,11 +4429,47 @@
         <v>1486.4318596673797</v>
       </c>
       <c r="AV29" s="12">
+        <f t="shared" si="37"/>
+        <v>4246.9481704782283</v>
+      </c>
+      <c r="AX29" s="4">
+        <v>2033</v>
+      </c>
+      <c r="AY29" s="27">
+        <f t="shared" si="28"/>
+        <v>24.442215000000001</v>
+      </c>
+      <c r="AZ29" s="27">
+        <f t="shared" si="29"/>
+        <v>81.474050000000005</v>
+      </c>
+      <c r="BA29" s="27">
+        <f t="shared" si="30"/>
+        <v>57.031835000000001</v>
+      </c>
+      <c r="BB29">
+        <v>162.94810000000001</v>
+      </c>
+      <c r="BD29" s="4">
+        <v>2033</v>
+      </c>
+      <c r="BE29" s="27">
         <f t="shared" si="31"/>
-        <v>4246.9481704782283</v>
+        <v>147</v>
+      </c>
+      <c r="BF29" s="27">
+        <f t="shared" si="32"/>
+        <v>490</v>
+      </c>
+      <c r="BG29" s="27">
+        <f t="shared" si="33"/>
+        <v>343</v>
+      </c>
+      <c r="BH29">
+        <v>980</v>
       </c>
     </row>
-    <row r="30" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B30" s="4">
         <v>2034</v>
       </c>
@@ -3913,7 +4505,7 @@
         <v>1478.3838928843236</v>
       </c>
       <c r="L30" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4223.9539796694962</v>
       </c>
       <c r="N30" s="4">
@@ -3951,7 +4543,7 @@
         <v>1606.9390140046999</v>
       </c>
       <c r="X30" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4591.2543257277139</v>
       </c>
       <c r="Z30" s="4">
@@ -3989,7 +4581,7 @@
         <v>1987.4463015184047</v>
       </c>
       <c r="AJ30" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5678.4180043382994</v>
       </c>
       <c r="AL30" s="4">
@@ -4027,11 +4619,47 @@
         <v>1499.809746404386</v>
       </c>
       <c r="AV30" s="12">
+        <f t="shared" si="37"/>
+        <v>4285.170704012532</v>
+      </c>
+      <c r="AX30" s="4">
+        <v>2034</v>
+      </c>
+      <c r="AY30" s="27">
+        <f t="shared" si="28"/>
+        <v>26.188087500000002</v>
+      </c>
+      <c r="AZ30" s="27">
+        <f t="shared" si="29"/>
+        <v>87.293625000000006</v>
+      </c>
+      <c r="BA30" s="27">
+        <f t="shared" si="30"/>
+        <v>61.105537499999997</v>
+      </c>
+      <c r="BB30">
+        <v>174.58725000000001</v>
+      </c>
+      <c r="BD30" s="4">
+        <v>2034</v>
+      </c>
+      <c r="BE30" s="27">
         <f t="shared" si="31"/>
-        <v>4285.170704012532</v>
+        <v>157.5</v>
+      </c>
+      <c r="BF30" s="27">
+        <f t="shared" si="32"/>
+        <v>525</v>
+      </c>
+      <c r="BG30" s="27">
+        <f t="shared" si="33"/>
+        <v>367.5</v>
+      </c>
+      <c r="BH30">
+        <v>1050</v>
       </c>
     </row>
-    <row r="31" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B31" s="4">
         <v>2035</v>
       </c>
@@ -4067,7 +4695,7 @@
         <v>1491.6893479202822</v>
       </c>
       <c r="L31" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4261.9695654865209</v>
       </c>
       <c r="N31" s="4">
@@ -4105,7 +4733,7 @@
         <v>1621.4014651307421</v>
       </c>
       <c r="X31" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4632.575614659263</v>
       </c>
       <c r="Z31" s="4">
@@ -4143,7 +4771,7 @@
         <v>2005.33331823207</v>
       </c>
       <c r="AJ31" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5729.5237663773432</v>
       </c>
       <c r="AL31" s="4">
@@ -4181,11 +4809,47 @@
         <v>1513.3080341220254</v>
       </c>
       <c r="AV31" s="12">
+        <f t="shared" si="37"/>
+        <v>4323.7372403486443</v>
+      </c>
+      <c r="AX31" s="4">
+        <v>2035</v>
+      </c>
+      <c r="AY31" s="27">
+        <f t="shared" si="28"/>
+        <v>27.933960000000003</v>
+      </c>
+      <c r="AZ31" s="27">
+        <f t="shared" si="29"/>
+        <v>93.113200000000006</v>
+      </c>
+      <c r="BA31" s="27">
+        <f t="shared" si="30"/>
+        <v>65.179240000000007</v>
+      </c>
+      <c r="BB31">
+        <v>186.22640000000001</v>
+      </c>
+      <c r="BD31" s="4">
+        <v>2035</v>
+      </c>
+      <c r="BE31" s="27">
         <f t="shared" si="31"/>
-        <v>4323.7372403486443</v>
+        <v>168</v>
+      </c>
+      <c r="BF31" s="27">
+        <f t="shared" si="32"/>
+        <v>560</v>
+      </c>
+      <c r="BG31" s="27">
+        <f t="shared" si="33"/>
+        <v>392</v>
+      </c>
+      <c r="BH31">
+        <v>1120</v>
       </c>
     </row>
-    <row r="32" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B32" s="4">
         <v>2036</v>
       </c>
@@ -4221,7 +4885,7 @@
         <v>1505.1145520515645</v>
       </c>
       <c r="L32" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4300.3272915758989</v>
       </c>
       <c r="N32" s="4">
@@ -4259,7 +4923,7 @@
         <v>1635.9940783169184</v>
       </c>
       <c r="X32" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4674.2687951911957</v>
       </c>
       <c r="Z32" s="4">
@@ -4297,7 +4961,7 @@
         <v>2023.3813180961586</v>
       </c>
       <c r="AJ32" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5781.0894802747389</v>
       </c>
       <c r="AL32" s="4">
@@ -4335,11 +4999,47 @@
         <v>1526.9278064291236</v>
       </c>
       <c r="AV32" s="12">
+        <f t="shared" si="37"/>
+        <v>4362.650875511782</v>
+      </c>
+      <c r="AX32" s="4">
+        <v>2036</v>
+      </c>
+      <c r="AY32" s="27">
+        <f t="shared" si="28"/>
+        <v>29.6798325</v>
+      </c>
+      <c r="AZ32" s="27">
+        <f t="shared" si="29"/>
+        <v>98.932775000000007</v>
+      </c>
+      <c r="BA32" s="27">
+        <f t="shared" si="30"/>
+        <v>69.252942500000003</v>
+      </c>
+      <c r="BB32">
+        <v>197.86555000000001</v>
+      </c>
+      <c r="BD32" s="4">
+        <v>2036</v>
+      </c>
+      <c r="BE32" s="27">
         <f t="shared" si="31"/>
-        <v>4362.650875511782</v>
+        <v>178.5</v>
+      </c>
+      <c r="BF32" s="27">
+        <f t="shared" si="32"/>
+        <v>595</v>
+      </c>
+      <c r="BG32" s="27">
+        <f t="shared" si="33"/>
+        <v>416.5</v>
+      </c>
+      <c r="BH32">
+        <v>1190</v>
       </c>
     </row>
-    <row r="33" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B33" s="4">
         <v>2037</v>
       </c>
@@ -4375,7 +5075,7 @@
         <v>1518.6605830200285</v>
       </c>
       <c r="L33" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4339.0302372000815</v>
       </c>
       <c r="N33" s="4">
@@ -4413,7 +5113,7 @@
         <v>1650.7180250217707</v>
       </c>
       <c r="X33" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4716.3372143479164</v>
       </c>
       <c r="Z33" s="4">
@@ -4451,7 +5151,7 @@
         <v>2041.5917499590239</v>
       </c>
       <c r="AJ33" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5833.1192855972113</v>
       </c>
       <c r="AL33" s="4">
@@ -4489,11 +5189,47 @@
         <v>1540.6701566869856</v>
       </c>
       <c r="AV33" s="12">
+        <f t="shared" si="37"/>
+        <v>4401.9147333913879</v>
+      </c>
+      <c r="AX33" s="4">
+        <v>2037</v>
+      </c>
+      <c r="AY33" s="27">
+        <f t="shared" si="28"/>
+        <v>31.425705000000001</v>
+      </c>
+      <c r="AZ33" s="27">
+        <f t="shared" si="29"/>
+        <v>104.75235000000001</v>
+      </c>
+      <c r="BA33" s="27">
+        <f t="shared" si="30"/>
+        <v>73.326644999999999</v>
+      </c>
+      <c r="BB33">
+        <v>209.50470000000001</v>
+      </c>
+      <c r="BD33" s="4">
+        <v>2037</v>
+      </c>
+      <c r="BE33" s="27">
         <f t="shared" si="31"/>
-        <v>4401.9147333913879</v>
+        <v>189</v>
+      </c>
+      <c r="BF33" s="27">
+        <f t="shared" si="32"/>
+        <v>630</v>
+      </c>
+      <c r="BG33" s="27">
+        <f t="shared" si="33"/>
+        <v>441</v>
+      </c>
+      <c r="BH33">
+        <v>1260</v>
       </c>
     </row>
-    <row r="34" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B34" s="4">
         <v>2038</v>
       </c>
@@ -4529,7 +5265,7 @@
         <v>1532.3285282672086</v>
       </c>
       <c r="L34" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4378.081509334882</v>
       </c>
       <c r="N34" s="4">
@@ -4567,7 +5303,7 @@
         <v>1665.5744872469663</v>
       </c>
       <c r="X34" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4758.7842492770469</v>
       </c>
       <c r="Z34" s="4">
@@ -4605,7 +5341,7 @@
         <v>2059.9660757086549</v>
       </c>
       <c r="AJ34" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5885.6173591675852</v>
       </c>
       <c r="AL34" s="4">
@@ -4643,11 +5379,47 @@
         <v>1554.5361880971682</v>
       </c>
       <c r="AV34" s="12">
+        <f t="shared" si="37"/>
+        <v>4441.5319659919096</v>
+      </c>
+      <c r="AX34" s="4">
+        <v>2038</v>
+      </c>
+      <c r="AY34" s="27">
+        <f t="shared" si="28"/>
+        <v>33.171577499999998</v>
+      </c>
+      <c r="AZ34" s="27">
+        <f t="shared" si="29"/>
+        <v>110.57192500000001</v>
+      </c>
+      <c r="BA34" s="27">
+        <f t="shared" si="30"/>
+        <v>77.400347499999995</v>
+      </c>
+      <c r="BB34">
+        <v>221.14385000000001</v>
+      </c>
+      <c r="BD34" s="4">
+        <v>2038</v>
+      </c>
+      <c r="BE34" s="27">
         <f t="shared" si="31"/>
-        <v>4441.5319659919096</v>
+        <v>199.5</v>
+      </c>
+      <c r="BF34" s="27">
+        <f t="shared" si="32"/>
+        <v>665</v>
+      </c>
+      <c r="BG34" s="27">
+        <f t="shared" si="33"/>
+        <v>465.49999999999994</v>
+      </c>
+      <c r="BH34">
+        <v>1330</v>
       </c>
     </row>
-    <row r="35" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B35" s="4">
         <v>2039</v>
       </c>
@@ -4683,7 +5455,7 @@
         <v>1546.1194850216134</v>
       </c>
       <c r="L35" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4417.4842429188957</v>
       </c>
       <c r="N35" s="4">
@@ -4721,7 +5493,7 @@
         <v>1680.5646576321888</v>
       </c>
       <c r="X35" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4801.6133075205398</v>
       </c>
       <c r="Z35" s="4">
@@ -4759,7 +5531,7 @@
         <v>2078.5057703900325</v>
       </c>
       <c r="AJ35" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5938.5879154000932</v>
       </c>
       <c r="AL35" s="4">
@@ -4797,11 +5569,47 @@
         <v>1568.5270137900427</v>
       </c>
       <c r="AV35" s="12">
+        <f t="shared" si="37"/>
+        <v>4481.5057536858367</v>
+      </c>
+      <c r="AX35" s="4">
+        <v>2039</v>
+      </c>
+      <c r="AY35" s="27">
+        <f t="shared" si="28"/>
+        <v>34.917450000000002</v>
+      </c>
+      <c r="AZ35" s="27">
+        <f t="shared" si="29"/>
+        <v>116.39150000000001</v>
+      </c>
+      <c r="BA35" s="27">
+        <f t="shared" si="30"/>
+        <v>81.474050000000005</v>
+      </c>
+      <c r="BB35">
+        <v>232.78300000000002</v>
+      </c>
+      <c r="BD35" s="4">
+        <v>2039</v>
+      </c>
+      <c r="BE35" s="27">
         <f t="shared" si="31"/>
-        <v>4481.5057536858367</v>
+        <v>210</v>
+      </c>
+      <c r="BF35" s="27">
+        <f t="shared" si="32"/>
+        <v>700</v>
+      </c>
+      <c r="BG35" s="27">
+        <f t="shared" si="33"/>
+        <v>489.99999999999994</v>
+      </c>
+      <c r="BH35">
+        <v>1400</v>
       </c>
     </row>
-    <row r="36" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B36" s="4">
         <v>2040</v>
       </c>
@@ -4837,7 +5645,7 @@
         <v>1560.0345603868079</v>
       </c>
       <c r="L36" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4457.2416011051655</v>
       </c>
       <c r="N36" s="4">
@@ -4875,7 +5683,7 @@
         <v>1695.6897395508784</v>
       </c>
       <c r="X36" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4844.8278272882244</v>
       </c>
       <c r="Z36" s="4">
@@ -4913,7 +5721,7 @@
         <v>2097.2123223235426</v>
       </c>
       <c r="AJ36" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>5992.0352066386931</v>
       </c>
       <c r="AL36" s="4">
@@ -4951,11 +5759,47 @@
         <v>1582.6437569141528</v>
       </c>
       <c r="AV36" s="12">
+        <f t="shared" si="37"/>
+        <v>4521.8393054690087</v>
+      </c>
+      <c r="AX36" s="4">
+        <v>2040</v>
+      </c>
+      <c r="AY36" s="27">
+        <f t="shared" si="28"/>
+        <v>36.6633225</v>
+      </c>
+      <c r="AZ36" s="27">
+        <f t="shared" si="29"/>
+        <v>122.21107500000001</v>
+      </c>
+      <c r="BA36" s="27">
+        <f t="shared" si="30"/>
+        <v>85.547752500000001</v>
+      </c>
+      <c r="BB36">
+        <v>244.42215000000002</v>
+      </c>
+      <c r="BD36" s="4">
+        <v>2040</v>
+      </c>
+      <c r="BE36" s="27">
         <f t="shared" si="31"/>
-        <v>4521.8393054690087</v>
+        <v>220.5</v>
+      </c>
+      <c r="BF36" s="27">
+        <f t="shared" si="32"/>
+        <v>735</v>
+      </c>
+      <c r="BG36" s="27">
+        <f t="shared" si="33"/>
+        <v>514.5</v>
+      </c>
+      <c r="BH36">
+        <v>1470</v>
       </c>
     </row>
-    <row r="37" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B37" s="4">
         <v>2041</v>
       </c>
@@ -4991,7 +5835,7 @@
         <v>1574.074871430289</v>
       </c>
       <c r="L37" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4497.3567755151116</v>
       </c>
       <c r="N37" s="4">
@@ -5029,7 +5873,7 @@
         <v>1710.9509472068362</v>
       </c>
       <c r="X37" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4888.4312777338182</v>
       </c>
       <c r="Z37" s="4">
@@ -5067,7 +5911,7 @@
         <v>2116.0872332244539</v>
       </c>
       <c r="AJ37" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>6045.9635234984407</v>
       </c>
       <c r="AL37" s="4">
@@ -5105,11 +5949,47 @@
         <v>1596.8875507263801</v>
       </c>
       <c r="AV37" s="12">
+        <f t="shared" si="37"/>
+        <v>4562.5358592182292</v>
+      </c>
+      <c r="AX37" s="4">
+        <v>2041</v>
+      </c>
+      <c r="AY37" s="27">
+        <f t="shared" si="28"/>
+        <v>38.409195000000004</v>
+      </c>
+      <c r="AZ37" s="27">
+        <f t="shared" si="29"/>
+        <v>128.03065000000001</v>
+      </c>
+      <c r="BA37" s="27">
+        <f t="shared" si="30"/>
+        <v>89.621454999999997</v>
+      </c>
+      <c r="BB37">
+        <v>256.06130000000002</v>
+      </c>
+      <c r="BD37" s="4">
+        <v>2041</v>
+      </c>
+      <c r="BE37" s="27">
         <f t="shared" si="31"/>
-        <v>4562.5358592182292</v>
+        <v>231</v>
+      </c>
+      <c r="BF37" s="27">
+        <f t="shared" si="32"/>
+        <v>770</v>
+      </c>
+      <c r="BG37" s="27">
+        <f t="shared" si="33"/>
+        <v>539</v>
+      </c>
+      <c r="BH37">
+        <v>1540</v>
       </c>
     </row>
-    <row r="38" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B38" s="4">
         <v>2042</v>
       </c>
@@ -5145,7 +6025,7 @@
         <v>1588.2415452731614</v>
       </c>
       <c r="L38" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4537.8329864947473</v>
       </c>
       <c r="N38" s="4">
@@ -5183,7 +6063,7 @@
         <v>1726.3495057316975</v>
       </c>
       <c r="X38" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4932.4271592334217</v>
       </c>
       <c r="Z38" s="4">
@@ -5221,7 +6101,7 @@
         <v>2135.1320183234739</v>
       </c>
       <c r="AJ38" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>6100.377195209926</v>
       </c>
       <c r="AL38" s="4">
@@ -5259,11 +6139,47 @@
         <v>1611.2595386829173</v>
       </c>
       <c r="AV38" s="12">
+        <f t="shared" si="37"/>
+        <v>4603.5986819511927</v>
+      </c>
+      <c r="AX38" s="4">
+        <v>2042</v>
+      </c>
+      <c r="AY38" s="27">
+        <f t="shared" si="28"/>
+        <v>40.155067500000008</v>
+      </c>
+      <c r="AZ38" s="27">
+        <f t="shared" si="29"/>
+        <v>133.85022500000002</v>
+      </c>
+      <c r="BA38" s="27">
+        <f t="shared" si="30"/>
+        <v>93.695157500000008</v>
+      </c>
+      <c r="BB38">
+        <v>267.70045000000005</v>
+      </c>
+      <c r="BD38" s="4">
+        <v>2042</v>
+      </c>
+      <c r="BE38" s="27">
         <f t="shared" si="31"/>
-        <v>4603.5986819511927</v>
+        <v>241.5</v>
+      </c>
+      <c r="BF38" s="27">
+        <f t="shared" si="32"/>
+        <v>805</v>
+      </c>
+      <c r="BG38" s="27">
+        <f t="shared" si="33"/>
+        <v>563.5</v>
+      </c>
+      <c r="BH38">
+        <v>1610</v>
       </c>
     </row>
-    <row r="39" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B39" s="4">
         <v>2043</v>
       </c>
@@ -5299,7 +6215,7 @@
         <v>1602.5357191806199</v>
       </c>
       <c r="L39" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4578.6734833731998</v>
       </c>
       <c r="N39" s="4">
@@ -5337,7 +6253,7 @@
         <v>1741.8866512832826</v>
       </c>
       <c r="X39" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>4976.8190036665219</v>
       </c>
       <c r="Z39" s="4">
@@ -5375,7 +6291,7 @@
         <v>2154.3482064883851</v>
       </c>
       <c r="AJ39" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>6155.2805899668147</v>
       </c>
       <c r="AL39" s="4">
@@ -5413,11 +6329,47 @@
         <v>1625.7608745310636</v>
       </c>
       <c r="AV39" s="12">
+        <f t="shared" si="37"/>
+        <v>4645.031070088753</v>
+      </c>
+      <c r="AX39" s="4">
+        <v>2043</v>
+      </c>
+      <c r="AY39" s="27">
+        <f t="shared" si="28"/>
+        <v>41.900939999999999</v>
+      </c>
+      <c r="AZ39" s="27">
+        <f t="shared" si="29"/>
+        <v>139.66980000000001</v>
+      </c>
+      <c r="BA39" s="27">
+        <f t="shared" si="30"/>
+        <v>97.768860000000004</v>
+      </c>
+      <c r="BB39">
+        <v>279.33960000000002</v>
+      </c>
+      <c r="BD39" s="4">
+        <v>2043</v>
+      </c>
+      <c r="BE39" s="27">
         <f t="shared" si="31"/>
-        <v>4645.031070088753</v>
+        <v>252</v>
+      </c>
+      <c r="BF39" s="27">
+        <f t="shared" si="32"/>
+        <v>840</v>
+      </c>
+      <c r="BG39" s="27">
+        <f t="shared" si="33"/>
+        <v>588</v>
+      </c>
+      <c r="BH39">
+        <v>1680</v>
       </c>
     </row>
-    <row r="40" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B40" s="4">
         <v>2044</v>
       </c>
@@ -5453,7 +6405,7 @@
         <v>1616.9585406532453</v>
       </c>
       <c r="L40" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4619.8815447235584</v>
       </c>
       <c r="N40" s="4">
@@ -5491,7 +6443,7 @@
         <v>1757.563631144832</v>
       </c>
       <c r="X40" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>5021.6103746995204</v>
       </c>
       <c r="Z40" s="4">
@@ -5529,7 +6481,7 @@
         <v>2173.73734034678</v>
       </c>
       <c r="AJ40" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>6210.6781152765152</v>
       </c>
       <c r="AL40" s="4">
@@ -5567,11 +6519,47 @@
         <v>1640.392722401843</v>
       </c>
       <c r="AV40" s="12">
+        <f t="shared" si="37"/>
+        <v>4686.8363497195514</v>
+      </c>
+      <c r="AX40" s="4">
+        <v>2044</v>
+      </c>
+      <c r="AY40" s="27">
+        <f t="shared" si="28"/>
+        <v>43.646812499999996</v>
+      </c>
+      <c r="AZ40" s="27">
+        <f t="shared" si="29"/>
+        <v>145.489375</v>
+      </c>
+      <c r="BA40" s="27">
+        <f t="shared" si="30"/>
+        <v>101.84256249999999</v>
+      </c>
+      <c r="BB40">
+        <v>290.97874999999999</v>
+      </c>
+      <c r="BD40" s="4">
+        <v>2044</v>
+      </c>
+      <c r="BE40" s="27">
         <f t="shared" si="31"/>
-        <v>4686.8363497195514</v>
+        <v>262.5</v>
+      </c>
+      <c r="BF40" s="27">
+        <f t="shared" si="32"/>
+        <v>875</v>
+      </c>
+      <c r="BG40" s="27">
+        <f t="shared" si="33"/>
+        <v>612.5</v>
+      </c>
+      <c r="BH40">
+        <v>1750</v>
       </c>
     </row>
-    <row r="41" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B41" s="4">
         <v>2045</v>
       </c>
@@ -5607,7 +6595,7 @@
         <v>1631.5111675191242</v>
       </c>
       <c r="L41" s="12">
-        <f t="shared" si="28"/>
+        <f t="shared" si="34"/>
         <v>4661.4604786260697</v>
       </c>
       <c r="N41" s="4">
@@ -5645,7 +6633,7 @@
         <v>1773.3817038251354</v>
       </c>
       <c r="X41" s="12">
-        <f t="shared" si="29"/>
+        <f t="shared" si="35"/>
         <v>5066.8048680718157</v>
       </c>
       <c r="Z41" s="4">
@@ -5683,7 +6671,7 @@
         <v>2193.3009764099006</v>
       </c>
       <c r="AJ41" s="12">
-        <f t="shared" si="30"/>
+        <f t="shared" si="36"/>
         <v>6266.5742183140028</v>
       </c>
       <c r="AL41" s="4">
@@ -5721,11 +6709,47 @@
         <v>1655.1562569034593</v>
       </c>
       <c r="AV41" s="12">
+        <f t="shared" si="37"/>
+        <v>4729.0178768670266</v>
+      </c>
+      <c r="AX41" s="4">
+        <v>2045</v>
+      </c>
+      <c r="AY41" s="27">
+        <f t="shared" si="28"/>
+        <v>45.392684999999993</v>
+      </c>
+      <c r="AZ41" s="27">
+        <f t="shared" si="29"/>
+        <v>151.30894999999998</v>
+      </c>
+      <c r="BA41" s="27">
+        <f t="shared" si="30"/>
+        <v>105.91626499999998</v>
+      </c>
+      <c r="BB41">
+        <v>302.61789999999996</v>
+      </c>
+      <c r="BD41" s="4">
+        <v>2045</v>
+      </c>
+      <c r="BE41" s="27">
         <f t="shared" si="31"/>
-        <v>4729.0178768670266</v>
+        <v>273</v>
+      </c>
+      <c r="BF41" s="27">
+        <f t="shared" si="32"/>
+        <v>910</v>
+      </c>
+      <c r="BG41" s="27">
+        <f t="shared" si="33"/>
+        <v>637</v>
+      </c>
+      <c r="BH41">
+        <v>1820</v>
       </c>
     </row>
-    <row r="44" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
         <v>3</v>
       </c>
@@ -5742,23 +6766,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="C45" s="42" t="s">
+    <row r="45" spans="2:60" x14ac:dyDescent="0.35">
+      <c r="C45" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
       <c r="F45" s="2"/>
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
       <c r="K45" s="2"/>
       <c r="L45" s="4"/>
       <c r="O45" s="4"/>
     </row>
-    <row r="46" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>4</v>
       </c>
@@ -5795,7 +6819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
@@ -5839,7 +6863,7 @@
         <v>3.06</v>
       </c>
     </row>
-    <row r="48" spans="2:48" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:60" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
@@ -5990,11 +7014,11 @@
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="C53" s="42" t="s">
+      <c r="C53" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
       <c r="G53" s="38" t="s">
         <v>137</v>
       </c>
@@ -6139,7 +7163,7 @@
         <v>1</v>
       </c>
       <c r="Z55" s="8">
-        <f t="shared" ref="Z55:Z97" si="32">AG55*AH55*1000/1000000</f>
+        <f t="shared" ref="Z55:Z97" si="38">AG55*AH55*1000/1000000</f>
         <v>39.666780000000003</v>
       </c>
       <c r="AB55" s="39">
@@ -6158,7 +7182,7 @@
         <v>12963</v>
       </c>
       <c r="AH55" s="6">
-        <f t="shared" ref="AH55:AH74" si="33">IF(EXACT(AF55,$R$47),$S$47,IF(EXACT(AF55,$R$48),$S$48,IF(EXACT(AF55,$R$49),$S$49,0)))</f>
+        <f t="shared" ref="AH55:AH74" si="39">IF(EXACT(AF55,$R$47),$S$47,IF(EXACT(AF55,$R$48),$S$48,IF(EXACT(AF55,$R$49),$S$49,0)))</f>
         <v>3.06</v>
       </c>
       <c r="AJ55" s="32">
@@ -6236,7 +7260,7 @@
         <v>2</v>
       </c>
       <c r="Z56" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>23.617080000000001</v>
       </c>
       <c r="AB56" s="39">
@@ -6255,7 +7279,7 @@
         <v>7718</v>
       </c>
       <c r="AH56" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ56" s="32">
@@ -6333,7 +7357,7 @@
         <v>3</v>
       </c>
       <c r="Z57" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>28.115279999999998</v>
       </c>
       <c r="AB57" s="39">
@@ -6352,7 +7376,7 @@
         <v>9188</v>
       </c>
       <c r="AH57" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ57" s="32">
@@ -6430,7 +7454,7 @@
         <v>4</v>
       </c>
       <c r="Z58" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>21.77496</v>
       </c>
       <c r="AB58" s="39">
@@ -6449,7 +7473,7 @@
         <v>7116</v>
       </c>
       <c r="AH58" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ58" s="32">
@@ -6527,7 +7551,7 @@
         <v>5</v>
       </c>
       <c r="Z59" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>23.94144</v>
       </c>
       <c r="AB59" s="39">
@@ -6546,7 +7570,7 @@
         <v>7824</v>
       </c>
       <c r="AH59" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ59" s="32">
@@ -6624,7 +7648,7 @@
         <v>6</v>
       </c>
       <c r="Z60" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>38.22552000000001</v>
       </c>
       <c r="AB60" s="39">
@@ -6643,7 +7667,7 @@
         <v>12492</v>
       </c>
       <c r="AH60" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ60" s="32">
@@ -6721,7 +7745,7 @@
         <v>7</v>
       </c>
       <c r="Z61" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>1.6982999999999999</v>
       </c>
       <c r="AB61" s="39">
@@ -6740,7 +7764,7 @@
         <v>555</v>
       </c>
       <c r="AH61" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ61" s="32">
@@ -6818,7 +7842,7 @@
         <v>8</v>
       </c>
       <c r="Z62" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>36.677160000000001</v>
       </c>
       <c r="AB62" s="39">
@@ -6837,7 +7861,7 @@
         <v>11986</v>
       </c>
       <c r="AH62" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ62" s="32">
@@ -6915,7 +7939,7 @@
         <v>9</v>
       </c>
       <c r="Z63" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>23.494679999999999</v>
       </c>
       <c r="AB63" s="39">
@@ -6934,7 +7958,7 @@
         <v>7678</v>
       </c>
       <c r="AH63" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ63" s="32">
@@ -7012,7 +8036,7 @@
         <v>10</v>
       </c>
       <c r="Z64" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>31.606739999999999</v>
       </c>
       <c r="AB64" s="39">
@@ -7031,7 +8055,7 @@
         <v>10329</v>
       </c>
       <c r="AH64" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ64" s="32">
@@ -7109,7 +8133,7 @@
         <v>11</v>
       </c>
       <c r="Z65" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>38.996639999999999</v>
       </c>
       <c r="AB65" s="39">
@@ -7128,7 +8152,7 @@
         <v>12744</v>
       </c>
       <c r="AH65" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ65" s="32">
@@ -7206,7 +8230,7 @@
         <v>12</v>
       </c>
       <c r="Z66" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>35.954999999999998</v>
       </c>
       <c r="AB66" s="39">
@@ -7225,7 +8249,7 @@
         <v>11750</v>
       </c>
       <c r="AH66" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ66" s="32">
@@ -7303,7 +8327,7 @@
         <v>13</v>
       </c>
       <c r="Z67" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>26.289359999999999</v>
       </c>
       <c r="AB67" s="39">
@@ -7322,7 +8346,7 @@
         <v>12171</v>
       </c>
       <c r="AH67" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>2.16</v>
       </c>
       <c r="AJ67" s="32">
@@ -7400,7 +8424,7 @@
         <v>14</v>
       </c>
       <c r="Z68" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>34.819740000000003</v>
       </c>
       <c r="AB68" s="39">
@@ -7419,7 +8443,7 @@
         <v>11379</v>
       </c>
       <c r="AH68" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ68" s="32">
@@ -7497,7 +8521,7 @@
         <v>15</v>
       </c>
       <c r="Z69" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>37.647179999999999</v>
       </c>
       <c r="AB69" s="39">
@@ -7516,7 +8540,7 @@
         <v>12303</v>
       </c>
       <c r="AH69" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ69" s="32">
@@ -7594,7 +8618,7 @@
         <v>16</v>
       </c>
       <c r="Z70" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>25.404119999999999</v>
       </c>
       <c r="AB70" s="39">
@@ -7613,7 +8637,7 @@
         <v>8302</v>
       </c>
       <c r="AH70" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ70" s="32">
@@ -7691,7 +8715,7 @@
         <v>17</v>
       </c>
       <c r="Z71" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>23.453280000000003</v>
       </c>
       <c r="AB71" s="39">
@@ -7710,7 +8734,7 @@
         <v>10858</v>
       </c>
       <c r="AH71" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>2.16</v>
       </c>
       <c r="AJ71" s="32">
@@ -7788,7 +8812,7 @@
         <v>18</v>
       </c>
       <c r="Z72" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>23.647680000000001</v>
       </c>
       <c r="AB72" s="39">
@@ -7807,7 +8831,7 @@
         <v>10948</v>
       </c>
       <c r="AH72" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>2.16</v>
       </c>
       <c r="AJ72" s="32">
@@ -7885,7 +8909,7 @@
         <v>19</v>
       </c>
       <c r="Z73" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>223.99503999999999</v>
       </c>
       <c r="AB73" s="39">
@@ -7904,7 +8928,7 @@
         <v>17834</v>
       </c>
       <c r="AH73" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>12.56</v>
       </c>
       <c r="AJ73" s="32">
@@ -7982,7 +9006,7 @@
         <v>20</v>
       </c>
       <c r="Z74" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>36.931139999999999</v>
       </c>
       <c r="AB74" s="39">
@@ -8001,7 +9025,7 @@
         <v>12069</v>
       </c>
       <c r="AH74" s="6">
-        <f t="shared" si="33"/>
+        <f t="shared" si="39"/>
         <v>3.06</v>
       </c>
       <c r="AJ74" s="32">
@@ -8043,14 +9067,14 @@
         <v>21</v>
       </c>
       <c r="H75" s="6">
-        <f t="shared" ref="H75:H94" si="34">$L$4*$G106*H$53</f>
+        <f t="shared" ref="H75:H94" si="40">$L$4*$G106*H$53</f>
         <v>14.05</v>
       </c>
       <c r="J75" s="35">
         <v>21</v>
       </c>
       <c r="K75" s="6">
-        <f t="shared" ref="K75:K94" si="35">$L$4*$G106*K$53</f>
+        <f t="shared" ref="K75:K94" si="41">$L$4*$G106*K$53</f>
         <v>19.669999999999998</v>
       </c>
       <c r="M75" s="35">
@@ -8064,7 +9088,7 @@
         <v>21</v>
       </c>
       <c r="Q75" s="6">
-        <f t="shared" ref="Q75:Q94" si="36">$L$4*$G106*Q$53</f>
+        <f t="shared" ref="Q75:Q94" si="42">$L$4*$G106*Q$53</f>
         <v>19.669999999999998</v>
       </c>
       <c r="S75" s="32">
@@ -8083,7 +9107,7 @@
         <v>21</v>
       </c>
       <c r="Z75" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB75" s="39">
@@ -8144,28 +9168,28 @@
         <v>22</v>
       </c>
       <c r="H76" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>12.5</v>
       </c>
       <c r="J76" s="35">
         <v>22</v>
       </c>
       <c r="K76" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>17.5</v>
       </c>
       <c r="M76" s="35">
         <v>22</v>
       </c>
       <c r="N76" s="6">
-        <f t="shared" ref="N76:N94" si="37">$L$4*$G107</f>
+        <f t="shared" ref="N76:N94" si="43">$L$4*$G107</f>
         <v>25</v>
       </c>
       <c r="P76" s="35">
         <v>22</v>
       </c>
       <c r="Q76" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>17.5</v>
       </c>
       <c r="S76" s="32">
@@ -8184,14 +9208,14 @@
         <v>22</v>
       </c>
       <c r="Z76" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB76" s="39">
         <v>22</v>
       </c>
       <c r="AC76" s="40">
-        <f t="shared" ref="AC76:AC94" si="38">Q76</f>
+        <f t="shared" ref="AC76:AC94" si="44">Q76</f>
         <v>17.5</v>
       </c>
       <c r="AE76" s="32">
@@ -8245,28 +9269,28 @@
         <v>23</v>
       </c>
       <c r="H77" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>35</v>
       </c>
       <c r="J77" s="35">
         <v>23</v>
       </c>
       <c r="K77" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>49</v>
       </c>
       <c r="M77" s="35">
         <v>23</v>
       </c>
       <c r="N77" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>70</v>
       </c>
       <c r="P77" s="35">
         <v>23</v>
       </c>
       <c r="Q77" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>49</v>
       </c>
       <c r="S77" s="32">
@@ -8285,14 +9309,14 @@
         <v>23</v>
       </c>
       <c r="Z77" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB77" s="39">
         <v>23</v>
       </c>
       <c r="AC77" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>49</v>
       </c>
       <c r="AE77" s="32">
@@ -8346,28 +9370,28 @@
         <v>24</v>
       </c>
       <c r="H78" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>15.3</v>
       </c>
       <c r="J78" s="35">
         <v>24</v>
       </c>
       <c r="K78" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>21.419999999999998</v>
       </c>
       <c r="M78" s="35">
         <v>24</v>
       </c>
       <c r="N78" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>30.6</v>
       </c>
       <c r="P78" s="35">
         <v>24</v>
       </c>
       <c r="Q78" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>21.419999999999998</v>
       </c>
       <c r="S78" s="32">
@@ -8386,14 +9410,14 @@
         <v>24</v>
       </c>
       <c r="Z78" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB78" s="39">
         <v>24</v>
       </c>
       <c r="AC78" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>21.419999999999998</v>
       </c>
       <c r="AE78" s="32">
@@ -8447,28 +9471,28 @@
         <v>25</v>
       </c>
       <c r="H79" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J79" s="35">
         <v>25</v>
       </c>
       <c r="K79" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M79" s="35">
         <v>25</v>
       </c>
       <c r="N79" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P79" s="35">
         <v>25</v>
       </c>
       <c r="Q79" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S79" s="32">
@@ -8487,14 +9511,14 @@
         <v>25</v>
       </c>
       <c r="Z79" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB79" s="39">
         <v>25</v>
       </c>
       <c r="AC79" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE79" s="32">
@@ -8548,28 +9572,28 @@
         <v>26</v>
       </c>
       <c r="H80" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J80" s="35">
         <v>26</v>
       </c>
       <c r="K80" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M80" s="35">
         <v>26</v>
       </c>
       <c r="N80" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P80" s="35">
         <v>26</v>
       </c>
       <c r="Q80" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S80" s="32">
@@ -8588,14 +9612,14 @@
         <v>26</v>
       </c>
       <c r="Z80" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB80" s="39">
         <v>26</v>
       </c>
       <c r="AC80" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE80" s="32">
@@ -8649,28 +9673,28 @@
         <v>27</v>
       </c>
       <c r="H81" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J81" s="35">
         <v>27</v>
       </c>
       <c r="K81" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M81" s="35">
         <v>27</v>
       </c>
       <c r="N81" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P81" s="35">
         <v>27</v>
       </c>
       <c r="Q81" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S81" s="32">
@@ -8689,14 +9713,14 @@
         <v>27</v>
       </c>
       <c r="Z81" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB81" s="39">
         <v>27</v>
       </c>
       <c r="AC81" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE81" s="32">
@@ -8750,28 +9774,28 @@
         <v>28</v>
       </c>
       <c r="H82" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>26.1</v>
       </c>
       <c r="J82" s="35">
         <v>28</v>
       </c>
       <c r="K82" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>36.54</v>
       </c>
       <c r="M82" s="35">
         <v>28</v>
       </c>
       <c r="N82" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>52.2</v>
       </c>
       <c r="P82" s="35">
         <v>28</v>
       </c>
       <c r="Q82" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>36.54</v>
       </c>
       <c r="S82" s="32">
@@ -8790,14 +9814,14 @@
         <v>28</v>
       </c>
       <c r="Z82" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB82" s="39">
         <v>28</v>
       </c>
       <c r="AC82" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>36.54</v>
       </c>
       <c r="AE82" s="32">
@@ -8851,28 +9875,28 @@
         <v>29</v>
       </c>
       <c r="H83" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J83" s="35">
         <v>29</v>
       </c>
       <c r="K83" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M83" s="35">
         <v>29</v>
       </c>
       <c r="N83" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P83" s="35">
         <v>29</v>
       </c>
       <c r="Q83" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S83" s="32">
@@ -8891,14 +9915,14 @@
         <v>29</v>
       </c>
       <c r="Z83" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB83" s="39">
         <v>29</v>
       </c>
       <c r="AC83" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE83" s="32">
@@ -8952,28 +9976,28 @@
         <v>30</v>
       </c>
       <c r="H84" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>10.1</v>
       </c>
       <c r="J84" s="35">
         <v>30</v>
       </c>
       <c r="K84" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>14.139999999999999</v>
       </c>
       <c r="M84" s="35">
         <v>30</v>
       </c>
       <c r="N84" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>20.2</v>
       </c>
       <c r="P84" s="35">
         <v>30</v>
       </c>
       <c r="Q84" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>14.139999999999999</v>
       </c>
       <c r="S84" s="32">
@@ -8992,14 +10016,14 @@
         <v>30</v>
       </c>
       <c r="Z84" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB84" s="39">
         <v>30</v>
       </c>
       <c r="AC84" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>14.139999999999999</v>
       </c>
       <c r="AE84" s="32">
@@ -9053,28 +10077,28 @@
         <v>31</v>
       </c>
       <c r="H85" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>35</v>
       </c>
       <c r="J85" s="35">
         <v>31</v>
       </c>
       <c r="K85" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>49</v>
       </c>
       <c r="M85" s="35">
         <v>31</v>
       </c>
       <c r="N85" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>70</v>
       </c>
       <c r="P85" s="35">
         <v>31</v>
       </c>
       <c r="Q85" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>49</v>
       </c>
       <c r="S85" s="32">
@@ -9093,14 +10117,14 @@
         <v>31</v>
       </c>
       <c r="Z85" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB85" s="39">
         <v>31</v>
       </c>
       <c r="AC85" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>49</v>
       </c>
       <c r="AE85" s="32">
@@ -9154,28 +10178,28 @@
         <v>32</v>
       </c>
       <c r="H86" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5.25</v>
       </c>
       <c r="J86" s="35">
         <v>32</v>
       </c>
       <c r="K86" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7.35</v>
       </c>
       <c r="M86" s="35">
         <v>32</v>
       </c>
       <c r="N86" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.5</v>
       </c>
       <c r="P86" s="35">
         <v>32</v>
       </c>
       <c r="Q86" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7.35</v>
       </c>
       <c r="S86" s="32">
@@ -9194,14 +10218,14 @@
         <v>32</v>
       </c>
       <c r="Z86" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB86" s="39">
         <v>32</v>
       </c>
       <c r="AC86" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7.35</v>
       </c>
       <c r="AE86" s="32">
@@ -9255,28 +10279,28 @@
         <v>33</v>
       </c>
       <c r="H87" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J87" s="35">
         <v>33</v>
       </c>
       <c r="K87" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M87" s="35">
         <v>33</v>
       </c>
       <c r="N87" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P87" s="35">
         <v>33</v>
       </c>
       <c r="Q87" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S87" s="32">
@@ -9295,14 +10319,14 @@
         <v>33</v>
       </c>
       <c r="Z87" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB87" s="39">
         <v>33</v>
       </c>
       <c r="AC87" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE87" s="32">
@@ -9356,28 +10380,28 @@
         <v>34</v>
       </c>
       <c r="H88" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J88" s="35">
         <v>34</v>
       </c>
       <c r="K88" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M88" s="35">
         <v>34</v>
       </c>
       <c r="N88" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P88" s="35">
         <v>34</v>
       </c>
       <c r="Q88" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S88" s="32">
@@ -9396,14 +10420,14 @@
         <v>34</v>
       </c>
       <c r="Z88" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB88" s="39">
         <v>34</v>
       </c>
       <c r="AC88" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE88" s="32">
@@ -9457,28 +10481,28 @@
         <v>35</v>
       </c>
       <c r="H89" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J89" s="35">
         <v>35</v>
       </c>
       <c r="K89" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M89" s="35">
         <v>35</v>
       </c>
       <c r="N89" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P89" s="35">
         <v>35</v>
       </c>
       <c r="Q89" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S89" s="32">
@@ -9497,14 +10521,14 @@
         <v>35</v>
       </c>
       <c r="Z89" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB89" s="39">
         <v>35</v>
       </c>
       <c r="AC89" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE89" s="32">
@@ -9558,28 +10582,28 @@
         <v>36</v>
       </c>
       <c r="H90" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J90" s="35">
         <v>36</v>
       </c>
       <c r="K90" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M90" s="35">
         <v>36</v>
       </c>
       <c r="N90" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P90" s="35">
         <v>36</v>
       </c>
       <c r="Q90" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S90" s="32">
@@ -9598,14 +10622,14 @@
         <v>36</v>
       </c>
       <c r="Z90" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB90" s="39">
         <v>36</v>
       </c>
       <c r="AC90" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE90" s="32">
@@ -9659,28 +10683,28 @@
         <v>37</v>
       </c>
       <c r="H91" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5.05</v>
       </c>
       <c r="J91" s="35">
         <v>37</v>
       </c>
       <c r="K91" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="M91" s="35">
         <v>37</v>
       </c>
       <c r="N91" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.1</v>
       </c>
       <c r="P91" s="35">
         <v>37</v>
       </c>
       <c r="Q91" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="S91" s="32">
@@ -9699,14 +10723,14 @@
         <v>37</v>
       </c>
       <c r="Z91" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB91" s="39">
         <v>37</v>
       </c>
       <c r="AC91" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="AE91" s="32">
@@ -9760,28 +10784,28 @@
         <v>38</v>
       </c>
       <c r="H92" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5.05</v>
       </c>
       <c r="J92" s="35">
         <v>38</v>
       </c>
       <c r="K92" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="M92" s="35">
         <v>38</v>
       </c>
       <c r="N92" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.1</v>
       </c>
       <c r="P92" s="35">
         <v>38</v>
       </c>
       <c r="Q92" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="S92" s="32">
@@ -9800,14 +10824,14 @@
         <v>38</v>
       </c>
       <c r="Z92" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB92" s="39">
         <v>38</v>
       </c>
       <c r="AC92" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7.0699999999999994</v>
       </c>
       <c r="AE92" s="32">
@@ -9861,28 +10885,28 @@
         <v>39</v>
       </c>
       <c r="H93" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="J93" s="35">
         <v>39</v>
       </c>
       <c r="K93" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>7</v>
       </c>
       <c r="M93" s="35">
         <v>39</v>
       </c>
       <c r="N93" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10</v>
       </c>
       <c r="P93" s="35">
         <v>39</v>
       </c>
       <c r="Q93" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7</v>
       </c>
       <c r="S93" s="32">
@@ -9901,14 +10925,14 @@
         <v>39</v>
       </c>
       <c r="Z93" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB93" s="39">
         <v>39</v>
       </c>
       <c r="AC93" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>7</v>
       </c>
       <c r="AE93" s="32">
@@ -9962,28 +10986,28 @@
         <v>40</v>
       </c>
       <c r="H94" s="6">
-        <f t="shared" si="34"/>
+        <f t="shared" si="40"/>
         <v>6</v>
       </c>
       <c r="J94" s="35">
         <v>40</v>
       </c>
       <c r="K94" s="6">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="M94" s="35">
         <v>40</v>
       </c>
       <c r="N94" s="6">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>12</v>
       </c>
       <c r="P94" s="35">
         <v>40</v>
       </c>
       <c r="Q94" s="6">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="S94" s="32">
@@ -10002,14 +11026,14 @@
         <v>40</v>
       </c>
       <c r="Z94" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB94" s="39">
         <v>40</v>
       </c>
       <c r="AC94" s="40">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="AE94" s="32">
@@ -10099,7 +11123,7 @@
         <v>41</v>
       </c>
       <c r="Z95" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB95" s="39">
@@ -10195,7 +11219,7 @@
         <v>42</v>
       </c>
       <c r="Z96" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB96" s="39">
@@ -10291,7 +11315,7 @@
         <v>43</v>
       </c>
       <c r="Z97" s="8">
-        <f t="shared" si="32"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="AB97" s="39">
@@ -10329,27 +11353,27 @@
       </c>
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D103" s="43" t="s">
+      <c r="D103" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="E103" s="45" t="s">
+      <c r="E103" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="F103" s="45"/>
-      <c r="G103" s="45" t="s">
+      <c r="F103" s="49"/>
+      <c r="G103" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="H103" s="54"/>
+      <c r="H103" s="56"/>
       <c r="N103" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D104" s="44"/>
-      <c r="E104" s="46"/>
-      <c r="F104" s="46"/>
-      <c r="G104" s="46"/>
-      <c r="H104" s="55"/>
+      <c r="D104" s="48"/>
+      <c r="E104" s="50"/>
+      <c r="F104" s="50"/>
+      <c r="G104" s="50"/>
+      <c r="H104" s="57"/>
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
@@ -10363,14 +11387,14 @@
       <c r="D106" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E106" s="47">
+      <c r="E106" s="51">
         <v>72154</v>
       </c>
-      <c r="F106" s="47"/>
-      <c r="G106" s="56">
+      <c r="F106" s="51"/>
+      <c r="G106" s="58">
         <v>28.1</v>
       </c>
-      <c r="H106" s="57"/>
+      <c r="H106" s="59"/>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C107" s="18">
@@ -10379,14 +11403,14 @@
       <c r="D107" s="19">
         <v>0.31</v>
       </c>
-      <c r="E107" s="48">
+      <c r="E107" s="52">
         <v>67811</v>
       </c>
-      <c r="F107" s="48"/>
-      <c r="G107" s="49">
+      <c r="F107" s="52"/>
+      <c r="G107" s="53">
         <v>25</v>
       </c>
-      <c r="H107" s="50"/>
+      <c r="H107" s="54"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C108" s="18">
@@ -10395,14 +11419,14 @@
       <c r="D108" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E108" s="48">
+      <c r="E108" s="52">
         <v>187455</v>
       </c>
-      <c r="F108" s="48"/>
-      <c r="G108" s="49">
+      <c r="F108" s="52"/>
+      <c r="G108" s="53">
         <v>70</v>
       </c>
-      <c r="H108" s="50"/>
+      <c r="H108" s="54"/>
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C109" s="18">
@@ -10411,14 +11435,14 @@
       <c r="D109" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E109" s="48">
+      <c r="E109" s="52">
         <v>63266</v>
       </c>
-      <c r="F109" s="48"/>
-      <c r="G109" s="49">
+      <c r="F109" s="52"/>
+      <c r="G109" s="53">
         <v>30.6</v>
       </c>
-      <c r="H109" s="50"/>
+      <c r="H109" s="54"/>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -10427,14 +11451,14 @@
       <c r="D110" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E110" s="48">
+      <c r="E110" s="52">
         <v>26553</v>
       </c>
-      <c r="F110" s="48"/>
-      <c r="G110" s="49">
+      <c r="F110" s="52"/>
+      <c r="G110" s="53">
         <v>10</v>
       </c>
-      <c r="H110" s="50"/>
+      <c r="H110" s="54"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -10443,14 +11467,14 @@
       <c r="D111" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E111" s="48">
+      <c r="E111" s="52">
         <v>24949</v>
       </c>
-      <c r="F111" s="48"/>
-      <c r="G111" s="49">
+      <c r="F111" s="52"/>
+      <c r="G111" s="53">
         <v>10</v>
       </c>
-      <c r="H111" s="50"/>
+      <c r="H111" s="54"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -10459,14 +11483,14 @@
       <c r="D112" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E112" s="48">
+      <c r="E112" s="52">
         <v>22870</v>
       </c>
-      <c r="F112" s="48"/>
-      <c r="G112" s="49">
+      <c r="F112" s="52"/>
+      <c r="G112" s="53">
         <v>10</v>
       </c>
-      <c r="H112" s="50"/>
+      <c r="H112" s="54"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -10475,14 +11499,14 @@
       <c r="D113" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E113" s="48">
+      <c r="E113" s="52">
         <v>139836</v>
       </c>
-      <c r="F113" s="48"/>
-      <c r="G113" s="49">
+      <c r="F113" s="52"/>
+      <c r="G113" s="53">
         <v>52.2</v>
       </c>
-      <c r="H113" s="50"/>
+      <c r="H113" s="54"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -10491,14 +11515,14 @@
       <c r="D114" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E114" s="48">
+      <c r="E114" s="52">
         <v>23515</v>
       </c>
-      <c r="F114" s="48"/>
-      <c r="G114" s="49">
+      <c r="F114" s="52"/>
+      <c r="G114" s="53">
         <v>10</v>
       </c>
-      <c r="H114" s="50"/>
+      <c r="H114" s="54"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -10507,14 +11531,14 @@
       <c r="D115" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E115" s="48">
+      <c r="E115" s="52">
         <v>49503</v>
       </c>
-      <c r="F115" s="48"/>
-      <c r="G115" s="49">
+      <c r="F115" s="52"/>
+      <c r="G115" s="53">
         <v>20.2</v>
       </c>
-      <c r="H115" s="50"/>
+      <c r="H115" s="54"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -10523,14 +11547,14 @@
       <c r="D116" s="19">
         <v>0.307</v>
       </c>
-      <c r="E116" s="48">
+      <c r="E116" s="52">
         <v>188420</v>
       </c>
-      <c r="F116" s="48"/>
-      <c r="G116" s="49">
+      <c r="F116" s="52"/>
+      <c r="G116" s="53">
         <v>70</v>
       </c>
-      <c r="H116" s="50"/>
+      <c r="H116" s="54"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -10539,14 +11563,14 @@
       <c r="D117" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E117" s="48">
+      <c r="E117" s="52">
         <v>26573</v>
       </c>
-      <c r="F117" s="48"/>
-      <c r="G117" s="49">
+      <c r="F117" s="52"/>
+      <c r="G117" s="53">
         <v>10.5</v>
       </c>
-      <c r="H117" s="50"/>
+      <c r="H117" s="54"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -10555,14 +11579,14 @@
       <c r="D118" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E118" s="48">
+      <c r="E118" s="52">
         <v>25253</v>
       </c>
-      <c r="F118" s="48"/>
-      <c r="G118" s="49">
+      <c r="F118" s="52"/>
+      <c r="G118" s="53">
         <v>10</v>
       </c>
-      <c r="H118" s="50"/>
+      <c r="H118" s="54"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -10571,14 +11595,14 @@
       <c r="D119" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E119" s="48">
+      <c r="E119" s="52">
         <v>17610</v>
       </c>
-      <c r="F119" s="48"/>
-      <c r="G119" s="49">
+      <c r="F119" s="52"/>
+      <c r="G119" s="53">
         <v>10</v>
       </c>
-      <c r="H119" s="50"/>
+      <c r="H119" s="54"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -10587,14 +11611,14 @@
       <c r="D120" s="19">
         <v>0.221</v>
       </c>
-      <c r="E120" s="48">
+      <c r="E120" s="52">
         <v>19372</v>
       </c>
-      <c r="F120" s="48"/>
-      <c r="G120" s="49">
+      <c r="F120" s="52"/>
+      <c r="G120" s="53">
         <v>10</v>
       </c>
-      <c r="H120" s="50"/>
+      <c r="H120" s="54"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -10603,14 +11627,14 @@
       <c r="D121" s="19">
         <v>0.216</v>
       </c>
-      <c r="E121" s="48">
+      <c r="E121" s="52">
         <v>18939</v>
       </c>
-      <c r="F121" s="48"/>
-      <c r="G121" s="49">
+      <c r="F121" s="52"/>
+      <c r="G121" s="53">
         <v>10</v>
       </c>
-      <c r="H121" s="50"/>
+      <c r="H121" s="54"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -10619,14 +11643,14 @@
       <c r="D122" s="19">
         <v>0.23</v>
       </c>
-      <c r="E122" s="48">
+      <c r="E122" s="52">
         <v>20382</v>
       </c>
-      <c r="F122" s="48"/>
-      <c r="G122" s="49">
+      <c r="F122" s="52"/>
+      <c r="G122" s="53">
         <v>10.1</v>
       </c>
-      <c r="H122" s="50"/>
+      <c r="H122" s="54"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -10635,14 +11659,14 @@
       <c r="D123" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E123" s="48">
+      <c r="E123" s="52">
         <v>19968</v>
       </c>
-      <c r="F123" s="48"/>
-      <c r="G123" s="49">
+      <c r="F123" s="52"/>
+      <c r="G123" s="53">
         <v>10.1</v>
       </c>
-      <c r="H123" s="50"/>
+      <c r="H123" s="54"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -10651,14 +11675,14 @@
       <c r="D124" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E124" s="48">
+      <c r="E124" s="52">
         <v>23240</v>
       </c>
-      <c r="F124" s="48"/>
-      <c r="G124" s="49">
+      <c r="F124" s="52"/>
+      <c r="G124" s="53">
         <v>10</v>
       </c>
-      <c r="H124" s="50"/>
+      <c r="H124" s="54"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="20">
@@ -10667,17 +11691,17 @@
       <c r="D125" s="21">
         <v>0.254</v>
       </c>
-      <c r="E125" s="53">
+      <c r="E125" s="55">
         <v>26709</v>
       </c>
-      <c r="F125" s="53"/>
-      <c r="G125" s="51">
+      <c r="F125" s="55"/>
+      <c r="G125" s="60">
         <v>12</v>
       </c>
-      <c r="H125" s="52"/>
+      <c r="H125" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="74">
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="S3:U3"/>
@@ -10685,12 +11709,13 @@
     <mergeCell ref="S7:U7"/>
     <mergeCell ref="S4:U4"/>
     <mergeCell ref="S5:U5"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E124:F124"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="G103:H104"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="G109:H109"/>
     <mergeCell ref="G123:H123"/>
     <mergeCell ref="G124:H124"/>
     <mergeCell ref="G125:H125"/>
@@ -10699,13 +11724,6 @@
     <mergeCell ref="G120:H120"/>
     <mergeCell ref="G121:H121"/>
     <mergeCell ref="G122:H122"/>
-    <mergeCell ref="E124:F124"/>
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="G103:H104"/>
-    <mergeCell ref="G106:H106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="G108:H108"/>
-    <mergeCell ref="G109:H109"/>
     <mergeCell ref="G110:H110"/>
     <mergeCell ref="G111:H111"/>
     <mergeCell ref="G112:H112"/>
@@ -10717,27 +11735,32 @@
     <mergeCell ref="E119:F119"/>
     <mergeCell ref="E120:F120"/>
     <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E122:F122"/>
     <mergeCell ref="E114:F114"/>
     <mergeCell ref="E115:F115"/>
     <mergeCell ref="E116:F116"/>
     <mergeCell ref="E117:F117"/>
     <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="E107:F107"/>
     <mergeCell ref="E108:F108"/>
     <mergeCell ref="E109:F109"/>
     <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
     <mergeCell ref="C53:E53"/>
     <mergeCell ref="D103:D104"/>
     <mergeCell ref="E103:F104"/>
-    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="S8:U8"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="N4:P4"/>
@@ -10748,6 +11771,11 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
     <mergeCell ref="N7:P7"/>
+    <mergeCell ref="AX14:BB14"/>
+    <mergeCell ref="BD14:BH14"/>
+    <mergeCell ref="AZ13:BA13"/>
+    <mergeCell ref="BF13:BG13"/>
+    <mergeCell ref="N9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding retrofits - does not run
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -22,6 +22,7 @@
     <definedName name="CAPEX_wind">Sheet2!$F$18:$F$43</definedName>
     <definedName name="CH4_rate">Sheet2!$AN$57:$AN$100</definedName>
     <definedName name="CO2_rate">Sheet2!$AM$57:$AM$100</definedName>
+    <definedName name="ConvUnitCap">Sheet2!$T$57:$T$76</definedName>
     <definedName name="DiscRate">Sheet2!$G$1</definedName>
     <definedName name="EV_subsidy_cost">Sheet2!$V$1</definedName>
     <definedName name="FallDemandOff">Sheet2!$BA$18:$BC$43</definedName>
@@ -58,6 +59,11 @@
     <definedName name="OPEX_wind">Sheet2!$Q$3</definedName>
     <definedName name="PeakHours">Sheet2!$C$6</definedName>
     <definedName name="RampRate">Sheet2!$AC$57:$AC$100</definedName>
+    <definedName name="retrofit_cap_cost">Sheet2!$L$8</definedName>
+    <definedName name="retrofit_CO2_removal">Sheet2!$L$12</definedName>
+    <definedName name="retrofit_NOx_removal">Sheet2!$L$10</definedName>
+    <definedName name="retrofit_opex_cost">Sheet2!$L$9</definedName>
+    <definedName name="retrofit_SO2_removal">Sheet2!$L$11</definedName>
     <definedName name="SO2_rate">Sheet2!$AL$57:$AL$100</definedName>
     <definedName name="solar_cap_factor">Sheet2!$L$4</definedName>
     <definedName name="solar_inc">Sheet2!$Q$7</definedName>
@@ -201,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="164">
   <si>
     <t>NumBuses</t>
   </si>
@@ -675,6 +681,24 @@
   </si>
   <si>
     <t>Solar Off-Peak Scale Factor</t>
+  </si>
+  <si>
+    <t>NGCC</t>
+  </si>
+  <si>
+    <t>Retrofit LCOE ($/MW):</t>
+  </si>
+  <si>
+    <t>Retrofit Levelized OPEX ($/MWh):</t>
+  </si>
+  <si>
+    <t>Retrofit NOx Removal</t>
+  </si>
+  <si>
+    <t>Retrofit SO2 Removal</t>
+  </si>
+  <si>
+    <t>Retrofit CO2 Removal</t>
   </si>
 </sst>
 </file>
@@ -859,7 +883,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -967,7 +991,13 @@
     </xf>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1303,7 +1333,7 @@
   <dimension ref="A1:BP128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1316,7 +1346,9 @@
     <col min="6" max="6" width="13.36328125" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.453125" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" customWidth="1"/>
     <col min="12" max="12" width="8.6328125" customWidth="1"/>
     <col min="14" max="14" width="9.26953125" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
@@ -1340,18 +1372,18 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="49"/>
+      <c r="F1" s="50"/>
       <c r="G1" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
@@ -1362,11 +1394,11 @@
       <c r="Q1" s="24">
         <v>0</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1378,14 +1410,14 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="49" t="s">
+      <c r="I2" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
@@ -1397,11 +1429,11 @@
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="49" t="s">
+      <c r="S2" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1419,11 +1451,11 @@
       <c r="F3" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="49" t="s">
+      <c r="I3" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -1434,11 +1466,11 @@
       <c r="Q3" s="24">
         <v>43560</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="49"/>
-      <c r="U3" s="49"/>
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1460,11 +1492,11 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="I4" s="50" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="15">
         <v>0.75</v>
       </c>
@@ -1475,11 +1507,11 @@
       <c r="Q4" s="24">
         <v>601000</v>
       </c>
-      <c r="S4" s="49" t="s">
+      <c r="S4" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1496,11 +1528,11 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="49" t="s">
+      <c r="I5" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
       <c r="L5" s="15">
         <v>0.5</v>
       </c>
@@ -1511,11 +1543,11 @@
       <c r="Q5" s="24">
         <v>15025</v>
       </c>
-      <c r="S5" s="49" t="s">
+      <c r="S5" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="50"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1531,11 +1563,11 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
       <c r="L6" s="15">
         <v>1</v>
       </c>
@@ -1546,11 +1578,11 @@
       <c r="Q6" s="26">
         <v>0.95</v>
       </c>
-      <c r="S6" s="49" t="s">
+      <c r="S6" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
+      <c r="T6" s="50"/>
+      <c r="U6" s="50"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1573,11 +1605,11 @@
       <c r="Q7" s="26">
         <v>50</v>
       </c>
-      <c r="S7" s="49" t="s">
+      <c r="S7" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
+      <c r="T7" s="50"/>
+      <c r="U7" s="50"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1593,6 +1625,14 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
+      <c r="I8" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="49">
+        <v>15.24</v>
+      </c>
       <c r="O8" s="41"/>
       <c r="P8" s="36" t="s">
         <v>86</v>
@@ -1600,11 +1640,11 @@
       <c r="Q8" s="26">
         <v>10</v>
       </c>
-      <c r="S8" s="49" t="s">
+      <c r="S8" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1619,6 +1659,14 @@
       </c>
       <c r="G9" s="6">
         <v>5009</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="49">
+        <v>9.83</v>
       </c>
       <c r="O9" s="41"/>
       <c r="P9" s="36" t="s">
@@ -1639,6 +1687,14 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
+      <c r="I10" s="50" t="s">
+        <v>161</v>
+      </c>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="27">
+        <v>0.73499999999999999</v>
+      </c>
       <c r="O10" s="41"/>
       <c r="P10" s="36" t="s">
         <v>140</v>
@@ -1657,6 +1713,14 @@
       </c>
       <c r="G11" s="6">
         <v>3780</v>
+      </c>
+      <c r="I11" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="27">
+        <v>0.65249999999999997</v>
       </c>
       <c r="O11" s="41"/>
       <c r="P11" s="36" t="s">
@@ -1674,10 +1738,14 @@
       <c r="F12" s="36"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
+      <c r="I12" s="51" t="s">
+        <v>163</v>
+      </c>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="27">
+        <v>0.81</v>
+      </c>
       <c r="M12" s="25"/>
       <c r="N12" s="43"/>
       <c r="O12" s="43"/>
@@ -1782,17 +1850,17 @@
         <f>92*8</f>
         <v>736</v>
       </c>
-      <c r="BH15" s="49" t="s">
+      <c r="BH15" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="BI15" s="49"/>
+      <c r="BI15" s="50"/>
       <c r="BJ15" s="48">
         <v>16054000</v>
       </c>
-      <c r="BN15" s="49" t="s">
+      <c r="BN15" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="BO15" s="49"/>
+      <c r="BO15" s="50"/>
       <c r="BP15" s="48">
         <v>10000000</v>
       </c>
@@ -1841,20 +1909,20 @@
       </c>
       <c r="BC16" s="33"/>
       <c r="BD16" s="34"/>
-      <c r="BF16" s="49" t="s">
+      <c r="BF16" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="BG16" s="49"/>
-      <c r="BH16" s="49"/>
-      <c r="BI16" s="49"/>
-      <c r="BJ16" s="49"/>
-      <c r="BL16" s="49" t="s">
+      <c r="BG16" s="50"/>
+      <c r="BH16" s="50"/>
+      <c r="BI16" s="50"/>
+      <c r="BJ16" s="50"/>
+      <c r="BL16" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="BM16" s="49"/>
-      <c r="BN16" s="49"/>
-      <c r="BO16" s="49"/>
-      <c r="BP16" s="49"/>
+      <c r="BM16" s="50"/>
+      <c r="BN16" s="50"/>
+      <c r="BO16" s="50"/>
+      <c r="BP16" s="50"/>
     </row>
     <row r="17" spans="2:68" x14ac:dyDescent="0.35">
       <c r="B17" s="44" t="s">
@@ -7611,17 +7679,17 @@
       </c>
     </row>
     <row r="47" spans="2:68" x14ac:dyDescent="0.35">
-      <c r="C47" s="50" t="s">
+      <c r="C47" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="50" t="s">
+      <c r="H47" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
       <c r="K47" s="2"/>
       <c r="L47" s="4"/>
       <c r="O47" s="4"/>
@@ -7858,11 +7926,11 @@
       </c>
     </row>
     <row r="55" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="C55" s="50" t="s">
+      <c r="C55" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
       <c r="G55" s="38" t="s">
         <v>132</v>
       </c>
@@ -12108,7 +12176,7 @@
         <v>100</v>
       </c>
       <c r="B99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C99" s="6">
         <v>0</v>
@@ -12120,56 +12188,59 @@
         <v>0</v>
       </c>
       <c r="G99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H99" s="6">
         <v>0</v>
       </c>
       <c r="J99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K99" s="6">
         <v>0</v>
       </c>
       <c r="M99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N99" s="6">
         <v>0</v>
       </c>
       <c r="P99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q99" s="6">
         <v>0</v>
       </c>
       <c r="S99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T99" s="6">
         <v>10000</v>
       </c>
       <c r="V99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W99" s="6">
         <v>-10000</v>
       </c>
       <c r="Y99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Z99" s="8">
         <f t="shared" ref="Z99" si="47">AG99*AH99*1000/1000000</f>
         <v>0</v>
       </c>
       <c r="AB99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AC99" s="40">
         <v>10000</v>
       </c>
       <c r="AE99" s="42">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>100</v>
       </c>
       <c r="AG99" s="6">
         <v>0</v>
@@ -12178,7 +12249,7 @@
         <v>0</v>
       </c>
       <c r="AJ99" s="42">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AK99" s="6">
         <v>0</v>
@@ -12240,6 +12311,9 @@
       <c r="AC100" s="40"/>
       <c r="AE100" s="42">
         <v>44</v>
+      </c>
+      <c r="AF100" t="s">
+        <v>158</v>
       </c>
       <c r="AG100" s="6"/>
       <c r="AH100" s="6"/>
@@ -12253,27 +12327,27 @@
       <c r="AO100" s="6"/>
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D106" s="51" t="s">
+      <c r="D106" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="53" t="s">
+      <c r="E106" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="53"/>
-      <c r="G106" s="53" t="s">
+      <c r="F106" s="55"/>
+      <c r="G106" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="H106" s="58"/>
+      <c r="H106" s="60"/>
       <c r="N106" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D107" s="52"/>
-      <c r="E107" s="54"/>
-      <c r="F107" s="54"/>
-      <c r="G107" s="54"/>
-      <c r="H107" s="59"/>
+      <c r="D107" s="54"/>
+      <c r="E107" s="56"/>
+      <c r="F107" s="56"/>
+      <c r="G107" s="56"/>
+      <c r="H107" s="61"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
@@ -12287,14 +12361,14 @@
       <c r="D109" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E109" s="55">
+      <c r="E109" s="57">
         <v>72154</v>
       </c>
-      <c r="F109" s="55"/>
-      <c r="G109" s="60">
+      <c r="F109" s="57"/>
+      <c r="G109" s="62">
         <v>28.1</v>
       </c>
-      <c r="H109" s="61"/>
+      <c r="H109" s="63"/>
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -12303,14 +12377,14 @@
       <c r="D110" s="19">
         <v>0.31</v>
       </c>
-      <c r="E110" s="56">
+      <c r="E110" s="58">
         <v>67811</v>
       </c>
-      <c r="F110" s="56"/>
-      <c r="G110" s="62">
+      <c r="F110" s="58"/>
+      <c r="G110" s="64">
         <v>25</v>
       </c>
-      <c r="H110" s="63"/>
+      <c r="H110" s="65"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -12319,14 +12393,14 @@
       <c r="D111" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E111" s="56">
+      <c r="E111" s="58">
         <v>187455</v>
       </c>
-      <c r="F111" s="56"/>
-      <c r="G111" s="62">
+      <c r="F111" s="58"/>
+      <c r="G111" s="64">
         <v>70</v>
       </c>
-      <c r="H111" s="63"/>
+      <c r="H111" s="65"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -12335,14 +12409,14 @@
       <c r="D112" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E112" s="56">
+      <c r="E112" s="58">
         <v>63266</v>
       </c>
-      <c r="F112" s="56"/>
-      <c r="G112" s="62">
+      <c r="F112" s="58"/>
+      <c r="G112" s="64">
         <v>30.6</v>
       </c>
-      <c r="H112" s="63"/>
+      <c r="H112" s="65"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -12351,14 +12425,14 @@
       <c r="D113" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E113" s="56">
+      <c r="E113" s="58">
         <v>26553</v>
       </c>
-      <c r="F113" s="56"/>
-      <c r="G113" s="62">
+      <c r="F113" s="58"/>
+      <c r="G113" s="64">
         <v>10</v>
       </c>
-      <c r="H113" s="63"/>
+      <c r="H113" s="65"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -12367,14 +12441,14 @@
       <c r="D114" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E114" s="56">
+      <c r="E114" s="58">
         <v>24949</v>
       </c>
-      <c r="F114" s="56"/>
-      <c r="G114" s="62">
+      <c r="F114" s="58"/>
+      <c r="G114" s="64">
         <v>10</v>
       </c>
-      <c r="H114" s="63"/>
+      <c r="H114" s="65"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -12383,14 +12457,14 @@
       <c r="D115" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E115" s="56">
+      <c r="E115" s="58">
         <v>22870</v>
       </c>
-      <c r="F115" s="56"/>
-      <c r="G115" s="62">
+      <c r="F115" s="58"/>
+      <c r="G115" s="64">
         <v>10</v>
       </c>
-      <c r="H115" s="63"/>
+      <c r="H115" s="65"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -12399,14 +12473,14 @@
       <c r="D116" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E116" s="56">
+      <c r="E116" s="58">
         <v>139836</v>
       </c>
-      <c r="F116" s="56"/>
-      <c r="G116" s="62">
+      <c r="F116" s="58"/>
+      <c r="G116" s="64">
         <v>52.2</v>
       </c>
-      <c r="H116" s="63"/>
+      <c r="H116" s="65"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -12415,14 +12489,14 @@
       <c r="D117" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E117" s="56">
+      <c r="E117" s="58">
         <v>23515</v>
       </c>
-      <c r="F117" s="56"/>
-      <c r="G117" s="62">
+      <c r="F117" s="58"/>
+      <c r="G117" s="64">
         <v>10</v>
       </c>
-      <c r="H117" s="63"/>
+      <c r="H117" s="65"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -12431,14 +12505,14 @@
       <c r="D118" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E118" s="56">
+      <c r="E118" s="58">
         <v>49503</v>
       </c>
-      <c r="F118" s="56"/>
-      <c r="G118" s="62">
+      <c r="F118" s="58"/>
+      <c r="G118" s="64">
         <v>20.2</v>
       </c>
-      <c r="H118" s="63"/>
+      <c r="H118" s="65"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -12447,14 +12521,14 @@
       <c r="D119" s="19">
         <v>0.307</v>
       </c>
-      <c r="E119" s="56">
+      <c r="E119" s="58">
         <v>188420</v>
       </c>
-      <c r="F119" s="56"/>
-      <c r="G119" s="62">
+      <c r="F119" s="58"/>
+      <c r="G119" s="64">
         <v>70</v>
       </c>
-      <c r="H119" s="63"/>
+      <c r="H119" s="65"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -12463,14 +12537,14 @@
       <c r="D120" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E120" s="56">
+      <c r="E120" s="58">
         <v>26573</v>
       </c>
-      <c r="F120" s="56"/>
-      <c r="G120" s="62">
+      <c r="F120" s="58"/>
+      <c r="G120" s="64">
         <v>10.5</v>
       </c>
-      <c r="H120" s="63"/>
+      <c r="H120" s="65"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -12479,14 +12553,14 @@
       <c r="D121" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E121" s="56">
+      <c r="E121" s="58">
         <v>25253</v>
       </c>
-      <c r="F121" s="56"/>
-      <c r="G121" s="62">
+      <c r="F121" s="58"/>
+      <c r="G121" s="64">
         <v>10</v>
       </c>
-      <c r="H121" s="63"/>
+      <c r="H121" s="65"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -12495,14 +12569,14 @@
       <c r="D122" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E122" s="56">
+      <c r="E122" s="58">
         <v>17610</v>
       </c>
-      <c r="F122" s="56"/>
-      <c r="G122" s="62">
+      <c r="F122" s="58"/>
+      <c r="G122" s="64">
         <v>10</v>
       </c>
-      <c r="H122" s="63"/>
+      <c r="H122" s="65"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -12511,14 +12585,14 @@
       <c r="D123" s="19">
         <v>0.221</v>
       </c>
-      <c r="E123" s="56">
+      <c r="E123" s="58">
         <v>19372</v>
       </c>
-      <c r="F123" s="56"/>
-      <c r="G123" s="62">
+      <c r="F123" s="58"/>
+      <c r="G123" s="64">
         <v>10</v>
       </c>
-      <c r="H123" s="63"/>
+      <c r="H123" s="65"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -12527,14 +12601,14 @@
       <c r="D124" s="19">
         <v>0.216</v>
       </c>
-      <c r="E124" s="56">
+      <c r="E124" s="58">
         <v>18939</v>
       </c>
-      <c r="F124" s="56"/>
-      <c r="G124" s="62">
+      <c r="F124" s="58"/>
+      <c r="G124" s="64">
         <v>10</v>
       </c>
-      <c r="H124" s="63"/>
+      <c r="H124" s="65"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="18">
@@ -12543,14 +12617,14 @@
       <c r="D125" s="19">
         <v>0.23</v>
       </c>
-      <c r="E125" s="56">
+      <c r="E125" s="58">
         <v>20382</v>
       </c>
-      <c r="F125" s="56"/>
-      <c r="G125" s="62">
+      <c r="F125" s="58"/>
+      <c r="G125" s="64">
         <v>10.1</v>
       </c>
-      <c r="H125" s="63"/>
+      <c r="H125" s="65"/>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C126" s="18">
@@ -12559,14 +12633,14 @@
       <c r="D126" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E126" s="56">
+      <c r="E126" s="58">
         <v>19968</v>
       </c>
-      <c r="F126" s="56"/>
-      <c r="G126" s="62">
+      <c r="F126" s="58"/>
+      <c r="G126" s="64">
         <v>10.1</v>
       </c>
-      <c r="H126" s="63"/>
+      <c r="H126" s="65"/>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C127" s="18">
@@ -12575,14 +12649,14 @@
       <c r="D127" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E127" s="56">
+      <c r="E127" s="58">
         <v>23240</v>
       </c>
-      <c r="F127" s="56"/>
-      <c r="G127" s="62">
+      <c r="F127" s="58"/>
+      <c r="G127" s="64">
         <v>10</v>
       </c>
-      <c r="H127" s="63"/>
+      <c r="H127" s="65"/>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C128" s="20">
@@ -12591,17 +12665,17 @@
       <c r="D128" s="21">
         <v>0.254</v>
       </c>
-      <c r="E128" s="57">
+      <c r="E128" s="59">
         <v>26709</v>
       </c>
-      <c r="F128" s="57"/>
-      <c r="G128" s="64">
+      <c r="F128" s="59"/>
+      <c r="G128" s="66">
         <v>12</v>
       </c>
-      <c r="H128" s="65"/>
+      <c r="H128" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="71">
     <mergeCell ref="S1:U1"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="S3:U3"/>
@@ -12668,6 +12742,11 @@
     <mergeCell ref="I5:K5"/>
     <mergeCell ref="I6:K6"/>
     <mergeCell ref="S8:U8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reverted Off Peak New Solar Generation to 0
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1036,36 +1036,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1077,20 +1077,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="AE60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AR57" sqref="AR57:AR76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,18 +1416,18 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="54"/>
+      <c r="F1" s="53"/>
       <c r="G1" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
@@ -1438,11 +1438,11 @@
       <c r="Q1" s="24">
         <v>0</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1454,14 +1454,14 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
@@ -1473,11 +1473,11 @@
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="54" t="s">
+      <c r="S2" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1495,11 +1495,11 @@
       <c r="F3" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -1510,11 +1510,11 @@
       <c r="Q3" s="24">
         <v>43560</v>
       </c>
-      <c r="S3" s="54" t="s">
+      <c r="S3" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1543,11 +1543,11 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
       <c r="L4" s="15">
         <v>0.75</v>
       </c>
@@ -1558,11 +1558,11 @@
       <c r="Q4" s="24">
         <v>601000</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="S4" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1581,11 +1581,11 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
@@ -1596,11 +1596,11 @@
       <c r="Q5" s="24">
         <v>15025</v>
       </c>
-      <c r="S5" s="54" t="s">
+      <c r="S5" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
+      <c r="T5" s="53"/>
+      <c r="U5" s="53"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1622,11 +1622,11 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
       <c r="L6" s="15">
         <v>1</v>
       </c>
@@ -1637,11 +1637,11 @@
       <c r="Q6" s="26">
         <v>0.95</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="S6" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1666,11 +1666,11 @@
       <c r="Q7" s="26">
         <v>50</v>
       </c>
-      <c r="S7" s="54" t="s">
+      <c r="S7" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
+      <c r="T7" s="53"/>
+      <c r="U7" s="53"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1692,11 +1692,11 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
       <c r="L8" s="49">
         <v>15.24</v>
       </c>
@@ -1707,11 +1707,11 @@
       <c r="Q8" s="26">
         <v>10</v>
       </c>
-      <c r="S8" s="54" t="s">
+      <c r="S8" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1729,11 +1729,11 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
       <c r="L9" s="49">
         <v>9.83</v>
       </c>
@@ -1762,11 +1762,11 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="53" t="s">
         <v>161</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
       <c r="L10" s="27">
         <v>0.73499999999999999</v>
       </c>
@@ -1791,11 +1791,11 @@
       <c r="G11" s="6">
         <v>3780</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="53" t="s">
         <v>162</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
       <c r="L11" s="27">
         <v>0.65249999999999997</v>
       </c>
@@ -1815,11 +1815,11 @@
       <c r="F12" s="36"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="71" t="s">
+      <c r="I12" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
       <c r="L12" s="27">
         <v>0.81</v>
       </c>
@@ -1927,17 +1927,17 @@
         <f>92*8</f>
         <v>736</v>
       </c>
-      <c r="BH15" s="54" t="s">
+      <c r="BH15" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="BI15" s="54"/>
+      <c r="BI15" s="53"/>
       <c r="BJ15" s="48">
         <v>16054000</v>
       </c>
-      <c r="BN15" s="54" t="s">
+      <c r="BN15" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="BO15" s="54"/>
+      <c r="BO15" s="53"/>
       <c r="BP15" s="48">
         <v>10000000</v>
       </c>
@@ -2006,20 +2006,20 @@
       </c>
       <c r="BC16" s="33"/>
       <c r="BD16" s="34"/>
-      <c r="BF16" s="54" t="s">
+      <c r="BF16" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="BG16" s="54"/>
-      <c r="BH16" s="54"/>
-      <c r="BI16" s="54"/>
-      <c r="BJ16" s="54"/>
-      <c r="BL16" s="54" t="s">
+      <c r="BG16" s="53"/>
+      <c r="BH16" s="53"/>
+      <c r="BI16" s="53"/>
+      <c r="BJ16" s="53"/>
+      <c r="BL16" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="BM16" s="54"/>
-      <c r="BN16" s="54"/>
-      <c r="BO16" s="54"/>
-      <c r="BP16" s="54"/>
+      <c r="BM16" s="53"/>
+      <c r="BN16" s="53"/>
+      <c r="BO16" s="53"/>
+      <c r="BP16" s="53"/>
       <c r="BT16" s="51" t="s">
         <v>169</v>
       </c>
@@ -9832,17 +9832,17 @@
       </c>
     </row>
     <row r="47" spans="2:92" x14ac:dyDescent="0.35">
-      <c r="C47" s="68" t="s">
+      <c r="C47" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="68"/>
-      <c r="E47" s="68"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="68" t="s">
+      <c r="H47" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="68"/>
-      <c r="J47" s="68"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
       <c r="K47" s="2"/>
       <c r="L47" s="4"/>
       <c r="O47" s="4"/>
@@ -10077,19 +10077,19 @@
       <c r="AO54" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AQ54" s="53" t="s">
+      <c r="AQ54" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="AR54" s="53"/>
-      <c r="AS54" s="53"/>
-      <c r="AT54" s="53"/>
+      <c r="AR54" s="71"/>
+      <c r="AS54" s="71"/>
+      <c r="AT54" s="71"/>
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
       <c r="G55" s="38" t="s">
         <v>132</v>
       </c>
@@ -14265,7 +14265,7 @@
         <v>41</v>
       </c>
       <c r="T97" s="6">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="V97" s="22">
         <v>41</v>
@@ -14569,26 +14569,26 @@
       <c r="AO100" s="6"/>
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D106" s="69" t="s">
+      <c r="D106" s="56" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="61" t="s">
+      <c r="E106" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="61"/>
-      <c r="G106" s="61" t="s">
+      <c r="F106" s="58"/>
+      <c r="G106" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="H106" s="62"/>
+      <c r="H106" s="63"/>
       <c r="N106" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D107" s="70"/>
-      <c r="E107" s="63"/>
-      <c r="F107" s="63"/>
-      <c r="G107" s="63"/>
+      <c r="D107" s="57"/>
+      <c r="E107" s="59"/>
+      <c r="F107" s="59"/>
+      <c r="G107" s="59"/>
       <c r="H107" s="64"/>
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.35">
@@ -14603,10 +14603,10 @@
       <c r="D109" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E109" s="67">
+      <c r="E109" s="60">
         <v>72154</v>
       </c>
-      <c r="F109" s="67"/>
+      <c r="F109" s="60"/>
       <c r="G109" s="65">
         <v>28.1</v>
       </c>
@@ -14619,14 +14619,14 @@
       <c r="D110" s="19">
         <v>0.31</v>
       </c>
-      <c r="E110" s="57">
+      <c r="E110" s="61">
         <v>67811</v>
       </c>
-      <c r="F110" s="57"/>
-      <c r="G110" s="55">
+      <c r="F110" s="61"/>
+      <c r="G110" s="67">
         <v>25</v>
       </c>
-      <c r="H110" s="56"/>
+      <c r="H110" s="68"/>
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -14635,14 +14635,14 @@
       <c r="D111" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E111" s="57">
+      <c r="E111" s="61">
         <v>187455</v>
       </c>
-      <c r="F111" s="57"/>
-      <c r="G111" s="55">
+      <c r="F111" s="61"/>
+      <c r="G111" s="67">
         <v>70</v>
       </c>
-      <c r="H111" s="56"/>
+      <c r="H111" s="68"/>
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -14651,14 +14651,14 @@
       <c r="D112" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E112" s="57">
+      <c r="E112" s="61">
         <v>63266</v>
       </c>
-      <c r="F112" s="57"/>
-      <c r="G112" s="55">
+      <c r="F112" s="61"/>
+      <c r="G112" s="67">
         <v>30.6</v>
       </c>
-      <c r="H112" s="56"/>
+      <c r="H112" s="68"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -14667,14 +14667,14 @@
       <c r="D113" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E113" s="57">
+      <c r="E113" s="61">
         <v>26553</v>
       </c>
-      <c r="F113" s="57"/>
-      <c r="G113" s="55">
+      <c r="F113" s="61"/>
+      <c r="G113" s="67">
         <v>10</v>
       </c>
-      <c r="H113" s="56"/>
+      <c r="H113" s="68"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -14683,14 +14683,14 @@
       <c r="D114" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E114" s="57">
+      <c r="E114" s="61">
         <v>24949</v>
       </c>
-      <c r="F114" s="57"/>
-      <c r="G114" s="55">
+      <c r="F114" s="61"/>
+      <c r="G114" s="67">
         <v>10</v>
       </c>
-      <c r="H114" s="56"/>
+      <c r="H114" s="68"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -14699,14 +14699,14 @@
       <c r="D115" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E115" s="57">
+      <c r="E115" s="61">
         <v>22870</v>
       </c>
-      <c r="F115" s="57"/>
-      <c r="G115" s="55">
+      <c r="F115" s="61"/>
+      <c r="G115" s="67">
         <v>10</v>
       </c>
-      <c r="H115" s="56"/>
+      <c r="H115" s="68"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -14715,14 +14715,14 @@
       <c r="D116" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E116" s="57">
+      <c r="E116" s="61">
         <v>139836</v>
       </c>
-      <c r="F116" s="57"/>
-      <c r="G116" s="55">
+      <c r="F116" s="61"/>
+      <c r="G116" s="67">
         <v>52.2</v>
       </c>
-      <c r="H116" s="56"/>
+      <c r="H116" s="68"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -14731,14 +14731,14 @@
       <c r="D117" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E117" s="57">
+      <c r="E117" s="61">
         <v>23515</v>
       </c>
-      <c r="F117" s="57"/>
-      <c r="G117" s="55">
+      <c r="F117" s="61"/>
+      <c r="G117" s="67">
         <v>10</v>
       </c>
-      <c r="H117" s="56"/>
+      <c r="H117" s="68"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -14747,14 +14747,14 @@
       <c r="D118" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E118" s="57">
+      <c r="E118" s="61">
         <v>49503</v>
       </c>
-      <c r="F118" s="57"/>
-      <c r="G118" s="55">
+      <c r="F118" s="61"/>
+      <c r="G118" s="67">
         <v>20.2</v>
       </c>
-      <c r="H118" s="56"/>
+      <c r="H118" s="68"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -14763,14 +14763,14 @@
       <c r="D119" s="19">
         <v>0.307</v>
       </c>
-      <c r="E119" s="57">
+      <c r="E119" s="61">
         <v>188420</v>
       </c>
-      <c r="F119" s="57"/>
-      <c r="G119" s="55">
+      <c r="F119" s="61"/>
+      <c r="G119" s="67">
         <v>70</v>
       </c>
-      <c r="H119" s="56"/>
+      <c r="H119" s="68"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -14779,14 +14779,14 @@
       <c r="D120" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E120" s="57">
+      <c r="E120" s="61">
         <v>26573</v>
       </c>
-      <c r="F120" s="57"/>
-      <c r="G120" s="55">
+      <c r="F120" s="61"/>
+      <c r="G120" s="67">
         <v>10.5</v>
       </c>
-      <c r="H120" s="56"/>
+      <c r="H120" s="68"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -14795,14 +14795,14 @@
       <c r="D121" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E121" s="57">
+      <c r="E121" s="61">
         <v>25253</v>
       </c>
-      <c r="F121" s="57"/>
-      <c r="G121" s="55">
+      <c r="F121" s="61"/>
+      <c r="G121" s="67">
         <v>10</v>
       </c>
-      <c r="H121" s="56"/>
+      <c r="H121" s="68"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -14811,14 +14811,14 @@
       <c r="D122" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E122" s="57">
+      <c r="E122" s="61">
         <v>17610</v>
       </c>
-      <c r="F122" s="57"/>
-      <c r="G122" s="55">
+      <c r="F122" s="61"/>
+      <c r="G122" s="67">
         <v>10</v>
       </c>
-      <c r="H122" s="56"/>
+      <c r="H122" s="68"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -14827,14 +14827,14 @@
       <c r="D123" s="19">
         <v>0.221</v>
       </c>
-      <c r="E123" s="57">
+      <c r="E123" s="61">
         <v>19372</v>
       </c>
-      <c r="F123" s="57"/>
-      <c r="G123" s="55">
+      <c r="F123" s="61"/>
+      <c r="G123" s="67">
         <v>10</v>
       </c>
-      <c r="H123" s="56"/>
+      <c r="H123" s="68"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -14843,14 +14843,14 @@
       <c r="D124" s="19">
         <v>0.216</v>
       </c>
-      <c r="E124" s="57">
+      <c r="E124" s="61">
         <v>18939</v>
       </c>
-      <c r="F124" s="57"/>
-      <c r="G124" s="55">
+      <c r="F124" s="61"/>
+      <c r="G124" s="67">
         <v>10</v>
       </c>
-      <c r="H124" s="56"/>
+      <c r="H124" s="68"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="18">
@@ -14859,14 +14859,14 @@
       <c r="D125" s="19">
         <v>0.23</v>
       </c>
-      <c r="E125" s="57">
+      <c r="E125" s="61">
         <v>20382</v>
       </c>
-      <c r="F125" s="57"/>
-      <c r="G125" s="55">
+      <c r="F125" s="61"/>
+      <c r="G125" s="67">
         <v>10.1</v>
       </c>
-      <c r="H125" s="56"/>
+      <c r="H125" s="68"/>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C126" s="18">
@@ -14875,14 +14875,14 @@
       <c r="D126" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E126" s="57">
+      <c r="E126" s="61">
         <v>19968</v>
       </c>
-      <c r="F126" s="57"/>
-      <c r="G126" s="55">
+      <c r="F126" s="61"/>
+      <c r="G126" s="67">
         <v>10.1</v>
       </c>
-      <c r="H126" s="56"/>
+      <c r="H126" s="68"/>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C127" s="18">
@@ -14891,14 +14891,14 @@
       <c r="D127" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E127" s="57">
+      <c r="E127" s="61">
         <v>23240</v>
       </c>
-      <c r="F127" s="57"/>
-      <c r="G127" s="55">
+      <c r="F127" s="61"/>
+      <c r="G127" s="67">
         <v>10</v>
       </c>
-      <c r="H127" s="56"/>
+      <c r="H127" s="68"/>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C128" s="20">
@@ -14907,42 +14907,48 @@
       <c r="D128" s="21">
         <v>0.254</v>
       </c>
-      <c r="E128" s="60">
+      <c r="E128" s="62">
         <v>26709</v>
       </c>
-      <c r="F128" s="60"/>
-      <c r="G128" s="58">
+      <c r="F128" s="62"/>
+      <c r="G128" s="69">
         <v>12</v>
       </c>
-      <c r="H128" s="59"/>
+      <c r="H128" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="BH15:BI15"/>
-    <mergeCell ref="BN15:BO15"/>
-    <mergeCell ref="BF16:BJ16"/>
-    <mergeCell ref="BL16:BP16"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:F107"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="AQ54:AT54"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G126:H126"/>
+    <mergeCell ref="E123:F123"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E124:F124"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
     <mergeCell ref="E127:F127"/>
     <mergeCell ref="E128:F128"/>
     <mergeCell ref="G106:H107"/>
@@ -14959,37 +14965,31 @@
     <mergeCell ref="G119:H119"/>
     <mergeCell ref="G120:H120"/>
     <mergeCell ref="E122:F122"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G126:H126"/>
-    <mergeCell ref="E123:F123"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="E124:F124"/>
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="AQ54:AT54"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:F107"/>
+    <mergeCell ref="BH15:BI15"/>
+    <mergeCell ref="BN15:BO15"/>
+    <mergeCell ref="BF16:BJ16"/>
+    <mergeCell ref="BL16:BP16"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adds existing generation opex
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -54,7 +54,7 @@
     <definedName name="NumUnits">Sheet2!$C$3</definedName>
     <definedName name="NumYears">Sheet2!$C$4</definedName>
     <definedName name="OffHours">Sheet2!$C$7</definedName>
-    <definedName name="OPEX_existing">Sheet2!$AR$57:$AR$76</definedName>
+    <definedName name="OPEX_existing">Sheet2!$AR$57:$AR$100</definedName>
     <definedName name="OPEX_NGCC">Sheet2!$Q$1</definedName>
     <definedName name="OPEX_solar">Sheet2!$Q$2</definedName>
     <definedName name="OPEX_storage">Sheet2!$Q$5</definedName>
@@ -706,9 +706,6 @@
     <t>Retrofit CO2 Removal</t>
   </si>
   <si>
-    <t>OPEX for Existing Generators ($/year)</t>
-  </si>
-  <si>
     <t>Peak Peak Demand Winter (MW)</t>
   </si>
   <si>
@@ -731,6 +728,9 @@
   </si>
   <si>
     <t>Fall Peak Peak Demand in Bus (MW)</t>
+  </si>
+  <si>
+    <t>OPEX for Existing Generators ($/MWh)</t>
   </si>
 </sst>
 </file>
@@ -915,7 +915,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1035,10 +1035,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1050,47 +1092,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1376,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE60" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AR57" sqref="AR57:AR76"/>
+    <sheetView tabSelected="1" topLeftCell="AE73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AV87" sqref="AV87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,18 +1419,18 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="53"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
@@ -1438,11 +1441,11 @@
       <c r="Q1" s="24">
         <v>0</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1454,14 +1457,14 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
@@ -1473,11 +1476,11 @@
       <c r="Q2" s="24">
         <v>19867.2</v>
       </c>
-      <c r="S2" s="53" t="s">
+      <c r="S2" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1495,11 +1498,11 @@
       <c r="F3" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="10">
         <v>8.9999999999999993E-3</v>
       </c>
@@ -1510,11 +1513,11 @@
       <c r="Q3" s="24">
         <v>43560</v>
       </c>
-      <c r="S3" s="53" t="s">
+      <c r="S3" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1523,7 +1526,7 @@
       </c>
       <c r="BS3" s="13"/>
       <c r="BU3" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BV3" s="6">
         <v>6189</v>
@@ -1543,11 +1546,11 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="55" t="s">
         <v>157</v>
       </c>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="15">
         <v>0.75</v>
       </c>
@@ -1558,11 +1561,11 @@
       <c r="Q4" s="24">
         <v>601000</v>
       </c>
-      <c r="S4" s="53" t="s">
+      <c r="S4" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1581,11 +1584,11 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="15">
         <v>1</v>
       </c>
@@ -1596,11 +1599,11 @@
       <c r="Q5" s="24">
         <v>15025</v>
       </c>
-      <c r="S5" s="53" t="s">
+      <c r="S5" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="T5" s="53"/>
-      <c r="U5" s="53"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1609,7 +1612,7 @@
         <v>99</v>
       </c>
       <c r="BU5" s="36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="BV5" s="6">
         <v>6951</v>
@@ -1622,11 +1625,11 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="15">
         <v>1</v>
       </c>
@@ -1637,11 +1640,11 @@
       <c r="Q6" s="26">
         <v>0.95</v>
       </c>
-      <c r="S6" s="53" t="s">
+      <c r="S6" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="T6" s="53"/>
-      <c r="U6" s="53"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="55"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1666,11 +1669,11 @@
       <c r="Q7" s="26">
         <v>50</v>
       </c>
-      <c r="S7" s="53" t="s">
+      <c r="S7" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="T7" s="53"/>
-      <c r="U7" s="53"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1679,7 +1682,7 @@
         <v>93</v>
       </c>
       <c r="BU7" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="BV7" s="6">
         <v>7618</v>
@@ -1692,11 +1695,11 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="I8" s="53" t="s">
+      <c r="I8" s="55" t="s">
         <v>159</v>
       </c>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
       <c r="L8" s="49">
         <v>15.24</v>
       </c>
@@ -1707,11 +1710,11 @@
       <c r="Q8" s="26">
         <v>10</v>
       </c>
-      <c r="S8" s="53" t="s">
+      <c r="S8" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="T8" s="53"/>
-      <c r="U8" s="53"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1729,11 +1732,11 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="49">
         <v>9.83</v>
       </c>
@@ -1749,7 +1752,7 @@
       <c r="U9" s="33"/>
       <c r="V9" s="25"/>
       <c r="BU9" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="BV9" s="6">
         <v>6653</v>
@@ -1762,11 +1765,11 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
-      <c r="I10" s="53" t="s">
+      <c r="I10" s="55" t="s">
         <v>161</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
       <c r="L10" s="27">
         <v>0.73499999999999999</v>
       </c>
@@ -1791,11 +1794,11 @@
       <c r="G11" s="6">
         <v>3780</v>
       </c>
-      <c r="I11" s="53" t="s">
+      <c r="I11" s="55" t="s">
         <v>162</v>
       </c>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="27">
         <v>0.65249999999999997</v>
       </c>
@@ -1815,11 +1818,11 @@
       <c r="F12" s="36"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="54" t="s">
+      <c r="I12" s="72" t="s">
         <v>163</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
       <c r="L12" s="27">
         <v>0.81</v>
       </c>
@@ -1927,17 +1930,17 @@
         <f>92*8</f>
         <v>736</v>
       </c>
-      <c r="BH15" s="53" t="s">
+      <c r="BH15" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="BI15" s="53"/>
+      <c r="BI15" s="55"/>
       <c r="BJ15" s="48">
         <v>16054000</v>
       </c>
-      <c r="BN15" s="53" t="s">
+      <c r="BN15" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="BO15" s="53"/>
+      <c r="BO15" s="55"/>
       <c r="BP15" s="48">
         <v>10000000</v>
       </c>
@@ -2006,37 +2009,37 @@
       </c>
       <c r="BC16" s="33"/>
       <c r="BD16" s="34"/>
-      <c r="BF16" s="53" t="s">
+      <c r="BF16" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="BG16" s="53"/>
-      <c r="BH16" s="53"/>
-      <c r="BI16" s="53"/>
-      <c r="BJ16" s="53"/>
-      <c r="BL16" s="53" t="s">
+      <c r="BG16" s="55"/>
+      <c r="BH16" s="55"/>
+      <c r="BI16" s="55"/>
+      <c r="BJ16" s="55"/>
+      <c r="BL16" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="BM16" s="53"/>
-      <c r="BN16" s="53"/>
-      <c r="BO16" s="53"/>
-      <c r="BP16" s="53"/>
+      <c r="BM16" s="55"/>
+      <c r="BN16" s="55"/>
+      <c r="BO16" s="55"/>
+      <c r="BP16" s="55"/>
       <c r="BT16" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="BU16" s="51"/>
       <c r="BV16" s="52"/>
       <c r="BZ16" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="CA16" s="51"/>
       <c r="CB16" s="52"/>
       <c r="CF16" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="CG16" s="51"/>
       <c r="CH16" s="52"/>
       <c r="CL16" s="51" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="CM16" s="51"/>
       <c r="CN16" s="52"/>
@@ -9832,17 +9835,17 @@
       </c>
     </row>
     <row r="47" spans="2:92" x14ac:dyDescent="0.35">
-      <c r="C47" s="55" t="s">
+      <c r="C47" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="55" t="s">
+      <c r="H47" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
       <c r="K47" s="2"/>
       <c r="L47" s="4"/>
       <c r="O47" s="4"/>
@@ -10077,19 +10080,19 @@
       <c r="AO54" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AQ54" s="71" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR54" s="71"/>
-      <c r="AS54" s="71"/>
-      <c r="AT54" s="71"/>
+      <c r="AQ54" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="AR54" s="54"/>
+      <c r="AS54" s="54"/>
+      <c r="AT54" s="54"/>
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="C55" s="55" t="s">
+      <c r="C55" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
       <c r="G55" s="38" t="s">
         <v>132</v>
       </c>
@@ -10280,7 +10283,9 @@
       <c r="AQ57" s="50">
         <v>1</v>
       </c>
-      <c r="AR57" s="27"/>
+      <c r="AR57" s="27">
+        <v>5.08</v>
+      </c>
     </row>
     <row r="58" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
@@ -10381,7 +10386,9 @@
       <c r="AQ58" s="50">
         <v>2</v>
       </c>
-      <c r="AR58" s="27"/>
+      <c r="AR58" s="27">
+        <v>5.08</v>
+      </c>
     </row>
     <row r="59" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
@@ -10482,7 +10489,9 @@
       <c r="AQ59" s="50">
         <v>3</v>
       </c>
-      <c r="AR59" s="27"/>
+      <c r="AR59" s="27">
+        <v>5.08</v>
+      </c>
     </row>
     <row r="60" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
@@ -10583,7 +10592,9 @@
       <c r="AQ60" s="50">
         <v>4</v>
       </c>
-      <c r="AR60" s="27"/>
+      <c r="AR60" s="27">
+        <v>5.08</v>
+      </c>
     </row>
     <row r="61" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
@@ -10684,7 +10695,9 @@
       <c r="AQ61" s="50">
         <v>5</v>
       </c>
-      <c r="AR61" s="27"/>
+      <c r="AR61" s="27">
+        <v>5.08</v>
+      </c>
     </row>
     <row r="62" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
@@ -10785,7 +10798,9 @@
       <c r="AQ62" s="50">
         <v>6</v>
       </c>
-      <c r="AR62" s="27"/>
+      <c r="AR62" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="63" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
@@ -10886,7 +10901,9 @@
       <c r="AQ63" s="50">
         <v>7</v>
       </c>
-      <c r="AR63" s="27"/>
+      <c r="AR63" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="64" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -10987,7 +11004,9 @@
       <c r="AQ64" s="50">
         <v>8</v>
       </c>
-      <c r="AR64" s="27"/>
+      <c r="AR64" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="65" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
@@ -11088,7 +11107,9 @@
       <c r="AQ65" s="50">
         <v>9</v>
       </c>
-      <c r="AR65" s="27"/>
+      <c r="AR65" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="66" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
@@ -11189,7 +11210,9 @@
       <c r="AQ66" s="50">
         <v>10</v>
       </c>
-      <c r="AR66" s="27"/>
+      <c r="AR66" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="67" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
@@ -11290,7 +11313,9 @@
       <c r="AQ67" s="50">
         <v>11</v>
       </c>
-      <c r="AR67" s="27"/>
+      <c r="AR67" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="68" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
@@ -11391,7 +11416,9 @@
       <c r="AQ68" s="50">
         <v>12</v>
       </c>
-      <c r="AR68" s="27"/>
+      <c r="AR68" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="69" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
@@ -11492,7 +11519,9 @@
       <c r="AQ69" s="50">
         <v>13</v>
       </c>
-      <c r="AR69" s="27"/>
+      <c r="AR69" s="27">
+        <v>5.36</v>
+      </c>
     </row>
     <row r="70" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
@@ -11593,7 +11622,9 @@
       <c r="AQ70" s="50">
         <v>14</v>
       </c>
-      <c r="AR70" s="27"/>
+      <c r="AR70" s="27">
+        <v>6.49</v>
+      </c>
     </row>
     <row r="71" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
@@ -11694,7 +11725,9 @@
       <c r="AQ71" s="50">
         <v>15</v>
       </c>
-      <c r="AR71" s="27"/>
+      <c r="AR71" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="72" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
@@ -11795,7 +11828,9 @@
       <c r="AQ72" s="50">
         <v>16</v>
       </c>
-      <c r="AR72" s="27"/>
+      <c r="AR72" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="73" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
@@ -11896,7 +11931,9 @@
       <c r="AQ73" s="50">
         <v>17</v>
       </c>
-      <c r="AR73" s="27"/>
+      <c r="AR73" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="74" spans="1:44" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
@@ -11997,7 +12034,9 @@
       <c r="AQ74" s="50">
         <v>18</v>
       </c>
-      <c r="AR74" s="27"/>
+      <c r="AR74" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="75" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -12098,7 +12137,9 @@
       <c r="AQ75" s="50">
         <v>19</v>
       </c>
-      <c r="AR75" s="27"/>
+      <c r="AR75" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="76" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
@@ -12199,7 +12240,9 @@
       <c r="AQ76" s="50">
         <v>20</v>
       </c>
-      <c r="AR76" s="27"/>
+      <c r="AR76" s="27">
+        <v>8.98</v>
+      </c>
     </row>
     <row r="77" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -12301,6 +12344,12 @@
       <c r="AO77" s="6">
         <v>0</v>
       </c>
+      <c r="AQ77" s="53">
+        <v>21</v>
+      </c>
+      <c r="AR77" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
@@ -12402,6 +12451,12 @@
       <c r="AO78" s="6">
         <v>0</v>
       </c>
+      <c r="AQ78" s="53">
+        <v>22</v>
+      </c>
+      <c r="AR78" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
@@ -12503,6 +12558,12 @@
       <c r="AO79" s="6">
         <v>0</v>
       </c>
+      <c r="AQ79" s="53">
+        <v>23</v>
+      </c>
+      <c r="AR79" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -12604,8 +12665,14 @@
       <c r="AO80" s="6">
         <v>0</v>
       </c>
+      <c r="AQ80" s="53">
+        <v>24</v>
+      </c>
+      <c r="AR80" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>40</v>
       </c>
@@ -12705,8 +12772,14 @@
       <c r="AO81" s="6">
         <v>0</v>
       </c>
+      <c r="AQ81" s="53">
+        <v>25</v>
+      </c>
+      <c r="AR81" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -12806,8 +12879,14 @@
       <c r="AO82" s="6">
         <v>0</v>
       </c>
+      <c r="AQ82" s="53">
+        <v>26</v>
+      </c>
+      <c r="AR82" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -12907,8 +12986,14 @@
       <c r="AO83" s="6">
         <v>0</v>
       </c>
+      <c r="AQ83" s="53">
+        <v>27</v>
+      </c>
+      <c r="AR83" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -13008,8 +13093,14 @@
       <c r="AO84" s="6">
         <v>0</v>
       </c>
+      <c r="AQ84" s="53">
+        <v>28</v>
+      </c>
+      <c r="AR84" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>44</v>
       </c>
@@ -13109,8 +13200,14 @@
       <c r="AO85" s="6">
         <v>0</v>
       </c>
+      <c r="AQ85" s="53">
+        <v>29</v>
+      </c>
+      <c r="AR85" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>45</v>
       </c>
@@ -13210,8 +13307,14 @@
       <c r="AO86" s="6">
         <v>0</v>
       </c>
+      <c r="AQ86" s="53">
+        <v>30</v>
+      </c>
+      <c r="AR86" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>46</v>
       </c>
@@ -13311,8 +13414,14 @@
       <c r="AO87" s="6">
         <v>0</v>
       </c>
+      <c r="AQ87" s="53">
+        <v>31</v>
+      </c>
+      <c r="AR87" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>47</v>
       </c>
@@ -13412,8 +13521,14 @@
       <c r="AO88" s="6">
         <v>0</v>
       </c>
+      <c r="AQ88" s="53">
+        <v>32</v>
+      </c>
+      <c r="AR88" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -13513,8 +13628,14 @@
       <c r="AO89" s="6">
         <v>0</v>
       </c>
+      <c r="AQ89" s="53">
+        <v>33</v>
+      </c>
+      <c r="AR89" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>49</v>
       </c>
@@ -13614,8 +13735,14 @@
       <c r="AO90" s="6">
         <v>0</v>
       </c>
+      <c r="AQ90" s="53">
+        <v>34</v>
+      </c>
+      <c r="AR90" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>50</v>
       </c>
@@ -13715,8 +13842,14 @@
       <c r="AO91" s="6">
         <v>0</v>
       </c>
+      <c r="AQ91" s="53">
+        <v>35</v>
+      </c>
+      <c r="AR91" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>51</v>
       </c>
@@ -13816,8 +13949,14 @@
       <c r="AO92" s="6">
         <v>0</v>
       </c>
+      <c r="AQ92" s="53">
+        <v>36</v>
+      </c>
+      <c r="AR92" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>52</v>
       </c>
@@ -13917,8 +14056,14 @@
       <c r="AO93" s="6">
         <v>0</v>
       </c>
+      <c r="AQ93" s="53">
+        <v>37</v>
+      </c>
+      <c r="AR93" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>53</v>
       </c>
@@ -14018,8 +14163,14 @@
       <c r="AO94" s="6">
         <v>0</v>
       </c>
+      <c r="AQ94" s="53">
+        <v>38</v>
+      </c>
+      <c r="AR94" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>54</v>
       </c>
@@ -14119,8 +14270,14 @@
       <c r="AO95" s="6">
         <v>0</v>
       </c>
+      <c r="AQ95" s="53">
+        <v>39</v>
+      </c>
+      <c r="AR95" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>55</v>
       </c>
@@ -14220,8 +14377,14 @@
       <c r="AO96" s="6">
         <v>0</v>
       </c>
+      <c r="AQ96" s="53">
+        <v>40</v>
+      </c>
+      <c r="AR96" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -14316,8 +14479,14 @@
       <c r="AO97" s="6">
         <v>0</v>
       </c>
+      <c r="AQ97" s="53">
+        <v>41</v>
+      </c>
+      <c r="AR97" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>82</v>
       </c>
@@ -14412,8 +14581,14 @@
       <c r="AO98" s="6">
         <v>0</v>
       </c>
+      <c r="AQ98" s="53">
+        <v>42</v>
+      </c>
+      <c r="AR98" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -14508,8 +14683,14 @@
       <c r="AO99" s="6">
         <v>0</v>
       </c>
+      <c r="AQ99" s="53">
+        <v>43</v>
+      </c>
+      <c r="AR99" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>143</v>
       </c>
@@ -14567,16 +14748,22 @@
       <c r="AM100" s="6"/>
       <c r="AN100" s="6"/>
       <c r="AO100" s="6"/>
+      <c r="AQ100" s="53">
+        <v>44</v>
+      </c>
+      <c r="AR100" s="6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D106" s="56" t="s">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="D106" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="58" t="s">
+      <c r="E106" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="58"/>
-      <c r="G106" s="58" t="s">
+      <c r="F106" s="62"/>
+      <c r="G106" s="62" t="s">
         <v>77</v>
       </c>
       <c r="H106" s="63"/>
@@ -14584,81 +14771,81 @@
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="D107" s="57"/>
-      <c r="E107" s="59"/>
-      <c r="F107" s="59"/>
-      <c r="G107" s="59"/>
-      <c r="H107" s="64"/>
+    <row r="107" spans="1:44" x14ac:dyDescent="0.35">
+      <c r="D107" s="71"/>
+      <c r="E107" s="64"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="64"/>
+      <c r="H107" s="65"/>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C109" s="16">
         <v>21</v>
       </c>
       <c r="D109" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E109" s="60">
+      <c r="E109" s="68">
         <v>72154</v>
       </c>
-      <c r="F109" s="60"/>
-      <c r="G109" s="65">
+      <c r="F109" s="68"/>
+      <c r="G109" s="66">
         <v>28.1</v>
       </c>
-      <c r="H109" s="66"/>
+      <c r="H109" s="67"/>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
         <v>22</v>
       </c>
       <c r="D110" s="19">
         <v>0.31</v>
       </c>
-      <c r="E110" s="61">
+      <c r="E110" s="58">
         <v>67811</v>
       </c>
-      <c r="F110" s="61"/>
-      <c r="G110" s="67">
+      <c r="F110" s="58"/>
+      <c r="G110" s="56">
         <v>25</v>
       </c>
-      <c r="H110" s="68"/>
+      <c r="H110" s="57"/>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
         <v>23</v>
       </c>
       <c r="D111" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E111" s="61">
+      <c r="E111" s="58">
         <v>187455</v>
       </c>
-      <c r="F111" s="61"/>
-      <c r="G111" s="67">
+      <c r="F111" s="58"/>
+      <c r="G111" s="56">
         <v>70</v>
       </c>
-      <c r="H111" s="68"/>
+      <c r="H111" s="57"/>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
         <v>24</v>
       </c>
       <c r="D112" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E112" s="61">
+      <c r="E112" s="58">
         <v>63266</v>
       </c>
-      <c r="F112" s="61"/>
-      <c r="G112" s="67">
+      <c r="F112" s="58"/>
+      <c r="G112" s="56">
         <v>30.6</v>
       </c>
-      <c r="H112" s="68"/>
+      <c r="H112" s="57"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -14667,14 +14854,14 @@
       <c r="D113" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E113" s="61">
+      <c r="E113" s="58">
         <v>26553</v>
       </c>
-      <c r="F113" s="61"/>
-      <c r="G113" s="67">
+      <c r="F113" s="58"/>
+      <c r="G113" s="56">
         <v>10</v>
       </c>
-      <c r="H113" s="68"/>
+      <c r="H113" s="57"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -14683,14 +14870,14 @@
       <c r="D114" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E114" s="61">
+      <c r="E114" s="58">
         <v>24949</v>
       </c>
-      <c r="F114" s="61"/>
-      <c r="G114" s="67">
+      <c r="F114" s="58"/>
+      <c r="G114" s="56">
         <v>10</v>
       </c>
-      <c r="H114" s="68"/>
+      <c r="H114" s="57"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -14699,14 +14886,14 @@
       <c r="D115" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E115" s="61">
+      <c r="E115" s="58">
         <v>22870</v>
       </c>
-      <c r="F115" s="61"/>
-      <c r="G115" s="67">
+      <c r="F115" s="58"/>
+      <c r="G115" s="56">
         <v>10</v>
       </c>
-      <c r="H115" s="68"/>
+      <c r="H115" s="57"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -14715,14 +14902,14 @@
       <c r="D116" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E116" s="61">
+      <c r="E116" s="58">
         <v>139836</v>
       </c>
-      <c r="F116" s="61"/>
-      <c r="G116" s="67">
+      <c r="F116" s="58"/>
+      <c r="G116" s="56">
         <v>52.2</v>
       </c>
-      <c r="H116" s="68"/>
+      <c r="H116" s="57"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -14731,14 +14918,14 @@
       <c r="D117" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E117" s="61">
+      <c r="E117" s="58">
         <v>23515</v>
       </c>
-      <c r="F117" s="61"/>
-      <c r="G117" s="67">
+      <c r="F117" s="58"/>
+      <c r="G117" s="56">
         <v>10</v>
       </c>
-      <c r="H117" s="68"/>
+      <c r="H117" s="57"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -14747,14 +14934,14 @@
       <c r="D118" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E118" s="61">
+      <c r="E118" s="58">
         <v>49503</v>
       </c>
-      <c r="F118" s="61"/>
-      <c r="G118" s="67">
+      <c r="F118" s="58"/>
+      <c r="G118" s="56">
         <v>20.2</v>
       </c>
-      <c r="H118" s="68"/>
+      <c r="H118" s="57"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -14763,14 +14950,14 @@
       <c r="D119" s="19">
         <v>0.307</v>
       </c>
-      <c r="E119" s="61">
+      <c r="E119" s="58">
         <v>188420</v>
       </c>
-      <c r="F119" s="61"/>
-      <c r="G119" s="67">
+      <c r="F119" s="58"/>
+      <c r="G119" s="56">
         <v>70</v>
       </c>
-      <c r="H119" s="68"/>
+      <c r="H119" s="57"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -14779,14 +14966,14 @@
       <c r="D120" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E120" s="61">
+      <c r="E120" s="58">
         <v>26573</v>
       </c>
-      <c r="F120" s="61"/>
-      <c r="G120" s="67">
+      <c r="F120" s="58"/>
+      <c r="G120" s="56">
         <v>10.5</v>
       </c>
-      <c r="H120" s="68"/>
+      <c r="H120" s="57"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -14795,14 +14982,14 @@
       <c r="D121" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E121" s="61">
+      <c r="E121" s="58">
         <v>25253</v>
       </c>
-      <c r="F121" s="61"/>
-      <c r="G121" s="67">
+      <c r="F121" s="58"/>
+      <c r="G121" s="56">
         <v>10</v>
       </c>
-      <c r="H121" s="68"/>
+      <c r="H121" s="57"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -14811,14 +14998,14 @@
       <c r="D122" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E122" s="61">
+      <c r="E122" s="58">
         <v>17610</v>
       </c>
-      <c r="F122" s="61"/>
-      <c r="G122" s="67">
+      <c r="F122" s="58"/>
+      <c r="G122" s="56">
         <v>10</v>
       </c>
-      <c r="H122" s="68"/>
+      <c r="H122" s="57"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -14827,14 +15014,14 @@
       <c r="D123" s="19">
         <v>0.221</v>
       </c>
-      <c r="E123" s="61">
+      <c r="E123" s="58">
         <v>19372</v>
       </c>
-      <c r="F123" s="61"/>
-      <c r="G123" s="67">
+      <c r="F123" s="58"/>
+      <c r="G123" s="56">
         <v>10</v>
       </c>
-      <c r="H123" s="68"/>
+      <c r="H123" s="57"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -14843,14 +15030,14 @@
       <c r="D124" s="19">
         <v>0.216</v>
       </c>
-      <c r="E124" s="61">
+      <c r="E124" s="58">
         <v>18939</v>
       </c>
-      <c r="F124" s="61"/>
-      <c r="G124" s="67">
+      <c r="F124" s="58"/>
+      <c r="G124" s="56">
         <v>10</v>
       </c>
-      <c r="H124" s="68"/>
+      <c r="H124" s="57"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="18">
@@ -14859,14 +15046,14 @@
       <c r="D125" s="19">
         <v>0.23</v>
       </c>
-      <c r="E125" s="61">
+      <c r="E125" s="58">
         <v>20382</v>
       </c>
-      <c r="F125" s="61"/>
-      <c r="G125" s="67">
+      <c r="F125" s="58"/>
+      <c r="G125" s="56">
         <v>10.1</v>
       </c>
-      <c r="H125" s="68"/>
+      <c r="H125" s="57"/>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C126" s="18">
@@ -14875,14 +15062,14 @@
       <c r="D126" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E126" s="61">
+      <c r="E126" s="58">
         <v>19968</v>
       </c>
-      <c r="F126" s="61"/>
-      <c r="G126" s="67">
+      <c r="F126" s="58"/>
+      <c r="G126" s="56">
         <v>10.1</v>
       </c>
-      <c r="H126" s="68"/>
+      <c r="H126" s="57"/>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C127" s="18">
@@ -14891,14 +15078,14 @@
       <c r="D127" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E127" s="61">
+      <c r="E127" s="58">
         <v>23240</v>
       </c>
-      <c r="F127" s="61"/>
-      <c r="G127" s="67">
+      <c r="F127" s="58"/>
+      <c r="G127" s="56">
         <v>10</v>
       </c>
-      <c r="H127" s="68"/>
+      <c r="H127" s="57"/>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C128" s="20">
@@ -14907,25 +15094,65 @@
       <c r="D128" s="21">
         <v>0.254</v>
       </c>
-      <c r="E128" s="62">
+      <c r="E128" s="61">
         <v>26709</v>
       </c>
-      <c r="F128" s="62"/>
-      <c r="G128" s="69">
+      <c r="F128" s="61"/>
+      <c r="G128" s="59">
         <v>12</v>
       </c>
-      <c r="H128" s="70"/>
+      <c r="H128" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="AQ54:AT54"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="BH15:BI15"/>
+    <mergeCell ref="BN15:BO15"/>
+    <mergeCell ref="BF16:BJ16"/>
+    <mergeCell ref="BL16:BP16"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:F107"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="G106:H107"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="E1:F1"/>
@@ -14942,54 +15169,14 @@
     <mergeCell ref="E116:F116"/>
     <mergeCell ref="E124:F124"/>
     <mergeCell ref="E125:F125"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="G106:H107"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:F107"/>
-    <mergeCell ref="BH15:BI15"/>
-    <mergeCell ref="BN15:BO15"/>
-    <mergeCell ref="BF16:BJ16"/>
-    <mergeCell ref="BL16:BP16"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="AQ54:AT54"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
letting storage generate negative power
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -1103,9 +1103,48 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1117,47 +1156,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1443,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="CX10" sqref="CX10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V95" sqref="V95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,18 +1480,18 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="54"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
@@ -1502,11 +1502,11 @@
       <c r="Q1" s="26">
         <v>0.95</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1518,14 +1518,14 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
@@ -1537,11 +1537,11 @@
       <c r="Q2" s="26">
         <v>50</v>
       </c>
-      <c r="S2" s="54" t="s">
+      <c r="S2" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1559,11 +1559,11 @@
       <c r="F3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
       <c r="L3" s="10">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -1574,11 +1574,11 @@
       <c r="Q3" s="26">
         <v>10</v>
       </c>
-      <c r="S3" s="54" t="s">
+      <c r="S3" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1607,11 +1607,11 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="54" t="s">
+      <c r="I4" s="55" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="15">
         <v>0.75</v>
       </c>
@@ -1622,11 +1622,11 @@
       <c r="Q4" s="26">
         <v>300</v>
       </c>
-      <c r="S4" s="54" t="s">
+      <c r="S4" s="55" t="s">
         <v>96</v>
       </c>
-      <c r="T4" s="54"/>
-      <c r="U4" s="54"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1645,11 +1645,11 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="54" t="s">
+      <c r="I5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="15">
         <v>0.25</v>
       </c>
@@ -1660,11 +1660,11 @@
       <c r="Q5" s="26">
         <v>1</v>
       </c>
-      <c r="S5" s="54" t="s">
+      <c r="S5" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="T5" s="54"/>
-      <c r="U5" s="54"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="55"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1686,11 +1686,11 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="55" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="15">
         <v>1</v>
       </c>
@@ -1701,11 +1701,11 @@
       <c r="Q6" s="26">
         <v>3</v>
       </c>
-      <c r="S6" s="54" t="s">
+      <c r="S6" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="T6" s="54"/>
-      <c r="U6" s="54"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="55"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1730,11 +1730,11 @@
       <c r="Q7" s="26">
         <v>3</v>
       </c>
-      <c r="S7" s="54" t="s">
+      <c r="S7" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="T7" s="54"/>
-      <c r="U7" s="54"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="55"/>
       <c r="V7" s="27">
         <f>V4*V6</f>
         <v>29903074042.27026</v>
@@ -1756,20 +1756,20 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="I8" s="54" t="s">
+      <c r="I8" s="55" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
       <c r="L8" s="47">
         <v>15.24</v>
       </c>
       <c r="O8" s="39"/>
-      <c r="S8" s="54" t="s">
+      <c r="S8" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="T8" s="54"/>
-      <c r="U8" s="54"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
       <c r="V8" s="27">
         <f>V5*V6</f>
         <v>5911072775.7976093</v>
@@ -1787,20 +1787,20 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="I9" s="54" t="s">
+      <c r="I9" s="55" t="s">
         <v>154</v>
       </c>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="47">
         <v>9.83</v>
       </c>
       <c r="O9" s="39"/>
-      <c r="S9" s="54" t="s">
+      <c r="S9" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="T9" s="54"/>
-      <c r="U9" s="54"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
       <c r="V9" s="27">
         <v>0</v>
       </c>
@@ -1818,11 +1818,11 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
-      <c r="I10" s="54" t="s">
+      <c r="I10" s="55" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
       <c r="L10" s="27">
         <v>0.73499999999999999</v>
       </c>
@@ -1841,11 +1841,11 @@
       <c r="G11" s="6">
         <v>3780</v>
       </c>
-      <c r="I11" s="54" t="s">
+      <c r="I11" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="27">
         <v>0.65249999999999997</v>
       </c>
@@ -1859,11 +1859,11 @@
       <c r="F12" s="34"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="55" t="s">
+      <c r="I12" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
+      <c r="J12" s="72"/>
+      <c r="K12" s="72"/>
       <c r="L12" s="27">
         <v>0.81</v>
       </c>
@@ -2013,24 +2013,24 @@
       </c>
     </row>
     <row r="16" spans="2:103" x14ac:dyDescent="0.35">
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54" t="s">
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55" t="s">
         <v>173</v>
       </c>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="55"/>
+      <c r="M16" s="55"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="55"/>
+      <c r="P16" s="55"/>
       <c r="S16" s="50" t="s">
         <v>101</v>
       </c>
@@ -2103,11 +2103,11 @@
       </c>
       <c r="CT16" s="50"/>
       <c r="CU16" s="51"/>
-      <c r="CW16" s="54" t="s">
+      <c r="CW16" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="CX16" s="54"/>
-      <c r="CY16" s="54"/>
+      <c r="CX16" s="55"/>
+      <c r="CY16" s="55"/>
     </row>
     <row r="17" spans="2:103" x14ac:dyDescent="0.35">
       <c r="B17" s="42" t="s">
@@ -10872,17 +10872,17 @@
       </c>
     </row>
     <row r="47" spans="2:103" x14ac:dyDescent="0.35">
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="56" t="s">
+      <c r="H47" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
       <c r="K47" s="2"/>
       <c r="L47" s="4"/>
     </row>
@@ -11130,19 +11130,19 @@
       <c r="AO54" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AQ54" s="72" t="s">
+      <c r="AQ54" s="54" t="s">
         <v>166</v>
       </c>
-      <c r="AR54" s="72"/>
-      <c r="AS54" s="72"/>
-      <c r="AT54" s="72"/>
+      <c r="AR54" s="54"/>
+      <c r="AS54" s="54"/>
+      <c r="AT54" s="54"/>
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="C55" s="56" t="s">
+      <c r="C55" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
       <c r="G55" s="36" t="s">
         <v>130</v>
       </c>
@@ -15478,7 +15478,7 @@
         <v>41</v>
       </c>
       <c r="T97" s="6">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="V97" s="22">
         <v>41</v>
@@ -15844,26 +15844,26 @@
       </c>
     </row>
     <row r="106" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="D106" s="57" t="s">
+      <c r="D106" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="59" t="s">
+      <c r="E106" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="59"/>
-      <c r="G106" s="59" t="s">
+      <c r="F106" s="62"/>
+      <c r="G106" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H106" s="64"/>
+      <c r="H106" s="63"/>
       <c r="N106" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="D107" s="58"/>
-      <c r="E107" s="60"/>
-      <c r="F107" s="60"/>
-      <c r="G107" s="60"/>
+      <c r="D107" s="71"/>
+      <c r="E107" s="64"/>
+      <c r="F107" s="64"/>
+      <c r="G107" s="64"/>
       <c r="H107" s="65"/>
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.35">
@@ -15878,10 +15878,10 @@
       <c r="D109" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E109" s="61">
+      <c r="E109" s="68">
         <v>72154</v>
       </c>
-      <c r="F109" s="61"/>
+      <c r="F109" s="68"/>
       <c r="G109" s="66">
         <v>28.1</v>
       </c>
@@ -15894,14 +15894,14 @@
       <c r="D110" s="19">
         <v>0.31</v>
       </c>
-      <c r="E110" s="62">
+      <c r="E110" s="58">
         <v>67811</v>
       </c>
-      <c r="F110" s="62"/>
-      <c r="G110" s="68">
+      <c r="F110" s="58"/>
+      <c r="G110" s="56">
         <v>25</v>
       </c>
-      <c r="H110" s="69"/>
+      <c r="H110" s="57"/>
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -15910,14 +15910,14 @@
       <c r="D111" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E111" s="62">
+      <c r="E111" s="58">
         <v>187455</v>
       </c>
-      <c r="F111" s="62"/>
-      <c r="G111" s="68">
+      <c r="F111" s="58"/>
+      <c r="G111" s="56">
         <v>70</v>
       </c>
-      <c r="H111" s="69"/>
+      <c r="H111" s="57"/>
     </row>
     <row r="112" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -15926,14 +15926,14 @@
       <c r="D112" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E112" s="62">
+      <c r="E112" s="58">
         <v>63266</v>
       </c>
-      <c r="F112" s="62"/>
-      <c r="G112" s="68">
+      <c r="F112" s="58"/>
+      <c r="G112" s="56">
         <v>30.6</v>
       </c>
-      <c r="H112" s="69"/>
+      <c r="H112" s="57"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -15942,14 +15942,14 @@
       <c r="D113" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E113" s="62">
+      <c r="E113" s="58">
         <v>26553</v>
       </c>
-      <c r="F113" s="62"/>
-      <c r="G113" s="68">
+      <c r="F113" s="58"/>
+      <c r="G113" s="56">
         <v>10</v>
       </c>
-      <c r="H113" s="69"/>
+      <c r="H113" s="57"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -15958,14 +15958,14 @@
       <c r="D114" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E114" s="62">
+      <c r="E114" s="58">
         <v>24949</v>
       </c>
-      <c r="F114" s="62"/>
-      <c r="G114" s="68">
+      <c r="F114" s="58"/>
+      <c r="G114" s="56">
         <v>10</v>
       </c>
-      <c r="H114" s="69"/>
+      <c r="H114" s="57"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -15974,14 +15974,14 @@
       <c r="D115" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E115" s="62">
+      <c r="E115" s="58">
         <v>22870</v>
       </c>
-      <c r="F115" s="62"/>
-      <c r="G115" s="68">
+      <c r="F115" s="58"/>
+      <c r="G115" s="56">
         <v>10</v>
       </c>
-      <c r="H115" s="69"/>
+      <c r="H115" s="57"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -15990,14 +15990,14 @@
       <c r="D116" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E116" s="62">
+      <c r="E116" s="58">
         <v>139836</v>
       </c>
-      <c r="F116" s="62"/>
-      <c r="G116" s="68">
+      <c r="F116" s="58"/>
+      <c r="G116" s="56">
         <v>52.2</v>
       </c>
-      <c r="H116" s="69"/>
+      <c r="H116" s="57"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -16006,14 +16006,14 @@
       <c r="D117" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E117" s="62">
+      <c r="E117" s="58">
         <v>23515</v>
       </c>
-      <c r="F117" s="62"/>
-      <c r="G117" s="68">
+      <c r="F117" s="58"/>
+      <c r="G117" s="56">
         <v>10</v>
       </c>
-      <c r="H117" s="69"/>
+      <c r="H117" s="57"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -16022,14 +16022,14 @@
       <c r="D118" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E118" s="62">
+      <c r="E118" s="58">
         <v>49503</v>
       </c>
-      <c r="F118" s="62"/>
-      <c r="G118" s="68">
+      <c r="F118" s="58"/>
+      <c r="G118" s="56">
         <v>20.2</v>
       </c>
-      <c r="H118" s="69"/>
+      <c r="H118" s="57"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -16038,14 +16038,14 @@
       <c r="D119" s="19">
         <v>0.307</v>
       </c>
-      <c r="E119" s="62">
+      <c r="E119" s="58">
         <v>188420</v>
       </c>
-      <c r="F119" s="62"/>
-      <c r="G119" s="68">
+      <c r="F119" s="58"/>
+      <c r="G119" s="56">
         <v>70</v>
       </c>
-      <c r="H119" s="69"/>
+      <c r="H119" s="57"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -16054,14 +16054,14 @@
       <c r="D120" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E120" s="62">
+      <c r="E120" s="58">
         <v>26573</v>
       </c>
-      <c r="F120" s="62"/>
-      <c r="G120" s="68">
+      <c r="F120" s="58"/>
+      <c r="G120" s="56">
         <v>10.5</v>
       </c>
-      <c r="H120" s="69"/>
+      <c r="H120" s="57"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -16070,14 +16070,14 @@
       <c r="D121" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E121" s="62">
+      <c r="E121" s="58">
         <v>25253</v>
       </c>
-      <c r="F121" s="62"/>
-      <c r="G121" s="68">
+      <c r="F121" s="58"/>
+      <c r="G121" s="56">
         <v>10</v>
       </c>
-      <c r="H121" s="69"/>
+      <c r="H121" s="57"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -16086,14 +16086,14 @@
       <c r="D122" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E122" s="62">
+      <c r="E122" s="58">
         <v>17610</v>
       </c>
-      <c r="F122" s="62"/>
-      <c r="G122" s="68">
+      <c r="F122" s="58"/>
+      <c r="G122" s="56">
         <v>10</v>
       </c>
-      <c r="H122" s="69"/>
+      <c r="H122" s="57"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -16102,14 +16102,14 @@
       <c r="D123" s="19">
         <v>0.221</v>
       </c>
-      <c r="E123" s="62">
+      <c r="E123" s="58">
         <v>19372</v>
       </c>
-      <c r="F123" s="62"/>
-      <c r="G123" s="68">
+      <c r="F123" s="58"/>
+      <c r="G123" s="56">
         <v>10</v>
       </c>
-      <c r="H123" s="69"/>
+      <c r="H123" s="57"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -16118,14 +16118,14 @@
       <c r="D124" s="19">
         <v>0.216</v>
       </c>
-      <c r="E124" s="62">
+      <c r="E124" s="58">
         <v>18939</v>
       </c>
-      <c r="F124" s="62"/>
-      <c r="G124" s="68">
+      <c r="F124" s="58"/>
+      <c r="G124" s="56">
         <v>10</v>
       </c>
-      <c r="H124" s="69"/>
+      <c r="H124" s="57"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="18">
@@ -16134,14 +16134,14 @@
       <c r="D125" s="19">
         <v>0.23</v>
       </c>
-      <c r="E125" s="62">
+      <c r="E125" s="58">
         <v>20382</v>
       </c>
-      <c r="F125" s="62"/>
-      <c r="G125" s="68">
+      <c r="F125" s="58"/>
+      <c r="G125" s="56">
         <v>10.1</v>
       </c>
-      <c r="H125" s="69"/>
+      <c r="H125" s="57"/>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C126" s="18">
@@ -16150,14 +16150,14 @@
       <c r="D126" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E126" s="62">
+      <c r="E126" s="58">
         <v>19968</v>
       </c>
-      <c r="F126" s="62"/>
-      <c r="G126" s="68">
+      <c r="F126" s="58"/>
+      <c r="G126" s="56">
         <v>10.1</v>
       </c>
-      <c r="H126" s="69"/>
+      <c r="H126" s="57"/>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C127" s="18">
@@ -16166,14 +16166,14 @@
       <c r="D127" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E127" s="62">
+      <c r="E127" s="58">
         <v>23240</v>
       </c>
-      <c r="F127" s="62"/>
-      <c r="G127" s="68">
+      <c r="F127" s="58"/>
+      <c r="G127" s="56">
         <v>10</v>
       </c>
-      <c r="H127" s="69"/>
+      <c r="H127" s="57"/>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C128" s="20">
@@ -16182,27 +16182,63 @@
       <c r="D128" s="21">
         <v>0.254</v>
       </c>
-      <c r="E128" s="63">
+      <c r="E128" s="61">
         <v>26709</v>
       </c>
-      <c r="F128" s="63"/>
-      <c r="G128" s="70">
+      <c r="F128" s="61"/>
+      <c r="G128" s="59">
         <v>12</v>
       </c>
-      <c r="H128" s="71"/>
+      <c r="H128" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="AQ54:AT54"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="CW16:CY16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:F107"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="G106:H107"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="E1:F1"/>
@@ -16219,52 +16255,16 @@
     <mergeCell ref="E116:F116"/>
     <mergeCell ref="E124:F124"/>
     <mergeCell ref="E125:F125"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="G106:H107"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:F107"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="CW16:CY16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="AQ54:AT54"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
emissions constraints - not running
</commit_message>
<xml_diff>
--- a/717A11_data_in.xlsx
+++ b/717A11_data_in.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfi\Google Drive\School\College\Semester 6 (Spring 2020)\ENV 717\Assignments\Assignment 11 (group project)\ENV717A11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jawessel\opl\ENV717A11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1143,9 +1143,54 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,52 +1202,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1489,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1524,18 +1524,18 @@
       <c r="C1" s="6">
         <v>3</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="56" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="55"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
       <c r="L1" s="15">
         <v>7256200.8565999996</v>
       </c>
@@ -1546,11 +1546,11 @@
       <c r="Q1" s="26">
         <v>0.95</v>
       </c>
-      <c r="S1" s="55" t="s">
+      <c r="S1" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
       <c r="V1" s="24">
         <v>8809340386.1000004</v>
       </c>
@@ -1562,14 +1562,14 @@
       <c r="C2" s="6">
         <v>3</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="25"/>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
       <c r="L2" s="23">
         <f>L1*0.25</f>
         <v>1814050.2141499999</v>
@@ -1581,11 +1581,11 @@
       <c r="Q2" s="26">
         <v>50</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="S2" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
       <c r="V2" s="27">
         <v>348494.96600000001</v>
       </c>
@@ -1603,11 +1603,11 @@
       <c r="F3" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="10">
         <v>1.7000000000000001E-2</v>
       </c>
@@ -1618,11 +1618,11 @@
       <c r="Q3" s="26">
         <v>10</v>
       </c>
-      <c r="S3" s="55" t="s">
+      <c r="S3" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="T3" s="55"/>
-      <c r="U3" s="55"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
       <c r="V3" s="28">
         <v>2066077.2990000001</v>
       </c>
@@ -1651,11 +1651,11 @@
       <c r="G4" s="6">
         <v>4198</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="56" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
       <c r="L4" s="15">
         <v>0.75</v>
       </c>
@@ -1666,11 +1666,11 @@
       <c r="Q4" s="26">
         <v>300</v>
       </c>
-      <c r="S4" s="55" t="s">
+      <c r="S4" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
       <c r="V4" s="27">
         <f>0.86*2489249.757</f>
         <v>2140754.7910200004</v>
@@ -1689,11 +1689,11 @@
       <c r="G5" s="6">
         <v>3726</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
       <c r="L5" s="15">
         <v>0.25</v>
       </c>
@@ -1704,11 +1704,11 @@
       <c r="Q5" s="26">
         <v>1</v>
       </c>
-      <c r="S5" s="55" t="s">
+      <c r="S5" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="T5" s="55"/>
-      <c r="U5" s="55"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
       <c r="V5" s="27">
         <f>0.17*2489249.757</f>
         <v>423172.45869000006</v>
@@ -1730,11 +1730,11 @@
       <c r="G6" s="6">
         <v>4765</v>
       </c>
-      <c r="I6" s="55" t="s">
+      <c r="I6" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
       <c r="L6" s="15">
         <v>1</v>
       </c>
@@ -1745,11 +1745,11 @@
       <c r="Q6" s="26">
         <v>3</v>
       </c>
-      <c r="S6" s="55" t="s">
+      <c r="S6" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
       <c r="V6" s="27">
         <f>(18000/25)*8.8*2.20462</f>
         <v>13968.472320000001</v>
@@ -1774,11 +1774,11 @@
       <c r="Q7" s="26">
         <v>3</v>
       </c>
-      <c r="S7" s="55" t="s">
+      <c r="S7" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="T7" s="55"/>
-      <c r="U7" s="55"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="56"/>
       <c r="V7" s="27">
         <v>13563822358</v>
       </c>
@@ -1799,20 +1799,20 @@
       <c r="G8" s="6">
         <v>5974</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="56" t="s">
         <v>153</v>
       </c>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
       <c r="L8" s="47">
         <v>15.24</v>
       </c>
       <c r="O8" s="39"/>
-      <c r="S8" s="55" t="s">
+      <c r="S8" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="T8" s="55"/>
-      <c r="U8" s="55"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="56"/>
       <c r="V8" s="27">
         <v>2681220699</v>
       </c>
@@ -1829,20 +1829,20 @@
       <c r="G9" s="6">
         <v>5009</v>
       </c>
-      <c r="I9" s="55" t="s">
+      <c r="I9" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
       <c r="L9" s="47">
         <v>9.83</v>
       </c>
       <c r="O9" s="39"/>
-      <c r="S9" s="74" t="s">
+      <c r="S9" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
       <c r="V9" s="54">
         <v>0</v>
       </c>
@@ -1860,11 +1860,11 @@
       <c r="G10" s="6">
         <v>4359</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="56" t="s">
         <v>155</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
       <c r="L10" s="27">
         <v>0.73499999999999999</v>
       </c>
@@ -1883,11 +1883,11 @@
       <c r="G11" s="6">
         <v>3780</v>
       </c>
-      <c r="I11" s="55" t="s">
+      <c r="I11" s="56" t="s">
         <v>156</v>
       </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
       <c r="L11" s="27">
         <v>0.65249999999999997</v>
       </c>
@@ -1901,11 +1901,11 @@
       <c r="F12" s="34"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
-      <c r="I12" s="56" t="s">
+      <c r="I12" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
       <c r="L12" s="27">
         <v>0.81</v>
       </c>
@@ -2055,24 +2055,24 @@
       </c>
     </row>
     <row r="16" spans="2:103" x14ac:dyDescent="0.35">
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55" t="s">
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
       <c r="S16" s="50" t="s">
         <v>101</v>
       </c>
@@ -2145,11 +2145,11 @@
       </c>
       <c r="CT16" s="50"/>
       <c r="CU16" s="51"/>
-      <c r="CW16" s="55" t="s">
+      <c r="CW16" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="CX16" s="55"/>
-      <c r="CY16" s="55"/>
+      <c r="CX16" s="56"/>
+      <c r="CY16" s="56"/>
     </row>
     <row r="17" spans="2:103" x14ac:dyDescent="0.35">
       <c r="B17" s="42" t="s">
@@ -10914,17 +10914,17 @@
       </c>
     </row>
     <row r="47" spans="2:103" x14ac:dyDescent="0.35">
-      <c r="C47" s="57" t="s">
+      <c r="C47" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="57"/>
-      <c r="E47" s="57"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
       <c r="F47" s="2"/>
-      <c r="H47" s="57" t="s">
+      <c r="H47" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
+      <c r="I47" s="72"/>
+      <c r="J47" s="72"/>
       <c r="K47" s="2"/>
       <c r="L47" s="4"/>
     </row>
@@ -11172,19 +11172,19 @@
       <c r="AO54" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="AQ54" s="73" t="s">
+      <c r="AQ54" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="AR54" s="73"/>
-      <c r="AS54" s="73"/>
-      <c r="AT54" s="73"/>
+      <c r="AR54" s="55"/>
+      <c r="AS54" s="55"/>
+      <c r="AT54" s="55"/>
     </row>
     <row r="55" spans="1:46" x14ac:dyDescent="0.35">
-      <c r="C55" s="57" t="s">
+      <c r="C55" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="57"/>
-      <c r="E55" s="57"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
       <c r="G55" s="36" t="s">
         <v>130</v>
       </c>
@@ -15886,27 +15886,27 @@
       </c>
     </row>
     <row r="106" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="D106" s="58" t="s">
+      <c r="D106" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="E106" s="60" t="s">
+      <c r="E106" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="F106" s="60"/>
-      <c r="G106" s="60" t="s">
+      <c r="F106" s="65"/>
+      <c r="G106" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="H106" s="65"/>
+      <c r="H106" s="66"/>
       <c r="N106" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:44" x14ac:dyDescent="0.35">
-      <c r="D107" s="59"/>
-      <c r="E107" s="61"/>
-      <c r="F107" s="61"/>
-      <c r="G107" s="61"/>
-      <c r="H107" s="66"/>
+      <c r="D107" s="74"/>
+      <c r="E107" s="67"/>
+      <c r="F107" s="67"/>
+      <c r="G107" s="67"/>
+      <c r="H107" s="68"/>
     </row>
     <row r="108" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
@@ -15920,14 +15920,14 @@
       <c r="D109" s="17">
         <v>0.29299999999999998</v>
       </c>
-      <c r="E109" s="62">
+      <c r="E109" s="71">
         <v>72154</v>
       </c>
-      <c r="F109" s="62"/>
-      <c r="G109" s="67">
+      <c r="F109" s="71"/>
+      <c r="G109" s="69">
         <v>28.1</v>
       </c>
-      <c r="H109" s="68"/>
+      <c r="H109" s="70"/>
     </row>
     <row r="110" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C110" s="18">
@@ -15936,14 +15936,14 @@
       <c r="D110" s="19">
         <v>0.31</v>
       </c>
-      <c r="E110" s="63">
+      <c r="E110" s="61">
         <v>67811</v>
       </c>
-      <c r="F110" s="63"/>
-      <c r="G110" s="69">
+      <c r="F110" s="61"/>
+      <c r="G110" s="59">
         <v>25</v>
       </c>
-      <c r="H110" s="70"/>
+      <c r="H110" s="60"/>
     </row>
     <row r="111" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C111" s="18">
@@ -15952,14 +15952,14 @@
       <c r="D111" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E111" s="63">
+      <c r="E111" s="61">
         <v>187455</v>
       </c>
-      <c r="F111" s="63"/>
-      <c r="G111" s="69">
+      <c r="F111" s="61"/>
+      <c r="G111" s="59">
         <v>70</v>
       </c>
-      <c r="H111" s="70"/>
+      <c r="H111" s="60"/>
     </row>
     <row r="112" spans="1:44" x14ac:dyDescent="0.35">
       <c r="C112" s="18">
@@ -15968,14 +15968,14 @@
       <c r="D112" s="19">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E112" s="63">
+      <c r="E112" s="61">
         <v>63266</v>
       </c>
-      <c r="F112" s="63"/>
-      <c r="G112" s="69">
+      <c r="F112" s="61"/>
+      <c r="G112" s="59">
         <v>30.6</v>
       </c>
-      <c r="H112" s="70"/>
+      <c r="H112" s="60"/>
     </row>
     <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" s="18">
@@ -15984,14 +15984,14 @@
       <c r="D113" s="19">
         <v>0.30299999999999999</v>
       </c>
-      <c r="E113" s="63">
+      <c r="E113" s="61">
         <v>26553</v>
       </c>
-      <c r="F113" s="63"/>
-      <c r="G113" s="69">
+      <c r="F113" s="61"/>
+      <c r="G113" s="59">
         <v>10</v>
       </c>
-      <c r="H113" s="70"/>
+      <c r="H113" s="60"/>
     </row>
     <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" s="18">
@@ -16000,14 +16000,14 @@
       <c r="D114" s="19">
         <v>0.28499999999999998</v>
       </c>
-      <c r="E114" s="63">
+      <c r="E114" s="61">
         <v>24949</v>
       </c>
-      <c r="F114" s="63"/>
-      <c r="G114" s="69">
+      <c r="F114" s="61"/>
+      <c r="G114" s="59">
         <v>10</v>
       </c>
-      <c r="H114" s="70"/>
+      <c r="H114" s="60"/>
     </row>
     <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" s="18">
@@ -16016,14 +16016,14 @@
       <c r="D115" s="19">
         <v>0.26100000000000001</v>
       </c>
-      <c r="E115" s="63">
+      <c r="E115" s="61">
         <v>22870</v>
       </c>
-      <c r="F115" s="63"/>
-      <c r="G115" s="69">
+      <c r="F115" s="61"/>
+      <c r="G115" s="59">
         <v>10</v>
       </c>
-      <c r="H115" s="70"/>
+      <c r="H115" s="60"/>
     </row>
     <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" s="18">
@@ -16032,14 +16032,14 @@
       <c r="D116" s="19">
         <v>0.30599999999999999</v>
       </c>
-      <c r="E116" s="63">
+      <c r="E116" s="61">
         <v>139836</v>
       </c>
-      <c r="F116" s="63"/>
-      <c r="G116" s="69">
+      <c r="F116" s="61"/>
+      <c r="G116" s="59">
         <v>52.2</v>
       </c>
-      <c r="H116" s="70"/>
+      <c r="H116" s="60"/>
     </row>
     <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" s="18">
@@ -16048,14 +16048,14 @@
       <c r="D117" s="19">
         <v>0.26800000000000002</v>
       </c>
-      <c r="E117" s="63">
+      <c r="E117" s="61">
         <v>23515</v>
       </c>
-      <c r="F117" s="63"/>
-      <c r="G117" s="69">
+      <c r="F117" s="61"/>
+      <c r="G117" s="59">
         <v>10</v>
       </c>
-      <c r="H117" s="70"/>
+      <c r="H117" s="60"/>
     </row>
     <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" s="18">
@@ -16064,14 +16064,14 @@
       <c r="D118" s="19">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E118" s="63">
+      <c r="E118" s="61">
         <v>49503</v>
       </c>
-      <c r="F118" s="63"/>
-      <c r="G118" s="69">
+      <c r="F118" s="61"/>
+      <c r="G118" s="59">
         <v>20.2</v>
       </c>
-      <c r="H118" s="70"/>
+      <c r="H118" s="60"/>
     </row>
     <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" s="18">
@@ -16080,14 +16080,14 @@
       <c r="D119" s="19">
         <v>0.307</v>
       </c>
-      <c r="E119" s="63">
+      <c r="E119" s="61">
         <v>188420</v>
       </c>
-      <c r="F119" s="63"/>
-      <c r="G119" s="69">
+      <c r="F119" s="61"/>
+      <c r="G119" s="59">
         <v>70</v>
       </c>
-      <c r="H119" s="70"/>
+      <c r="H119" s="60"/>
     </row>
     <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" s="18">
@@ -16096,14 +16096,14 @@
       <c r="D120" s="19">
         <v>0.28899999999999998</v>
       </c>
-      <c r="E120" s="63">
+      <c r="E120" s="61">
         <v>26573</v>
       </c>
-      <c r="F120" s="63"/>
-      <c r="G120" s="69">
+      <c r="F120" s="61"/>
+      <c r="G120" s="59">
         <v>10.5</v>
       </c>
-      <c r="H120" s="70"/>
+      <c r="H120" s="60"/>
     </row>
     <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" s="18">
@@ -16112,14 +16112,14 @@
       <c r="D121" s="19">
         <v>0.28799999999999998</v>
       </c>
-      <c r="E121" s="63">
+      <c r="E121" s="61">
         <v>25253</v>
       </c>
-      <c r="F121" s="63"/>
-      <c r="G121" s="69">
+      <c r="F121" s="61"/>
+      <c r="G121" s="59">
         <v>10</v>
       </c>
-      <c r="H121" s="70"/>
+      <c r="H121" s="60"/>
     </row>
     <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" s="18">
@@ -16128,14 +16128,14 @@
       <c r="D122" s="19">
         <v>0.20100000000000001</v>
       </c>
-      <c r="E122" s="63">
+      <c r="E122" s="61">
         <v>17610</v>
       </c>
-      <c r="F122" s="63"/>
-      <c r="G122" s="69">
+      <c r="F122" s="61"/>
+      <c r="G122" s="59">
         <v>10</v>
       </c>
-      <c r="H122" s="70"/>
+      <c r="H122" s="60"/>
     </row>
     <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" s="18">
@@ -16144,14 +16144,14 @@
       <c r="D123" s="19">
         <v>0.221</v>
       </c>
-      <c r="E123" s="63">
+      <c r="E123" s="61">
         <v>19372</v>
       </c>
-      <c r="F123" s="63"/>
-      <c r="G123" s="69">
+      <c r="F123" s="61"/>
+      <c r="G123" s="59">
         <v>10</v>
       </c>
-      <c r="H123" s="70"/>
+      <c r="H123" s="60"/>
     </row>
     <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" s="18">
@@ -16160,14 +16160,14 @@
       <c r="D124" s="19">
         <v>0.216</v>
       </c>
-      <c r="E124" s="63">
+      <c r="E124" s="61">
         <v>18939</v>
       </c>
-      <c r="F124" s="63"/>
-      <c r="G124" s="69">
+      <c r="F124" s="61"/>
+      <c r="G124" s="59">
         <v>10</v>
       </c>
-      <c r="H124" s="70"/>
+      <c r="H124" s="60"/>
     </row>
     <row r="125" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C125" s="18">
@@ -16176,14 +16176,14 @@
       <c r="D125" s="19">
         <v>0.23</v>
       </c>
-      <c r="E125" s="63">
+      <c r="E125" s="61">
         <v>20382</v>
       </c>
-      <c r="F125" s="63"/>
-      <c r="G125" s="69">
+      <c r="F125" s="61"/>
+      <c r="G125" s="59">
         <v>10.1</v>
       </c>
-      <c r="H125" s="70"/>
+      <c r="H125" s="60"/>
     </row>
     <row r="126" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C126" s="18">
@@ -16192,14 +16192,14 @@
       <c r="D126" s="19">
         <v>0.22600000000000001</v>
       </c>
-      <c r="E126" s="63">
+      <c r="E126" s="61">
         <v>19968</v>
       </c>
-      <c r="F126" s="63"/>
-      <c r="G126" s="69">
+      <c r="F126" s="61"/>
+      <c r="G126" s="59">
         <v>10.1</v>
       </c>
-      <c r="H126" s="70"/>
+      <c r="H126" s="60"/>
     </row>
     <row r="127" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C127" s="18">
@@ -16208,14 +16208,14 @@
       <c r="D127" s="19">
         <v>0.26500000000000001</v>
       </c>
-      <c r="E127" s="63">
+      <c r="E127" s="61">
         <v>23240</v>
       </c>
-      <c r="F127" s="63"/>
-      <c r="G127" s="69">
+      <c r="F127" s="61"/>
+      <c r="G127" s="59">
         <v>10</v>
       </c>
-      <c r="H127" s="70"/>
+      <c r="H127" s="60"/>
     </row>
     <row r="128" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C128" s="20">
@@ -16228,23 +16228,59 @@
         <v>26709</v>
       </c>
       <c r="F128" s="64"/>
-      <c r="G128" s="71">
+      <c r="G128" s="62">
         <v>12</v>
       </c>
-      <c r="H128" s="72"/>
+      <c r="H128" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="AQ54:AT54"/>
-    <mergeCell ref="S1:U1"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="S6:U6"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="CW16:CY16"/>
+    <mergeCell ref="J16:P16"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="D106:D107"/>
+    <mergeCell ref="E106:F107"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="E127:F127"/>
+    <mergeCell ref="E128:F128"/>
+    <mergeCell ref="G106:H107"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="E122:F122"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="E1:F1"/>
@@ -16261,52 +16297,16 @@
     <mergeCell ref="E116:F116"/>
     <mergeCell ref="E124:F124"/>
     <mergeCell ref="E125:F125"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="E127:F127"/>
-    <mergeCell ref="E128:F128"/>
-    <mergeCell ref="G106:H107"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="E122:F122"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="D106:D107"/>
-    <mergeCell ref="E106:F107"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="CW16:CY16"/>
-    <mergeCell ref="J16:P16"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="AQ54:AT54"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="S6:U6"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S9:U9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>